<commit_message>
Change '*' to '+' for number of options choices if >0
</commit_message>
<xml_diff>
--- a/media/questions.xlsx
+++ b/media/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ju5315jo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4AB1695-0CCC-4B82-953E-777A309B850F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADEB1DD-13A5-490B-B8B0-716EC3F139B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>1a</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
   <si>
     <t>1c</t>
@@ -908,6 +905,9 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1740,6 +1740,18 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2057,8 +2069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF3ACC6-6455-42D3-BCE3-944B33DD47DC}">
   <dimension ref="A1:AC248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2111,22 +2123,22 @@
         <v>8</v>
       </c>
       <c r="J1" s="115" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="116" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="116" t="s">
+      <c r="L1" s="115" t="s">
+        <v>195</v>
+      </c>
+      <c r="M1" s="115" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="115" t="s">
-        <v>196</v>
-      </c>
-      <c r="M1" s="115" t="s">
+      <c r="N1" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="116" t="s">
+      <c r="O1" s="116" t="s">
         <v>54</v>
-      </c>
-      <c r="O1" s="116" t="s">
-        <v>55</v>
       </c>
       <c r="P1" s="15"/>
       <c r="Q1" s="14"/>
@@ -2148,7 +2160,7 @@
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
@@ -2156,22 +2168,22 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="117" t="s">
+        <v>199</v>
+      </c>
+      <c r="K2" s="118" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="118" t="s">
         <v>200</v>
       </c>
-      <c r="K2" s="118" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="118" t="s">
+      <c r="M2" s="118" t="s">
         <v>201</v>
       </c>
-      <c r="M2" s="118" t="s">
+      <c r="N2" s="119" t="s">
         <v>202</v>
       </c>
-      <c r="N2" s="119" t="s">
+      <c r="O2" s="118" t="s">
         <v>203</v>
-      </c>
-      <c r="O2" s="118" t="s">
-        <v>204</v>
       </c>
       <c r="P2" s="9"/>
       <c r="Q2" s="8"/>
@@ -2199,22 +2211,22 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="110" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K3" s="110" t="s">
+        <v>204</v>
+      </c>
+      <c r="L3" s="110" t="s">
         <v>205</v>
       </c>
-      <c r="L3" s="110" t="s">
+      <c r="M3" s="110" t="s">
         <v>206</v>
       </c>
-      <c r="M3" s="110" t="s">
-        <v>207</v>
-      </c>
       <c r="N3" s="110" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O3" s="111" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="1"/>
@@ -2243,7 +2255,7 @@
       </c>
       <c r="D4" s="56"/>
       <c r="E4" s="100" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="32" t="s">
         <v>10</v>
@@ -2468,7 +2480,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="131" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
@@ -2692,7 +2704,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
@@ -2918,7 +2930,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G22" s="31"/>
       <c r="H22" s="31"/>
@@ -3144,7 +3156,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="120" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G28" s="31"/>
       <c r="H28" s="31"/>
@@ -3376,7 +3388,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="120" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -3604,7 +3616,7 @@
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G40" s="31"/>
       <c r="H40" s="31"/>
@@ -3808,7 +3820,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="121" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G46" s="31"/>
       <c r="H46" s="31"/>
@@ -4038,20 +4050,20 @@
         <v>15</v>
       </c>
       <c r="B52" s="123" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52" s="62">
         <v>1</v>
       </c>
       <c r="D52" s="177" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
       <c r="G52" s="18"/>
       <c r="H52" s="18"/>
       <c r="I52" s="127" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J52" s="158"/>
       <c r="K52" s="159"/>
@@ -4079,14 +4091,14 @@
       <c r="B53" s="77"/>
       <c r="C53" s="77"/>
       <c r="D53" s="96" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
       <c r="G53" s="18"/>
       <c r="H53" s="18"/>
       <c r="I53" s="128" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J53" s="158"/>
       <c r="K53" s="159"/>
@@ -4119,7 +4131,7 @@
       <c r="G54" s="18"/>
       <c r="H54" s="18"/>
       <c r="I54" s="129" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J54" s="158"/>
       <c r="K54" s="159"/>
@@ -4152,7 +4164,7 @@
       <c r="G55" s="18"/>
       <c r="H55" s="18"/>
       <c r="I55" s="129" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J55" s="158"/>
       <c r="K55" s="159"/>
@@ -4177,25 +4189,25 @@
     </row>
     <row r="56" spans="1:29" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A56" s="29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B56" s="122" t="s">
-        <v>60</v>
-      </c>
-      <c r="C56" s="54" t="s">
-        <v>16</v>
+        <v>59</v>
+      </c>
+      <c r="C56" s="186" t="s">
+        <v>262</v>
       </c>
       <c r="D56" s="97" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F56" s="78"/>
       <c r="G56" s="78"/>
       <c r="H56" s="31"/>
       <c r="I56" s="120" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J56" s="161"/>
       <c r="K56" s="162"/>
@@ -4221,12 +4233,12 @@
     <row r="57" spans="1:29" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A57" s="27"/>
       <c r="D57" s="97" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E57" s="11"/>
       <c r="H57" s="13"/>
       <c r="I57" s="124" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J57" s="158"/>
       <c r="K57" s="165"/>
@@ -4257,7 +4269,7 @@
       <c r="E58" s="1"/>
       <c r="H58" s="11"/>
       <c r="I58" s="125" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J58" s="158"/>
       <c r="K58" s="165"/>
@@ -4290,7 +4302,7 @@
       <c r="G59" s="22"/>
       <c r="H59" s="66"/>
       <c r="I59" s="126" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J59" s="167"/>
       <c r="K59" s="168"/>
@@ -4315,25 +4327,25 @@
     </row>
     <row r="60" spans="1:29" ht="42" x14ac:dyDescent="0.3">
       <c r="A60" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B60" s="130" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="187" t="s">
+        <v>262</v>
+      </c>
+      <c r="D60" s="99" t="s">
+        <v>251</v>
+      </c>
+      <c r="E60" s="34" t="s">
         <v>70</v>
-      </c>
-      <c r="C60" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D60" s="99" t="s">
-        <v>252</v>
-      </c>
-      <c r="E60" s="34" t="s">
-        <v>71</v>
       </c>
       <c r="F60" s="64"/>
       <c r="G60" s="64"/>
       <c r="H60" s="34"/>
       <c r="I60" s="133" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J60" s="158"/>
       <c r="K60" s="171"/>
@@ -4359,12 +4371,12 @@
     <row r="61" spans="1:29" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A61" s="27"/>
       <c r="D61" s="99" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E61" s="11"/>
       <c r="H61" s="11"/>
       <c r="I61" s="125" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J61" s="158"/>
       <c r="K61" s="165"/>
@@ -4395,7 +4407,7 @@
       <c r="E62" s="1"/>
       <c r="H62" s="11"/>
       <c r="I62" s="125" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J62" s="158"/>
       <c r="K62" s="165"/>
@@ -4426,7 +4438,7 @@
       <c r="E63" s="1"/>
       <c r="H63" s="13"/>
       <c r="I63" s="124" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J63" s="158"/>
       <c r="K63" s="165"/>
@@ -4457,7 +4469,7 @@
       <c r="E64" s="1"/>
       <c r="H64" s="11"/>
       <c r="I64" s="125" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J64" s="158"/>
       <c r="K64" s="165"/>
@@ -4490,7 +4502,7 @@
       <c r="G65" s="75"/>
       <c r="H65" s="66"/>
       <c r="I65" s="126" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J65" s="172"/>
       <c r="K65" s="173"/>
@@ -4515,25 +4527,25 @@
     </row>
     <row r="66" spans="1:29" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A66" s="27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B66" s="123" t="s">
-        <v>77</v>
-      </c>
-      <c r="C66" s="56" t="s">
-        <v>16</v>
+        <v>76</v>
+      </c>
+      <c r="C66" s="188" t="s">
+        <v>262</v>
       </c>
       <c r="D66" s="98" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E66" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F66" s="64"/>
       <c r="G66" s="64"/>
       <c r="H66" s="35"/>
       <c r="I66" s="128" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J66" s="158"/>
       <c r="K66" s="159"/>
@@ -4561,12 +4573,12 @@
       <c r="B67" s="11"/>
       <c r="C67" s="11"/>
       <c r="D67" s="98" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E67" s="11"/>
       <c r="H67" s="13"/>
       <c r="I67" s="124" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J67" s="158"/>
       <c r="K67" s="166"/>
@@ -4597,7 +4609,7 @@
       <c r="E68" s="11"/>
       <c r="H68" s="11"/>
       <c r="I68" s="125" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J68" s="158"/>
       <c r="K68" s="166"/>
@@ -4628,7 +4640,7 @@
       <c r="E69" s="1"/>
       <c r="H69" s="13"/>
       <c r="I69" s="124" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J69" s="158"/>
       <c r="K69" s="166"/>
@@ -4659,7 +4671,7 @@
       <c r="E70" s="1"/>
       <c r="H70" s="13"/>
       <c r="I70" s="124" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J70" s="158"/>
       <c r="K70" s="166"/>
@@ -4690,7 +4702,7 @@
       <c r="E71" s="1"/>
       <c r="H71" s="13"/>
       <c r="I71" s="124" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J71" s="158"/>
       <c r="K71" s="166"/>
@@ -4721,7 +4733,7 @@
       <c r="E72" s="1"/>
       <c r="H72" s="11"/>
       <c r="I72" s="125" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J72" s="158"/>
       <c r="K72" s="166"/>
@@ -4746,23 +4758,23 @@
     </row>
     <row r="73" spans="1:29" ht="42" x14ac:dyDescent="0.3">
       <c r="A73" s="29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B73" s="122" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C73" s="55">
         <v>1</v>
       </c>
       <c r="D73" s="96" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E73" s="26"/>
       <c r="F73" s="78"/>
       <c r="G73" s="78"/>
       <c r="H73" s="32"/>
       <c r="I73" s="134" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J73" s="161"/>
       <c r="K73" s="163"/>
@@ -4790,14 +4802,14 @@
       <c r="B74" s="18"/>
       <c r="C74" s="18"/>
       <c r="D74" s="96" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E74" s="18"/>
       <c r="F74" s="64"/>
       <c r="G74" s="64"/>
       <c r="H74" s="34"/>
       <c r="I74" s="133" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J74" s="158"/>
       <c r="K74" s="159"/>
@@ -4830,7 +4842,7 @@
       <c r="G75" s="22"/>
       <c r="H75" s="106"/>
       <c r="I75" s="135" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J75" s="167"/>
       <c r="K75" s="169"/>
@@ -4855,19 +4867,19 @@
     </row>
     <row r="76" spans="1:29" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A76" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B76" s="136" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="107" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E76" s="1"/>
       <c r="H76" s="11"/>
       <c r="I76" s="125" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J76" s="158"/>
       <c r="K76" s="166"/>
@@ -4895,12 +4907,12 @@
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="107" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E77" s="1"/>
       <c r="H77" s="11"/>
       <c r="I77" s="125" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J77" s="158"/>
       <c r="K77" s="166"/>
@@ -4931,7 +4943,7 @@
       <c r="E78" s="1"/>
       <c r="H78" s="11"/>
       <c r="I78" s="125" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J78" s="158"/>
       <c r="K78" s="166"/>
@@ -4959,20 +4971,20 @@
         <v>2</v>
       </c>
       <c r="B79" s="51" t="s">
-        <v>218</v>
-      </c>
-      <c r="C79" s="51" t="s">
-        <v>16</v>
+        <v>217</v>
+      </c>
+      <c r="C79" s="189" t="s">
+        <v>262</v>
       </c>
       <c r="D79" s="51"/>
       <c r="E79" s="34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F79" s="78"/>
       <c r="G79" s="78"/>
       <c r="H79" s="31"/>
       <c r="I79" s="120" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J79" s="43">
         <v>1</v>
@@ -5010,7 +5022,7 @@
       <c r="E80" s="11"/>
       <c r="H80" s="13"/>
       <c r="I80" s="124" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J80" s="44"/>
       <c r="K80" s="2"/>
@@ -5049,7 +5061,7 @@
       <c r="E81" s="1"/>
       <c r="H81" s="13"/>
       <c r="I81" s="124" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J81" s="44">
         <v>1</v>
@@ -5086,7 +5098,7 @@
       <c r="E82" s="1"/>
       <c r="H82" s="13"/>
       <c r="I82" s="124" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J82" s="44"/>
       <c r="K82" s="2"/>
@@ -5123,7 +5135,7 @@
       <c r="E83" s="1"/>
       <c r="H83" s="13"/>
       <c r="I83" s="124" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J83" s="44">
         <v>1</v>
@@ -5158,7 +5170,7 @@
       <c r="E84" s="1"/>
       <c r="H84" s="13"/>
       <c r="I84" s="124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J84" s="44"/>
       <c r="K84" s="2"/>
@@ -5186,7 +5198,7 @@
         <v>3</v>
       </c>
       <c r="B85" s="137" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C85" s="51"/>
       <c r="D85" s="51"/>
@@ -5195,7 +5207,7 @@
       <c r="G85" s="78"/>
       <c r="H85" s="23"/>
       <c r="I85" s="120" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J85" s="43">
         <v>1</v>
@@ -5230,7 +5242,7 @@
       <c r="E86" s="1"/>
       <c r="H86" s="17"/>
       <c r="I86" s="124" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J86" s="44"/>
       <c r="K86" s="2"/>
@@ -5267,7 +5279,7 @@
       <c r="E87" s="1"/>
       <c r="H87" s="17"/>
       <c r="I87" s="124" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J87" s="44"/>
       <c r="K87" s="2"/>
@@ -5304,7 +5316,7 @@
       <c r="E88" s="1"/>
       <c r="H88" s="17"/>
       <c r="I88" s="124" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J88" s="44"/>
       <c r="K88" s="2"/>
@@ -5337,7 +5349,7 @@
       <c r="E89" s="1"/>
       <c r="H89" s="17"/>
       <c r="I89" s="124" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J89" s="44"/>
       <c r="K89" s="2"/>
@@ -5372,7 +5384,7 @@
       <c r="E90" s="1"/>
       <c r="H90" s="17"/>
       <c r="I90" s="124" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J90" s="44"/>
       <c r="K90" s="2"/>
@@ -5407,7 +5419,7 @@
       <c r="E91" s="1"/>
       <c r="H91" s="17"/>
       <c r="I91" s="124" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J91" s="44"/>
       <c r="K91" s="2"/>
@@ -5437,24 +5449,24 @@
         <v>4</v>
       </c>
       <c r="B92" s="122" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C92" s="51"/>
       <c r="D92" s="53"/>
       <c r="E92" s="132" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F92" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="G92" s="185" t="s">
+        <v>261</v>
+      </c>
+      <c r="H92" s="120" t="s">
         <v>100</v>
       </c>
-      <c r="G92" s="185" t="s">
-        <v>262</v>
-      </c>
-      <c r="H92" s="120" t="s">
-        <v>101</v>
-      </c>
       <c r="I92" s="120" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J92" s="43">
         <v>1</v>
@@ -5486,7 +5498,7 @@
       <c r="E93" s="1"/>
       <c r="H93" s="14"/>
       <c r="I93" s="124" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J93" s="44">
         <v>1</v>
@@ -5521,7 +5533,7 @@
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
       <c r="I94" s="124" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J94" s="44">
         <v>1</v>
@@ -5558,7 +5570,7 @@
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
       <c r="I95" s="124" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J95" s="44">
         <v>1</v>
@@ -5595,7 +5607,7 @@
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
       <c r="I96" s="124" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J96" s="44"/>
       <c r="K96" s="2"/>
@@ -5630,7 +5642,7 @@
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
       <c r="I97" s="124" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J97" s="44">
         <v>1</v>
@@ -5665,7 +5677,7 @@
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
       <c r="I98" s="124" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J98" s="44">
         <v>1</v>
@@ -5702,7 +5714,7 @@
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
       <c r="I99" s="124" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J99" s="44">
         <v>1</v>
@@ -5737,7 +5749,7 @@
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
       <c r="I100" s="124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J100" s="44">
         <v>1</v>
@@ -5774,7 +5786,7 @@
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
       <c r="I101" s="124" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J101" s="44">
         <v>1</v>
@@ -5809,7 +5821,7 @@
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
       <c r="I102" s="124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J102" s="44"/>
       <c r="K102" s="2">
@@ -5844,7 +5856,7 @@
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
       <c r="I103" s="124" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J103" s="44">
         <v>1</v>
@@ -5881,7 +5893,7 @@
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
       <c r="I104" s="124" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J104" s="44">
         <v>1</v>
@@ -5918,7 +5930,7 @@
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
       <c r="I105" s="124" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J105" s="44">
         <v>1</v>
@@ -5955,7 +5967,7 @@
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
       <c r="I106" s="124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J106" s="44"/>
       <c r="K106" s="2"/>
@@ -5985,14 +5997,14 @@
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="54" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G107" s="1"/>
       <c r="H107" s="120" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I107" s="120" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J107" s="151">
         <v>1</v>
@@ -6026,10 +6038,10 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I108" s="124" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J108" s="154">
         <v>1</v>
@@ -6064,7 +6076,7 @@
       <c r="G109" s="1"/>
       <c r="H109" s="12"/>
       <c r="I109" s="124" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J109" s="154">
         <v>1</v>
@@ -6099,7 +6111,7 @@
       <c r="G110" s="1"/>
       <c r="H110" s="12"/>
       <c r="I110" s="124" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J110" s="154">
         <v>1</v>
@@ -6134,7 +6146,7 @@
       <c r="G111" s="1"/>
       <c r="H111" s="12"/>
       <c r="I111" s="124" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J111" s="154">
         <v>1</v>
@@ -6169,7 +6181,7 @@
       <c r="G112" s="1"/>
       <c r="H112" s="12"/>
       <c r="I112" s="124" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J112" s="154">
         <v>1</v>
@@ -6204,7 +6216,7 @@
       <c r="G113" s="1"/>
       <c r="H113" s="12"/>
       <c r="I113" s="124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J113" s="154"/>
       <c r="K113" s="155">
@@ -6239,7 +6251,7 @@
       <c r="G114" s="1"/>
       <c r="H114" s="12"/>
       <c r="I114" s="124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J114" s="154">
         <v>1</v>
@@ -6276,7 +6288,7 @@
       <c r="G115" s="1"/>
       <c r="H115" s="12"/>
       <c r="I115" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J115" s="154">
         <v>1</v>
@@ -6311,7 +6323,7 @@
       <c r="G116" s="1"/>
       <c r="H116" s="12"/>
       <c r="I116" s="124" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J116" s="154">
         <v>1</v>
@@ -6348,7 +6360,7 @@
       <c r="G117" s="1"/>
       <c r="H117" s="12"/>
       <c r="I117" s="124" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J117" s="154">
         <v>1</v>
@@ -6385,7 +6397,7 @@
       <c r="G118" s="1"/>
       <c r="H118" s="12"/>
       <c r="I118" s="124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J118" s="154"/>
       <c r="K118" s="155"/>
@@ -6415,14 +6427,14 @@
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="138" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G119" s="55"/>
       <c r="H119" s="120" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I119" s="120" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J119" s="43"/>
       <c r="K119" s="24"/>
@@ -6459,7 +6471,7 @@
       <c r="G120" s="17"/>
       <c r="H120" s="17"/>
       <c r="I120" s="124" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J120" s="44"/>
       <c r="K120" s="2"/>
@@ -6498,7 +6510,7 @@
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
       <c r="I121" s="124" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J121" s="44"/>
       <c r="K121" s="2"/>
@@ -6537,7 +6549,7 @@
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
       <c r="I122" s="124" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J122" s="44"/>
       <c r="K122" s="2"/>
@@ -6576,7 +6588,7 @@
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
       <c r="I123" s="124" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J123" s="44"/>
       <c r="K123" s="2"/>
@@ -6615,7 +6627,7 @@
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
       <c r="I124" s="124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J124" s="44"/>
       <c r="K124" s="2"/>
@@ -6652,7 +6664,7 @@
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
       <c r="I125" s="124" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J125" s="44"/>
       <c r="K125" s="2"/>
@@ -6691,7 +6703,7 @@
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
       <c r="I126" s="124" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J126" s="44"/>
       <c r="K126" s="2">
@@ -6726,7 +6738,7 @@
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
       <c r="I127" s="124" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J127" s="44"/>
       <c r="K127" s="2">
@@ -6763,7 +6775,7 @@
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
       <c r="I128" s="124" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J128" s="44"/>
       <c r="K128" s="2"/>
@@ -6802,7 +6814,7 @@
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
       <c r="I129" s="124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J129" s="44"/>
       <c r="K129" s="2">
@@ -6837,7 +6849,7 @@
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
       <c r="I130" s="124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J130" s="44"/>
       <c r="K130" s="2"/>
@@ -6867,14 +6879,14 @@
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
       <c r="F131" s="122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G131" s="54"/>
       <c r="H131" s="120" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I131" s="120" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J131" s="43"/>
       <c r="K131" s="24"/>
@@ -6911,7 +6923,7 @@
       <c r="G132" s="17"/>
       <c r="H132" s="17"/>
       <c r="I132" s="124" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J132" s="44"/>
       <c r="K132" s="2"/>
@@ -6948,7 +6960,7 @@
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
       <c r="I133" s="124" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J133" s="44"/>
       <c r="K133" s="2"/>
@@ -6985,7 +6997,7 @@
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
       <c r="I134" s="124" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J134" s="44"/>
       <c r="K134" s="2"/>
@@ -7022,7 +7034,7 @@
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
       <c r="I135" s="124" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J135" s="44"/>
       <c r="K135" s="2"/>
@@ -7057,7 +7069,7 @@
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
       <c r="I136" s="124" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J136" s="44"/>
       <c r="K136" s="2"/>
@@ -7092,7 +7104,7 @@
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
       <c r="I137" s="124" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J137" s="44"/>
       <c r="K137" s="2"/>
@@ -7131,7 +7143,7 @@
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
       <c r="I138" s="124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J138" s="44"/>
       <c r="K138" s="2">
@@ -7166,7 +7178,7 @@
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
       <c r="I139" s="124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J139" s="44"/>
       <c r="K139" s="2"/>
@@ -7203,7 +7215,7 @@
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
       <c r="I140" s="124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J140" s="44"/>
       <c r="K140" s="2"/>
@@ -7233,14 +7245,14 @@
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="138" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G141" s="55"/>
       <c r="H141" s="120" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I141" s="120" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J141" s="43"/>
       <c r="K141" s="24"/>
@@ -7277,7 +7289,7 @@
       <c r="G142" s="17"/>
       <c r="H142" s="17"/>
       <c r="I142" s="124" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J142" s="44"/>
       <c r="K142" s="2"/>
@@ -7316,7 +7328,7 @@
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
       <c r="I143" s="124" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J143" s="44"/>
       <c r="K143" s="2"/>
@@ -7353,7 +7365,7 @@
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
       <c r="I144" s="124" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J144" s="44"/>
       <c r="K144" s="2"/>
@@ -7390,7 +7402,7 @@
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
       <c r="I145" s="124" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J145" s="44"/>
       <c r="K145" s="2"/>
@@ -7425,7 +7437,7 @@
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
       <c r="I146" s="124" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J146" s="44"/>
       <c r="K146" s="2"/>
@@ -7460,7 +7472,7 @@
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
       <c r="I147" s="124" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J147" s="44"/>
       <c r="K147" s="2"/>
@@ -7495,7 +7507,7 @@
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
       <c r="I148" s="124" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J148" s="44"/>
       <c r="K148" s="2"/>
@@ -7530,7 +7542,7 @@
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
       <c r="I149" s="124" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J149" s="44"/>
       <c r="K149" s="2"/>
@@ -7567,7 +7579,7 @@
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
       <c r="I150" s="124" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J150" s="44"/>
       <c r="K150" s="2">
@@ -7604,7 +7616,7 @@
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
       <c r="I151" s="124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J151" s="44"/>
       <c r="K151" s="2">
@@ -7639,7 +7651,7 @@
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
       <c r="I152" s="124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J152" s="44"/>
       <c r="K152" s="2"/>
@@ -7676,7 +7688,7 @@
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
       <c r="I153" s="124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J153" s="44"/>
       <c r="K153" s="2"/>
@@ -7706,14 +7718,14 @@
       <c r="D154" s="18"/>
       <c r="E154" s="18"/>
       <c r="F154" s="137" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G154" s="51"/>
       <c r="H154" s="120" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I154" s="120" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J154" s="43"/>
       <c r="K154" s="24"/>
@@ -7746,7 +7758,7 @@
       <c r="E155" s="1"/>
       <c r="H155" s="17"/>
       <c r="I155" s="124" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J155" s="44"/>
       <c r="K155" s="2"/>
@@ -7783,7 +7795,7 @@
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
       <c r="I156" s="124" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J156" s="44"/>
       <c r="K156" s="2"/>
@@ -7818,7 +7830,7 @@
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
       <c r="I157" s="124" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J157" s="44"/>
       <c r="K157" s="2"/>
@@ -7853,7 +7865,7 @@
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
       <c r="I158" s="124" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J158" s="44"/>
       <c r="K158" s="2"/>
@@ -7888,7 +7900,7 @@
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
       <c r="I159" s="124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J159" s="44"/>
       <c r="K159" s="2">
@@ -7923,7 +7935,7 @@
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
       <c r="I160" s="124" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J160" s="44"/>
       <c r="K160" s="2"/>
@@ -7960,7 +7972,7 @@
       <c r="G161" s="63"/>
       <c r="H161" s="63"/>
       <c r="I161" s="124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J161" s="67"/>
       <c r="K161" s="68"/>
@@ -7988,22 +8000,22 @@
         <v>5</v>
       </c>
       <c r="B162" s="123" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C162" s="56">
         <v>3</v>
       </c>
       <c r="D162" s="98" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E162" s="128" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F162" s="18"/>
       <c r="G162" s="18"/>
       <c r="H162" s="18"/>
       <c r="I162" s="128" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J162" s="44"/>
       <c r="K162" s="36"/>
@@ -8031,14 +8043,14 @@
       <c r="B163" s="13"/>
       <c r="C163" s="13"/>
       <c r="D163" s="98" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E163" s="13"/>
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
       <c r="I163" s="124" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J163" s="44"/>
       <c r="K163" s="2"/>
@@ -8071,7 +8083,7 @@
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
       <c r="I164" s="124" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J164" s="44"/>
       <c r="K164" s="2"/>
@@ -8104,7 +8116,7 @@
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
       <c r="I165" s="124" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J165" s="44"/>
       <c r="K165" s="2"/>
@@ -8137,7 +8149,7 @@
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
       <c r="I166" s="124" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J166" s="44"/>
       <c r="K166" s="2"/>
@@ -8170,7 +8182,7 @@
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
       <c r="I167" s="124" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J167" s="44"/>
       <c r="K167" s="2"/>
@@ -8203,7 +8215,7 @@
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
       <c r="I168" s="124" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J168" s="44"/>
       <c r="K168" s="2"/>
@@ -8236,7 +8248,7 @@
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
       <c r="I169" s="139" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J169" s="44"/>
       <c r="K169" s="2"/>
@@ -8269,7 +8281,7 @@
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
       <c r="I170" s="124" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J170" s="44"/>
       <c r="K170" s="2"/>
@@ -8302,7 +8314,7 @@
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
       <c r="I171" s="124" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J171" s="44"/>
       <c r="K171" s="2"/>
@@ -8335,7 +8347,7 @@
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
       <c r="I172" s="124" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J172" s="44"/>
       <c r="K172" s="2"/>
@@ -8368,7 +8380,7 @@
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
       <c r="I173" s="124" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J173" s="44"/>
       <c r="K173" s="2"/>
@@ -8401,7 +8413,7 @@
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
       <c r="I174" s="124" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J174" s="44"/>
       <c r="K174" s="2"/>
@@ -8434,7 +8446,7 @@
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
       <c r="I175" s="124" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J175" s="44"/>
       <c r="K175" s="2"/>
@@ -8467,7 +8479,7 @@
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
       <c r="I176" s="124" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J176" s="44"/>
       <c r="K176" s="2"/>
@@ -8500,7 +8512,7 @@
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
       <c r="I177" s="124" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J177" s="44"/>
       <c r="K177" s="2"/>
@@ -8533,7 +8545,7 @@
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
       <c r="I178" s="124" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J178" s="44"/>
       <c r="K178" s="2"/>
@@ -8566,7 +8578,7 @@
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
       <c r="I179" s="124" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J179" s="44"/>
       <c r="K179" s="2"/>
@@ -8599,7 +8611,7 @@
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
       <c r="I180" s="124" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J180" s="44"/>
       <c r="K180" s="2"/>
@@ -8632,7 +8644,7 @@
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
       <c r="I181" s="124" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J181" s="44"/>
       <c r="K181" s="2"/>
@@ -8665,7 +8677,7 @@
       <c r="G182" s="63"/>
       <c r="H182" s="63"/>
       <c r="I182" s="126" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J182" s="67"/>
       <c r="K182" s="68"/>
@@ -8693,20 +8705,20 @@
         <v>6</v>
       </c>
       <c r="B183" s="130" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C183" s="52">
         <v>1</v>
       </c>
       <c r="D183" s="52"/>
       <c r="E183" s="132" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F183" s="64"/>
       <c r="G183" s="35"/>
       <c r="H183" s="35"/>
       <c r="I183" s="128" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J183" s="44"/>
       <c r="K183" s="36"/>
@@ -8737,7 +8749,7 @@
       <c r="G184" s="35"/>
       <c r="H184" s="35"/>
       <c r="I184" s="128" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J184" s="44"/>
       <c r="K184" s="36"/>
@@ -8769,7 +8781,7 @@
       <c r="G185" s="13"/>
       <c r="H185" s="13"/>
       <c r="I185" s="124" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J185" s="44"/>
       <c r="K185" s="2"/>
@@ -8801,7 +8813,7 @@
       <c r="G186" s="13"/>
       <c r="H186" s="13"/>
       <c r="I186" s="124" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J186" s="44"/>
       <c r="K186" s="2"/>
@@ -8833,7 +8845,7 @@
       <c r="G187" s="13"/>
       <c r="H187" s="13"/>
       <c r="I187" s="124" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J187" s="44"/>
       <c r="K187" s="2"/>
@@ -8865,7 +8877,7 @@
       <c r="G188" s="13"/>
       <c r="H188" s="13"/>
       <c r="I188" s="124" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J188" s="44"/>
       <c r="K188" s="2"/>
@@ -8898,7 +8910,7 @@
       <c r="G189" s="72"/>
       <c r="H189" s="72"/>
       <c r="I189" s="126" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J189" s="67"/>
       <c r="K189" s="68"/>
@@ -8926,7 +8938,7 @@
         <v>7</v>
       </c>
       <c r="B190" s="130" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C190" s="52"/>
       <c r="D190" s="52"/>
@@ -8935,7 +8947,7 @@
       <c r="G190" s="35"/>
       <c r="H190" s="35"/>
       <c r="I190" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J190" s="44"/>
       <c r="K190" s="36"/>
@@ -8967,7 +8979,7 @@
       <c r="G191" s="13"/>
       <c r="H191" s="13"/>
       <c r="I191" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J191" s="44"/>
       <c r="K191" s="2"/>
@@ -9000,7 +9012,7 @@
       <c r="G192" s="72"/>
       <c r="H192" s="72"/>
       <c r="I192" s="126" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J192" s="67"/>
       <c r="K192" s="68"/>
@@ -9028,7 +9040,7 @@
         <v>8</v>
       </c>
       <c r="B193" s="123" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C193" s="64"/>
       <c r="D193" s="184">
@@ -9039,7 +9051,7 @@
       <c r="G193" s="35"/>
       <c r="H193" s="35"/>
       <c r="I193" s="128" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J193" s="44"/>
       <c r="K193" s="36"/>
@@ -9067,13 +9079,13 @@
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="98" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E194" s="1"/>
       <c r="G194" s="13"/>
       <c r="H194" s="13"/>
       <c r="I194" s="124" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J194" s="44"/>
       <c r="K194" s="2"/>
@@ -9105,7 +9117,7 @@
       <c r="G195" s="13"/>
       <c r="H195" s="13"/>
       <c r="I195" s="124" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J195" s="44"/>
       <c r="K195" s="2"/>
@@ -9137,7 +9149,7 @@
       <c r="G196" s="13"/>
       <c r="H196" s="13"/>
       <c r="I196" s="124" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J196" s="44"/>
       <c r="K196" s="2"/>
@@ -9169,7 +9181,7 @@
       <c r="G197" s="13"/>
       <c r="H197" s="13"/>
       <c r="I197" s="124" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J197" s="44"/>
       <c r="K197" s="2"/>
@@ -9195,7 +9207,7 @@
     <row r="198" spans="1:29" s="16" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="29"/>
       <c r="B198" s="178" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C198" s="179"/>
       <c r="D198" s="179"/>
@@ -9228,7 +9240,7 @@
     <row r="199" spans="1:29" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="27"/>
       <c r="B199" s="140" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C199" s="83"/>
       <c r="D199" s="83"/>
@@ -9294,17 +9306,17 @@
         <v>9</v>
       </c>
       <c r="B201" s="130" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C201" s="52"/>
       <c r="D201" s="34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E201" s="52"/>
       <c r="G201" s="35"/>
       <c r="H201" s="35"/>
       <c r="I201" s="128" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J201" s="100"/>
       <c r="K201" s="35"/>
@@ -9334,14 +9346,14 @@
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="96" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E202" s="1"/>
       <c r="F202" s="124"/>
       <c r="G202" s="13"/>
       <c r="H202" s="13"/>
       <c r="I202" s="124" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J202" s="44"/>
       <c r="K202" s="2"/>
@@ -9371,7 +9383,7 @@
         <v>10</v>
       </c>
       <c r="B203" s="122" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C203" s="54"/>
       <c r="D203" s="54"/>
@@ -9380,7 +9392,7 @@
       <c r="G203" s="31"/>
       <c r="H203" s="31"/>
       <c r="I203" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J203" s="43">
         <v>1</v>
@@ -9417,7 +9429,7 @@
       <c r="G204" s="13"/>
       <c r="H204" s="13"/>
       <c r="I204" s="124" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J204" s="44"/>
       <c r="K204" s="2"/>
@@ -9452,7 +9464,7 @@
       <c r="G205" s="13"/>
       <c r="H205" s="13"/>
       <c r="I205" s="124" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J205" s="44"/>
       <c r="K205" s="2"/>
@@ -9489,7 +9501,7 @@
       <c r="G206" s="19"/>
       <c r="H206" s="19"/>
       <c r="I206" s="141" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J206" s="44"/>
       <c r="K206" s="2"/>
@@ -9522,7 +9534,7 @@
       <c r="G207" s="19"/>
       <c r="H207" s="19"/>
       <c r="I207" s="141" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J207" s="44"/>
       <c r="K207" s="2"/>
@@ -9550,7 +9562,7 @@
         <v>11</v>
       </c>
       <c r="B208" s="142" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C208" s="59"/>
       <c r="D208" s="59"/>
@@ -9559,7 +9571,7 @@
       <c r="G208" s="31"/>
       <c r="H208" s="31"/>
       <c r="I208" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J208" s="43"/>
       <c r="K208" s="24"/>
@@ -9596,7 +9608,7 @@
       <c r="G209" s="13"/>
       <c r="H209" s="13"/>
       <c r="I209" s="124" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J209" s="44">
         <v>1</v>
@@ -9637,7 +9649,7 @@
       <c r="G210" s="13"/>
       <c r="H210" s="13"/>
       <c r="I210" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J210" s="44"/>
       <c r="K210" s="2">
@@ -9667,7 +9679,7 @@
         <v>12</v>
       </c>
       <c r="B211" s="54" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C211" s="54"/>
       <c r="D211" s="54"/>
@@ -9676,7 +9688,7 @@
       <c r="G211" s="31"/>
       <c r="H211" s="31"/>
       <c r="I211" s="120" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J211" s="43">
         <v>1</v>
@@ -9715,7 +9727,7 @@
       <c r="G212" s="13"/>
       <c r="H212" s="13"/>
       <c r="I212" s="124" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J212" s="44"/>
       <c r="K212" s="2"/>
@@ -9749,18 +9761,18 @@
         <v>13</v>
       </c>
       <c r="B213" s="123" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C213" s="56"/>
       <c r="D213" s="96" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E213" s="56"/>
       <c r="F213" s="128"/>
       <c r="G213" s="35"/>
       <c r="H213" s="35"/>
       <c r="I213" s="128" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J213" s="44"/>
       <c r="K213" s="36"/>
@@ -9788,14 +9800,14 @@
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E214" s="1"/>
       <c r="F214" s="124"/>
       <c r="G214" s="13"/>
       <c r="H214" s="13"/>
       <c r="I214" s="124" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J214" s="44"/>
       <c r="K214" s="2"/>
@@ -9823,18 +9835,18 @@
         <v>14</v>
       </c>
       <c r="B215" s="123" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C215" s="56"/>
       <c r="D215" s="97" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E215" s="56"/>
       <c r="F215" s="128"/>
       <c r="G215" s="35"/>
       <c r="H215" s="35"/>
       <c r="I215" s="128" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J215" s="44"/>
       <c r="K215" s="36"/>
@@ -9862,14 +9874,14 @@
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="97" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E216" s="1"/>
       <c r="F216" s="124"/>
       <c r="G216" s="13"/>
       <c r="H216" s="13"/>
       <c r="I216" s="124" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J216" s="44"/>
       <c r="K216" s="2"/>
@@ -9895,7 +9907,7 @@
     <row r="217" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A217" s="29"/>
       <c r="B217" s="180" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C217" s="181"/>
       <c r="D217" s="181"/>
@@ -9930,13 +9942,13 @@
         <v>15</v>
       </c>
       <c r="B218" s="143" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C218" s="57"/>
       <c r="D218" s="57"/>
       <c r="E218" s="57"/>
       <c r="F218" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G218" s="34"/>
       <c r="H218" s="34"/>
@@ -9969,7 +9981,7 @@
       <c r="D219" s="1"/>
       <c r="E219" s="1"/>
       <c r="F219" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G219" s="34"/>
       <c r="H219" s="34"/>
@@ -10002,7 +10014,7 @@
       <c r="D220" s="1"/>
       <c r="E220" s="1"/>
       <c r="F220" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G220" s="18"/>
       <c r="H220" s="18"/>
@@ -10033,13 +10045,13 @@
         <v>16</v>
       </c>
       <c r="B221" s="143" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C221" s="57"/>
       <c r="D221" s="57"/>
       <c r="E221" s="57"/>
       <c r="F221" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G221" s="61"/>
       <c r="H221" s="61"/>
@@ -10070,13 +10082,13 @@
         <v>17</v>
       </c>
       <c r="B222" s="145" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C222" s="58"/>
       <c r="D222" s="58"/>
       <c r="E222" s="58"/>
       <c r="F222" s="150" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G222" s="18"/>
       <c r="H222" s="18"/>
@@ -10107,7 +10119,7 @@
         <v>18</v>
       </c>
       <c r="B223" s="145" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C223" s="58"/>
       <c r="D223" s="58"/>
@@ -10142,13 +10154,13 @@
         <v>19</v>
       </c>
       <c r="B224" s="145" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C224" s="58"/>
       <c r="D224" s="58"/>
       <c r="E224" s="58"/>
       <c r="F224" s="148" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G224" s="35"/>
       <c r="H224" s="35"/>
@@ -10181,7 +10193,7 @@
       <c r="D225" s="14"/>
       <c r="E225" s="14"/>
       <c r="F225" s="149" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G225" s="35"/>
       <c r="H225" s="35"/>
@@ -10214,7 +10226,7 @@
       <c r="D226" s="14"/>
       <c r="E226" s="14"/>
       <c r="F226" s="149" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G226" s="35"/>
       <c r="H226" s="35"/>
@@ -10247,7 +10259,7 @@
       <c r="D227" s="14"/>
       <c r="E227" s="14"/>
       <c r="F227" s="149" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G227" s="35"/>
       <c r="H227" s="35"/>
@@ -10280,7 +10292,7 @@
       <c r="D228" s="14"/>
       <c r="E228" s="14"/>
       <c r="F228" s="149" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G228" s="35"/>
       <c r="H228" s="35"/>
@@ -10316,7 +10328,7 @@
       <c r="G229" s="26"/>
       <c r="H229" s="26"/>
       <c r="I229" s="47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J229" s="43">
         <f>SUM(J2:J228)</f>
@@ -10392,15 +10404,15 @@
         <v>20</v>
       </c>
       <c r="B231" s="146" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C231" s="26"/>
       <c r="D231" s="26"/>
       <c r="E231" s="102" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F231" s="112" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G231" s="26"/>
       <c r="H231" s="26"/>
@@ -10433,7 +10445,7 @@
       <c r="D232" s="63"/>
       <c r="E232" s="63"/>
       <c r="F232" s="126" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G232" s="63"/>
       <c r="H232" s="63"/>
@@ -10464,13 +10476,13 @@
         <v>21</v>
       </c>
       <c r="B233" s="147" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C233" s="1"/>
       <c r="D233" s="11"/>
       <c r="E233" s="11"/>
       <c r="F233" s="125" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G233" s="1"/>
       <c r="H233" s="1"/>
@@ -10532,15 +10544,15 @@
         <v>22</v>
       </c>
       <c r="B235" s="146" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C235" s="26"/>
       <c r="D235" s="78"/>
       <c r="E235" s="176" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F235" s="125" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G235" s="26"/>
       <c r="H235" s="26"/>
@@ -10572,10 +10584,10 @@
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
       <c r="E236" s="176" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F236" s="134" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G236" s="1"/>
       <c r="H236" s="1"/>
@@ -10607,10 +10619,10 @@
       <c r="C237" s="1"/>
       <c r="D237" s="1"/>
       <c r="E237" s="176" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F237" s="124" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G237" s="1"/>
       <c r="H237" s="1"/>
@@ -10643,7 +10655,7 @@
       <c r="D238" s="1"/>
       <c r="E238" s="1"/>
       <c r="F238" s="144" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G238" s="1"/>
       <c r="H238" s="1"/>
@@ -10704,11 +10716,11 @@
         <v>23</v>
       </c>
       <c r="B240" s="114" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C240" s="1"/>
       <c r="D240" s="98" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E240" s="1"/>
       <c r="F240" s="1"/>
@@ -10739,7 +10751,7 @@
     <row r="241" spans="1:29" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="27"/>
       <c r="B241" s="113" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
@@ -10772,7 +10784,7 @@
     <row r="242" spans="1:29" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="27"/>
       <c r="B242" s="113" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C242" s="1"/>
       <c r="D242" s="1"/>
@@ -10805,7 +10817,7 @@
     <row r="243" spans="1:29" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="27"/>
       <c r="B243" s="113" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C243" s="1"/>
       <c r="D243" s="1"/>
@@ -11020,14 +11032,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="183" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="183"/>
       <c r="C1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="182" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" s="182" t="s">
-        <v>32</v>
       </c>
       <c r="E1" s="182"/>
       <c r="F1" s="22"/>
@@ -11035,68 +11047,68 @@
     </row>
     <row r="2" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A2" s="115" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="110" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="157" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" s="110" t="s">
-        <v>206</v>
-      </c>
-      <c r="C2" s="157" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="115" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="110" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C3" s="157" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" s="116" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="110" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" s="157" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="116" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="111" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C5" s="157" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="115" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="110" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C6" s="157" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="116" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="110" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C7" s="157" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separate translation with "//"
</commit_message>
<xml_diff>
--- a/media/questions.xlsx
+++ b/media/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ju5315jo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{074806AF-F5DA-462F-94C4-C281F8E84916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C180C471-E4D6-4FDE-9483-C0891E4141E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,40 +40,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="264">
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>Kysymys/Fråga/Question</t>
-  </si>
-  <si>
-    <t>Valintojen määrä/Antal alternativ/Number of 
-choices(default=1)</t>
-  </si>
-  <si>
-    <t>Ehto/Vilkor/Condition</t>
-  </si>
-  <si>
-    <t>Kuvas/beskrivning/Description</t>
-  </si>
-  <si>
-    <t>Alikysymys/delfråga/Subquestion</t>
-  </si>
-  <si>
-    <t>Moneenko alikysymykseen tulee vastata/Hur många delfrågor bör svaras/How many subquestion should be answered. (default=all)</t>
-  </si>
-  <si>
-    <t>Alikysymyksen kuvas/Delfrågans
- beskrivning/Subquestion description</t>
-  </si>
-  <si>
-    <t>Alikysymyksen ehto/delfrågans vilkor /subquestion condition</t>
-  </si>
-  <si>
-    <t>Vaihtoehto/Alternativ/option</t>
-  </si>
-  <si>
     <t>Autoilija/Bilist/Car traveler</t>
   </si>
   <si>
@@ -98,24 +69,6 @@
     <t>Jos ehtoa ei ole alikysymys kysytään aina, mutta jos ehto on niin sen on täytyttävä, että kysymys tulee näkyville. esim  jos on 3.0 niin alikysymys näytetään vain jos kysymyksessä kolme on vastattu vaihtoehto 0 (auto).</t>
   </si>
   <si>
-    <t>Matkustaja, jonka on vaikea luopua autosta./En passagerare som har svårt att ge upp bilen./Traveler who has trouble giving up their car.</t>
-  </si>
-  <si>
-    <t>Matkustaa autolla tottumuksesta, avoin muille matkustusmuodoille, kun hän oppii käyttämään./Reser med bil av vana, är öppen för andra former av transport när resenären lär sig använda dem./Travels by car out of habit, open to other modes of travel as he becomes familiar with them.</t>
-  </si>
-  <si>
-    <t>Kulkee kävellen tai pyörällä ympäri vuoden, jos etäisyys sallii. Käyttää joukkoliikennettä pitkillä matkoilla. /Färdas till fots eller med cykel året runt, om avståndet tillåter. Använder kollektivtrafik för långa avstånd./Travels by foot or by bicycle if distance permits, uses public transport for long distances.</t>
-  </si>
-  <si>
-    <t>Kulkee aina julkisilla kulkuvälineillä, ei omaa autoa./Reser alltid med kollektivtrafik, ingen egen bil./Always travels by public transport, does not have a car.</t>
-  </si>
-  <si>
-    <t>Hän kokeilee mielellään uusia kulkumuotoja ja etsii, mitkä ovelta ovelle -ratkaisut sopivat hänelle parhaiten./Resenären gillar att prova nya transportsätt och hitta vilka dörr-till-dörr-lösningar som passar resenären bäst./Likes to try out new forms of mobility and looks for which door-to-door solutions suit them best.</t>
-  </si>
-  <si>
-    <t>Ennen matkaa tutkii, mikä kulkumuoto sopii parhaiten. Mikäli mahdollista, käyttää joukkoliikennettä, mutta jos se vie liikaa aikaa tai vaatii useita vaihtoja, hän käyttää autoa./Undersöker vilket transportsätt passar bäst innan resan. Om möjligt använder resenären kollektivtrafik, men om det tar för mycket tid eller kräver flera byten, kommer resenären att använda bil./Prior to their journey, examines which modality best suits their journey. If possible, they use public transport, but if this takes extra time or if they have to make frequent transfers, they take the car.</t>
-  </si>
-  <si>
     <t>Helppo Hirvi/Enkel Älg/Easy Elk</t>
   </si>
   <si>
@@ -128,21 +81,9 @@
     <t>Nokkela Näätä/Vettig Vessla/Witty Weasel</t>
   </si>
   <si>
-    <t>Kokeileva Kauris/Hugad Hjort/Daring Deer</t>
-  </si>
-  <si>
     <t>Määrätietoinen Metso/Käck Tjäder/Goal-oriented Grouse</t>
   </si>
   <si>
-    <t xml:space="preserve">Kuinka monena päivänä viikossa liikut seuraavin kulkumuodoin?/Hur många gånger i veckan använder du följande transportmedel/How many times a week do you use the following means of transport? </t>
-  </si>
-  <si>
-    <t>Jos sinulla ei ole mahdollisuutta johonkin kulkumuotoon, valitse "ei koskaan"/Om du inte har tillgång till ett transportsätt, välj "aldrig". /If you do not have an opportunity to use a mode, choose "never".</t>
-  </si>
-  <si>
-    <t>Auto/Bil/Car</t>
-  </si>
-  <si>
     <t>2-3</t>
   </si>
   <si>
@@ -152,58 +93,18 @@
     <t>6-7</t>
   </si>
   <si>
-    <t>Moottoripyörä/Motorcykel/Motorbike</t>
-  </si>
-  <si>
-    <t>Juna/Tåg/Train</t>
-  </si>
-  <si>
-    <t>Linja-auto/Bus/Buss</t>
-  </si>
-  <si>
-    <t>Mopo tai skootteri/Moped eller skoter/Moped or scooter</t>
-  </si>
-  <si>
-    <t>Polkupyörä tai sähköpyörä/Cykel eller elcykel/Bicycle or e-bike</t>
-  </si>
-  <si>
-    <t>Kävellen/Gående/On foot</t>
-  </si>
-  <si>
-    <t>Sähköpotkulauta, segway tai muu vastaava/Elsparkcykel, segway eller liknande/Scooter, segway or similar</t>
-  </si>
-  <si>
     <t>1a</t>
   </si>
   <si>
-    <t>Kun kuljet autolla, kuka auton omistaa?/När du kör bil, vem äger bilen?/When you drive a car, who owns the car?</t>
-  </si>
-  <si>
     <t>1.0,1-2-3-4-5</t>
   </si>
   <si>
-    <t>Oma tai perheeni/Egen eller familjens/Mine or my family's</t>
-  </si>
-  <si>
     <t>*Esitä vain, jos vastaus auton kohdalla "&lt;1 eller mer".</t>
   </si>
   <si>
-    <t>Yrityksen omistama auto tai työsuhdeauto/Företagsägd bil eller tjänstebil/
-Company-owned car or company car</t>
-  </si>
-  <si>
-    <t>Yhteiskäyttöauto/Bil för delat bruk/Shared car</t>
-  </si>
-  <si>
-    <t>Joku muu/Någon annan/Something else</t>
-  </si>
-  <si>
     <t>1b1</t>
   </si>
   <si>
-    <t>Miksi et koskaan kulje autolla?/Varför använder du aldrig bil?/Why do you never use a car?</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
@@ -211,630 +112,99 @@
   </si>
   <si>
     <t>(kan välja mer än ett alternativ)</t>
-  </si>
-  <si>
-    <t>Minulla ei ole autoa./Jag har ingen bil./I don't own a car.</t>
   </si>
   <si>
     <t xml:space="preserve">
 *Esitä vain, jos vastaus auton kohdalla "aldrig". (1.0, 0)</t>
   </si>
   <si>
-    <t>Suosin muita kulkutapoja./Jag föredrar andra transportsätt./I prefer using other means of transport.</t>
-  </si>
-  <si>
-    <t>Ympäristöön liittyvät syyt/Miljöskäl/For environmental reasons</t>
-  </si>
-  <si>
-    <t>Minulla ei ole ajokorttia./Jag har inte körkort./I don’t have a driving licence.</t>
-  </si>
-  <si>
     <t>1b2</t>
   </si>
   <si>
-    <t>Miksi et koskaan kulje pyörällä tai sähköpyörällä?/Varför anväder du aldrig cykel eller elcykel?/Why do you never use a bike or e-bike?</t>
-  </si>
-  <si>
     <t>1.5,0</t>
   </si>
   <si>
-    <t>(voi valita useamman vaihtoehdon)/(kan välja mer än ett alternativ)/(multiple answers possible)</t>
-  </si>
-  <si>
-    <t>En omista pyörää./Jag äger ingen cykel./I don’t own a bike.</t>
-  </si>
-  <si>
     <t>** Esitä vain, jos vastaus polkupyörän kohdalla "aldrig" (1.5, 0)</t>
   </si>
   <si>
-    <t>Matkan pituus (liian lyhyt tai pitkä)/Resans längd (för kort eller lång)/The travel distance (too short or long)</t>
-  </si>
-  <si>
-    <t>En halua saapua paikalle hikisenä./Jag vill inte anlända svettig./I don't want to arrive sweaty at the destination.</t>
-  </si>
-  <si>
-    <t>En pysty terveydentilani tai fyysisen kuntoni vuoksi käyttämään polkupyörää./Jag kan inte använda en cykel på grund av min hälsa eller fysiska tillstånd./I can’t use a bike because of a physical disability or my state of health.</t>
-  </si>
-  <si>
-    <t>En pysty kuljettamaan kaikkea tarvitsemaani tavaraa pyörällä./Jag kan inte transportera alla saker jag behöver på cykel./I can't transport the necessities that I need on a bike.</t>
-  </si>
-  <si>
-    <t>En pysty yhdistämään pyöräilyä muihin tehtäviini, kuten lasten vientiin ja hakemiseen./Jag kan inte kombinera cykling med mina andra uppgifter, som att föra och hämta barn./I can't combine a bike with my other activities, e.g., dropping off and picking up children.</t>
-  </si>
-  <si>
-    <t>Muu/Annat/Other</t>
-  </si>
-  <si>
     <t>1b3</t>
   </si>
   <si>
-    <t xml:space="preserve">Miksi et koskaan kulje joukkoliikenteellä?/Varför åker du aldrig kollektivt?/Why do you never use public transport? </t>
-  </si>
-  <si>
     <t>1.2,0:1.3,0</t>
   </si>
   <si>
-    <t>Matkanteko kestää kauemmin tai matka on pidempi muihin kulkutapoihin verrattuna./Resan tar längre tid eller är längre jämfört med andra transportsätt./Longer travel time or travel distance compared with other means of transport.</t>
-  </si>
-  <si>
     <t>* Esitä vain jos vastaus joukkoliikenteen kohdalla "aldrig". (tåg eller buss)</t>
   </si>
   <si>
-    <t>Ei sopivia yhteyksiä tai vaihtomahdollisuuksia./Inga lämpliga anslutningar eller bytesalternativ./No good connection or transfer options.</t>
-  </si>
-  <si>
-    <t>En pysty kuljettamaan kaikkea tarvitsemaani tavaraa joukkoliikenteessä./Jag kan inte transportera alla saker jag behöver i kollektiv trafiken./I can't transport the stuff that I need on public transportation.</t>
-  </si>
-  <si>
-    <t>Joukkoliikenne ei ole riittävän mukava tapa matkustaa esim. kiireestä, palveluiden puutteesta tai turvallisuudesta johtuen./Kollektivtrafik är inte ett tillräckligt bekvämt sätt att resa t.ex. på grund av brådska, brist på tjänster eller säkerhet./I don’t find public transport sufficiently comfortable because it is too busy, lack of facilities or safety.</t>
-  </si>
-  <si>
-    <t>En pysty yhdistämään joukkoliikennettä muihin tehtäviini , kuten lasten vientiin ja hakemiseen./Jag kan inte kombinera kollektivtrafik med mina andra uppgifter, som att föra och hämta barn./I cannot combine public transport with my other activities, e.g., dropping off and picking up children.</t>
-  </si>
-  <si>
-    <t>Suosin muita kulkutapoja. /Jag föredrar andra transportsätt./I prefer using other means of transport.</t>
-  </si>
-  <si>
-    <t>Minulla on vaikeuksia käyttää joukkoliikennettä fyysisen kuntoni tai terveydentilani takia. /Jag har svårt att använda kollektivtrafik på grund av mitt fysiska tillstånd eller hälsotillstånd./I find public transport difficult to access because of my (physical) disability or for health reasons.</t>
-  </si>
-  <si>
     <t>1c</t>
   </si>
   <si>
-    <t>Pyöräiletkö ympäri vuoden, myös silloin kun on lunta ja jäätä?/Cyklar du året runt, även när det finns snö och is?/Do you cycle all year round, even when there is snow and ice?</t>
-  </si>
-  <si>
     <t>1.5,4-5</t>
   </si>
   <si>
-    <t xml:space="preserve">Pyöräilen ympäri vuoden./Jag cyklar året runt./ I cycle all year round. </t>
-  </si>
-  <si>
     <t>* Esitä vain jos vastaus pyöräilyn kohdalla "4-5" tai enemmän</t>
   </si>
   <si>
-    <t>Pyöräilen vain lumettomana ja jäättömänä aikana./Jag cyklar bara när det är snö- och isfritt./I only cycle when there is no snow or ice.</t>
-  </si>
-  <si>
-    <t>Pyöräilen vain kesäkaudella./Jag cyklar bara under sommarsäsongen./I only cycle in the summer season.</t>
-  </si>
-  <si>
     <t>1d</t>
   </si>
   <si>
-    <t>Vaihdatko pyörään nastarenkaat talveksi?/Byter du  dubbdäck till din cykel för vintern?/Are you changing to studded tires on your bike for the winter?</t>
-  </si>
-  <si>
     <t>1c,0-1</t>
   </si>
   <si>
-    <t>Kyllä/Ja/Yes</t>
-  </si>
-  <si>
     <t>*Esitä vain, jos vastaus kysymykseen 1c on "Jag cyklar året runt" tai " Jag cyklar när det är snö- och isfritt"</t>
   </si>
   <si>
-    <t>Joskus/Ibland/Sometimes</t>
-  </si>
-  <si>
-    <t>En/Nej/No</t>
-  </si>
-  <si>
-    <t>Mitä kulkutapoja yhdistät toisinaan saman matkan aikana?/Vilka transportsätt kombinerar du ibland under samma resa?/Which modes of transport do you combine sometimes during the same travel?</t>
-  </si>
-  <si>
-    <t>Auto ja joukkoliikenne/Bil och kollektivtrafik/Car and public transport</t>
-  </si>
-  <si>
-    <t>Polkupyörä tai sähköpotkulauta ja joukkoliikenne/Cykel eller elsparkcykel och kollektivtrafik/Bicycle or scooter and public transport</t>
-  </si>
-  <si>
-    <t>Polkupyörä tai sähköpotkulauta ja auto/Cykel eller elsparkcykel och bil/Bicycle or scooter and car</t>
-  </si>
-  <si>
-    <t>Mopo tai skootteri ja joukkoliikenne/Moped eller skoter och kollektivtrafik/Moped or motorcycle and public transport</t>
-  </si>
-  <si>
-    <t>Pyörä ja kävely/Cykel och gång/Bicycle and walking</t>
-  </si>
-  <si>
-    <t>En koskaan yhdistele erilaisia kulkutapoja./Jag kombinerar aldrig olika transportsätt./I never combine different means of transport.</t>
-  </si>
-  <si>
-    <t>Päivän aikana tekemistäni matkoista suurimman etäisyyden kuljen: /Av de resor jag har gjort under dagen reser jag den största sträckan:/During my daily journeys I cover the greatest distance by:</t>
-  </si>
-  <si>
-    <t>Autolla/Med bil/Car</t>
-  </si>
-  <si>
-    <t>Junalla/Med tåg/Train</t>
-  </si>
-  <si>
-    <t>Linja-autolla/Med buss/Bus</t>
-  </si>
-  <si>
-    <t>Mopolla tai skootterilla/Med moped eller skoter/Moped or motorcycle</t>
-  </si>
-  <si>
-    <t>Polkupyörällä tai sähköpyörällä/Med cykel eller el-cykel/Bicycle or e-bike</t>
-  </si>
-  <si>
-    <t>Sähköpotkulaudalla tai muulla vastaavalla/Med elsparkcykel eller likannde/E-scooter or similar</t>
-  </si>
-  <si>
-    <t>Jalkaisin/Til fots/On Foot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tärkein syy, että käytän kulkumuotoa &lt;&lt;kysymyksen 3 vastaus tähän&gt;&gt;:/Den främsta anledningen till att jag använder transportsätt &lt;&lt;svar på fråga 3 här&gt;&gt;:/The main reason why &lt;&lt;answer from question 3 here&gt;&gt; I use  is: </t>
-  </si>
-  <si>
-    <t>(valitse yksi)/(välj en)/(choose one)</t>
-  </si>
-  <si>
-    <t>auto/bil/car</t>
-  </si>
-  <si>
-    <t>Tärkein syy, miksi käytän autoa, on: /Den främsta anledningen till att jag använder bil är:/The main reason why I use car is:</t>
-  </si>
-  <si>
     <t>3.0</t>
   </si>
   <si>
-    <t>matkan hinta/resans pris/cost of the joyrney</t>
-  </si>
-  <si>
-    <t>matkan pituus/resans längd/travel distance</t>
-  </si>
-  <si>
-    <t>matkan kesto/resans längd i tid/travel time</t>
-  </si>
-  <si>
-    <t>säätila (sade, tuuli, jne.)/väder (regn, vind, etc)/the weather (rain, wind etc)</t>
-  </si>
-  <si>
-    <t>Vien tai haen lapset./Jag för eller hämtar barnen./I drop off or pick up children.</t>
-  </si>
-  <si>
-    <t>Työni edellyttää asiakastapaamisia ja minun tulee näyttää edustavalta. /Mitt jobb kräver kundmöten och jag måste se representabel ut./My job involves a lot of contact with customers and I need to look presentable.</t>
-  </si>
-  <si>
-    <t>Minun pitää liikkua päivän aikana usean sijainnin välillä. /Jag måste flytta mellan flera platser under dagen./I have appointments in different locations.</t>
-  </si>
-  <si>
-    <t>Minulla on mukanani paljon tavaraa tai työvälineitä./Jag har många saker eller verktyg med mig./I have a lot of luggage or work equipment.</t>
-  </si>
-  <si>
-    <t>Haluan tuntea oloni mukavaksi matkan ajan. /Jag vill känna mig bekväm under resan./I like to be comfortable during my journey.</t>
-  </si>
-  <si>
-    <t>Pidän omasta rauhasta./Jag gillar att få vara i fred./I like my privacy.</t>
-  </si>
-  <si>
-    <t>tavan vuoksi. /för vanans skull./out of habit.</t>
-  </si>
-  <si>
-    <t>Minulla on yrityksen tai työnantajan auto käytössäni./Jag har en företags- eller arbetsgivarbil till mitt förfogande./I use a company car.</t>
-  </si>
-  <si>
-    <t>Minulla on puutteelliset tiedot muista kulkumuodoista reitilläni./ Jag har ofullständig information om andra transportsätt på min rutt./I have insufficient information about other means of transport (for my route).</t>
-  </si>
-  <si>
-    <t>Minulla ei ole sopivia yhteyksiä tai vaihtomahdollisuuksia joukkoliikenteellä (sisältäen riittävän vuorovälin)./Jag har inte lämpliga anslutningar eller bytesmöjligheter med kollektivtrafik (inklusive tillräcklig frekvens)./I don't have a good connection or transfer options (including good frequency) with public transport.</t>
-  </si>
-  <si>
-    <t>moottoripyörä/motorcykel/motorbike</t>
-  </si>
-  <si>
-    <t>Tärkein syy, miksi käytän moottoripyörää on:/Den främsta anledningen till att jag använder motorcykel är: /The main reason why I use motorbike is:</t>
-  </si>
-  <si>
     <t>3.1</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Haluan välttää liikenneruuhkat. /Jag vill undvika trafikstockningar./I want to avoid traffic jams.</t>
-  </si>
-  <si>
-    <t>vapauden tunne/en känsla av frihet/the sense of freedom</t>
-  </si>
-  <si>
-    <t>joukkoliikenne (juna, linja-auto)/kollektivtrafik (tåg, buss)/public transportation (train, bus)</t>
-  </si>
-  <si>
-    <t>Tärkein syy, miksi käytän joukkoliikennettä on:/Den främsta anledningen till att jag använder kollektivtrafik är: /The main reason why I use public transportation is:</t>
-  </si>
-  <si>
     <t>3.2</t>
   </si>
   <si>
-    <t>Voin käyttää matka-ajan työskentelyyn tai muihin tehtäviin. /Jag kan använda restiden till arbete eller andra uppgifter./I use the travel time for work or other tasks</t>
-  </si>
-  <si>
-    <t>Minulla on hyvät yhteydet joukkoliikenteellä (sisältäen riittävän vuorovälin)./Jag har goda förbindelser med kollektivtrafik (inklusive tillräcklig frekvens)./I havea good connection with transfer options (including good frequency) with public transport</t>
-  </si>
-  <si>
-    <t>Työnantajani edellyttää minulta joukkoliikenteen käyttöä. /Min arbetsgivare kräver att jag använder kollektivtrafiken./My employer requires me to use public transport.</t>
-  </si>
-  <si>
-    <t>mopo tai skootteri/moped eller skoter/moped or scooter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tärkein syy, miksi käytän mopa tai skootteria on:/Den främsta anledningen till att jag använder moped or skoter är: /The main reason why I use my moped/motorcycle is: </t>
-  </si>
-  <si>
     <t>3.3</t>
   </si>
   <si>
-    <t>Työni edellyttää asiakastapaamisia ja minun tulee näyttää edustavalta. /Mitt jobb kräver kundmöten och jag måste se presentabel ut./My job involves a lot of contact with customers and I need to look presentable.</t>
-  </si>
-  <si>
-    <t>Minulla ei ole sopivia yhteyksiä tai vaihtomahdollisuuksia joukkoliikenteellä (sisältäen riittävän vuorovälin)./Jag har inte lämpliga anslutningar eller bytesmöjligheter med kollektivtrafik (inklusive tillräcklig frekvens)./I don't have a good connection or transfer options with public transport (frequency).</t>
-  </si>
-  <si>
-    <t>polkupyörä tai sähköpyörä tms/cykel eller elsparkcykel,o.d./bicycle or e-bike etc</t>
-  </si>
-  <si>
-    <t>Tärkein syy, miksi käytän pyörää tai sähköpyörää on:/Viktigaste orsaken att jag använder cykel eller elsparkcykel eller o.d. är:/The main reason why I use my bicycle or e-bike is:</t>
-  </si>
-  <si>
     <t>3.4</t>
   </si>
   <si>
-    <t>ympäristölliset syyt/miljöskäl/the environment</t>
-  </si>
-  <si>
-    <t>terveyteni/hälsoskäl/my health</t>
-  </si>
-  <si>
-    <t>Minulla ei ole sopivia yhteyksiä tai vaihtomahdollisuuksia joukkoliikenteellä (sisältäen riittävän vuorovälin)./Jag har inte lämpliga anslutningar eller bytessmöjligheter med kollektivtrafik (inklusive tillräcklig frekvens)./I don't have a good connection or transfer options with public transport (frequency).</t>
-  </si>
-  <si>
-    <t>Pidän tästä matkustustavasta./Jag gillar det här sättet att resa./I like traveling like this.</t>
-  </si>
-  <si>
-    <t>kävellen/till fots/on foot</t>
-  </si>
-  <si>
-    <t>Tärkein syy, miksi kävelen on:/Den främsta anledningen till att jag går är:/The main reason why I walk is:</t>
-  </si>
-  <si>
     <t>3.5</t>
   </si>
   <si>
-    <t>matkan hinta/resans pris/cost of the journey</t>
-  </si>
-  <si>
-    <t>Muu:/Annat:/Other:</t>
-  </si>
-  <si>
-    <t>Mikä/Mitkä seuraavista saisivat sinut muuttamaan liikkumistottumuksiasi?/Vad skulle få dig att ändra dina mobilitetsvanor?/What would inspire you to change your travel habits?</t>
-  </si>
-  <si>
     <t>1.0,3-4-5</t>
   </si>
   <si>
-    <t xml:space="preserve">Valitse 3 tärkeintä (Vedä tai tuplaklikkaa vastausvaihtoehtoja)/Välj de 3 viktigaste (Dra eller dubbelklicka på svarsalternativen)/List your top 3 (Drag or double-click your choices) </t>
-  </si>
-  <si>
-    <t>Ajansäästö/Tidsbesparande/Time gains</t>
-  </si>
-  <si>
     <t>&lt;&lt;kysy vain, jos henkilö vastasi kysymykseen 1 "bil"&gt;&gt;</t>
   </si>
   <si>
-    <t>Hyvät joukkoliikenneyhteydet/Bra förbindelser med kollektivtrafik/A good connection with public transport</t>
-  </si>
-  <si>
-    <t>Mahdollisuus käyttää joukkoliikennettä maksutta/Möjlighet att använda kollektivtrafiken gratis/A free public transport pass</t>
-  </si>
-  <si>
-    <t>Liityntäpysäköinti- eli park and ride -mahdollisuuksien lisääntyminen/Fler infartsparkeringsmöjligheter (Park &amp; Ride)/More Park &amp; Ride (P+R) options</t>
-  </si>
-  <si>
-    <t>Turvallinen pyöräpysäköinti niissä sijainneissa, joihin pysäköin pyöräni./Säker cykelparkering på platser där jag parkerar min cykel./A secure bicycle parking at the location where I park my bike.</t>
-  </si>
-  <si>
-    <t>Mahdollisuus käydä suihkussa työpaikalla./Möjlighet att duscha på arbetsplatsen./Shower facilities at work.</t>
-  </si>
-  <si>
-    <t>Työsuhdepolkupyörä/Företagscykel/Company bicycle through my employer</t>
-  </si>
-  <si>
-    <t>Reaaliaikaisen tiedon saaminen vaihtoyhteyksistä./Realtidsinformation om bytesanslutningar i kollektivtrafiken./Real-time information about transfer options.</t>
-  </si>
-  <si>
-    <t>Työnantajan antama liikkumisbudjetti./Arbetsgivarens budget för mobilitet./A mobility budget from my employer.</t>
-  </si>
-  <si>
-    <t>Kestävää liikkumista tukevat työsuhde-edut./Hållbar rörlighet stöds av anställningsförmåner./Sustainable mobility is supported by employment benefits.</t>
-  </si>
-  <si>
-    <t>Sovellus, joka antaa reaaliaikaista tietoa liikenneruuhkista ja vaihtoehtoisista reiteistä./En app som ger information i realtid om trafikstockningar och alternativa rutter./A mobility app that provides real time information about traffic jams and the available alternatives.</t>
-  </si>
-  <si>
-    <t>Kaupunkipyöräasema lähellä kotiani./Stadscykelstation nära mitt hem./A bike sharing station in my neighbourhood.</t>
-  </si>
-  <si>
-    <t>Yhteiskäyttöauto lähellä kotiani./Bil för delat bruk nära mitt hem./A car sharing car in my neighbourhood.</t>
-  </si>
-  <si>
-    <t>Kaupunkipyöräjärjestelmän testausmahdollisuus./Testperiod för stadscykelsystemet./A test subscription to a bike sharing system.</t>
-  </si>
-  <si>
-    <t>Yhteiskäyttöautojen testausmahdollisuus./Testperiod för bil med delat bruk./A test subscription to a car sharing system.</t>
-  </si>
-  <si>
-    <t>Parempi ja turvallisempi pyöräilyverkosto./Ett bättre och säkrare cykelnät./Better and safer cycling infrastructure.</t>
-  </si>
-  <si>
-    <t>Sovellus, joka kannustaa minua tekemään parempia valintoja päivittäin./En app som uppmuntrar mig att göra bättre val varje dag./An app that encourages me to make better choices daily.</t>
-  </si>
-  <si>
-    <t>Ratkaisu, joka mahdollistaa lasten kuljettamisen auton sijaan. /Någon lösning för att föra och hämta barn./A solution for dropping off and picking up the children.</t>
-  </si>
-  <si>
-    <t>Ei ole tapaa, jolla minut saisi muuttamaan käyttäytymistäni. /Det finns inget sätt att få mig att ändra mitt beteende./You can't convince me to change my behaviour.</t>
-  </si>
-  <si>
-    <t>Vaihtoehto, joka on yhtä mukava ja luotettava kuin nykyinen. /Ett alternativ som är lika bekvämt och pålitligt som det nuvarande ./An alternative that is just as comfortable and reliable as current one.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Työskenteletkö kotoa käsin?/Arbetar du hemifrån?/Do you sometimes work from home? </t>
-  </si>
-  <si>
-    <t>Kyllä, mutta korkeintaan päivän viikossa./Ja, men inte mer än en dag i veckan./Yes, but no more than 1 day a week.</t>
-  </si>
-  <si>
-    <t>Kyllä, 2-3 päivää viikossa./Ja, 2-3 dagar i veckan./Yes, 2-3 days a week.</t>
-  </si>
-  <si>
-    <t>Kyllä, useammin kuin kolmena päivänä viikossa. /Ja, mer än tre dagar i veckan./Yes, more that 3 days a week.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En, työtäni ei pysty tekemään kotoa./Nej, jag kan inte göra mitt jobb hemifrån./No, I can't do my job at home. </t>
-  </si>
-  <si>
-    <t>En. Haluaisin, mutta työnantajani ei salli etätyötä. /Nej. Jag skulle vilja, men min arbetsgivare tillåter inte distansarbete./No, I'd like to but my employer doesn't let me.</t>
-  </si>
-  <si>
-    <t>En, sillä en halua työskennellä kotoa käsin./Nej, för jag vill inte jobba hemifrån./No, I don't want to work from home.</t>
-  </si>
-  <si>
-    <t>Jokin muu tai ei sopivaa vastausvaihtoehtoa./Annat eller inget lämpligt svarsalternativ./Not applicable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Onko sinun mahdollista kulkea kodin ja työpaikan välillä ruuhka-aikojen ulkopuolella?/Är det möjligt för dig att pendla mellan hemmet och jobbet under lågtrafik?/Would you be able to commute at other times of the day, i.e., outside of the rush hour? </t>
-  </si>
-  <si>
-    <t>Ei/Nej/No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mikset voi matkustaa ruuhka-aikojen ulkopuolella?/Varför kan du inte resa under lågtrafik?/Why can’t you commute outside of the rush hour? </t>
-  </si>
-  <si>
-    <t>Teen kiinteitä työvuoroja./Jag arbetar fasta skift./I work fixed hours.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;&lt;kysy vain, jos vastaus kysymykseen 7 on "nej"&gt;&gt; 7, 1</t>
   </si>
   <si>
-    <t>Työnantajani ei mahdollista tätä./Min arbetsgivare gör inte detta möjligt./My employer doesn't allow this.</t>
-  </si>
-  <si>
-    <t>En ole valmis mukauttamaan työaikojani./Jag är inte beredd att anpassa min arbetstid./I'm not prepared to adapt my working hours.</t>
-  </si>
-  <si>
-    <t>Kategoria 2: Mitä tai miten ajattelet liikkumisesta(si)?/Kategori 2: Vad eller hur tänker du kring (din) mobilitet? Category 2: How you think about (your) mobility?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  &lt;&lt;valitse yksi vastaus per väittämä)/&lt;&lt;välj ett svar per påstående)/&lt;&lt;choose one option per statement&gt;&gt;</t>
-  </si>
-  <si>
-    <t>Mikä seuraavista kulkumuodoista on mielestäsi välttämättömin? (Valitse sinua parhaiten kuvaava vaihtoehto.)/Vilket av följande transportsätt tycker du är det mest nödvändiga?</t>
-  </si>
-  <si>
-    <t>polkupyörä tai sähköpotkulauta/cykel tai elsparkcykel/bicycle or e-scooter</t>
-  </si>
-  <si>
-    <t>joukkoliikenne/kollektivtrafik/public transportation</t>
-  </si>
-  <si>
-    <t>ei mikään näistä/ingen av dessa/none of these</t>
-  </si>
-  <si>
-    <t>kaikki ovat välttämättömiä kulkumuotoja/alla är oumbärliga transportsätt/all are indispensable means of transport</t>
-  </si>
-  <si>
-    <t>Tarkastatko ennen liikkeelle lähtöä, onko reitilläsi ruuhkaa? (Valitse sinua parhaiten kuvaava vaihtoehto.)/Innan du ger dig av, kontrollerar du om det är trafikstockning på din rutt? (Välj det alternativ som bäst beskriver dig.)/Do you check whether there are traffic jams on my route before leaving? (Please indicate the answer that suits you best.)</t>
-  </si>
-  <si>
-    <t>joka kerta/alltid/every time</t>
-  </si>
-  <si>
-    <t>silloin tällöin/ibland/now and then</t>
-  </si>
-  <si>
-    <t>en koskaan/aldrig/never</t>
-  </si>
-  <si>
-    <t>Kategoria 3: Henkilötiedot/Kategori 3: Personuppgifter/Category 3: Personal data</t>
-  </si>
-  <si>
-    <t>Sukupuoli/Kön/Gender</t>
-  </si>
-  <si>
-    <t>Mies/Man/Male</t>
-  </si>
-  <si>
-    <t>Nainen/Kvinna/Female</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
-    <t>Syntymävuosi/Födelseår/Year of birth</t>
-  </si>
-  <si>
     <t>(Pudotusvalikko)</t>
   </si>
   <si>
-    <t>Kotiosoitteeni postinumero/Postnummer för min hemadress/Post code of my home address</t>
-  </si>
-  <si>
     <t>Pudotusvalikko Turun alueen postinumeroista ja "muu" (sulkee ulkopaikkakuntalaiset ulos datasta), vaihtoehtoisesti kotikunnat (Turun alue ja "muu"), Turun alueella asuville kysymys postinumerosta</t>
   </si>
   <si>
-    <t>Työ- tai opiskelupaikan postinumero: (Ohita kysymys, jos et opiskele tai käy töissä)/Postnumret på din arbetsplats eller studieort: (Hoppa över frågan om du inte studerar eller arbetar)/Post code of my work or study address: (In case you don't work or study, you can skip this question)</t>
-  </si>
-  <si>
-    <t>Asuminen/Boende/Living situation</t>
-  </si>
-  <si>
-    <t>Asun yksin ilman lapsia./Jag bor ensam utan barn./Single without children.</t>
-  </si>
-  <si>
-    <t>Asun yksin lasten kanssa./Jag bor ensam med barn./Single with children.</t>
-  </si>
-  <si>
-    <t>Asun puolison kanssa kaksin./Jag bor tillsammans med min partner./Co-habiting without children.</t>
-  </si>
-  <si>
-    <t>Asun puolison ja lasten kanssa./Jag bor med min partner och barn./Co-habiting with children.</t>
-  </si>
-  <si>
     <t>Yhteensä</t>
   </si>
   <si>
-    <t>Miksi tein testin?/Varför gjorde jag testet?/Why did I do the test?</t>
-  </si>
-  <si>
     <t>Tähän joku keino, miten saadaan erotettua hupitäyttelijät ja oikeaan dataan kuuluvat</t>
   </si>
   <si>
-    <t>Huvin vuoksi/Bara för skojs skull/Just for fun</t>
-  </si>
-  <si>
-    <t>Haluan saada minulle räätälöityä tietoa liikkumisesta./Jag vill få skräddarsydd information om mobilitet./I want to receive customized information about mobility.</t>
-  </si>
-  <si>
-    <t>Ehdot/Vilkoren/Conditions</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Hyväksyn, että Turun kaupunki tallentaa vastauksiini perustuvan liikkumisprofiilini ja voi käyttää vastauksiani osana yleistettyä liikkumisdataa (Kyselydataa ei yhdistetä henkilötietoihin, se näytetään yleiskuvana osana palvelukartan liikkumisnäkymää https://palvelukartta.turku.fi/fi/mobility/). /Jag godkänner att Åbo stad lagrar min mobilitetsprofil baserat på mina svar och kan använda mina svar som en del av generaliserad mobilitetsdata (Undersökningsdata inte är kopplad till personuppgifter visas den som en översikt som en del av mobilitetsvyn av tjänstekartan https://palvelukartta.turku.fi/sv/mobility/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>)./I accept that the city of Turku saves my mobility profile based on my answers and can use my answers as part of generalized mobility data (Survey data is not combined with personal data, it is shown as an overview as part of the mobility view of the service map https://palvelukartta.turku.fi/en/mobility/).</t>
-    </r>
-  </si>
-  <si>
-    <t>Uutiskirje/Nyhetsbrev/Newsletter</t>
-  </si>
-  <si>
     <t>Tällä valinnalla kootaan kustakin profiilista oma viestintälista.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">Haluan tilata kestävän liikkumisen uutiskirjeen. (Liikenteen ja liikkumisen uutiskirjeen henkilörekisteri https://rekisteri.turku.fi/Saabe_data/ )/Jag vill prenumerera på nyhetsbrevet om hållbar rörlighet. (
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF305496"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Trafik- och mobilitetnyhetsbrevets personregister</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> https://rekisteri.turku.fi/Saabe_data/)/I want to subscribe to the sustainable mobility newsletter (Traffic and mobility newsletter's personal register https://rekisteri.turku.fi/Saabe_data/)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>En halua</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>./Jag vill inte./I do not want.</t>
-    </r>
-  </si>
-  <si>
-    <t>Lisätiedot/Ytterligare information/More information</t>
-  </si>
-  <si>
     <t>kysy vain, jos vastaus kysymykseen 25 on kyllä (vaihtoehdot 1-3)</t>
   </si>
   <si>
-    <t>Etunimi/Förnamn/First name</t>
-  </si>
-  <si>
-    <t>Sukunimi/Efternamn/Last name</t>
-  </si>
-  <si>
-    <t>Sähköposti/E-post/E-mail</t>
-  </si>
-  <si>
     <t>Profiili</t>
   </si>
   <si>
@@ -863,13 +233,617 @@
   </si>
   <si>
     <t xml:space="preserve">Tiedät päivittäiset kohteesi ja miten niihin pääsee. Et pidä yllätyksistä matkan aikana; elämä on sellaisenaan jo tarpeeksi stressaavaa. Olet valmis kokeilemaan nopeampia tai mukavampia vaihtoehtoja, mutta vain jos saat selkeää tietoa niistä – mieluiten yksityiskohtaisen matkasuunnitelman kera./Du vet dina dagliga resmål och hur du tar dig till dem. Du gillar inte överraskningar under resan; livet är tillräckligt stressigt som det är. Du är villig att prova snabbare eller bekvämare alternativ, men bara om du får tydlig information om dem – gärna med en detaljerad resplan./You know where you're going every day and how to get there. You don't like surprises en route; life is already sufficiently stressful as it is. You are willing to try out faster or more comfortable alternatives. But only if you get clear information about this, preferably with a detailed travel plan. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ad </t>
+  </si>
+  <si>
+    <t>Valveutunut matkustaja//Medveten resenär//Conscious traveler</t>
+  </si>
+  <si>
+    <t>Maas-matkustaja//MaaS-resenär//MaaS traveler</t>
+  </si>
+  <si>
+    <t>Joukkoliikenteen käyttäjä//Använder kollektivtrafiken//Public transport passenger</t>
+  </si>
+  <si>
+    <t>Kävelijä-Pyöräilijä//Fotgängare-Cyklist//Walker-Cyclist</t>
+  </si>
+  <si>
+    <t>Tavan mukaan kulkeva//Rör sig enligt vana//Habit traveler</t>
+  </si>
+  <si>
+    <t>Autoilija//Bilist//Car traveler</t>
+  </si>
+  <si>
+    <t>Vaihtoehto//Alternativ//option</t>
+  </si>
+  <si>
+    <t>Alikysymyksen ehto//delfrågans vilkor //subquestion condition</t>
+  </si>
+  <si>
+    <t>Alikysymyksen kuvas//Delfrågans
+ beskrivning//Subquestion description</t>
+  </si>
+  <si>
+    <t>Moneenko alikysymykseen tulee vastata//Hur många delfrågor bör svaras//How many subquestion should be answered. (default=all)</t>
+  </si>
+  <si>
+    <t>Alikysymys//delfråga//Subquestion</t>
+  </si>
+  <si>
+    <t>Kuvas//beskrivning//Description</t>
+  </si>
+  <si>
+    <t>Ehto//Vilkor//Condition</t>
+  </si>
+  <si>
+    <t>Valintojen määrä//Antal alternativ//Number of 
+choices(default=1)</t>
+  </si>
+  <si>
+    <t>Kysymys//Fråga//Question</t>
+  </si>
+  <si>
+    <t>Sähköposti//E-post//E-mail</t>
+  </si>
+  <si>
+    <t>Sukunimi//Efternamn//Last name</t>
+  </si>
+  <si>
+    <t>Etunimi//Förnamn//First name</t>
+  </si>
+  <si>
+    <t>Lisätiedot//Ytterligare information//More information</t>
+  </si>
+  <si>
+    <t>En halua.//Jag vill inte.//I do not want.</t>
+  </si>
+  <si>
+    <t>Haluan tilata kestävän liikkumisen uutiskirjeen. (Liikenteen ja liikkumisen uutiskirjeen henkilörekisteri https:////rekisteri.turku.fi//Saabe_data// )//Jag vill prenumerera på nyhetsbrevet om hållbar rörlighet. (
+Trafik- och mobilitetnyhetsbrevets personregister https:////rekisteri.turku.fi//Saabe_data//)//I want to subscribe to the sustainable mobility newsletter (Traffic and mobility newsletter's personal register https:////rekisteri.turku.fi//Saabe_data//)</t>
+  </si>
+  <si>
+    <t>Uutiskirje//Nyhetsbrev//Newsletter</t>
+  </si>
+  <si>
+    <t>Hyväksyn, että Turun kaupunki tallentaa vastauksiini perustuvan liikkumisprofiilini ja voi käyttää vastauksiani osana yleistettyä liikkumisdataa (Kyselydataa ei yhdistetä henkilötietoihin, se näytetään yleiskuvana osana palvelukartan liikkumisnäkymää https:////palvelukartta.turku.fi//fi//mobility//). //Jag godkänner att Åbo stad lagrar min mobilitetsprofil baserat på mina svar och kan använda mina svar som en del av generaliserad mobilitetsdata (Undersökningsdata inte är kopplad till personuppgifter visas den som en översikt som en del av mobilitetsvyn av tjänstekartan https:////palvelukartta.turku.fi//sv//mobility// ).//I accept that the city of Turku saves my mobility profile based on my answers and can use my answers as part of generalized mobility data (Survey data is not combined with personal data, it is shown as an overview as part of the mobility view of the service map https:////palvelukartta.turku.fi//en//mobility//).</t>
+  </si>
+  <si>
+    <t>Ehdot//Vilkoren//Conditions</t>
+  </si>
+  <si>
+    <t>Haluan saada minulle räätälöityä tietoa liikkumisesta.//Jag vill få skräddarsydd information om mobilitet.//I want to receive customized information about mobility.</t>
+  </si>
+  <si>
+    <t>Huvin vuoksi//Bara för skojs skull//Just for fun</t>
+  </si>
+  <si>
+    <t>Miksi tein testin?//Varför gjorde jag testet?//Why did I do the test?</t>
+  </si>
+  <si>
+    <t>Muu://Annat://Other:</t>
+  </si>
+  <si>
+    <t>Asun puolison ja lasten kanssa.//Jag bor med min partner och barn.//Co-habiting with children.</t>
+  </si>
+  <si>
+    <t>Asun puolison kanssa kaksin.//Jag bor tillsammans med min partner.//Co-habiting without children.</t>
+  </si>
+  <si>
+    <t>Asun yksin lasten kanssa.//Jag bor ensam med barn.//Single with children.</t>
+  </si>
+  <si>
+    <t>Asun yksin ilman lapsia.//Jag bor ensam utan barn.//Single without children.</t>
+  </si>
+  <si>
+    <t>Asuminen//Boende//Living situation</t>
+  </si>
+  <si>
+    <t>Työ- tai opiskelupaikan postinumero: (Ohita kysymys, jos et opiskele tai käy töissä)//Postnumret på din arbetsplats eller studieort: (Hoppa över frågan om du inte studerar eller arbetar)//Post code of my work or study address: (In case you don't work or study, you can skip this question)</t>
+  </si>
+  <si>
+    <t>Kotiosoitteeni postinumero//Postnummer för min hemadress//Post code of my home address</t>
+  </si>
+  <si>
+    <t>Syntymävuosi//Födelseår//Year of birth</t>
+  </si>
+  <si>
+    <t>Nainen//Kvinna//Female</t>
+  </si>
+  <si>
+    <t>Mies//Man//Male</t>
+  </si>
+  <si>
+    <t>Sukupuoli//Kön//Gender</t>
+  </si>
+  <si>
+    <t>Kategoria 3: Henkilötiedot//Kategori 3: Personuppgifter//Category 3: Personal data</t>
+  </si>
+  <si>
+    <t>en koskaan//aldrig//never</t>
+  </si>
+  <si>
+    <t>silloin tällöin//ibland//now and then</t>
+  </si>
+  <si>
+    <t>joka kerta//alltid//every time</t>
+  </si>
+  <si>
+    <t>Tarkastatko ennen liikkeelle lähtöä, onko reitilläsi ruuhkaa? (Valitse sinua parhaiten kuvaava vaihtoehto.)//Innan du ger dig av, kontrollerar du om det är trafikstockning på din rutt? (Välj det alternativ som bäst beskriver dig.)//Do you check whether there are traffic jams on my route before leaving? (Please indicate the answer that suits you best.)</t>
+  </si>
+  <si>
+    <t>kaikki ovat välttämättömiä kulkumuotoja//alla är oumbärliga transportsätt//all are indispensable means of transport</t>
+  </si>
+  <si>
+    <t>ei mikään näistä//ingen av dessa//none of these</t>
+  </si>
+  <si>
+    <t>joukkoliikenne//kollektivtrafik//public transportation</t>
+  </si>
+  <si>
+    <t>polkupyörä tai sähköpotkulauta//cykel tai elsparkcykel//bicycle or e-scooter</t>
+  </si>
+  <si>
+    <t>auto//bil//car</t>
+  </si>
+  <si>
+    <t>Mikä seuraavista kulkumuodoista on mielestäsi välttämättömin? (Valitse sinua parhaiten kuvaava vaihtoehto.)//Vilket av följande transportsätt tycker du är det mest nödvändiga?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;&lt;valitse yksi vastaus per väittämä)//&lt;&lt;välj ett svar per påstående)//&lt;&lt;choose one option per statement&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Kategoria 2: Mitä tai miten ajattelet liikkumisesta(si)?//Kategori 2: Vad eller hur tänker du kring (din) mobilitet? Category 2: How you think about (your) mobility?</t>
+  </si>
+  <si>
+    <t>Vien tai haen lapset.//Jag för eller hämtar barnen.//I drop off or pick up children.</t>
+  </si>
+  <si>
+    <t>En ole valmis mukauttamaan työaikojani.//Jag är inte beredd att anpassa min arbetstid.//I'm not prepared to adapt my working hours.</t>
+  </si>
+  <si>
+    <t>Työnantajani ei mahdollista tätä.//Min arbetsgivare gör inte detta möjligt.//My employer doesn't allow this.</t>
+  </si>
+  <si>
+    <t>Teen kiinteitä työvuoroja.//Jag arbetar fasta skift.//I work fixed hours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mikset voi matkustaa ruuhka-aikojen ulkopuolella?//Varför kan du inte resa under lågtrafik?//Why can’t you commute outside of the rush hour? </t>
+  </si>
+  <si>
+    <t>Jokin muu tai ei sopivaa vastausvaihtoehtoa.//Annat eller inget lämpligt svarsalternativ.//Not applicable.</t>
+  </si>
+  <si>
+    <t>Ei//Nej//No</t>
+  </si>
+  <si>
+    <t>Kyllä//Ja//Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onko sinun mahdollista kulkea kodin ja työpaikan välillä ruuhka-aikojen ulkopuolella?//Är det möjligt för dig att pendla mellan hemmet och jobbet under lågtrafik?//Would you be able to commute at other times of the day, i.e., outside of the rush hour? </t>
+  </si>
+  <si>
+    <t>En, sillä en halua työskennellä kotoa käsin.//Nej, för jag vill inte jobba hemifrån.//No, I don't want to work from home.</t>
+  </si>
+  <si>
+    <t>En. Haluaisin, mutta työnantajani ei salli etätyötä. //Nej. Jag skulle vilja, men min arbetsgivare tillåter inte distansarbete.//No, I'd like to but my employer doesn't let me.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En, työtäni ei pysty tekemään kotoa.//Nej, jag kan inte göra mitt jobb hemifrån.//No, I can't do my job at home. </t>
+  </si>
+  <si>
+    <t>Kyllä, useammin kuin kolmena päivänä viikossa. //Ja, mer än tre dagar i veckan.//Yes, more that 3 days a week.</t>
+  </si>
+  <si>
+    <t>Kyllä, 2-3 päivää viikossa.//Ja, 2-3 dagar i veckan.//Yes, 2-3 days a week.</t>
+  </si>
+  <si>
+    <t>Kyllä, mutta korkeintaan päivän viikossa.//Ja, men inte mer än en dag i veckan.//Yes, but no more than 1 day a week.</t>
+  </si>
+  <si>
+    <t>(valitse yksi)//(välj en)//(choose one)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Työskenteletkö kotoa käsin?//Arbetar du hemifrån?//Do you sometimes work from home? </t>
+  </si>
+  <si>
+    <t>Muu//Annat//Other</t>
+  </si>
+  <si>
+    <t>Vaihtoehto, joka on yhtä mukava ja luotettava kuin nykyinen. //Ett alternativ som är lika bekvämt och pålitligt som det nuvarande .//An alternative that is just as comfortable and reliable as current one.</t>
+  </si>
+  <si>
+    <t>Ei ole tapaa, jolla minut saisi muuttamaan käyttäytymistäni. //Det finns inget sätt att få mig att ändra mitt beteende.//You can't convince me to change my behaviour.</t>
+  </si>
+  <si>
+    <t>Ratkaisu, joka mahdollistaa lasten kuljettamisen auton sijaan. //Någon lösning för att föra och hämta barn.//A solution for dropping off and picking up the children.</t>
+  </si>
+  <si>
+    <t>Sovellus, joka kannustaa minua tekemään parempia valintoja päivittäin.//En app som uppmuntrar mig att göra bättre val varje dag.//An app that encourages me to make better choices daily.</t>
+  </si>
+  <si>
+    <t>Parempi ja turvallisempi pyöräilyverkosto.//Ett bättre och säkrare cykelnät.//Better and safer cycling infrastructure.</t>
+  </si>
+  <si>
+    <t>Yhteiskäyttöautojen testausmahdollisuus.//Testperiod för bil med delat bruk.//A test subscription to a car sharing system.</t>
+  </si>
+  <si>
+    <t>Kaupunkipyöräjärjestelmän testausmahdollisuus.//Testperiod för stadscykelsystemet.//A test subscription to a bike sharing system.</t>
+  </si>
+  <si>
+    <t>Yhteiskäyttöauto lähellä kotiani.//Bil för delat bruk nära mitt hem.//A car sharing car in my neighbourhood.</t>
+  </si>
+  <si>
+    <t>Kaupunkipyöräasema lähellä kotiani.//Stadscykelstation nära mitt hem.//A bike sharing station in my neighbourhood.</t>
+  </si>
+  <si>
+    <t>Sovellus, joka antaa reaaliaikaista tietoa liikenneruuhkista ja vaihtoehtoisista reiteistä.//En app som ger information i realtid om trafikstockningar och alternativa rutter.//A mobility app that provides real time information about traffic jams and the available alternatives.</t>
+  </si>
+  <si>
+    <t>Kestävää liikkumista tukevat työsuhde-edut.//Hållbar rörlighet stöds av anställningsförmåner.//Sustainable mobility is supported by employment benefits.</t>
+  </si>
+  <si>
+    <t>Työnantajan antama liikkumisbudjetti.//Arbetsgivarens budget för mobilitet.//A mobility budget from my employer.</t>
+  </si>
+  <si>
+    <t>Reaaliaikaisen tiedon saaminen vaihtoyhteyksistä.//Realtidsinformation om bytesanslutningar i kollektivtrafiken.//Real-time information about transfer options.</t>
+  </si>
+  <si>
+    <t>Työsuhdepolkupyörä//Företagscykel//Company bicycle through my employer</t>
+  </si>
+  <si>
+    <t>Mahdollisuus käydä suihkussa työpaikalla.//Möjlighet att duscha på arbetsplatsen.//Shower facilities at work.</t>
+  </si>
+  <si>
+    <t>Turvallinen pyöräpysäköinti niissä sijainneissa, joihin pysäköin pyöräni.//Säker cykelparkering på platser där jag parkerar min cykel.//A secure bicycle parking at the location where I park my bike.</t>
+  </si>
+  <si>
+    <t>Liityntäpysäköinti- eli park and ride -mahdollisuuksien lisääntyminen//Fler infartsparkeringsmöjligheter (Park &amp; Ride)//More Park &amp; Ride (P+R) options</t>
+  </si>
+  <si>
+    <t>Mahdollisuus käyttää joukkoliikennettä maksutta//Möjlighet att använda kollektivtrafiken gratis//A free public transport pass</t>
+  </si>
+  <si>
+    <t>Hyvät joukkoliikenneyhteydet//Bra förbindelser med kollektivtrafik//A good connection with public transport</t>
+  </si>
+  <si>
+    <t>Ajansäästö//Tidsbesparande//Time gains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valitse 3 tärkeintä (Vedä tai tuplaklikkaa vastausvaihtoehtoja)//Välj de 3 viktigaste (Dra eller dubbelklicka på svarsalternativen)//List your top 3 (Drag or double-click your choices) </t>
+  </si>
+  <si>
+    <t>Haluan tuntea oloni mukavaksi matkan ajan. //Jag vill känna mig bekväm under resan.//I like to be comfortable during my journey.</t>
+  </si>
+  <si>
+    <t>tavan vuoksi. //för vanans skull.//out of habit.</t>
+  </si>
+  <si>
+    <t>terveyteni//hälsoskäl//my health</t>
+  </si>
+  <si>
+    <t>ympäristölliset syyt//miljöskäl//the environment</t>
+  </si>
+  <si>
+    <t>matkan kesto//resans längd i tid//travel time</t>
+  </si>
+  <si>
+    <t>matkan pituus//resans längd//travel distance</t>
+  </si>
+  <si>
+    <t>matkan hinta//resans pris//cost of the journey</t>
+  </si>
+  <si>
+    <t>Tärkein syy, miksi kävelen on://Den främsta anledningen till att jag går är://The main reason why I walk is:</t>
+  </si>
+  <si>
+    <t>kävellen//till fots//on foot</t>
+  </si>
+  <si>
+    <t>Minulla ei ole autoa.//Jag har ingen bil.//I don't own a car.</t>
+  </si>
+  <si>
+    <t>Haluan välttää liikenneruuhkat. //Jag vill undvika trafikstockningar.//I want to avoid traffic jams.</t>
+  </si>
+  <si>
+    <t>Pidän tästä matkustustavasta.//Jag gillar det här sättet att resa.//I like traveling like this.</t>
+  </si>
+  <si>
+    <t>Minulla ei ole sopivia yhteyksiä tai vaihtomahdollisuuksia joukkoliikenteellä (sisältäen riittävän vuorovälin).//Jag har inte lämpliga anslutningar eller bytessmöjligheter med kollektivtrafik (inklusive tillräcklig frekvens).//I don't have a good connection or transfer options with public transport (frequency).</t>
+  </si>
+  <si>
+    <t>Pidän omasta rauhasta.//Jag gillar att få vara i fred.//I like my privacy.</t>
+  </si>
+  <si>
+    <t>matkan hinta//resans pris//cost of the joyrney</t>
+  </si>
+  <si>
+    <t>Tärkein syy, miksi käytän pyörää tai sähköpyörää on://Viktigaste orsaken att jag använder cykel eller elsparkcykel eller o.d. är://The main reason why I use my bicycle or e-bike is:</t>
+  </si>
+  <si>
+    <t>polkupyörä tai sähköpyörä tms//cykel eller elsparkcykel,o.d.//bicycle or e-bike etc</t>
+  </si>
+  <si>
+    <t>Minulla ei ole sopivia yhteyksiä tai vaihtomahdollisuuksia joukkoliikenteellä (sisältäen riittävän vuorovälin).//Jag har inte lämpliga anslutningar eller bytesmöjligheter med kollektivtrafik (inklusive tillräcklig frekvens).//I don't have a good connection or transfer options with public transport (frequency).</t>
+  </si>
+  <si>
+    <t>Työni edellyttää asiakastapaamisia ja minun tulee näyttää edustavalta. //Mitt jobb kräver kundmöten och jag måste se presentabel ut.//My job involves a lot of contact with customers and I need to look presentable.</t>
+  </si>
+  <si>
+    <t>Minun pitää liikkua päivän aikana usean sijainnin välillä. //Jag måste flytta mellan flera platser under dagen.//I have appointments in different locations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tärkein syy, miksi käytän mopa tai skootteria on://Den främsta anledningen till att jag använder moped or skoter är: //The main reason why I use my moped//motorcycle is: </t>
+  </si>
+  <si>
+    <t>mopo tai skootteri//moped eller skoter//moped or scooter</t>
+  </si>
+  <si>
+    <t>Työnantajani edellyttää minulta joukkoliikenteen käyttöä. //Min arbetsgivare kräver att jag använder kollektivtrafiken.//My employer requires me to use public transport.</t>
+  </si>
+  <si>
+    <t>Minulla on hyvät yhteydet joukkoliikenteellä (sisältäen riittävän vuorovälin).//Jag har goda förbindelser med kollektivtrafik (inklusive tillräcklig frekvens).//I havea good connection with transfer options (including good frequency) with public transport</t>
+  </si>
+  <si>
+    <t>Voin käyttää matka-ajan työskentelyyn tai muihin tehtäviin. //Jag kan använda restiden till arbete eller andra uppgifter.//I use the travel time for work or other tasks</t>
+  </si>
+  <si>
+    <t>säätila (sade, tuuli, jne.)//väder (regn, vind, etc)//the weather (rain, wind etc)</t>
+  </si>
+  <si>
+    <t>Tärkein syy, miksi käytän joukkoliikennettä on://Den främsta anledningen till att jag använder kollektivtrafik är: //The main reason why I use public transportation is:</t>
+  </si>
+  <si>
+    <t>joukkoliikenne (juna, linja-auto)//kollektivtrafik (tåg, buss)//public transportation (train, bus)</t>
+  </si>
+  <si>
+    <t>Minulla ei ole sopivia yhteyksiä tai vaihtomahdollisuuksia joukkoliikenteellä (sisältäen riittävän vuorovälin).//Jag har inte lämpliga anslutningar eller bytesmöjligheter med kollektivtrafik (inklusive tillräcklig frekvens).//I don't have a good connection or transfer options (including good frequency) with public transport.</t>
+  </si>
+  <si>
+    <t>Minulla on puutteelliset tiedot muista kulkumuodoista reitilläni.// Jag har ofullständig information om andra transportsätt på min rutt.//I have insufficient information about other means of transport (for my route).</t>
+  </si>
+  <si>
+    <t>vapauden tunne//en känsla av frihet//the sense of freedom</t>
+  </si>
+  <si>
+    <t>Tärkein syy, miksi käytän moottoripyörää on://Den främsta anledningen till att jag använder motorcykel är: //The main reason why I use motorbike is:</t>
+  </si>
+  <si>
+    <t>moottoripyörä//motorcykel//motorbike</t>
+  </si>
+  <si>
+    <t>Minulla on yrityksen tai työnantajan auto käytössäni.//Jag har en företags- eller arbetsgivarbil till mitt förfogande.//I use a company car.</t>
+  </si>
+  <si>
+    <t>Minulla on mukanani paljon tavaraa tai työvälineitä.//Jag har många saker eller verktyg med mig.//I have a lot of luggage or work equipment.</t>
+  </si>
+  <si>
+    <t>Työni edellyttää asiakastapaamisia ja minun tulee näyttää edustavalta. //Mitt jobb kräver kundmöten och jag måste se representabel ut.//My job involves a lot of contact with customers and I need to look presentable.</t>
+  </si>
+  <si>
+    <t>Tärkein syy, miksi käytän autoa, on: //Den främsta anledningen till att jag använder bil är://The main reason why I use car is:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tärkein syy, että käytän kulkumuotoa &lt;&lt;kysymyksen 3 vastaus tähän&gt;&gt;://Den främsta anledningen till att jag använder transportsätt &lt;&lt;svar på fråga 3 här&gt;&gt;://The main reason why &lt;&lt;answer from question 3 here&gt;&gt; I use  is: </t>
+  </si>
+  <si>
+    <t>Jalkaisin//Til fots//On Foot</t>
+  </si>
+  <si>
+    <t>Sähköpotkulaudalla tai muulla vastaavalla//Med elsparkcykel eller likannde//E-scooter or similar</t>
+  </si>
+  <si>
+    <t>Polkupyörällä tai sähköpyörällä//Med cykel eller el-cykel//Bicycle or e-bike</t>
+  </si>
+  <si>
+    <t>Mopolla tai skootterilla//Med moped eller skoter//Moped or motorcycle</t>
+  </si>
+  <si>
+    <t>Linja-autolla//Med buss//Bus</t>
+  </si>
+  <si>
+    <t>Junalla//Med tåg//Train</t>
+  </si>
+  <si>
+    <t>Autolla//Med bil//Car</t>
+  </si>
+  <si>
+    <t>Päivän aikana tekemistäni matkoista suurimman etäisyyden kuljen: //Av de resor jag har gjort under dagen reser jag den största sträckan://During my daily journeys I cover the greatest distance by:</t>
+  </si>
+  <si>
+    <t>En koskaan yhdistele erilaisia kulkutapoja.//Jag kombinerar aldrig olika transportsätt.//I never combine different means of transport.</t>
+  </si>
+  <si>
+    <t>Pyörä ja kävely//Cykel och gång//Bicycle and walking</t>
+  </si>
+  <si>
+    <t>Mopo tai skootteri ja joukkoliikenne//Moped eller skoter och kollektivtrafik//Moped or motorcycle and public transport</t>
+  </si>
+  <si>
+    <t>Polkupyörä tai sähköpotkulauta ja auto//Cykel eller elsparkcykel och bil//Bicycle or scooter and car</t>
+  </si>
+  <si>
+    <t>Polkupyörä tai sähköpotkulauta ja joukkoliikenne//Cykel eller elsparkcykel och kollektivtrafik//Bicycle or scooter and public transport</t>
+  </si>
+  <si>
+    <t>Auto ja joukkoliikenne//Bil och kollektivtrafik//Car and public transport</t>
+  </si>
+  <si>
+    <t>(voi valita useamman vaihtoehdon)//(kan välja mer än ett alternativ)//(multiple answers possible)</t>
+  </si>
+  <si>
+    <t>Mitä kulkutapoja yhdistät toisinaan saman matkan aikana?//Vilka transportsätt kombinerar du ibland under samma resa?//Which modes of transport do you combine sometimes during the same travel?</t>
+  </si>
+  <si>
+    <t>En//Nej//No</t>
+  </si>
+  <si>
+    <t>Joskus//Ibland//Sometimes</t>
+  </si>
+  <si>
+    <t>Vaihdatko pyörään nastarenkaat talveksi?//Byter du  dubbdäck till din cykel för vintern?//Are you changing to studded tires on your bike for the winter?</t>
+  </si>
+  <si>
+    <t>Pyöräilen vain kesäkaudella.//Jag cyklar bara under sommarsäsongen.//I only cycle in the summer season.</t>
+  </si>
+  <si>
+    <t>Pyöräilen vain lumettomana ja jäättömänä aikana.//Jag cyklar bara när det är snö- och isfritt.//I only cycle when there is no snow or ice.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyöräilen ympäri vuoden.//Jag cyklar året runt.// I cycle all year round. </t>
+  </si>
+  <si>
+    <t>Pyöräiletkö ympäri vuoden, myös silloin kun on lunta ja jäätä?//Cyklar du året runt, även när det finns snö och is?//Do you cycle all year round, even when there is snow and ice?</t>
+  </si>
+  <si>
+    <t>Minulla on vaikeuksia käyttää joukkoliikennettä fyysisen kuntoni tai terveydentilani takia. //Jag har svårt att använda kollektivtrafik på grund av mitt fysiska tillstånd eller hälsotillstånd.//I find public transport difficult to access because of my (physical) disability or for health reasons.</t>
+  </si>
+  <si>
+    <t>Suosin muita kulkutapoja. //Jag föredrar andra transportsätt.//I prefer using other means of transport.</t>
+  </si>
+  <si>
+    <t>En pysty yhdistämään joukkoliikennettä muihin tehtäviini , kuten lasten vientiin ja hakemiseen.//Jag kan inte kombinera kollektivtrafik med mina andra uppgifter, som att föra och hämta barn.//I cannot combine public transport with my other activities, e.g., dropping off and picking up children.</t>
+  </si>
+  <si>
+    <t>Joukkoliikenne ei ole riittävän mukava tapa matkustaa esim. kiireestä, palveluiden puutteesta tai turvallisuudesta johtuen.//Kollektivtrafik är inte ett tillräckligt bekvämt sätt att resa t.ex. på grund av brådska, brist på tjänster eller säkerhet.//I don’t find public transport sufficiently comfortable because it is too busy, lack of facilities or safety.</t>
+  </si>
+  <si>
+    <t>En pysty kuljettamaan kaikkea tarvitsemaani tavaraa joukkoliikenteessä.//Jag kan inte transportera alla saker jag behöver i kollektiv trafiken.//I can't transport the stuff that I need on public transportation.</t>
+  </si>
+  <si>
+    <t>Ei sopivia yhteyksiä tai vaihtomahdollisuuksia.//Inga lämpliga anslutningar eller bytesalternativ.//No good connection or transfer options.</t>
+  </si>
+  <si>
+    <t>Matkanteko kestää kauemmin tai matka on pidempi muihin kulkutapoihin verrattuna.//Resan tar längre tid eller är längre jämfört med andra transportsätt.//Longer travel time or travel distance compared with other means of transport.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miksi et koskaan kulje joukkoliikenteellä?//Varför åker du aldrig kollektivt?//Why do you never use public transport? </t>
+  </si>
+  <si>
+    <t>En pysty yhdistämään pyöräilyä muihin tehtäviini, kuten lasten vientiin ja hakemiseen.//Jag kan inte kombinera cykling med mina andra uppgifter, som att föra och hämta barn.//I can't combine a bike with my other activities, e.g., dropping off and picking up children.</t>
+  </si>
+  <si>
+    <t>En pysty kuljettamaan kaikkea tarvitsemaani tavaraa pyörällä.//Jag kan inte transportera alla saker jag behöver på cykel.//I can't transport the necessities that I need on a bike.</t>
+  </si>
+  <si>
+    <t>En pysty terveydentilani tai fyysisen kuntoni vuoksi käyttämään polkupyörää.//Jag kan inte använda en cykel på grund av min hälsa eller fysiska tillstånd.//I can’t use a bike because of a physical disability or my state of health.</t>
+  </si>
+  <si>
+    <t>En halua saapua paikalle hikisenä.//Jag vill inte anlända svettig.//I don't want to arrive sweaty at the destination.</t>
+  </si>
+  <si>
+    <t>Matkan pituus (liian lyhyt tai pitkä)//Resans längd (för kort eller lång)//The travel distance (too short or long)</t>
+  </si>
+  <si>
+    <t>En omista pyörää.//Jag äger ingen cykel.//I don’t own a bike.</t>
+  </si>
+  <si>
+    <t>Miksi et koskaan kulje pyörällä tai sähköpyörällä?//Varför anväder du aldrig cykel eller elcykel?//Why do you never use a bike or e-bike?</t>
+  </si>
+  <si>
+    <t>Minulla ei ole ajokorttia.//Jag har inte körkort.//I don’t have a driving licence.</t>
+  </si>
+  <si>
+    <t>Ympäristöön liittyvät syyt//Miljöskäl//For environmental reasons</t>
+  </si>
+  <si>
+    <t>Suosin muita kulkutapoja.//Jag föredrar andra transportsätt.//I prefer using other means of transport.</t>
+  </si>
+  <si>
+    <t>Miksi et koskaan kulje autolla?//Varför använder du aldrig bil?//Why do you never use a car?</t>
+  </si>
+  <si>
+    <t>Joku muu//Någon annan//Something else</t>
+  </si>
+  <si>
+    <t>Yhteiskäyttöauto//Bil för delat bruk//Shared car</t>
+  </si>
+  <si>
+    <t>Yrityksen omistama auto tai työsuhdeauto//Företagsägd bil eller tjänstebil//
+Company-owned car or company car</t>
+  </si>
+  <si>
+    <t>Oma tai perheeni//Egen eller familjens//Mine or my family's</t>
+  </si>
+  <si>
+    <t>Kun kuljet autolla, kuka auton omistaa?//När du kör bil, vem äger bilen?//When you drive a car, who owns the car?</t>
+  </si>
+  <si>
+    <t>Sähköpotkulauta, segway tai muu vastaava//Elsparkcykel, segway eller liknande//Scooter, segway or similar</t>
+  </si>
+  <si>
+    <t>Kävellen//Gående//On foot</t>
+  </si>
+  <si>
+    <t>Polkupyörä tai sähköpyörä//Cykel eller elcykel//Bicycle or e-bike</t>
+  </si>
+  <si>
+    <t>Mopo tai skootteri//Moped eller skoter//Moped or scooter</t>
+  </si>
+  <si>
+    <t>Linja-auto//Bus//Buss</t>
+  </si>
+  <si>
+    <t>Juna//Tåg//Train</t>
+  </si>
+  <si>
+    <t>Moottoripyörä//Motorcykel//Motorbike</t>
+  </si>
+  <si>
+    <t>Auto//Bil//Car</t>
+  </si>
+  <si>
+    <t>Jos sinulla ei ole mahdollisuutta johonkin kulkumuotoon, valitse "ei koskaan"//Om du inte har tillgång till ett transportsätt, välj "aldrig". //If you do not have an opportunity to use a mode, choose "never".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuinka monena päivänä viikossa liikut seuraavin kulkumuodoin?//Hur många gånger i veckan använder du följande transportmedel//How many times a week do you use the following means of transport? </t>
+  </si>
+  <si>
+    <t>Määrätietoinen Metso//Käck Tjäder//Goal-oriented Grouse</t>
+  </si>
+  <si>
+    <t>Kokeileva Kauris//Hugad Hjort//Daring Deer</t>
+  </si>
+  <si>
+    <t>Nokkela Näätä//Vettig Vessla//Witty Weasel</t>
+  </si>
+  <si>
+    <t>Joustava Jänis//Hinderfri Hare//Hassle-free Hare</t>
+  </si>
+  <si>
+    <t>Käytännöllinen Kettu//Rutinerad Räv//Faithful Fox</t>
+  </si>
+  <si>
+    <t>Helppo Hirvi//Enkel Älg//Easy Elk</t>
+  </si>
+  <si>
+    <t>Ennen matkaa tutkii, mikä kulkumuoto sopii parhaiten. Mikäli mahdollista, käyttää joukkoliikennettä, mutta jos se vie liikaa aikaa tai vaatii useita vaihtoja, hän käyttää autoa.//Undersöker vilket transportsätt passar bäst innan resan. Om möjligt använder resenären kollektivtrafik, men om det tar för mycket tid eller kräver flera byten, kommer resenären att använda bil.//Prior to their journey, examines which modality best suits their journey. If possible, they use public transport, but if this takes extra time or if they have to make frequent transfers, they take the car.</t>
+  </si>
+  <si>
+    <t>Hän kokeilee mielellään uusia kulkumuotoja ja etsii, mitkä ovelta ovelle -ratkaisut sopivat hänelle parhaiten.//Resenären gillar att prova nya transportsätt och hitta vilka dörr-till-dörr-lösningar som passar resenären bäst.//Likes to try out new forms of mobility and looks for which door-to-door solutions suit them best.</t>
+  </si>
+  <si>
+    <t>Kulkee aina julkisilla kulkuvälineillä, ei omaa autoa.//Reser alltid med kollektivtrafik, ingen egen bil.//Always travels by public transport, does not have a car.</t>
+  </si>
+  <si>
+    <t>Kulkee kävellen tai pyörällä ympäri vuoden, jos etäisyys sallii. Käyttää joukkoliikennettä pitkillä matkoilla. //Färdas till fots eller med cykel året runt, om avståndet tillåter. Använder kollektivtrafik för långa avstånd.//Travels by foot or by bicycle if distance permits, uses public transport for long distances.</t>
+  </si>
+  <si>
+    <t>Matkustaa autolla tottumuksesta, avoin muille matkustusmuodoille, kun hän oppii käyttämään.//Reser med bil av vana, är öppen för andra former av transport när resenären lär sig använda dem.//Travels by car out of habit, open to other modes of travel as he becomes familiar with them.</t>
+  </si>
+  <si>
+    <t>Matkustaja, jonka on vaikea luopua autosta.//En passagerare som har svårt att ge upp bilen.//Traveler who has trouble giving up their car.</t>
+  </si>
+  <si>
+    <t>Mikä/Mitkä seuraavista saisivat sinut muuttamaan liikkumistottumuksiasi?//Vad skulle få dig att ändra dina mobilitetsvanor?//What would inspire you to change your travel habits?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -987,26 +961,10 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF305496"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1762,10 +1720,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1807,6 +1765,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2108,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF3ACC6-6455-42D3-BCE3-944B33DD47DC}">
   <dimension ref="A1:AD232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
@@ -2138,49 +2100,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>2</v>
+        <v>78</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="K1" s="110" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="L1" s="111" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="M1" s="110" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="N1" s="110" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="O1" s="111" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="P1" s="111" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="Q1" s="15"/>
       <c r="R1" s="14"/>
@@ -2202,33 +2164,33 @@
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="112" t="s">
-        <v>18</v>
+        <v>262</v>
       </c>
       <c r="L2" s="113" t="s">
-        <v>19</v>
+        <v>261</v>
       </c>
       <c r="M2" s="113" t="s">
-        <v>20</v>
+        <v>260</v>
       </c>
       <c r="N2" s="113" t="s">
-        <v>21</v>
+        <v>259</v>
       </c>
       <c r="O2" s="114" t="s">
-        <v>22</v>
+        <v>258</v>
       </c>
       <c r="P2" s="113" t="s">
-        <v>23</v>
+        <v>257</v>
       </c>
       <c r="Q2" s="9"/>
       <c r="R2" s="8"/>
@@ -2257,22 +2219,22 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="105" t="s">
-        <v>24</v>
+        <v>256</v>
       </c>
       <c r="L3" s="105" t="s">
-        <v>25</v>
+        <v>255</v>
       </c>
       <c r="M3" s="105" t="s">
-        <v>26</v>
+        <v>254</v>
       </c>
       <c r="N3" s="105" t="s">
-        <v>27</v>
+        <v>253</v>
       </c>
       <c r="O3" s="105" t="s">
-        <v>28</v>
+        <v>252</v>
       </c>
       <c r="P3" s="106" t="s">
-        <v>29</v>
+        <v>251</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="1"/>
@@ -2294,17 +2256,17 @@
         <v>1</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>30</v>
+        <v>250</v>
       </c>
       <c r="C4" s="54">
         <v>1</v>
       </c>
       <c r="D4" s="54"/>
       <c r="E4" s="95" t="s">
-        <v>31</v>
+        <v>249</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>32</v>
+        <v>248</v>
       </c>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
@@ -2385,7 +2347,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K6" s="43"/>
       <c r="L6" s="2">
@@ -2423,7 +2385,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K7" s="43">
         <v>1</v>
@@ -2461,7 +2423,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K8" s="43">
         <v>1</v>
@@ -2495,7 +2457,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="126" t="s">
-        <v>36</v>
+        <v>247</v>
       </c>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
@@ -2577,7 +2539,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K11" s="146"/>
       <c r="L11" s="147"/>
@@ -2611,7 +2573,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K12" s="146">
         <v>1</v>
@@ -2649,7 +2611,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K13" s="146">
         <v>1</v>
@@ -2683,7 +2645,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="31" t="s">
-        <v>37</v>
+        <v>246</v>
       </c>
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
@@ -2763,7 +2725,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K16" s="43"/>
       <c r="L16" s="2"/>
@@ -2805,7 +2767,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K17" s="43"/>
       <c r="L17" s="2"/>
@@ -2845,7 +2807,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K18" s="43"/>
       <c r="L18" s="2"/>
@@ -2877,7 +2839,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="31" t="s">
-        <v>38</v>
+        <v>245</v>
       </c>
       <c r="G19" s="31"/>
       <c r="H19" s="31"/>
@@ -2957,7 +2919,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K21" s="43"/>
       <c r="L21" s="2"/>
@@ -2999,7 +2961,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K22" s="43"/>
       <c r="L22" s="2"/>
@@ -3039,7 +3001,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K23" s="43"/>
       <c r="L23" s="2"/>
@@ -3071,7 +3033,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="115" t="s">
-        <v>39</v>
+        <v>244</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -3157,7 +3119,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="2"/>
@@ -3197,7 +3159,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K27" s="43"/>
       <c r="L27" s="2"/>
@@ -3235,7 +3197,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K28" s="43"/>
       <c r="L28" s="2"/>
@@ -3267,7 +3229,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="115" t="s">
-        <v>40</v>
+        <v>243</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
@@ -3351,7 +3313,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K31" s="43"/>
       <c r="L31" s="2"/>
@@ -3391,7 +3353,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K32" s="43"/>
       <c r="L32" s="2"/>
@@ -3431,7 +3393,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K33" s="43"/>
       <c r="L33" s="2"/>
@@ -3463,7 +3425,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="31" t="s">
-        <v>41</v>
+        <v>242</v>
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -3537,7 +3499,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K36" s="43"/>
       <c r="L36" s="2"/>
@@ -3571,7 +3533,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K37" s="43"/>
       <c r="L37" s="2"/>
@@ -3607,7 +3569,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K38" s="43"/>
       <c r="L38" s="2"/>
@@ -3639,7 +3601,7 @@
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="116" t="s">
-        <v>42</v>
+        <v>241</v>
       </c>
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
@@ -3725,7 +3687,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="K41" s="43"/>
       <c r="L41" s="2"/>
@@ -3763,7 +3725,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="K42" s="43"/>
       <c r="L42" s="2"/>
@@ -3801,7 +3763,7 @@
       <c r="H43" s="61"/>
       <c r="I43" s="61"/>
       <c r="J43" s="71" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="K43" s="65"/>
       <c r="L43" s="66"/>
@@ -3830,16 +3792,16 @@
     </row>
     <row r="44" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B44" s="118" t="s">
-        <v>44</v>
+        <v>240</v>
       </c>
       <c r="C44" s="60">
         <v>1</v>
       </c>
       <c r="D44" s="164" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
@@ -3847,7 +3809,7 @@
       <c r="H44" s="18"/>
       <c r="I44" s="18"/>
       <c r="J44" s="122" t="s">
-        <v>46</v>
+        <v>239</v>
       </c>
       <c r="K44" s="149"/>
       <c r="L44" s="150"/>
@@ -3875,7 +3837,7 @@
       <c r="B45" s="72"/>
       <c r="C45" s="72"/>
       <c r="D45" s="91" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
@@ -3883,7 +3845,7 @@
       <c r="H45" s="18"/>
       <c r="I45" s="18"/>
       <c r="J45" s="123" t="s">
-        <v>48</v>
+        <v>238</v>
       </c>
       <c r="K45" s="149"/>
       <c r="L45" s="150"/>
@@ -3917,7 +3879,7 @@
       <c r="H46" s="18"/>
       <c r="I46" s="18"/>
       <c r="J46" s="124" t="s">
-        <v>49</v>
+        <v>237</v>
       </c>
       <c r="K46" s="149"/>
       <c r="L46" s="150"/>
@@ -3951,7 +3913,7 @@
       <c r="H47" s="18"/>
       <c r="I47" s="18"/>
       <c r="J47" s="124" t="s">
-        <v>50</v>
+        <v>236</v>
       </c>
       <c r="K47" s="149"/>
       <c r="L47" s="150"/>
@@ -3976,26 +3938,26 @@
     </row>
     <row r="48" spans="1:30" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A48" s="29" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="B48" s="117" t="s">
-        <v>52</v>
+        <v>235</v>
       </c>
       <c r="C48" s="167" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D48" s="92" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="F48" s="73"/>
       <c r="G48" s="73"/>
       <c r="H48" s="31"/>
       <c r="I48" s="31"/>
       <c r="J48" s="115" t="s">
-        <v>56</v>
+        <v>165</v>
       </c>
       <c r="K48" s="152"/>
       <c r="L48" s="153"/>
@@ -4018,16 +3980,16 @@
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:30" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A49" s="27"/>
       <c r="D49" s="92" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="E49" s="11"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="119" t="s">
-        <v>58</v>
+        <v>234</v>
       </c>
       <c r="K49" s="149"/>
       <c r="L49" s="156"/>
@@ -4059,7 +4021,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
       <c r="J50" s="120" t="s">
-        <v>59</v>
+        <v>233</v>
       </c>
       <c r="K50" s="149"/>
       <c r="L50" s="156"/>
@@ -4093,7 +4055,7 @@
       <c r="H51" s="64"/>
       <c r="I51" s="64"/>
       <c r="J51" s="121" t="s">
-        <v>60</v>
+        <v>232</v>
       </c>
       <c r="K51" s="158"/>
       <c r="L51" s="159"/>
@@ -4118,26 +4080,26 @@
     </row>
     <row r="52" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A52" s="27" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="B52" s="125" t="s">
-        <v>62</v>
+        <v>231</v>
       </c>
       <c r="C52" s="168" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D52" s="94" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="E52" s="34" t="s">
-        <v>64</v>
+        <v>208</v>
       </c>
       <c r="F52" s="62"/>
       <c r="G52" s="62"/>
       <c r="H52" s="34"/>
       <c r="I52" s="34"/>
       <c r="J52" s="128" t="s">
-        <v>65</v>
+        <v>230</v>
       </c>
       <c r="K52" s="149"/>
       <c r="L52" s="162"/>
@@ -4163,13 +4125,13 @@
     <row r="53" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A53" s="27"/>
       <c r="D53" s="94" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="E53" s="11"/>
       <c r="H53" s="11"/>
       <c r="I53" s="11"/>
       <c r="J53" s="120" t="s">
-        <v>67</v>
+        <v>229</v>
       </c>
       <c r="K53" s="149"/>
       <c r="L53" s="156"/>
@@ -4201,7 +4163,7 @@
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
       <c r="J54" s="120" t="s">
-        <v>68</v>
+        <v>228</v>
       </c>
       <c r="K54" s="149"/>
       <c r="L54" s="156"/>
@@ -4233,7 +4195,7 @@
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
       <c r="J55" s="119" t="s">
-        <v>69</v>
+        <v>227</v>
       </c>
       <c r="K55" s="149"/>
       <c r="L55" s="156"/>
@@ -4256,7 +4218,7 @@
       <c r="AC55" s="1"/>
       <c r="AD55" s="1"/>
     </row>
-    <row r="56" spans="1:30" s="62" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:30" s="62" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A56" s="27"/>
       <c r="B56" s="18"/>
       <c r="C56" s="18"/>
@@ -4265,7 +4227,7 @@
       <c r="H56" s="34"/>
       <c r="I56" s="34"/>
       <c r="J56" s="128" t="s">
-        <v>70</v>
+        <v>226</v>
       </c>
       <c r="K56" s="149"/>
       <c r="L56" s="162"/>
@@ -4288,7 +4250,7 @@
       <c r="AC56" s="18"/>
       <c r="AD56" s="18"/>
     </row>
-    <row r="57" spans="1:30" s="179" customFormat="1" ht="81.599999999999994" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:30" s="179" customFormat="1" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A57" s="192"/>
       <c r="B57" s="178"/>
       <c r="C57" s="178"/>
@@ -4297,7 +4259,7 @@
       <c r="H57" s="35"/>
       <c r="I57" s="35"/>
       <c r="J57" s="123" t="s">
-        <v>71</v>
+        <v>225</v>
       </c>
       <c r="K57" s="181"/>
       <c r="L57" s="180"/>
@@ -4329,7 +4291,7 @@
       <c r="H58" s="185"/>
       <c r="I58" s="185"/>
       <c r="J58" s="186" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="K58" s="187"/>
       <c r="L58" s="188"/>
@@ -4354,24 +4316,24 @@
     </row>
     <row r="59" spans="1:30" s="62" customFormat="1" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="B59" s="118" t="s">
-        <v>74</v>
+        <v>224</v>
       </c>
       <c r="C59" s="169" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D59" s="93" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="E59" s="34" t="s">
-        <v>64</v>
+        <v>208</v>
       </c>
       <c r="H59" s="35"/>
       <c r="I59" s="35"/>
       <c r="J59" s="123" t="s">
-        <v>76</v>
+        <v>223</v>
       </c>
       <c r="K59" s="149"/>
       <c r="L59" s="150"/>
@@ -4399,13 +4361,13 @@
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
       <c r="D60" s="93" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="E60" s="11"/>
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
       <c r="J60" s="119" t="s">
-        <v>78</v>
+        <v>222</v>
       </c>
       <c r="K60" s="149"/>
       <c r="L60" s="157"/>
@@ -4437,7 +4399,7 @@
       <c r="H61" s="11"/>
       <c r="I61" s="11"/>
       <c r="J61" s="120" t="s">
-        <v>79</v>
+        <v>221</v>
       </c>
       <c r="K61" s="149"/>
       <c r="L61" s="157"/>
@@ -4469,7 +4431,7 @@
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
       <c r="J62" s="119" t="s">
-        <v>80</v>
+        <v>220</v>
       </c>
       <c r="K62" s="149"/>
       <c r="L62" s="157"/>
@@ -4501,7 +4463,7 @@
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
       <c r="J63" s="119" t="s">
-        <v>81</v>
+        <v>219</v>
       </c>
       <c r="K63" s="149"/>
       <c r="L63" s="157"/>
@@ -4533,7 +4495,7 @@
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
       <c r="J64" s="119" t="s">
-        <v>82</v>
+        <v>218</v>
       </c>
       <c r="K64" s="149"/>
       <c r="L64" s="157"/>
@@ -4565,7 +4527,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="11"/>
       <c r="J65" s="120" t="s">
-        <v>83</v>
+        <v>217</v>
       </c>
       <c r="K65" s="149"/>
       <c r="L65" s="157"/>
@@ -4590,16 +4552,16 @@
     </row>
     <row r="66" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A66" s="29" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="B66" s="117" t="s">
-        <v>85</v>
+        <v>216</v>
       </c>
       <c r="C66" s="53">
         <v>1</v>
       </c>
       <c r="D66" s="91" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="E66" s="26"/>
       <c r="F66" s="73"/>
@@ -4607,7 +4569,7 @@
       <c r="H66" s="32"/>
       <c r="I66" s="32"/>
       <c r="J66" s="129" t="s">
-        <v>87</v>
+        <v>215</v>
       </c>
       <c r="K66" s="152"/>
       <c r="L66" s="154"/>
@@ -4630,12 +4592,12 @@
       <c r="AC66" s="1"/>
       <c r="AD66" s="1"/>
     </row>
-    <row r="67" spans="1:30" ht="42" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:30" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A67" s="27"/>
       <c r="B67" s="18"/>
       <c r="C67" s="18"/>
       <c r="D67" s="91" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="E67" s="18"/>
       <c r="F67" s="62"/>
@@ -4643,7 +4605,7 @@
       <c r="H67" s="34"/>
       <c r="I67" s="34"/>
       <c r="J67" s="128" t="s">
-        <v>89</v>
+        <v>214</v>
       </c>
       <c r="K67" s="149"/>
       <c r="L67" s="150"/>
@@ -4677,7 +4639,7 @@
       <c r="H68" s="101"/>
       <c r="I68" s="101"/>
       <c r="J68" s="130" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="K68" s="158"/>
       <c r="L68" s="160"/>
@@ -4700,22 +4662,22 @@
       <c r="AC68" s="1"/>
       <c r="AD68" s="1"/>
     </row>
-    <row r="69" spans="1:30" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A69" s="27" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="B69" s="131" t="s">
-        <v>92</v>
+        <v>212</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="102" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="E69" s="1"/>
       <c r="H69" s="11"/>
       <c r="I69" s="11"/>
       <c r="J69" s="120" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="K69" s="149"/>
       <c r="L69" s="157"/>
@@ -4743,13 +4705,13 @@
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="102" t="s">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="E70" s="1"/>
       <c r="H70" s="11"/>
       <c r="I70" s="11"/>
       <c r="J70" s="120" t="s">
-        <v>96</v>
+        <v>211</v>
       </c>
       <c r="K70" s="149"/>
       <c r="L70" s="157"/>
@@ -4781,7 +4743,7 @@
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
       <c r="J71" s="120" t="s">
-        <v>97</v>
+        <v>210</v>
       </c>
       <c r="K71" s="149"/>
       <c r="L71" s="157"/>
@@ -4809,21 +4771,21 @@
         <v>2</v>
       </c>
       <c r="B72" s="49" t="s">
-        <v>98</v>
+        <v>209</v>
       </c>
       <c r="C72" s="170" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="D72" s="49"/>
       <c r="E72" s="34" t="s">
-        <v>64</v>
+        <v>208</v>
       </c>
       <c r="F72" s="73"/>
       <c r="G72" s="73"/>
       <c r="H72" s="31"/>
       <c r="I72" s="31"/>
       <c r="J72" s="115" t="s">
-        <v>99</v>
+        <v>207</v>
       </c>
       <c r="K72" s="42">
         <v>1</v>
@@ -4862,7 +4824,7 @@
       <c r="H73" s="13"/>
       <c r="I73" s="13"/>
       <c r="J73" s="119" t="s">
-        <v>100</v>
+        <v>206</v>
       </c>
       <c r="K73" s="43"/>
       <c r="L73" s="2"/>
@@ -4902,7 +4864,7 @@
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
       <c r="J74" s="119" t="s">
-        <v>101</v>
+        <v>205</v>
       </c>
       <c r="K74" s="43">
         <v>1</v>
@@ -4940,7 +4902,7 @@
       <c r="H75" s="13"/>
       <c r="I75" s="13"/>
       <c r="J75" s="119" t="s">
-        <v>102</v>
+        <v>204</v>
       </c>
       <c r="K75" s="43"/>
       <c r="L75" s="2"/>
@@ -4978,7 +4940,7 @@
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
       <c r="J76" s="119" t="s">
-        <v>103</v>
+        <v>203</v>
       </c>
       <c r="K76" s="43"/>
       <c r="L76" s="2"/>
@@ -5016,7 +4978,7 @@
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
       <c r="J77" s="119" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="K77" s="43">
         <v>1</v>
@@ -5052,7 +5014,7 @@
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
       <c r="J78" s="34" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="K78" s="43"/>
       <c r="L78" s="2"/>
@@ -5080,7 +5042,7 @@
         <v>3</v>
       </c>
       <c r="B79" s="132" t="s">
-        <v>105</v>
+        <v>201</v>
       </c>
       <c r="C79" s="49"/>
       <c r="D79" s="49"/>
@@ -5090,7 +5052,7 @@
       <c r="H79" s="23"/>
       <c r="I79" s="23"/>
       <c r="J79" s="115" t="s">
-        <v>106</v>
+        <v>200</v>
       </c>
       <c r="K79" s="42">
         <v>1</v>
@@ -5126,7 +5088,7 @@
       <c r="H80" s="17"/>
       <c r="I80" s="17"/>
       <c r="J80" s="119" t="s">
-        <v>107</v>
+        <v>199</v>
       </c>
       <c r="K80" s="43"/>
       <c r="L80" s="2"/>
@@ -5164,7 +5126,7 @@
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
       <c r="J81" s="119" t="s">
-        <v>108</v>
+        <v>198</v>
       </c>
       <c r="K81" s="43"/>
       <c r="L81" s="2"/>
@@ -5202,7 +5164,7 @@
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
       <c r="J82" s="119" t="s">
-        <v>109</v>
+        <v>197</v>
       </c>
       <c r="K82" s="43"/>
       <c r="L82" s="2"/>
@@ -5236,7 +5198,7 @@
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
       <c r="J83" s="119" t="s">
-        <v>110</v>
+        <v>196</v>
       </c>
       <c r="K83" s="43"/>
       <c r="L83" s="2"/>
@@ -5272,7 +5234,7 @@
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
       <c r="J84" s="119" t="s">
-        <v>111</v>
+        <v>195</v>
       </c>
       <c r="K84" s="43"/>
       <c r="L84" s="2"/>
@@ -5308,7 +5270,7 @@
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
       <c r="J85" s="119" t="s">
-        <v>112</v>
+        <v>194</v>
       </c>
       <c r="K85" s="43"/>
       <c r="L85" s="2"/>
@@ -5338,25 +5300,25 @@
         <v>4</v>
       </c>
       <c r="B86" s="117" t="s">
-        <v>113</v>
+        <v>193</v>
       </c>
       <c r="C86" s="49"/>
       <c r="D86" s="51"/>
       <c r="E86" s="127" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="F86" s="52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G86" s="166"/>
       <c r="H86" s="115" t="s">
-        <v>116</v>
+        <v>192</v>
       </c>
       <c r="I86" s="176" t="s">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="J86" s="115" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="K86" s="42">
         <v>1</v>
@@ -5389,7 +5351,7 @@
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
       <c r="J87" s="119" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="K87" s="43">
         <v>1</v>
@@ -5425,7 +5387,7 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
       <c r="J88" s="119" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="K88" s="43">
         <v>1</v>
@@ -5463,7 +5425,7 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
       <c r="J89" s="119" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="K89" s="43">
         <v>1</v>
@@ -5501,7 +5463,7 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="119" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K90" s="43"/>
       <c r="L90" s="2"/>
@@ -5537,7 +5499,7 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="119" t="s">
-        <v>123</v>
+        <v>191</v>
       </c>
       <c r="K91" s="43">
         <v>1</v>
@@ -5573,7 +5535,7 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="119" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="K92" s="43">
         <v>1</v>
@@ -5611,7 +5573,7 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
       <c r="J93" s="119" t="s">
-        <v>125</v>
+        <v>190</v>
       </c>
       <c r="K93" s="43">
         <v>1</v>
@@ -5647,7 +5609,7 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="119" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="K94" s="43">
         <v>1</v>
@@ -5685,7 +5647,7 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
       <c r="J95" s="119" t="s">
-        <v>127</v>
+        <v>169</v>
       </c>
       <c r="K95" s="43">
         <v>1</v>
@@ -5721,7 +5683,7 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="119" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="K96" s="43"/>
       <c r="L96" s="2">
@@ -5757,7 +5719,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="119" t="s">
-        <v>129</v>
+        <v>189</v>
       </c>
       <c r="K97" s="43">
         <v>1</v>
@@ -5795,7 +5757,7 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="119" t="s">
-        <v>130</v>
+        <v>185</v>
       </c>
       <c r="K98" s="43">
         <v>1</v>
@@ -5833,7 +5795,7 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="119" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="K99" s="43">
         <v>1</v>
@@ -5871,7 +5833,7 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="34" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="K100" s="43"/>
       <c r="L100" s="2"/>
@@ -5901,17 +5863,17 @@
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="52" t="s">
-        <v>132</v>
+        <v>188</v>
       </c>
       <c r="G101" s="1"/>
       <c r="H101" s="115" t="s">
-        <v>133</v>
+        <v>187</v>
       </c>
       <c r="I101" s="177" t="s">
-        <v>134</v>
+        <v>38</v>
       </c>
       <c r="J101" s="115" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="K101" s="143">
         <v>1</v>
@@ -5945,11 +5907,11 @@
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="12" t="s">
-        <v>135</v>
+        <v>39</v>
       </c>
       <c r="I102" s="12"/>
       <c r="J102" s="119" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="K102" s="146">
         <v>1</v>
@@ -5985,7 +5947,7 @@
       <c r="H103" s="12"/>
       <c r="I103" s="12"/>
       <c r="J103" s="119" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="K103" s="146">
         <v>1</v>
@@ -6021,7 +5983,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="12"/>
       <c r="J104" s="119" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="K104" s="146">
         <v>1</v>
@@ -6057,7 +6019,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="12"/>
       <c r="J105" s="119" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="K105" s="146">
         <v>1</v>
@@ -6093,7 +6055,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
       <c r="J106" s="119" t="s">
-        <v>127</v>
+        <v>169</v>
       </c>
       <c r="K106" s="146">
         <v>1</v>
@@ -6129,7 +6091,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
       <c r="J107" s="119" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="K107" s="146"/>
       <c r="L107" s="147">
@@ -6165,7 +6127,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
       <c r="J108" s="119" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="K108" s="146">
         <v>1</v>
@@ -6203,7 +6165,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
       <c r="J109" s="13" t="s">
-        <v>137</v>
+        <v>186</v>
       </c>
       <c r="K109" s="146">
         <v>1</v>
@@ -6239,7 +6201,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
       <c r="J110" s="119" t="s">
-        <v>130</v>
+        <v>185</v>
       </c>
       <c r="K110" s="146">
         <v>1</v>
@@ -6277,7 +6239,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
       <c r="J111" s="119" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="K111" s="146">
         <v>1</v>
@@ -6315,7 +6277,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
       <c r="J112" s="34" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="K112" s="146"/>
       <c r="L112" s="147"/>
@@ -6345,17 +6307,17 @@
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="133" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
       <c r="G113" s="53"/>
       <c r="H113" s="115" t="s">
-        <v>139</v>
+        <v>182</v>
       </c>
       <c r="I113" s="177" t="s">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="J113" s="115" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="K113" s="42"/>
       <c r="L113" s="24"/>
@@ -6393,7 +6355,7 @@
       <c r="H114" s="17"/>
       <c r="I114" s="17"/>
       <c r="J114" s="119" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="K114" s="43"/>
       <c r="L114" s="2"/>
@@ -6433,7 +6395,7 @@
       <c r="H115" s="1"/>
       <c r="I115" s="1"/>
       <c r="J115" s="119" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="K115" s="43"/>
       <c r="L115" s="2"/>
@@ -6473,7 +6435,7 @@
       <c r="H116" s="1"/>
       <c r="I116" s="1"/>
       <c r="J116" s="119" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="K116" s="43"/>
       <c r="L116" s="2"/>
@@ -6513,7 +6475,7 @@
       <c r="H117" s="1"/>
       <c r="I117" s="1"/>
       <c r="J117" s="119" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="K117" s="43"/>
       <c r="L117" s="2"/>
@@ -6553,7 +6515,7 @@
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
       <c r="J118" s="119" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="K118" s="43"/>
       <c r="L118" s="2"/>
@@ -6591,7 +6553,7 @@
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
       <c r="J119" s="119" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="K119" s="43"/>
       <c r="L119" s="2"/>
@@ -6631,7 +6593,7 @@
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
       <c r="J120" s="119" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="K120" s="43"/>
       <c r="L120" s="2">
@@ -6667,7 +6629,7 @@
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="119" t="s">
-        <v>56</v>
+        <v>165</v>
       </c>
       <c r="K121" s="43"/>
       <c r="L121" s="2">
@@ -6705,7 +6667,7 @@
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
       <c r="J122" s="119" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="K122" s="43"/>
       <c r="L122" s="2"/>
@@ -6745,7 +6707,7 @@
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
       <c r="J123" s="119" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="K123" s="43"/>
       <c r="L123" s="2">
@@ -6781,7 +6743,7 @@
       <c r="H124" s="1"/>
       <c r="I124" s="1"/>
       <c r="J124" s="34" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="K124" s="43"/>
       <c r="L124" s="2"/>
@@ -6811,17 +6773,17 @@
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="117" t="s">
-        <v>144</v>
+        <v>177</v>
       </c>
       <c r="G125" s="52"/>
       <c r="H125" s="115" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="I125" s="177" t="s">
-        <v>146</v>
+        <v>41</v>
       </c>
       <c r="J125" s="115" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="K125" s="42"/>
       <c r="L125" s="24"/>
@@ -6859,7 +6821,7 @@
       <c r="H126" s="17"/>
       <c r="I126" s="17"/>
       <c r="J126" s="119" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="K126" s="43"/>
       <c r="L126" s="2"/>
@@ -6897,7 +6859,7 @@
       <c r="H127" s="1"/>
       <c r="I127" s="1"/>
       <c r="J127" s="119" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="K127" s="43"/>
       <c r="L127" s="2"/>
@@ -6935,7 +6897,7 @@
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
       <c r="J128" s="119" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="K128" s="43"/>
       <c r="L128" s="2"/>
@@ -6973,7 +6935,7 @@
       <c r="H129" s="1"/>
       <c r="I129" s="1"/>
       <c r="J129" s="119" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="K129" s="43"/>
       <c r="L129" s="2"/>
@@ -7009,7 +6971,7 @@
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
       <c r="J130" s="119" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="K130" s="43"/>
       <c r="L130" s="2"/>
@@ -7045,7 +7007,7 @@
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
       <c r="J131" s="119" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="K131" s="43"/>
       <c r="L131" s="2"/>
@@ -7085,7 +7047,7 @@
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
       <c r="J132" s="119" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="K132" s="43"/>
       <c r="L132" s="2">
@@ -7121,7 +7083,7 @@
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
       <c r="J133" s="119" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="K133" s="43"/>
       <c r="L133" s="2"/>
@@ -7159,7 +7121,7 @@
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
       <c r="J134" s="34" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="K134" s="43"/>
       <c r="L134" s="2"/>
@@ -7189,17 +7151,17 @@
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
       <c r="F135" s="133" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="G135" s="53"/>
       <c r="H135" s="115" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="I135" s="177" t="s">
-        <v>151</v>
+        <v>42</v>
       </c>
       <c r="J135" s="115" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="K135" s="42"/>
       <c r="L135" s="24"/>
@@ -7237,7 +7199,7 @@
       <c r="H136" s="17"/>
       <c r="I136" s="17"/>
       <c r="J136" s="119" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="K136" s="43"/>
       <c r="L136" s="2"/>
@@ -7277,7 +7239,7 @@
       <c r="H137" s="1"/>
       <c r="I137" s="1"/>
       <c r="J137" s="119" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="K137" s="43"/>
       <c r="L137" s="2"/>
@@ -7315,7 +7277,7 @@
       <c r="H138" s="1"/>
       <c r="I138" s="1"/>
       <c r="J138" s="119" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="K138" s="43"/>
       <c r="L138" s="2"/>
@@ -7353,7 +7315,7 @@
       <c r="H139" s="1"/>
       <c r="I139" s="1"/>
       <c r="J139" s="119" t="s">
-        <v>127</v>
+        <v>169</v>
       </c>
       <c r="K139" s="43"/>
       <c r="L139" s="2"/>
@@ -7389,7 +7351,7 @@
       <c r="H140" s="1"/>
       <c r="I140" s="1"/>
       <c r="J140" s="119" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="K140" s="43"/>
       <c r="L140" s="2"/>
@@ -7425,7 +7387,7 @@
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
       <c r="J141" s="119" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="K141" s="43"/>
       <c r="L141" s="2"/>
@@ -7461,7 +7423,7 @@
       <c r="H142" s="1"/>
       <c r="I142" s="1"/>
       <c r="J142" s="119" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="K142" s="43"/>
       <c r="L142" s="2"/>
@@ -7497,7 +7459,7 @@
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
       <c r="J143" s="119" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="K143" s="43"/>
       <c r="L143" s="2"/>
@@ -7535,7 +7497,7 @@
       <c r="H144" s="1"/>
       <c r="I144" s="1"/>
       <c r="J144" s="119" t="s">
-        <v>56</v>
+        <v>165</v>
       </c>
       <c r="K144" s="43"/>
       <c r="L144" s="2">
@@ -7573,7 +7535,7 @@
       <c r="H145" s="1"/>
       <c r="I145" s="1"/>
       <c r="J145" s="119" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="K145" s="43"/>
       <c r="L145" s="2">
@@ -7609,7 +7571,7 @@
       <c r="H146" s="1"/>
       <c r="I146" s="1"/>
       <c r="J146" s="119" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="K146" s="43"/>
       <c r="L146" s="2"/>
@@ -7647,7 +7609,7 @@
       <c r="H147" s="1"/>
       <c r="I147" s="1"/>
       <c r="J147" s="34" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="K147" s="43"/>
       <c r="L147" s="2"/>
@@ -7677,17 +7639,17 @@
       <c r="D148" s="18"/>
       <c r="E148" s="18"/>
       <c r="F148" s="132" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="G148" s="49"/>
       <c r="H148" s="115" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="I148" s="177" t="s">
-        <v>158</v>
+        <v>43</v>
       </c>
       <c r="J148" s="115" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="K148" s="42"/>
       <c r="L148" s="24"/>
@@ -7721,7 +7683,7 @@
       <c r="H149" s="17"/>
       <c r="I149" s="17"/>
       <c r="J149" s="119" t="s">
-        <v>119</v>
+        <v>161</v>
       </c>
       <c r="K149" s="43"/>
       <c r="L149" s="2"/>
@@ -7759,7 +7721,7 @@
       <c r="H150" s="1"/>
       <c r="I150" s="1"/>
       <c r="J150" s="119" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="K150" s="43"/>
       <c r="L150" s="2"/>
@@ -7795,7 +7757,7 @@
       <c r="H151" s="1"/>
       <c r="I151" s="1"/>
       <c r="J151" s="119" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="K151" s="43"/>
       <c r="L151" s="2"/>
@@ -7831,7 +7793,7 @@
       <c r="H152" s="1"/>
       <c r="I152" s="1"/>
       <c r="J152" s="119" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="K152" s="43"/>
       <c r="L152" s="2"/>
@@ -7867,7 +7829,7 @@
       <c r="H153" s="1"/>
       <c r="I153" s="1"/>
       <c r="J153" s="119" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="K153" s="43"/>
       <c r="L153" s="2">
@@ -7903,7 +7865,7 @@
       <c r="H154" s="1"/>
       <c r="I154" s="1"/>
       <c r="J154" s="119" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="K154" s="43"/>
       <c r="L154" s="2"/>
@@ -7941,7 +7903,7 @@
       <c r="H155" s="61"/>
       <c r="I155" s="18"/>
       <c r="J155" s="119" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="K155" s="65"/>
       <c r="L155" s="66"/>
@@ -7969,23 +7931,23 @@
         <v>5</v>
       </c>
       <c r="B156" s="118" t="s">
-        <v>161</v>
+        <v>263</v>
       </c>
       <c r="C156" s="54">
         <v>3</v>
       </c>
       <c r="D156" s="93" t="s">
-        <v>162</v>
+        <v>44</v>
       </c>
       <c r="E156" s="123" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F156" s="18"/>
       <c r="G156" s="18"/>
       <c r="H156" s="18"/>
       <c r="I156" s="18"/>
       <c r="J156" s="123" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="K156" s="43"/>
       <c r="L156" s="36"/>
@@ -8013,7 +7975,7 @@
       <c r="B157" s="13"/>
       <c r="C157" s="13"/>
       <c r="D157" s="93" t="s">
-        <v>165</v>
+        <v>45</v>
       </c>
       <c r="E157" s="13"/>
       <c r="F157" s="1"/>
@@ -8021,7 +7983,7 @@
       <c r="H157" s="1"/>
       <c r="I157" s="1"/>
       <c r="J157" s="34" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="K157" s="43"/>
       <c r="L157" s="2"/>
@@ -8055,7 +8017,7 @@
       <c r="H158" s="1"/>
       <c r="I158" s="1"/>
       <c r="J158" s="119" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="K158" s="43"/>
       <c r="L158" s="2"/>
@@ -8089,7 +8051,7 @@
       <c r="H159" s="1"/>
       <c r="I159" s="1"/>
       <c r="J159" s="34" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="K159" s="43"/>
       <c r="L159" s="2"/>
@@ -8123,7 +8085,7 @@
       <c r="H160" s="1"/>
       <c r="I160" s="1"/>
       <c r="J160" s="119" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="K160" s="43"/>
       <c r="L160" s="2"/>
@@ -8157,7 +8119,7 @@
       <c r="H161" s="1"/>
       <c r="I161" s="1"/>
       <c r="J161" s="34" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="K161" s="43"/>
       <c r="L161" s="2"/>
@@ -8191,7 +8153,7 @@
       <c r="H162" s="1"/>
       <c r="I162" s="1"/>
       <c r="J162" s="119" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="K162" s="43"/>
       <c r="L162" s="2"/>
@@ -8225,7 +8187,7 @@
       <c r="H163" s="1"/>
       <c r="I163" s="1"/>
       <c r="J163" s="34" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="K163" s="43"/>
       <c r="L163" s="2"/>
@@ -8259,7 +8221,7 @@
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
       <c r="J164" s="119" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="K164" s="43"/>
       <c r="L164" s="2"/>
@@ -8293,7 +8255,7 @@
       <c r="H165" s="1"/>
       <c r="I165" s="1"/>
       <c r="J165" s="34" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="K165" s="43"/>
       <c r="L165" s="2"/>
@@ -8316,7 +8278,7 @@
       <c r="AC165" s="1"/>
       <c r="AD165" s="1"/>
     </row>
-    <row r="166" spans="1:30" ht="81.599999999999994" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:30" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A166" s="27"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -8327,7 +8289,7 @@
       <c r="H166" s="1"/>
       <c r="I166" s="1"/>
       <c r="J166" s="119" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="K166" s="43"/>
       <c r="L166" s="2"/>
@@ -8361,7 +8323,7 @@
       <c r="H167" s="1"/>
       <c r="I167" s="1"/>
       <c r="J167" s="119" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="K167" s="43"/>
       <c r="L167" s="2"/>
@@ -8395,7 +8357,7 @@
       <c r="H168" s="1"/>
       <c r="I168" s="1"/>
       <c r="J168" s="119" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="K168" s="43"/>
       <c r="L168" s="2"/>
@@ -8429,7 +8391,7 @@
       <c r="H169" s="1"/>
       <c r="I169" s="1"/>
       <c r="J169" s="34" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="K169" s="43"/>
       <c r="L169" s="2"/>
@@ -8463,7 +8425,7 @@
       <c r="H170" s="1"/>
       <c r="I170" s="1"/>
       <c r="J170" s="34" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
       <c r="K170" s="43"/>
       <c r="L170" s="2"/>
@@ -8497,7 +8459,7 @@
       <c r="H171" s="1"/>
       <c r="I171" s="1"/>
       <c r="J171" s="119" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="K171" s="43"/>
       <c r="L171" s="2"/>
@@ -8531,7 +8493,7 @@
       <c r="H172" s="1"/>
       <c r="I172" s="1"/>
       <c r="J172" s="34" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="K172" s="43"/>
       <c r="L172" s="2"/>
@@ -8554,7 +8516,7 @@
       <c r="AC172" s="1"/>
       <c r="AD172" s="1"/>
     </row>
-    <row r="173" spans="1:30" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:30" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A173" s="27"/>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -8565,7 +8527,7 @@
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
       <c r="J173" s="34" t="s">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="K173" s="43"/>
       <c r="L173" s="2"/>
@@ -8588,7 +8550,7 @@
       <c r="AC173" s="1"/>
       <c r="AD173" s="1"/>
     </row>
-    <row r="174" spans="1:30" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:30" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A174" s="27"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -8599,7 +8561,7 @@
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
       <c r="J174" s="34" t="s">
-        <v>183</v>
+        <v>136</v>
       </c>
       <c r="K174" s="43"/>
       <c r="L174" s="2"/>
@@ -8633,7 +8595,7 @@
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
       <c r="J175" s="34" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="K175" s="43"/>
       <c r="L175" s="2"/>
@@ -8667,7 +8629,7 @@
       <c r="H176" s="61"/>
       <c r="I176" s="61"/>
       <c r="J176" s="101" t="s">
-        <v>72</v>
+        <v>134</v>
       </c>
       <c r="K176" s="65"/>
       <c r="L176" s="66"/>
@@ -8695,21 +8657,21 @@
         <v>6</v>
       </c>
       <c r="B177" s="125" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="C177" s="50">
         <v>1</v>
       </c>
       <c r="D177" s="50"/>
       <c r="E177" s="127" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="F177" s="62"/>
       <c r="G177" s="35"/>
       <c r="H177" s="35"/>
       <c r="I177" s="35"/>
       <c r="J177" s="123" t="s">
-        <v>186</v>
+        <v>131</v>
       </c>
       <c r="K177" s="43"/>
       <c r="L177" s="36"/>
@@ -8741,7 +8703,7 @@
       <c r="H178" s="35"/>
       <c r="I178" s="35"/>
       <c r="J178" s="34" t="s">
-        <v>187</v>
+        <v>130</v>
       </c>
       <c r="K178" s="43"/>
       <c r="L178" s="36"/>
@@ -8774,7 +8736,7 @@
       <c r="H179" s="13"/>
       <c r="I179" s="13"/>
       <c r="J179" s="119" t="s">
-        <v>188</v>
+        <v>129</v>
       </c>
       <c r="K179" s="43"/>
       <c r="L179" s="2"/>
@@ -8807,7 +8769,7 @@
       <c r="H180" s="13"/>
       <c r="I180" s="13"/>
       <c r="J180" s="119" t="s">
-        <v>189</v>
+        <v>128</v>
       </c>
       <c r="K180" s="43"/>
       <c r="L180" s="2"/>
@@ -8840,7 +8802,7 @@
       <c r="H181" s="13"/>
       <c r="I181" s="13"/>
       <c r="J181" s="34" t="s">
-        <v>190</v>
+        <v>127</v>
       </c>
       <c r="K181" s="43"/>
       <c r="L181" s="2"/>
@@ -8873,7 +8835,7 @@
       <c r="H182" s="13"/>
       <c r="I182" s="13"/>
       <c r="J182" s="119" t="s">
-        <v>191</v>
+        <v>126</v>
       </c>
       <c r="K182" s="43"/>
       <c r="L182" s="2"/>
@@ -8907,7 +8869,7 @@
       <c r="H183" s="70"/>
       <c r="I183" s="70"/>
       <c r="J183" s="121" t="s">
-        <v>192</v>
+        <v>122</v>
       </c>
       <c r="K183" s="65"/>
       <c r="L183" s="66"/>
@@ -8935,7 +8897,7 @@
         <v>7</v>
       </c>
       <c r="B184" s="125" t="s">
-        <v>193</v>
+        <v>125</v>
       </c>
       <c r="C184" s="50"/>
       <c r="D184" s="50"/>
@@ -8945,7 +8907,7 @@
       <c r="H184" s="35"/>
       <c r="I184" s="35"/>
       <c r="J184" s="35" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="K184" s="43"/>
       <c r="L184" s="36"/>
@@ -8978,7 +8940,7 @@
       <c r="H185" s="13"/>
       <c r="I185" s="13"/>
       <c r="J185" s="13" t="s">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="K185" s="43"/>
       <c r="L185" s="2"/>
@@ -9012,7 +8974,7 @@
       <c r="H186" s="70"/>
       <c r="I186" s="70"/>
       <c r="J186" s="121" t="s">
-        <v>192</v>
+        <v>122</v>
       </c>
       <c r="K186" s="65"/>
       <c r="L186" s="66"/>
@@ -9040,7 +9002,7 @@
         <v>8</v>
       </c>
       <c r="B187" s="118" t="s">
-        <v>195</v>
+        <v>121</v>
       </c>
       <c r="C187" s="62"/>
       <c r="D187" s="165">
@@ -9052,7 +9014,7 @@
       <c r="H187" s="35"/>
       <c r="I187" s="35"/>
       <c r="J187" s="123" t="s">
-        <v>196</v>
+        <v>120</v>
       </c>
       <c r="K187" s="43"/>
       <c r="L187" s="36"/>
@@ -9080,14 +9042,14 @@
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="93" t="s">
-        <v>197</v>
+        <v>46</v>
       </c>
       <c r="E188" s="1"/>
       <c r="G188" s="13"/>
       <c r="H188" s="13"/>
       <c r="I188" s="13"/>
       <c r="J188" s="119" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="K188" s="43"/>
       <c r="L188" s="2"/>
@@ -9120,7 +9082,7 @@
       <c r="H189" s="13"/>
       <c r="I189" s="13"/>
       <c r="J189" s="119" t="s">
-        <v>199</v>
+        <v>118</v>
       </c>
       <c r="K189" s="43"/>
       <c r="L189" s="2"/>
@@ -9153,7 +9115,7 @@
       <c r="H190" s="13"/>
       <c r="I190" s="13"/>
       <c r="J190" s="119" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="K190" s="43"/>
       <c r="L190" s="2"/>
@@ -9186,7 +9148,7 @@
       <c r="H191" s="13"/>
       <c r="I191" s="13"/>
       <c r="J191" s="119" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="K191" s="43"/>
       <c r="L191" s="2"/>
@@ -9212,7 +9174,7 @@
     <row r="192" spans="1:30" s="16" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="29"/>
       <c r="B192" s="197" t="s">
-        <v>200</v>
+        <v>116</v>
       </c>
       <c r="C192" s="198"/>
       <c r="D192" s="198"/>
@@ -9246,7 +9208,7 @@
     <row r="193" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="27"/>
       <c r="B193" s="134" t="s">
-        <v>201</v>
+        <v>115</v>
       </c>
       <c r="C193" s="78"/>
       <c r="D193" s="78"/>
@@ -9314,7 +9276,7 @@
         <v>9</v>
       </c>
       <c r="B195" s="117" t="s">
-        <v>202</v>
+        <v>114</v>
       </c>
       <c r="C195" s="52"/>
       <c r="D195" s="52"/>
@@ -9324,7 +9286,7 @@
       <c r="H195" s="31"/>
       <c r="I195" s="31"/>
       <c r="J195" s="31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K195" s="42">
         <v>1</v>
@@ -9355,14 +9317,16 @@
       <c r="A196" s="27"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
-      <c r="D196" s="1"/>
+      <c r="D196" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="E196" s="1"/>
       <c r="F196" s="119"/>
       <c r="G196" s="13"/>
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
       <c r="J196" s="119" t="s">
-        <v>203</v>
+        <v>112</v>
       </c>
       <c r="K196" s="43"/>
       <c r="L196" s="2"/>
@@ -9398,7 +9362,7 @@
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
       <c r="J197" s="119" t="s">
-        <v>204</v>
+        <v>111</v>
       </c>
       <c r="K197" s="43"/>
       <c r="L197" s="2"/>
@@ -9436,7 +9400,7 @@
       <c r="H198" s="19"/>
       <c r="I198" s="19"/>
       <c r="J198" s="135" t="s">
-        <v>205</v>
+        <v>110</v>
       </c>
       <c r="K198" s="43"/>
       <c r="L198" s="2"/>
@@ -9470,7 +9434,7 @@
       <c r="H199" s="19"/>
       <c r="I199" s="19"/>
       <c r="J199" s="72" t="s">
-        <v>206</v>
+        <v>109</v>
       </c>
       <c r="K199" s="43"/>
       <c r="L199" s="2"/>
@@ -9498,7 +9462,7 @@
         <v>10</v>
       </c>
       <c r="B200" s="52" t="s">
-        <v>207</v>
+        <v>108</v>
       </c>
       <c r="C200" s="57"/>
       <c r="D200" s="57"/>
@@ -9508,7 +9472,7 @@
       <c r="H200" s="31"/>
       <c r="I200" s="31"/>
       <c r="J200" s="31" t="s">
-        <v>208</v>
+        <v>107</v>
       </c>
       <c r="K200" s="42"/>
       <c r="L200" s="24"/>
@@ -9535,7 +9499,7 @@
       <c r="AC200" s="1"/>
       <c r="AD200" s="1"/>
     </row>
-    <row r="201" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A201" s="27"/>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -9546,7 +9510,7 @@
       <c r="H201" s="13"/>
       <c r="I201" s="13"/>
       <c r="J201" s="119" t="s">
-        <v>209</v>
+        <v>106</v>
       </c>
       <c r="K201" s="43">
         <v>1</v>
@@ -9588,7 +9552,7 @@
       <c r="H202" s="13"/>
       <c r="I202" s="13"/>
       <c r="J202" s="13" t="s">
-        <v>210</v>
+        <v>105</v>
       </c>
       <c r="K202" s="43"/>
       <c r="L202" s="2">
@@ -9616,7 +9580,7 @@
     <row r="203" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A203" s="29"/>
       <c r="B203" s="199" t="s">
-        <v>211</v>
+        <v>104</v>
       </c>
       <c r="C203" s="200"/>
       <c r="D203" s="200"/>
@@ -9652,13 +9616,13 @@
         <v>12</v>
       </c>
       <c r="B204" s="136" t="s">
-        <v>212</v>
+        <v>103</v>
       </c>
       <c r="C204" s="55"/>
       <c r="D204" s="55"/>
       <c r="E204" s="55"/>
       <c r="F204" s="39" t="s">
-        <v>213</v>
+        <v>102</v>
       </c>
       <c r="G204" s="34"/>
       <c r="H204" s="34"/>
@@ -9692,7 +9656,7 @@
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
       <c r="F205" s="40" t="s">
-        <v>214</v>
+        <v>101</v>
       </c>
       <c r="G205" s="34"/>
       <c r="H205" s="34"/>
@@ -9726,7 +9690,7 @@
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
       <c r="F206" s="104" t="s">
-        <v>215</v>
+        <v>47</v>
       </c>
       <c r="G206" s="18"/>
       <c r="H206" s="18"/>
@@ -9758,13 +9722,13 @@
         <v>13</v>
       </c>
       <c r="B207" s="136" t="s">
-        <v>216</v>
+        <v>100</v>
       </c>
       <c r="C207" s="55"/>
       <c r="D207" s="55"/>
       <c r="E207" s="55"/>
       <c r="F207" s="41" t="s">
-        <v>217</v>
+        <v>48</v>
       </c>
       <c r="G207" s="59"/>
       <c r="H207" s="59"/>
@@ -9796,13 +9760,13 @@
         <v>14</v>
       </c>
       <c r="B208" s="138" t="s">
-        <v>218</v>
+        <v>99</v>
       </c>
       <c r="C208" s="56"/>
       <c r="D208" s="56"/>
       <c r="E208" s="56"/>
       <c r="F208" s="142" t="s">
-        <v>219</v>
+        <v>49</v>
       </c>
       <c r="G208" s="18"/>
       <c r="H208" s="18"/>
@@ -9834,7 +9798,7 @@
         <v>15</v>
       </c>
       <c r="B209" s="138" t="s">
-        <v>220</v>
+        <v>98</v>
       </c>
       <c r="C209" s="56"/>
       <c r="D209" s="56"/>
@@ -9870,13 +9834,13 @@
         <v>16</v>
       </c>
       <c r="B210" s="138" t="s">
-        <v>221</v>
+        <v>97</v>
       </c>
       <c r="C210" s="56"/>
       <c r="D210" s="56"/>
       <c r="E210" s="56"/>
       <c r="F210" s="140" t="s">
-        <v>222</v>
+        <v>96</v>
       </c>
       <c r="G210" s="35"/>
       <c r="H210" s="35"/>
@@ -9910,7 +9874,7 @@
       <c r="D211" s="14"/>
       <c r="E211" s="14"/>
       <c r="F211" s="141" t="s">
-        <v>223</v>
+        <v>95</v>
       </c>
       <c r="G211" s="35"/>
       <c r="H211" s="35"/>
@@ -9944,7 +9908,7 @@
       <c r="D212" s="14"/>
       <c r="E212" s="14"/>
       <c r="F212" s="141" t="s">
-        <v>224</v>
+        <v>94</v>
       </c>
       <c r="G212" s="35"/>
       <c r="H212" s="35"/>
@@ -9978,7 +9942,7 @@
       <c r="D213" s="14"/>
       <c r="E213" s="14"/>
       <c r="F213" s="141" t="s">
-        <v>225</v>
+        <v>93</v>
       </c>
       <c r="G213" s="35"/>
       <c r="H213" s="35"/>
@@ -10012,7 +9976,7 @@
       <c r="D214" s="14"/>
       <c r="E214" s="14"/>
       <c r="F214" s="141" t="s">
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="G214" s="35"/>
       <c r="H214" s="35"/>
@@ -10050,7 +10014,7 @@
       <c r="H215" s="26"/>
       <c r="I215" s="26"/>
       <c r="J215" s="46" t="s">
-        <v>226</v>
+        <v>50</v>
       </c>
       <c r="K215" s="42">
         <f>SUM(K2:K214)</f>
@@ -10127,15 +10091,15 @@
         <v>17</v>
       </c>
       <c r="B217" s="139" t="s">
-        <v>227</v>
+        <v>91</v>
       </c>
       <c r="C217" s="26"/>
       <c r="D217" s="26"/>
       <c r="E217" s="97" t="s">
-        <v>228</v>
+        <v>51</v>
       </c>
       <c r="F217" s="107" t="s">
-        <v>229</v>
+        <v>90</v>
       </c>
       <c r="G217" s="26"/>
       <c r="H217" s="26"/>
@@ -10169,7 +10133,7 @@
       <c r="D218" s="61"/>
       <c r="E218" s="61"/>
       <c r="F218" s="121" t="s">
-        <v>230</v>
+        <v>89</v>
       </c>
       <c r="G218" s="61"/>
       <c r="H218" s="61"/>
@@ -10201,13 +10165,13 @@
         <v>18</v>
       </c>
       <c r="B219" s="171" t="s">
-        <v>231</v>
+        <v>88</v>
       </c>
       <c r="C219" s="172"/>
       <c r="D219" s="173"/>
       <c r="E219" s="173"/>
       <c r="F219" s="195" t="s">
-        <v>232</v>
+        <v>87</v>
       </c>
       <c r="G219" s="1"/>
       <c r="H219" s="1"/>
@@ -10271,15 +10235,15 @@
         <v>19</v>
       </c>
       <c r="B221" s="139" t="s">
-        <v>233</v>
+        <v>86</v>
       </c>
       <c r="C221" s="26"/>
       <c r="D221" s="73"/>
       <c r="E221" s="174" t="s">
-        <v>135</v>
+        <v>39</v>
       </c>
       <c r="F221" s="174" t="s">
-        <v>135</v>
+        <v>39</v>
       </c>
       <c r="G221" s="26"/>
       <c r="H221" s="26"/>
@@ -10312,10 +10276,10 @@
       <c r="C222" s="1"/>
       <c r="D222" s="1"/>
       <c r="E222" s="163" t="s">
-        <v>234</v>
+        <v>52</v>
       </c>
       <c r="F222" s="196" t="s">
-        <v>235</v>
+        <v>85</v>
       </c>
       <c r="G222" s="1"/>
       <c r="H222" s="1"/>
@@ -10349,7 +10313,7 @@
       <c r="D223" s="1"/>
       <c r="E223" s="1"/>
       <c r="F223" s="137" t="s">
-        <v>236</v>
+        <v>84</v>
       </c>
       <c r="G223" s="1"/>
       <c r="H223" s="1"/>
@@ -10381,11 +10345,11 @@
         <v>20</v>
       </c>
       <c r="B224" s="109" t="s">
-        <v>237</v>
+        <v>83</v>
       </c>
       <c r="C224" s="1"/>
       <c r="D224" s="93" t="s">
-        <v>238</v>
+        <v>53</v>
       </c>
       <c r="E224" s="1"/>
       <c r="F224" s="1"/>
@@ -10417,7 +10381,7 @@
     <row r="225" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="27"/>
       <c r="B225" s="175" t="s">
-        <v>239</v>
+        <v>82</v>
       </c>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
@@ -10451,7 +10415,7 @@
     <row r="226" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="27"/>
       <c r="B226" s="175" t="s">
-        <v>240</v>
+        <v>81</v>
       </c>
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
@@ -10485,7 +10449,7 @@
     <row r="227" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="27"/>
       <c r="B227" s="108" t="s">
-        <v>241</v>
+        <v>80</v>
       </c>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
@@ -10706,14 +10670,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="202" t="s">
-        <v>242</v>
+        <v>54</v>
       </c>
       <c r="B1" s="202"/>
       <c r="C1" s="21" t="s">
-        <v>243</v>
+        <v>55</v>
       </c>
       <c r="D1" s="201" t="s">
-        <v>244</v>
+        <v>56</v>
       </c>
       <c r="E1" s="201"/>
       <c r="F1" s="22"/>
@@ -10721,68 +10685,68 @@
     </row>
     <row r="2" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A2" s="110" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B2" s="105" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C2" s="193" t="s">
-        <v>245</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="110" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C3" s="194" t="s">
-        <v>246</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" s="111" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>247</v>
+        <v>59</v>
       </c>
       <c r="C4" s="194" t="s">
-        <v>248</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="111" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>249</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="110" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C6" s="194" t="s">
-        <v>250</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="111" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C7" s="194" t="s">
-        <v>251</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -11081,16 +11045,16 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix question 16 and errors
</commit_message>
<xml_diff>
--- a/media/questions.xlsx
+++ b/media/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ju5315jo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4902A36-EDF7-4252-B4C4-EF507AE07E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E636B75D-A305-404C-AF31-B68E041D71E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-216" yWindow="0" windowWidth="23256" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Yhdistetty" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="265">
   <si>
     <t>#</t>
   </si>
@@ -223,9 +223,15 @@
     <t>Suosin muita kulkutapoja.//Jag föredrar andra transportsätt.//I prefer using other means of transport.</t>
   </si>
   <si>
+    <t>Ympäristöön liittyvät syyt.//Miljöskäl.//For environmental reasons.</t>
+  </si>
+  <si>
     <t>Minulla ei ole ajokorttia.//Jag har inte körkort.//I don’t have a driving licence.</t>
   </si>
   <si>
+    <t>Muu//Annat//Other</t>
+  </si>
+  <si>
     <t>1b2</t>
   </si>
   <si>
@@ -244,6 +250,9 @@
     <t>** Esitä vain, jos vastaus polkupyörän kohdalla "aldrig" (1.5, 0)</t>
   </si>
   <si>
+    <t>Matkan pituus (liian lyhyt tai pitkä).//Resans längd (för kort eller lång).//The travel distance (too short or long).</t>
+  </si>
+  <si>
     <t>En halua saapua paikalle hikisenä.//Jag vill inte anlända svettig.//I don't want to arrive sweaty at the destination.</t>
   </si>
   <si>
@@ -256,9 +265,6 @@
     <t>En pysty yhdistämään pyöräilyä muihin tehtäviini, kuten lasten vientiin ja hakemiseen.//Jag kan inte kombinera cykling med mina andra uppgifter, som att föra och hämta barn.//I can't combine a bike with my other activities, e.g., dropping off and picking up children.</t>
   </si>
   <si>
-    <t>Muu//Annat//Other</t>
-  </si>
-  <si>
     <t>1b3</t>
   </si>
   <si>
@@ -337,6 +343,21 @@
     <t>Mitä kulkutapoja yhdistät toisinaan saman matkan aikana?//Vilka transportsätt kombinerar du ibland under samma resa?//Which modes of transport do you combine sometimes during the same travel?</t>
   </si>
   <si>
+    <t>Auto ja joukkoliikenne.//Bil och kollektivtrafik.//Car and public transport.</t>
+  </si>
+  <si>
+    <t>Polkupyörä tai sähköpotkulauta ja joukkoliikenne.//Cykel eller elsparkcykel och kollektivtrafik.//Bicycle or scooter and public transport.</t>
+  </si>
+  <si>
+    <t>Polkupyörä tai sähköpotkulauta ja auto.//Cykel eller elsparkcykel och bil.//Bicycle or scooter and car.</t>
+  </si>
+  <si>
+    <t>Mopo tai skootteri ja joukkoliikenne.//Moped eller skoter och kollektivtrafik.//Moped or motorcycle and public transport.</t>
+  </si>
+  <si>
+    <t>Pyörä ja kävely.//Cykel och gång.//Bicycle and walking.</t>
+  </si>
+  <si>
     <t>En koskaan yhdistele erilaisia kulkutapoja.//Jag kombinerar aldrig olika transportsätt.//I never combine different means of transport.</t>
   </si>
   <si>
@@ -379,6 +400,18 @@
     <t>3.0</t>
   </si>
   <si>
+    <t>Matkan hinta.//Resans pris.//Cost of the joyrney.</t>
+  </si>
+  <si>
+    <t>Matkan pituus.//Resans längd.//Travel distance.</t>
+  </si>
+  <si>
+    <t>Matkan kesto.//Resans längd i tid.//Travel time.</t>
+  </si>
+  <si>
+    <t>Säätila (sade, tuuli, jne.).//Väder (regn, vind, etc).//The weather (rain, wind etc).</t>
+  </si>
+  <si>
     <t>Vien tai haen lapset.//Jag för eller hämtar barnen.//I drop off or pick up children.</t>
   </si>
   <si>
@@ -397,6 +430,9 @@
     <t>Pidän omasta rauhasta.//Jag gillar att få vara i fred.//I like my privacy.</t>
   </si>
   <si>
+    <t>Tavan vuoksi. //För vanans skull.//Out of habit.</t>
+  </si>
+  <si>
     <t>Minulla on yrityksen tai työnantajan auto käytössäni.//Jag har en företags- eller arbetsgivarbil till mitt förfogande.//I use a company car.</t>
   </si>
   <si>
@@ -421,6 +457,9 @@
     <t>Haluan välttää liikenneruuhkat. //Jag vill undvika trafikstockningar.//I want to avoid traffic jams.</t>
   </si>
   <si>
+    <t>Vapauden tunne.//En känsla av frihet.//The sense of freedom.</t>
+  </si>
+  <si>
     <t>joukkoliikenne (juna, linja-auto)//kollektivtrafik (tåg, buss)//public transportation (train, bus)</t>
   </si>
   <si>
@@ -430,6 +469,12 @@
     <t>3.2</t>
   </si>
   <si>
+    <t>Voin käyttää matka-ajan työskentelyyn tai muihin tehtäviin. //Jag kan använda restiden till arbete eller andra uppgifter.//I use the travel time for work or other tasks.</t>
+  </si>
+  <si>
+    <t>Minulla on hyvät yhteydet joukkoliikenteellä (sisältäen riittävän vuorovälin).//Jag har goda förbindelser med kollektivtrafik (inklusive tillräcklig frekvens).//I havea good connection with transfer options (including good frequency) with public transport.</t>
+  </si>
+  <si>
     <t>Työnantajani edellyttää minulta joukkoliikenteen käyttöä. //Min arbetsgivare kräver att jag använder kollektivtrafiken.//My employer requires me to use public transport.</t>
   </si>
   <si>
@@ -442,6 +487,9 @@
     <t>3.3</t>
   </si>
   <si>
+    <t>Matkan kesto.//Resans längd i tid.//Tavel time.</t>
+  </si>
+  <si>
     <t>Työni edellyttää asiakastapaamisia ja minun tulee näyttää edustavalta. //Mitt jobb kräver kundmöten och jag måste se presentabel ut.//My job involves a lot of contact with customers and I need to look presentable.</t>
   </si>
   <si>
@@ -457,6 +505,12 @@
     <t>3.4</t>
   </si>
   <si>
+    <t>Ympäristölliset syyt.//Miljöskäl.//The environment.</t>
+  </si>
+  <si>
+    <t>Terveyteni.//Hälsoskäl.//My health.</t>
+  </si>
+  <si>
     <t>Minulla ei ole sopivia yhteyksiä tai vaihtomahdollisuuksia joukkoliikenteellä (sisältäen riittävän vuorovälin).//Jag har inte lämpliga anslutningar eller bytessmöjligheter med kollektivtrafik (inklusive tillräcklig frekvens).//I don't have a good connection or transfer options with public transport (frequency).</t>
   </si>
   <si>
@@ -472,160 +526,211 @@
     <t>3.5</t>
   </si>
   <si>
+    <t>Matkan hinta.//Resans pris.//Cost of the journey.</t>
+  </si>
+  <si>
+    <t>Mikä tai mitkä seuraavista saisivat sinut muuttamaan liikkumistottumuksiasi?//Vad skulle få dig att ändra dina mobilitetsvanor?//What would inspire you to change your travel habits?</t>
+  </si>
+  <si>
+    <t>1.0,3-4-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valitse 3 tärkeintä (Vedä tai tuplaklikkaa vastausvaihtoehtoja)//Välj de 3 viktigaste (Dra eller dubbelklicka på svarsalternativen)//List your top 3 (Drag or double-click your choices) </t>
+  </si>
+  <si>
+    <t>Ajansäästö.//Tidsbesparande.//Time gains.</t>
+  </si>
+  <si>
+    <t>&lt;&lt;kysy vain, jos henkilö vastasi kysymykseen 1 "bil"&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Hyvät joukkoliikenneyhteydet.//Bra förbindelser med kollektivtrafik.//A good connection with public transport.</t>
+  </si>
+  <si>
+    <t>Mahdollisuus käyttää joukkoliikennettä maksutta.//Möjlighet att använda kollektivtrafiken gratis.//A free public transport pass.</t>
+  </si>
+  <si>
+    <t>Liityntäpysäköinti- eli park and ride -mahdollisuuksien lisääntyminen.//Fler infartsparkeringsmöjligheter (Park &amp; Ride).//More Park &amp; Ride (P+R) options.</t>
+  </si>
+  <si>
+    <t>Turvallinen pyöräpysäköinti niissä sijainneissa, joihin pysäköin pyöräni.//Säker cykelparkering på platser där jag parkerar min cykel.//A secure bicycle parking at the location where I park my bike.</t>
+  </si>
+  <si>
+    <t>Mahdollisuus käydä suihkussa työpaikalla.//Möjlighet att duscha på arbetsplatsen.//Shower facilities at work.</t>
+  </si>
+  <si>
+    <t>Työsuhdepolkupyörä.//Företagscykel.//Company bicycle through my employer.</t>
+  </si>
+  <si>
+    <t>Reaaliaikaisen tiedon saaminen vaihtoyhteyksistä.//Realtidsinformation om bytesanslutningar i kollektivtrafiken.//Real-time information about transfer options.</t>
+  </si>
+  <si>
+    <t>Kestävää liikkumista tukevat työsuhde-edut.//Hållbar rörlighet stöds av anställningsförmåner.//Sustainable mobility is supported by employment benefits.</t>
+  </si>
+  <si>
+    <t>Sovellus, joka antaa reaaliaikaista tietoa liikenneruuhkista ja vaihtoehtoisista reiteistä.//En app som ger information i realtid om trafikstockningar och alternativa rutter.//A mobility app that provides real time information about traffic jams and the available alternatives.</t>
+  </si>
+  <si>
+    <t>Kaupunkipyöräasema lähellä kotiani.//Stadscykelstation nära mitt hem.//A bike sharing station in my neighbourhood.</t>
+  </si>
+  <si>
+    <t>Yhteiskäyttöauto lähellä kotiani.//Bil för delat bruk nära mitt hem.//A car sharing car in my neighbourhood.</t>
+  </si>
+  <si>
+    <t>Kaupunkipyöräjärjestelmän testausmahdollisuus.//Testperiod för stadscykelsystemet.//A test subscription to a bike sharing system.</t>
+  </si>
+  <si>
+    <t>Yhteiskäyttöautojen testausmahdollisuus.//Testperiod för bil med delat bruk.//A test subscription to a car sharing system.</t>
+  </si>
+  <si>
+    <t>Parempi ja turvallisempi pyöräilyverkosto.//Ett bättre och säkrare cykelnät.//Better and safer cycling infrastructure.</t>
+  </si>
+  <si>
+    <t>Sovellus, joka kannustaa minua tekemään parempia valintoja päivittäin.//En app som uppmuntrar mig att göra bättre val varje dag.//An app that encourages me to make better choices daily.</t>
+  </si>
+  <si>
+    <t>Ratkaisu, joka mahdollistaa lasten kuljettamisen auton sijaan. //Någon lösning för att föra och hämta barn.//A solution for dropping off and picking up the children.</t>
+  </si>
+  <si>
+    <t>Ei ole tapaa, jolla minut saisi muuttamaan käyttäytymistäni. //Det finns inget sätt att få mig att ändra mitt beteende.//You can't convince me to change my behaviour.</t>
+  </si>
+  <si>
+    <t>Vaihtoehto, joka on yhtä mukava ja luotettava kuin nykyinen. //Ett alternativ som är lika bekvämt och pålitligt som det nuvarande .//An alternative that is just as comfortable and reliable as current one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Työskenteletkö kotoa käsin?//Arbetar du hemifrån?//Do you sometimes work from home? </t>
+  </si>
+  <si>
+    <t>Kyllä, mutta korkeintaan päivän viikossa.//Ja, men inte mer än en dag i veckan.//Yes, but no more than 1 day a week.</t>
+  </si>
+  <si>
+    <t>Kyllä, 2-3 päivää viikossa.//Ja, 2-3 dagar i veckan.//Yes, 2-3 days a week.</t>
+  </si>
+  <si>
+    <t>Kyllä, useammin kuin kolmena päivänä viikossa. //Ja, mer än tre dagar i veckan.//Yes, more that 3 days a week.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En, työtäni ei pysty tekemään kotoa.//Nej, jag kan inte göra mitt jobb hemifrån.//No, I can't do my job at home. </t>
+  </si>
+  <si>
+    <t>En. Haluaisin, mutta työnantajani ei salli etätyötä. //Nej. Jag skulle vilja, men min arbetsgivare tillåter inte distansarbete.//No, I'd like to but my employer doesn't let me.</t>
+  </si>
+  <si>
+    <t>En, sillä en halua työskennellä kotoa käsin.//Nej, för jag vill inte jobba hemifrån.//No, I don't want to work from home.</t>
+  </si>
+  <si>
+    <t>Jokin muu tai ei sopivaa vastausvaihtoehtoa.//Annat eller inget lämpligt svarsalternativ.//Not applicable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onko sinun mahdollista kulkea kodin ja työpaikan välillä ruuhka-aikojen ulkopuolella?//Är det möjligt för dig att pendla mellan hemmet och jobbet under lågtrafik?//Would you be able to commute at other times of the day, i.e., outside of the rush hour? </t>
+  </si>
+  <si>
+    <t>Kyllä.//Ja.//Yes.</t>
+  </si>
+  <si>
+    <t>Ei.//Nej.//No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mikset voi matkustaa ruuhka-aikojen ulkopuolella?//Varför kan du inte resa under lågtrafik?//Why can’t you commute outside of the rush hour? </t>
+  </si>
+  <si>
+    <t>Teen kiinteitä työvuoroja.//Jag arbetar fasta skift.//I work fixed hours.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;&lt;kysy vain, jos vastaus kysymykseen 7 on "nej"&gt;&gt; 7, 1</t>
+  </si>
+  <si>
+    <t>Työnantajani ei mahdollista tätä.//Min arbetsgivare gör inte detta möjligt.//My employer doesn't allow this.</t>
+  </si>
+  <si>
+    <t>En ole valmis mukauttamaan työaikojani.//Jag är inte beredd att anpassa min arbetstid.//I'm not prepared to adapt my working hours.</t>
+  </si>
+  <si>
+    <t>Kategoria 2: Mitä tai miten ajattelet liikkumisesta(si)?//Kategori 2: Vad eller hur tänker du kring (din) mobilitet? Category 2: How you think about (your) mobility?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;&lt;valitse yksi vastaus per väittämä)//&lt;&lt;välj ett svar per påstående)//&lt;&lt;choose one option per statement&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Mikä seuraavista kulkumuodoista on mielestäsi välttämättömin? (Valitse sinua parhaiten kuvaava vaihtoehto.)//Vilket av följande transportsätt tycker du är det mest nödvändiga? (Välj det alternativ som bäst beskriver dig.) // Which of the following modes of transportation do you think is the most necessary? (Choose the option that best describes you.)</t>
+  </si>
+  <si>
+    <t>Auto.//Bil.//Car.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ad </t>
+  </si>
+  <si>
+    <t>Polkupyörä tai sähköpotkulauta.//Cykel tai elsparkcykel.//Bicycle or e-scooter.</t>
+  </si>
+  <si>
+    <t>Joukkoliikenne.//Kollektivtrafik.//Public transportation.</t>
+  </si>
+  <si>
+    <t>Ei mikään näistä.//Ingen av dessa.//None of these.</t>
+  </si>
+  <si>
+    <t>Kaikki ovat välttämättömiä kulkumuotoja.//Alla är oumbärliga transportsätt.//All are indispensable means of transport.</t>
+  </si>
+  <si>
+    <t>Tarkastatko ennen liikkeelle lähtöä, onko reitilläsi ruuhkaa? (Valitse sinua parhaiten kuvaava vaihtoehto.)//Innan du ger dig av, kontrollerar du om det är trafikstockning på din rutt? (Välj det alternativ som bäst beskriver dig.)//Do you check whether there are traffic jams on my route before leaving? (Please indicate the answer that suits you best.)</t>
+  </si>
+  <si>
+    <t>Joka kerta.//Alltid.//Every time.</t>
+  </si>
+  <si>
+    <t>Silloin tällöin.//Ibland.//Now and then.</t>
+  </si>
+  <si>
+    <t>En koskaan.//Aldrig.//Never.</t>
+  </si>
+  <si>
+    <t>Kategoria 3: Henkilötiedot//Kategori 3: Personuppgifter//Category 3: Personal data</t>
+  </si>
+  <si>
+    <t>Sukupuoli//Kön//Gender</t>
+  </si>
+  <si>
+    <t>Mies//Man//Male</t>
+  </si>
+  <si>
+    <t>Nainen//Kvinna//Female</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Syntymävuosi//Födelseår//Year of birth</t>
+  </si>
+  <si>
+    <t>(Pudotusvalikko)</t>
+  </si>
+  <si>
+    <t>Kotiosoitteeni postinumero//Postnummer för min hemadress//Post code of my home address</t>
+  </si>
+  <si>
+    <t>Pudotusvalikko Turun alueen postinumeroista ja "muu" (sulkee ulkopaikkakuntalaiset ulos datasta), vaihtoehtoisesti kotikunnat (Turun alue ja "muu"), Turun alueella asuville kysymys postinumerosta</t>
+  </si>
+  <si>
+    <t>Työ- tai opiskelupaikan postinumero: (Ohita kysymys, jos et opiskele tai käy töissä)//Postnumret på din arbetsplats eller studieort: (Hoppa över frågan om du inte studerar eller arbetar)//Post code of my work or study address: (In case you don't work or study, you can skip this question)</t>
+  </si>
+  <si>
+    <t>Asuminen//Boende//Living situation</t>
+  </si>
+  <si>
+    <t>Asun yksin ilman lapsia.//Jag bor ensam utan barn.//Single without children.</t>
+  </si>
+  <si>
+    <t>Asun yksin lasten kanssa.//Jag bor ensam med barn.//Single with children.</t>
+  </si>
+  <si>
+    <t>Asun puolison kanssa kaksin.//Jag bor tillsammans med min partner.//Co-habiting without children.</t>
+  </si>
+  <si>
+    <t>Asun puolison ja lasten kanssa.//Jag bor med min partner och barn.//Co-habiting with children.</t>
+  </si>
+  <si>
     <t>Muu://Annat://Other:</t>
-  </si>
-  <si>
-    <t>1.0,3-4-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valitse 3 tärkeintä (Vedä tai tuplaklikkaa vastausvaihtoehtoja)//Välj de 3 viktigaste (Dra eller dubbelklicka på svarsalternativen)//List your top 3 (Drag or double-click your choices) </t>
-  </si>
-  <si>
-    <t>&lt;&lt;kysy vain, jos henkilö vastasi kysymykseen 1 "bil"&gt;&gt;</t>
-  </si>
-  <si>
-    <t>Turvallinen pyöräpysäköinti niissä sijainneissa, joihin pysäköin pyöräni.//Säker cykelparkering på platser där jag parkerar min cykel.//A secure bicycle parking at the location where I park my bike.</t>
-  </si>
-  <si>
-    <t>Mahdollisuus käydä suihkussa työpaikalla.//Möjlighet att duscha på arbetsplatsen.//Shower facilities at work.</t>
-  </si>
-  <si>
-    <t>Reaaliaikaisen tiedon saaminen vaihtoyhteyksistä.//Realtidsinformation om bytesanslutningar i kollektivtrafiken.//Real-time information about transfer options.</t>
-  </si>
-  <si>
-    <t>Kestävää liikkumista tukevat työsuhde-edut.//Hållbar rörlighet stöds av anställningsförmåner.//Sustainable mobility is supported by employment benefits.</t>
-  </si>
-  <si>
-    <t>Sovellus, joka antaa reaaliaikaista tietoa liikenneruuhkista ja vaihtoehtoisista reiteistä.//En app som ger information i realtid om trafikstockningar och alternativa rutter.//A mobility app that provides real time information about traffic jams and the available alternatives.</t>
-  </si>
-  <si>
-    <t>Kaupunkipyöräasema lähellä kotiani.//Stadscykelstation nära mitt hem.//A bike sharing station in my neighbourhood.</t>
-  </si>
-  <si>
-    <t>Yhteiskäyttöauto lähellä kotiani.//Bil för delat bruk nära mitt hem.//A car sharing car in my neighbourhood.</t>
-  </si>
-  <si>
-    <t>Kaupunkipyöräjärjestelmän testausmahdollisuus.//Testperiod för stadscykelsystemet.//A test subscription to a bike sharing system.</t>
-  </si>
-  <si>
-    <t>Yhteiskäyttöautojen testausmahdollisuus.//Testperiod för bil med delat bruk.//A test subscription to a car sharing system.</t>
-  </si>
-  <si>
-    <t>Parempi ja turvallisempi pyöräilyverkosto.//Ett bättre och säkrare cykelnät.//Better and safer cycling infrastructure.</t>
-  </si>
-  <si>
-    <t>Sovellus, joka kannustaa minua tekemään parempia valintoja päivittäin.//En app som uppmuntrar mig att göra bättre val varje dag.//An app that encourages me to make better choices daily.</t>
-  </si>
-  <si>
-    <t>Ratkaisu, joka mahdollistaa lasten kuljettamisen auton sijaan. //Någon lösning för att föra och hämta barn.//A solution for dropping off and picking up the children.</t>
-  </si>
-  <si>
-    <t>Ei ole tapaa, jolla minut saisi muuttamaan käyttäytymistäni. //Det finns inget sätt att få mig att ändra mitt beteende.//You can't convince me to change my behaviour.</t>
-  </si>
-  <si>
-    <t>Vaihtoehto, joka on yhtä mukava ja luotettava kuin nykyinen. //Ett alternativ som är lika bekvämt och pålitligt som det nuvarande .//An alternative that is just as comfortable and reliable as current one.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Työskenteletkö kotoa käsin?//Arbetar du hemifrån?//Do you sometimes work from home? </t>
-  </si>
-  <si>
-    <t>Kyllä, mutta korkeintaan päivän viikossa.//Ja, men inte mer än en dag i veckan.//Yes, but no more than 1 day a week.</t>
-  </si>
-  <si>
-    <t>Kyllä, 2-3 päivää viikossa.//Ja, 2-3 dagar i veckan.//Yes, 2-3 days a week.</t>
-  </si>
-  <si>
-    <t>Kyllä, useammin kuin kolmena päivänä viikossa. //Ja, mer än tre dagar i veckan.//Yes, more that 3 days a week.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En, työtäni ei pysty tekemään kotoa.//Nej, jag kan inte göra mitt jobb hemifrån.//No, I can't do my job at home. </t>
-  </si>
-  <si>
-    <t>En. Haluaisin, mutta työnantajani ei salli etätyötä. //Nej. Jag skulle vilja, men min arbetsgivare tillåter inte distansarbete.//No, I'd like to but my employer doesn't let me.</t>
-  </si>
-  <si>
-    <t>En, sillä en halua työskennellä kotoa käsin.//Nej, för jag vill inte jobba hemifrån.//No, I don't want to work from home.</t>
-  </si>
-  <si>
-    <t>Jokin muu tai ei sopivaa vastausvaihtoehtoa.//Annat eller inget lämpligt svarsalternativ.//Not applicable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Onko sinun mahdollista kulkea kodin ja työpaikan välillä ruuhka-aikojen ulkopuolella?//Är det möjligt för dig att pendla mellan hemmet och jobbet under lågtrafik?//Would you be able to commute at other times of the day, i.e., outside of the rush hour? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mikset voi matkustaa ruuhka-aikojen ulkopuolella?//Varför kan du inte resa under lågtrafik?//Why can’t you commute outside of the rush hour? </t>
-  </si>
-  <si>
-    <t>Teen kiinteitä työvuoroja.//Jag arbetar fasta skift.//I work fixed hours.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;&lt;kysy vain, jos vastaus kysymykseen 7 on "nej"&gt;&gt; 7, 1</t>
-  </si>
-  <si>
-    <t>Työnantajani ei mahdollista tätä.//Min arbetsgivare gör inte detta möjligt.//My employer doesn't allow this.</t>
-  </si>
-  <si>
-    <t>En ole valmis mukauttamaan työaikojani.//Jag är inte beredd att anpassa min arbetstid.//I'm not prepared to adapt my working hours.</t>
-  </si>
-  <si>
-    <t>Kategoria 2: Mitä tai miten ajattelet liikkumisesta(si)?//Kategori 2: Vad eller hur tänker du kring (din) mobilitet? Category 2: How you think about (your) mobility?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  &lt;&lt;valitse yksi vastaus per väittämä)//&lt;&lt;välj ett svar per påstående)//&lt;&lt;choose one option per statement&gt;&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ad </t>
-  </si>
-  <si>
-    <t>Tarkastatko ennen liikkeelle lähtöä, onko reitilläsi ruuhkaa? (Valitse sinua parhaiten kuvaava vaihtoehto.)//Innan du ger dig av, kontrollerar du om det är trafikstockning på din rutt? (Välj det alternativ som bäst beskriver dig.)//Do you check whether there are traffic jams on my route before leaving? (Please indicate the answer that suits you best.)</t>
-  </si>
-  <si>
-    <t>Kategoria 3: Henkilötiedot//Kategori 3: Personuppgifter//Category 3: Personal data</t>
-  </si>
-  <si>
-    <t>Sukupuoli//Kön//Gender</t>
-  </si>
-  <si>
-    <t>Mies//Man//Male</t>
-  </si>
-  <si>
-    <t>Nainen//Kvinna//Female</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Syntymävuosi//Födelseår//Year of birth</t>
-  </si>
-  <si>
-    <t>(Pudotusvalikko)</t>
-  </si>
-  <si>
-    <t>Kotiosoitteeni postinumero//Postnummer för min hemadress//Post code of my home address</t>
-  </si>
-  <si>
-    <t>Pudotusvalikko Turun alueen postinumeroista ja "muu" (sulkee ulkopaikkakuntalaiset ulos datasta), vaihtoehtoisesti kotikunnat (Turun alue ja "muu"), Turun alueella asuville kysymys postinumerosta</t>
-  </si>
-  <si>
-    <t>Työ- tai opiskelupaikan postinumero: (Ohita kysymys, jos et opiskele tai käy töissä)//Postnumret på din arbetsplats eller studieort: (Hoppa över frågan om du inte studerar eller arbetar)//Post code of my work or study address: (In case you don't work or study, you can skip this question)</t>
-  </si>
-  <si>
-    <t>Asuminen//Boende//Living situation</t>
-  </si>
-  <si>
-    <t>Asun yksin ilman lapsia.//Jag bor ensam utan barn.//Single without children.</t>
-  </si>
-  <si>
-    <t>Asun yksin lasten kanssa.//Jag bor ensam med barn.//Single with children.</t>
-  </si>
-  <si>
-    <t>Asun puolison kanssa kaksin.//Jag bor tillsammans med min partner.//Co-habiting without children.</t>
-  </si>
-  <si>
-    <t>Asun puolison ja lasten kanssa.//Jag bor med min partner och barn.//Co-habiting with children.</t>
-  </si>
-  <si>
-    <t>Yhteensä</t>
   </si>
   <si>
     <t>Miksi tein testin?//Varför gjorde jag testet?//Why did I do the test?</t>
@@ -735,120 +840,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tiedät päivittäiset kohteesi ja miten niihin pääsee. Et pidä yllätyksistä matkan aikana; elämä on sellaisenaan jo tarpeeksi stressaavaa. Olet valmis kokeilemaan nopeampia tai mukavampia vaihtoehtoja, mutta vain jos saat selkeää tietoa niistä – mieluiten yksityiskohtaisen matkasuunnitelman kera./Du vet dina dagliga resmål och hur du tar dig till dem. Du gillar inte överraskningar under resan; livet är tillräckligt stressigt som det är. Du är villig att prova snabbare eller bekvämare alternativ, men bara om du får tydlig information om dem – gärna med en detaljerad resplan./You know where you're going every day and how to get there. You don't like surprises en route; life is already sufficiently stressful as it is. You are willing to try out faster or more comfortable alternatives. But only if you get clear information about this, preferably with a detailed travel plan. </t>
-  </si>
-  <si>
-    <t>Mikä tai mitkä seuraavista saisivat sinut muuttamaan liikkumistottumuksiasi?//Vad skulle få dig att ändra dina mobilitetsvanor?//What would inspire you to change your travel habits?</t>
-  </si>
-  <si>
-    <t>Mikä seuraavista kulkumuodoista on mielestäsi välttämättömin? (Valitse sinua parhaiten kuvaava vaihtoehto.)//Vilket av följande transportsätt tycker du är det mest nödvändiga? (Välj det alternativ som bäst beskriver dig.) // Which of the following modes of transportation do you think is the most necessary? (Choose the option that best describes you.)</t>
-  </si>
-  <si>
-    <t>Tavan vuoksi. //För vanans skull.//Out of habit.</t>
-  </si>
-  <si>
-    <t>Matkan hinta.//Resans pris.//Cost of the joyrney.</t>
-  </si>
-  <si>
-    <t>Matkan pituus.//Resans längd.//Travel distance.</t>
-  </si>
-  <si>
-    <t>Matkan kesto.//Resans längd i tid.//Travel time.</t>
-  </si>
-  <si>
-    <t>Säätila (sade, tuuli, jne.).//Väder (regn, vind, etc).//The weather (rain, wind etc).</t>
-  </si>
-  <si>
-    <t>Vapauden tunne.//En känsla av frihet.//The sense of freedom.</t>
-  </si>
-  <si>
-    <t>Voin käyttää matka-ajan työskentelyyn tai muihin tehtäviin. //Jag kan använda restiden till arbete eller andra uppgifter.//I use the travel time for work or other tasks.</t>
-  </si>
-  <si>
-    <t>Minulla on hyvät yhteydet joukkoliikenteellä (sisältäen riittävän vuorovälin).//Jag har goda förbindelser med kollektivtrafik (inklusive tillräcklig frekvens).//I havea good connection with transfer options (including good frequency) with public transport.</t>
-  </si>
-  <si>
-    <t>;atkan hinta.//Resans pris.//Cost of the joyrney.</t>
-  </si>
-  <si>
-    <t>Matkan kesto.//Resans längd i tid.//Tavel time.</t>
-  </si>
-  <si>
-    <t>Ympäristölliset syyt.//Miljöskäl.//The environment.</t>
-  </si>
-  <si>
-    <t>Terveyteni.//Hälsoskäl.//My health.</t>
-  </si>
-  <si>
-    <t>Matkan hinta.//Resans pris.//Cost of the journey.</t>
-  </si>
-  <si>
-    <t>Ajansäästö.//Tidsbesparande.//Time gains.</t>
-  </si>
-  <si>
-    <t>Hyvät joukkoliikenneyhteydet.//Bra förbindelser med kollektivtrafik.//A good connection with public transport.</t>
-  </si>
-  <si>
-    <t>Mahdollisuus käyttää joukkoliikennettä maksutta.//Möjlighet att använda kollektivtrafiken gratis.//A free public transport pass.</t>
-  </si>
-  <si>
-    <t>Liityntäpysäköinti- eli park and ride -mahdollisuuksien lisääntyminen.//Fler infartsparkeringsmöjligheter (Park &amp; Ride).//More Park &amp; Ride (P+R) options.</t>
-  </si>
-  <si>
-    <t>Työsuhdepolkupyörä.//Företagscykel.//Company bicycle through my employer.</t>
-  </si>
-  <si>
-    <t>Kyllä.//Ja.//Yes.</t>
-  </si>
-  <si>
-    <t>Ei.//Nej.//No.</t>
-  </si>
-  <si>
-    <t>Polkupyörä tai sähköpotkulauta.//Cykel tai elsparkcykel.//Bicycle or e-scooter.</t>
-  </si>
-  <si>
-    <t>Auto.//Bil.//Car.</t>
-  </si>
-  <si>
-    <t>Joukkoliikenne.//Kollektivtrafik.//Public transportation.</t>
-  </si>
-  <si>
-    <t>Ei mikään näistä.//Ingen av dessa.//None of these.</t>
-  </si>
-  <si>
-    <t>Kaikki ovat välttämättömiä kulkumuotoja.//Alla är oumbärliga transportsätt.//All are indispensable means of transport.</t>
-  </si>
-  <si>
-    <t>Joka kerta.//Alltid.//Every time.</t>
-  </si>
-  <si>
-    <t>Silloin tällöin.//Ibland.//Now and then.</t>
-  </si>
-  <si>
-    <t>En koskaan.//Aldrig.//Never.</t>
-  </si>
-  <si>
-    <t>Kestävää liikkumista tukevat työsuhde-edut./Hållbar rörlighet stöds av anställningsförmåner./Sustainable mobility is supported by employment benefits.</t>
-  </si>
-  <si>
-    <t>Ympäristöön liittyvät syyt.//Miljöskäl.//For environmental reasons.</t>
-  </si>
-  <si>
-    <t>Matkan pituus (liian lyhyt tai pitkä).//Resans längd (för kort eller lång).//The travel distance (too short or long).</t>
-  </si>
-  <si>
-    <t>Auto ja joukkoliikenne.//Bil och kollektivtrafik.//Car and public transport.</t>
-  </si>
-  <si>
-    <t>Polkupyörä tai sähköpotkulauta ja joukkoliikenne.//Cykel eller elsparkcykel och kollektivtrafik.//Bicycle or scooter and public transport.</t>
-  </si>
-  <si>
-    <t>Polkupyörä tai sähköpotkulauta ja auto.//Cykel eller elsparkcykel och bil.//Bicycle or scooter and car.</t>
-  </si>
-  <si>
-    <t>Mopo tai skootteri ja joukkoliikenne.//Moped eller skoter och kollektivtrafik.//Moped or motorcycle and public transport.</t>
-  </si>
-  <si>
-    <t>Pyörä ja kävely.//Cykel och gång.//Bicycle and walking.</t>
   </si>
 </sst>
 </file>
@@ -2082,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF3ACC6-6455-42D3-BCE3-944B33DD47DC}">
   <dimension ref="A1:AD233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B196" sqref="B196"/>
+    <sheetView tabSelected="1" topLeftCell="B156" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I163" sqref="I163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4033,7 +4024,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
       <c r="J50" s="120" t="s">
-        <v>261</v>
+        <v>59</v>
       </c>
       <c r="K50" s="149"/>
       <c r="L50" s="156"/>
@@ -4065,7 +4056,7 @@
       <c r="H51" s="35"/>
       <c r="I51" s="35"/>
       <c r="J51" s="123" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K51" s="150"/>
       <c r="L51" s="162"/>
@@ -4096,8 +4087,8 @@
       <c r="E52" s="61"/>
       <c r="H52" s="64"/>
       <c r="I52" s="64"/>
-      <c r="J52" s="11" t="s">
-        <v>70</v>
+      <c r="J52" s="34" t="s">
+        <v>61</v>
       </c>
       <c r="K52" s="158"/>
       <c r="L52" s="159"/>
@@ -4122,26 +4113,26 @@
     </row>
     <row r="53" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B53" s="125" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C53" s="168" t="s">
         <v>53</v>
       </c>
       <c r="D53" s="94" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E53" s="34" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F53" s="62"/>
       <c r="G53" s="62"/>
       <c r="H53" s="34"/>
       <c r="I53" s="34"/>
       <c r="J53" s="128" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K53" s="149"/>
       <c r="L53" s="162"/>
@@ -4167,13 +4158,13 @@
     <row r="54" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A54" s="27"/>
       <c r="D54" s="94" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E54" s="11"/>
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
       <c r="J54" s="120" t="s">
-        <v>262</v>
+        <v>68</v>
       </c>
       <c r="K54" s="149"/>
       <c r="L54" s="156"/>
@@ -4205,7 +4196,7 @@
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
       <c r="J55" s="120" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K55" s="149"/>
       <c r="L55" s="156"/>
@@ -4237,7 +4228,7 @@
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
       <c r="J56" s="119" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K56" s="149"/>
       <c r="L56" s="156"/>
@@ -4269,7 +4260,7 @@
       <c r="H57" s="34"/>
       <c r="I57" s="34"/>
       <c r="J57" s="128" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="K57" s="149"/>
       <c r="L57" s="162"/>
@@ -4301,7 +4292,7 @@
       <c r="H58" s="35"/>
       <c r="I58" s="35"/>
       <c r="J58" s="123" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="K58" s="181"/>
       <c r="L58" s="180"/>
@@ -4333,7 +4324,7 @@
       <c r="H59" s="185"/>
       <c r="I59" s="185"/>
       <c r="J59" s="186" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K59" s="187"/>
       <c r="L59" s="188"/>
@@ -4358,24 +4349,24 @@
     </row>
     <row r="60" spans="1:30" s="62" customFormat="1" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A60" s="27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B60" s="118" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C60" s="169" t="s">
         <v>53</v>
       </c>
       <c r="D60" s="93" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E60" s="34" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H60" s="35"/>
       <c r="I60" s="35"/>
       <c r="J60" s="123" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K60" s="149"/>
       <c r="L60" s="150"/>
@@ -4403,13 +4394,13 @@
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
       <c r="D61" s="93" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E61" s="11"/>
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
       <c r="J61" s="119" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K61" s="149"/>
       <c r="L61" s="157"/>
@@ -4441,7 +4432,7 @@
       <c r="H62" s="11"/>
       <c r="I62" s="11"/>
       <c r="J62" s="120" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K62" s="149"/>
       <c r="L62" s="157"/>
@@ -4473,7 +4464,7 @@
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
       <c r="J63" s="119" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K63" s="149"/>
       <c r="L63" s="157"/>
@@ -4505,7 +4496,7 @@
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
       <c r="J64" s="119" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="K64" s="149"/>
       <c r="L64" s="157"/>
@@ -4537,7 +4528,7 @@
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
       <c r="J65" s="119" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K65" s="149"/>
       <c r="L65" s="157"/>
@@ -4569,7 +4560,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
       <c r="J66" s="120" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K66" s="149"/>
       <c r="L66" s="157"/>
@@ -4594,16 +4585,16 @@
     </row>
     <row r="67" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A67" s="29" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B67" s="117" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C67" s="53">
         <v>1</v>
       </c>
       <c r="D67" s="91" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E67" s="26"/>
       <c r="F67" s="73"/>
@@ -4611,7 +4602,7 @@
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
       <c r="J67" s="129" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K67" s="152"/>
       <c r="L67" s="154"/>
@@ -4639,7 +4630,7 @@
       <c r="B68" s="18"/>
       <c r="C68" s="18"/>
       <c r="D68" s="91" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E68" s="18"/>
       <c r="F68" s="62"/>
@@ -4647,7 +4638,7 @@
       <c r="H68" s="34"/>
       <c r="I68" s="34"/>
       <c r="J68" s="128" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K68" s="149"/>
       <c r="L68" s="150"/>
@@ -4681,7 +4672,7 @@
       <c r="H69" s="101"/>
       <c r="I69" s="101"/>
       <c r="J69" s="130" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K69" s="158"/>
       <c r="L69" s="160"/>
@@ -4706,20 +4697,20 @@
     </row>
     <row r="70" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A70" s="27" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B70" s="131" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="102" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E70" s="1"/>
       <c r="H70" s="11"/>
       <c r="I70" s="11"/>
       <c r="J70" s="120" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K70" s="149"/>
       <c r="L70" s="157"/>
@@ -4747,13 +4738,13 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="102" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E71" s="1"/>
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
       <c r="J71" s="120" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K71" s="149"/>
       <c r="L71" s="157"/>
@@ -4785,7 +4776,7 @@
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
       <c r="J72" s="120" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="K72" s="149"/>
       <c r="L72" s="157"/>
@@ -4813,21 +4804,21 @@
         <v>2</v>
       </c>
       <c r="B73" s="49" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C73" s="170" t="s">
         <v>53</v>
       </c>
       <c r="D73" s="49"/>
       <c r="E73" s="34" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F73" s="73"/>
       <c r="G73" s="73"/>
       <c r="H73" s="31"/>
       <c r="I73" s="31"/>
       <c r="J73" s="115" t="s">
-        <v>263</v>
+        <v>99</v>
       </c>
       <c r="K73" s="42">
         <v>1</v>
@@ -4866,7 +4857,7 @@
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
       <c r="J74" s="119" t="s">
-        <v>264</v>
+        <v>100</v>
       </c>
       <c r="K74" s="43"/>
       <c r="L74" s="2"/>
@@ -4906,7 +4897,7 @@
       <c r="H75" s="13"/>
       <c r="I75" s="13"/>
       <c r="J75" s="119" t="s">
-        <v>265</v>
+        <v>101</v>
       </c>
       <c r="K75" s="43">
         <v>1</v>
@@ -4944,7 +4935,7 @@
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
       <c r="J76" s="119" t="s">
-        <v>266</v>
+        <v>102</v>
       </c>
       <c r="K76" s="43"/>
       <c r="L76" s="2"/>
@@ -4982,7 +4973,7 @@
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
       <c r="J77" s="119" t="s">
-        <v>267</v>
+        <v>103</v>
       </c>
       <c r="K77" s="43"/>
       <c r="L77" s="2"/>
@@ -5020,7 +5011,7 @@
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
       <c r="J78" s="119" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="K78" s="43">
         <v>1</v>
@@ -5056,7 +5047,7 @@
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
       <c r="J79" s="34" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K79" s="43"/>
       <c r="L79" s="2"/>
@@ -5084,7 +5075,7 @@
         <v>3</v>
       </c>
       <c r="B80" s="132" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C80" s="49"/>
       <c r="D80" s="49"/>
@@ -5094,7 +5085,7 @@
       <c r="H80" s="23"/>
       <c r="I80" s="23"/>
       <c r="J80" s="115" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="K80" s="42">
         <v>1</v>
@@ -5130,7 +5121,7 @@
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
       <c r="J81" s="119" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="K81" s="43"/>
       <c r="L81" s="2"/>
@@ -5168,7 +5159,7 @@
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
       <c r="J82" s="119" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="K82" s="43"/>
       <c r="L82" s="2"/>
@@ -5206,7 +5197,7 @@
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
       <c r="J83" s="119" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="K83" s="43"/>
       <c r="L83" s="2"/>
@@ -5240,7 +5231,7 @@
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
       <c r="J84" s="119" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="K84" s="43"/>
       <c r="L84" s="2"/>
@@ -5276,7 +5267,7 @@
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
       <c r="J85" s="119" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="K85" s="43"/>
       <c r="L85" s="2"/>
@@ -5312,7 +5303,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
       <c r="J86" s="119" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="K86" s="43"/>
       <c r="L86" s="2"/>
@@ -5342,25 +5333,25 @@
         <v>4</v>
       </c>
       <c r="B87" s="117" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C87" s="49"/>
       <c r="D87" s="51"/>
       <c r="E87" s="127" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F87" s="52" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="G87" s="166"/>
       <c r="H87" s="115" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="I87" s="176" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="J87" s="115" t="s">
-        <v>233</v>
+        <v>118</v>
       </c>
       <c r="K87" s="42">
         <v>1</v>
@@ -5393,7 +5384,7 @@
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
       <c r="J88" s="119" t="s">
-        <v>234</v>
+        <v>119</v>
       </c>
       <c r="K88" s="43">
         <v>1</v>
@@ -5429,7 +5420,7 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
       <c r="J89" s="119" t="s">
-        <v>235</v>
+        <v>120</v>
       </c>
       <c r="K89" s="43">
         <v>1</v>
@@ -5467,7 +5458,7 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="119" t="s">
-        <v>236</v>
+        <v>121</v>
       </c>
       <c r="K90" s="43">
         <v>1</v>
@@ -5505,7 +5496,7 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="119" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="K91" s="43"/>
       <c r="L91" s="2"/>
@@ -5541,7 +5532,7 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="119" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="K92" s="43">
         <v>1</v>
@@ -5577,7 +5568,7 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
       <c r="J93" s="119" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="K93" s="43">
         <v>1</v>
@@ -5615,7 +5606,7 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="119" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="K94" s="43">
         <v>1</v>
@@ -5651,7 +5642,7 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
       <c r="J95" s="119" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="K95" s="43">
         <v>1</v>
@@ -5689,7 +5680,7 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="119" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K96" s="43">
         <v>1</v>
@@ -5725,7 +5716,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="119" t="s">
-        <v>232</v>
+        <v>128</v>
       </c>
       <c r="K97" s="43"/>
       <c r="L97" s="2">
@@ -5761,7 +5752,7 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="119" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="K98" s="43">
         <v>1</v>
@@ -5799,7 +5790,7 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="119" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="K99" s="43">
         <v>1</v>
@@ -5837,7 +5828,7 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="119" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="K100" s="43">
         <v>1</v>
@@ -5875,7 +5866,7 @@
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
       <c r="J101" s="34" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K101" s="43"/>
       <c r="L101" s="2"/>
@@ -5905,17 +5896,17 @@
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="52" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="G102" s="1"/>
       <c r="H102" s="115" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="I102" s="177" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="J102" s="115" t="s">
-        <v>233</v>
+        <v>118</v>
       </c>
       <c r="K102" s="143">
         <v>1</v>
@@ -5949,11 +5940,11 @@
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="12" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="I103" s="12"/>
       <c r="J103" s="119" t="s">
-        <v>234</v>
+        <v>119</v>
       </c>
       <c r="K103" s="146">
         <v>1</v>
@@ -5989,7 +5980,7 @@
       <c r="H104" s="12"/>
       <c r="I104" s="12"/>
       <c r="J104" s="119" t="s">
-        <v>235</v>
+        <v>120</v>
       </c>
       <c r="K104" s="146">
         <v>1</v>
@@ -6025,7 +6016,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="12"/>
       <c r="J105" s="119" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="K105" s="146">
         <v>1</v>
@@ -6061,7 +6052,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
       <c r="J106" s="119" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="K106" s="146">
         <v>1</v>
@@ -6097,7 +6088,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
       <c r="J107" s="119" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K107" s="146">
         <v>1</v>
@@ -6133,7 +6124,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
       <c r="J108" s="119" t="s">
-        <v>232</v>
+        <v>128</v>
       </c>
       <c r="K108" s="146"/>
       <c r="L108" s="147">
@@ -6169,7 +6160,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
       <c r="J109" s="119" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="K109" s="146">
         <v>1</v>
@@ -6207,7 +6198,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
       <c r="J110" s="13" t="s">
-        <v>237</v>
+        <v>137</v>
       </c>
       <c r="K110" s="146">
         <v>1</v>
@@ -6243,7 +6234,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
       <c r="J111" s="119" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="K111" s="146">
         <v>1</v>
@@ -6281,7 +6272,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
       <c r="J112" s="119" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="K112" s="146">
         <v>1</v>
@@ -6319,7 +6310,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="12"/>
       <c r="J113" s="34" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K113" s="146"/>
       <c r="L113" s="147"/>
@@ -6349,17 +6340,17 @@
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="133" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="G114" s="53"/>
       <c r="H114" s="115" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="I114" s="177" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="J114" s="115" t="s">
-        <v>233</v>
+        <v>118</v>
       </c>
       <c r="K114" s="42"/>
       <c r="L114" s="24"/>
@@ -6397,7 +6388,7 @@
       <c r="H115" s="17"/>
       <c r="I115" s="17"/>
       <c r="J115" s="119" t="s">
-        <v>234</v>
+        <v>119</v>
       </c>
       <c r="K115" s="43"/>
       <c r="L115" s="2"/>
@@ -6437,7 +6428,7 @@
       <c r="H116" s="1"/>
       <c r="I116" s="1"/>
       <c r="J116" s="119" t="s">
-        <v>235</v>
+        <v>120</v>
       </c>
       <c r="K116" s="43"/>
       <c r="L116" s="2"/>
@@ -6477,7 +6468,7 @@
       <c r="H117" s="1"/>
       <c r="I117" s="1"/>
       <c r="J117" s="119" t="s">
-        <v>236</v>
+        <v>121</v>
       </c>
       <c r="K117" s="43"/>
       <c r="L117" s="2"/>
@@ -6517,7 +6508,7 @@
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
       <c r="J118" s="119" t="s">
-        <v>238</v>
+        <v>141</v>
       </c>
       <c r="K118" s="43"/>
       <c r="L118" s="2"/>
@@ -6557,7 +6548,7 @@
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
       <c r="J119" s="119" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="K119" s="43"/>
       <c r="L119" s="2"/>
@@ -6595,7 +6586,7 @@
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
       <c r="J120" s="119" t="s">
-        <v>239</v>
+        <v>142</v>
       </c>
       <c r="K120" s="43"/>
       <c r="L120" s="2"/>
@@ -6635,7 +6626,7 @@
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="119" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="K121" s="43"/>
       <c r="L121" s="2">
@@ -6709,7 +6700,7 @@
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
       <c r="J123" s="119" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="K123" s="43"/>
       <c r="L123" s="2"/>
@@ -6749,7 +6740,7 @@
       <c r="H124" s="1"/>
       <c r="I124" s="1"/>
       <c r="J124" s="119" t="s">
-        <v>232</v>
+        <v>128</v>
       </c>
       <c r="K124" s="43"/>
       <c r="L124" s="2">
@@ -6785,7 +6776,7 @@
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
       <c r="J125" s="34" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K125" s="43"/>
       <c r="L125" s="2"/>
@@ -6815,17 +6806,17 @@
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="117" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="G126" s="52"/>
       <c r="H126" s="115" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="I126" s="177" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="J126" s="115" t="s">
-        <v>240</v>
+        <v>118</v>
       </c>
       <c r="K126" s="42"/>
       <c r="L126" s="24"/>
@@ -6863,7 +6854,7 @@
       <c r="H127" s="17"/>
       <c r="I127" s="17"/>
       <c r="J127" s="119" t="s">
-        <v>234</v>
+        <v>119</v>
       </c>
       <c r="K127" s="43"/>
       <c r="L127" s="2"/>
@@ -6901,7 +6892,7 @@
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
       <c r="J128" s="119" t="s">
-        <v>241</v>
+        <v>147</v>
       </c>
       <c r="K128" s="43"/>
       <c r="L128" s="2"/>
@@ -6939,7 +6930,7 @@
       <c r="H129" s="1"/>
       <c r="I129" s="1"/>
       <c r="J129" s="119" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="K129" s="43"/>
       <c r="L129" s="2"/>
@@ -6977,7 +6968,7 @@
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
       <c r="J130" s="119" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="K130" s="43"/>
       <c r="L130" s="2"/>
@@ -7013,7 +7004,7 @@
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
       <c r="J131" s="119" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="K131" s="43"/>
       <c r="L131" s="2"/>
@@ -7049,7 +7040,7 @@
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
       <c r="J132" s="119" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="K132" s="43"/>
       <c r="L132" s="2"/>
@@ -7089,7 +7080,7 @@
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
       <c r="J133" s="119" t="s">
-        <v>232</v>
+        <v>128</v>
       </c>
       <c r="K133" s="43"/>
       <c r="L133" s="2">
@@ -7125,7 +7116,7 @@
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
       <c r="J134" s="119" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="K134" s="43"/>
       <c r="L134" s="2"/>
@@ -7163,7 +7154,7 @@
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
       <c r="J135" s="34" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K135" s="43"/>
       <c r="L135" s="2"/>
@@ -7193,17 +7184,17 @@
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="133" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="G136" s="53"/>
       <c r="H136" s="115" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="I136" s="177" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="J136" s="115" t="s">
-        <v>233</v>
+        <v>118</v>
       </c>
       <c r="K136" s="42"/>
       <c r="L136" s="24"/>
@@ -7241,7 +7232,7 @@
       <c r="H137" s="17"/>
       <c r="I137" s="17"/>
       <c r="J137" s="119" t="s">
-        <v>234</v>
+        <v>119</v>
       </c>
       <c r="K137" s="43"/>
       <c r="L137" s="2"/>
@@ -7281,7 +7272,7 @@
       <c r="H138" s="1"/>
       <c r="I138" s="1"/>
       <c r="J138" s="119" t="s">
-        <v>235</v>
+        <v>120</v>
       </c>
       <c r="K138" s="43"/>
       <c r="L138" s="2"/>
@@ -7319,7 +7310,7 @@
       <c r="H139" s="1"/>
       <c r="I139" s="1"/>
       <c r="J139" s="119" t="s">
-        <v>242</v>
+        <v>153</v>
       </c>
       <c r="K139" s="43"/>
       <c r="L139" s="2"/>
@@ -7357,7 +7348,7 @@
       <c r="H140" s="1"/>
       <c r="I140" s="1"/>
       <c r="J140" s="119" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="K140" s="43"/>
       <c r="L140" s="2"/>
@@ -7393,7 +7384,7 @@
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
       <c r="J141" s="119" t="s">
-        <v>243</v>
+        <v>154</v>
       </c>
       <c r="K141" s="43"/>
       <c r="L141" s="2"/>
@@ -7429,7 +7420,7 @@
       <c r="H142" s="1"/>
       <c r="I142" s="1"/>
       <c r="J142" s="119" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="K142" s="43"/>
       <c r="L142" s="2"/>
@@ -7465,7 +7456,7 @@
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
       <c r="J143" s="119" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="K143" s="43"/>
       <c r="L143" s="2"/>
@@ -7501,7 +7492,7 @@
       <c r="H144" s="1"/>
       <c r="I144" s="1"/>
       <c r="J144" s="119" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="K144" s="43"/>
       <c r="L144" s="2"/>
@@ -7577,7 +7568,7 @@
       <c r="H146" s="1"/>
       <c r="I146" s="1"/>
       <c r="J146" s="119" t="s">
-        <v>232</v>
+        <v>128</v>
       </c>
       <c r="K146" s="43"/>
       <c r="L146" s="2">
@@ -7613,7 +7604,7 @@
       <c r="H147" s="1"/>
       <c r="I147" s="1"/>
       <c r="J147" s="119" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="K147" s="43"/>
       <c r="L147" s="2"/>
@@ -7651,7 +7642,7 @@
       <c r="H148" s="1"/>
       <c r="I148" s="1"/>
       <c r="J148" s="34" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K148" s="43"/>
       <c r="L148" s="2"/>
@@ -7681,17 +7672,17 @@
       <c r="D149" s="18"/>
       <c r="E149" s="18"/>
       <c r="F149" s="132" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="G149" s="49"/>
       <c r="H149" s="115" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="I149" s="177" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="J149" s="115" t="s">
-        <v>244</v>
+        <v>160</v>
       </c>
       <c r="K149" s="42"/>
       <c r="L149" s="24"/>
@@ -7725,7 +7716,7 @@
       <c r="H150" s="17"/>
       <c r="I150" s="17"/>
       <c r="J150" s="119" t="s">
-        <v>234</v>
+        <v>119</v>
       </c>
       <c r="K150" s="43"/>
       <c r="L150" s="2"/>
@@ -7763,7 +7754,7 @@
       <c r="H151" s="1"/>
       <c r="I151" s="1"/>
       <c r="J151" s="119" t="s">
-        <v>235</v>
+        <v>120</v>
       </c>
       <c r="K151" s="43"/>
       <c r="L151" s="2"/>
@@ -7799,7 +7790,7 @@
       <c r="H152" s="1"/>
       <c r="I152" s="1"/>
       <c r="J152" s="119" t="s">
-        <v>242</v>
+        <v>153</v>
       </c>
       <c r="K152" s="43"/>
       <c r="L152" s="2"/>
@@ -7835,7 +7826,7 @@
       <c r="H153" s="1"/>
       <c r="I153" s="1"/>
       <c r="J153" s="119" t="s">
-        <v>243</v>
+        <v>154</v>
       </c>
       <c r="K153" s="43"/>
       <c r="L153" s="2"/>
@@ -7871,7 +7862,7 @@
       <c r="H154" s="1"/>
       <c r="I154" s="1"/>
       <c r="J154" s="119" t="s">
-        <v>232</v>
+        <v>128</v>
       </c>
       <c r="K154" s="43"/>
       <c r="L154" s="2">
@@ -7907,7 +7898,7 @@
       <c r="H155" s="1"/>
       <c r="I155" s="1"/>
       <c r="J155" s="119" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="K155" s="43"/>
       <c r="L155" s="2"/>
@@ -7945,7 +7936,7 @@
       <c r="H156" s="61"/>
       <c r="I156" s="18"/>
       <c r="J156" s="119" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K156" s="65"/>
       <c r="L156" s="66"/>
@@ -7973,23 +7964,23 @@
         <v>5</v>
       </c>
       <c r="B157" s="118" t="s">
-        <v>230</v>
+        <v>161</v>
       </c>
       <c r="C157" s="54">
         <v>3</v>
       </c>
       <c r="D157" s="93" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="E157" s="123" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="F157" s="18"/>
       <c r="G157" s="18"/>
       <c r="H157" s="18"/>
       <c r="I157" s="18"/>
       <c r="J157" s="123" t="s">
-        <v>245</v>
+        <v>164</v>
       </c>
       <c r="K157" s="43"/>
       <c r="L157" s="36"/>
@@ -8017,7 +8008,7 @@
       <c r="B158" s="13"/>
       <c r="C158" s="13"/>
       <c r="D158" s="93" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="E158" s="13"/>
       <c r="F158" s="1"/>
@@ -8025,7 +8016,7 @@
       <c r="H158" s="1"/>
       <c r="I158" s="1"/>
       <c r="J158" s="34" t="s">
-        <v>246</v>
+        <v>166</v>
       </c>
       <c r="K158" s="43"/>
       <c r="L158" s="2"/>
@@ -8059,7 +8050,7 @@
       <c r="H159" s="1"/>
       <c r="I159" s="1"/>
       <c r="J159" s="119" t="s">
-        <v>247</v>
+        <v>167</v>
       </c>
       <c r="K159" s="43"/>
       <c r="L159" s="2"/>
@@ -8093,7 +8084,7 @@
       <c r="H160" s="1"/>
       <c r="I160" s="1"/>
       <c r="J160" s="34" t="s">
-        <v>248</v>
+        <v>168</v>
       </c>
       <c r="K160" s="43"/>
       <c r="L160" s="2"/>
@@ -8127,7 +8118,7 @@
       <c r="H161" s="1"/>
       <c r="I161" s="1"/>
       <c r="J161" s="119" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="K161" s="43"/>
       <c r="L161" s="2"/>
@@ -8161,7 +8152,7 @@
       <c r="H162" s="1"/>
       <c r="I162" s="1"/>
       <c r="J162" s="34" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="K162" s="43"/>
       <c r="L162" s="2"/>
@@ -8195,7 +8186,7 @@
       <c r="H163" s="1"/>
       <c r="I163" s="1"/>
       <c r="J163" s="119" t="s">
-        <v>249</v>
+        <v>171</v>
       </c>
       <c r="K163" s="43"/>
       <c r="L163" s="2"/>
@@ -8229,7 +8220,7 @@
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
       <c r="J164" s="34" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="K164" s="43"/>
       <c r="L164" s="2"/>
@@ -8263,7 +8254,7 @@
       <c r="H165" s="1"/>
       <c r="I165" s="1"/>
       <c r="J165" s="119" t="s">
-        <v>260</v>
+        <v>173</v>
       </c>
       <c r="K165" s="43"/>
       <c r="L165" s="2"/>
@@ -8297,7 +8288,7 @@
       <c r="H166" s="1"/>
       <c r="I166" s="1"/>
       <c r="J166" s="34" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="K166" s="43"/>
       <c r="L166" s="2"/>
@@ -8331,7 +8322,7 @@
       <c r="H167" s="1"/>
       <c r="I167" s="1"/>
       <c r="J167" s="119" t="s">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="K167" s="43"/>
       <c r="L167" s="2"/>
@@ -8365,7 +8356,7 @@
       <c r="H168" s="1"/>
       <c r="I168" s="1"/>
       <c r="J168" s="119" t="s">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="K168" s="43"/>
       <c r="L168" s="2"/>
@@ -8399,7 +8390,7 @@
       <c r="H169" s="1"/>
       <c r="I169" s="1"/>
       <c r="J169" s="119" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="K169" s="43"/>
       <c r="L169" s="2"/>
@@ -8433,7 +8424,7 @@
       <c r="H170" s="1"/>
       <c r="I170" s="1"/>
       <c r="J170" s="34" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="K170" s="43"/>
       <c r="L170" s="2"/>
@@ -8467,7 +8458,7 @@
       <c r="H171" s="1"/>
       <c r="I171" s="1"/>
       <c r="J171" s="34" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="K171" s="43"/>
       <c r="L171" s="2"/>
@@ -8501,7 +8492,7 @@
       <c r="H172" s="1"/>
       <c r="I172" s="1"/>
       <c r="J172" s="119" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="K172" s="43"/>
       <c r="L172" s="2"/>
@@ -8535,7 +8526,7 @@
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
       <c r="J173" s="34" t="s">
-        <v>156</v>
+        <v>180</v>
       </c>
       <c r="K173" s="43"/>
       <c r="L173" s="2"/>
@@ -8569,7 +8560,7 @@
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
       <c r="J174" s="34" t="s">
-        <v>157</v>
+        <v>181</v>
       </c>
       <c r="K174" s="43"/>
       <c r="L174" s="2"/>
@@ -8603,7 +8594,7 @@
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
       <c r="J175" s="34" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="K175" s="43"/>
       <c r="L175" s="2"/>
@@ -8637,7 +8628,7 @@
       <c r="H176" s="1"/>
       <c r="I176" s="1"/>
       <c r="J176" s="34" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="K176" s="43"/>
       <c r="L176" s="2"/>
@@ -8671,7 +8662,7 @@
       <c r="H177" s="61"/>
       <c r="I177" s="61"/>
       <c r="J177" s="101" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K177" s="65"/>
       <c r="L177" s="66"/>
@@ -8699,21 +8690,21 @@
         <v>6</v>
       </c>
       <c r="B178" s="125" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="C178" s="50">
         <v>1</v>
       </c>
       <c r="D178" s="50"/>
       <c r="E178" s="127" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F178" s="62"/>
       <c r="G178" s="35"/>
       <c r="H178" s="35"/>
       <c r="I178" s="35"/>
       <c r="J178" s="123" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="K178" s="43"/>
       <c r="L178" s="36"/>
@@ -8745,7 +8736,7 @@
       <c r="H179" s="35"/>
       <c r="I179" s="35"/>
       <c r="J179" s="34" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="K179" s="43"/>
       <c r="L179" s="36"/>
@@ -8778,7 +8769,7 @@
       <c r="H180" s="13"/>
       <c r="I180" s="13"/>
       <c r="J180" s="119" t="s">
-        <v>163</v>
+        <v>187</v>
       </c>
       <c r="K180" s="43"/>
       <c r="L180" s="2"/>
@@ -8811,7 +8802,7 @@
       <c r="H181" s="13"/>
       <c r="I181" s="13"/>
       <c r="J181" s="119" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="K181" s="43"/>
       <c r="L181" s="2"/>
@@ -8844,7 +8835,7 @@
       <c r="H182" s="13"/>
       <c r="I182" s="13"/>
       <c r="J182" s="34" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="K182" s="43"/>
       <c r="L182" s="2"/>
@@ -8877,7 +8868,7 @@
       <c r="H183" s="13"/>
       <c r="I183" s="13"/>
       <c r="J183" s="119" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="K183" s="43"/>
       <c r="L183" s="2"/>
@@ -8911,7 +8902,7 @@
       <c r="H184" s="70"/>
       <c r="I184" s="70"/>
       <c r="J184" s="121" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="K184" s="65"/>
       <c r="L184" s="66"/>
@@ -8939,7 +8930,7 @@
         <v>7</v>
       </c>
       <c r="B185" s="125" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="C185" s="50"/>
       <c r="D185" s="50"/>
@@ -8949,7 +8940,7 @@
       <c r="H185" s="35"/>
       <c r="I185" s="35"/>
       <c r="J185" s="35" t="s">
-        <v>250</v>
+        <v>193</v>
       </c>
       <c r="K185" s="43"/>
       <c r="L185" s="36"/>
@@ -8982,7 +8973,7 @@
       <c r="H186" s="13"/>
       <c r="I186" s="13"/>
       <c r="J186" s="13" t="s">
-        <v>251</v>
+        <v>194</v>
       </c>
       <c r="K186" s="43"/>
       <c r="L186" s="2"/>
@@ -9016,7 +9007,7 @@
       <c r="H187" s="70"/>
       <c r="I187" s="70"/>
       <c r="J187" s="121" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="K187" s="65"/>
       <c r="L187" s="66"/>
@@ -9044,7 +9035,7 @@
         <v>8</v>
       </c>
       <c r="B188" s="118" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="C188" s="62"/>
       <c r="D188" s="165">
@@ -9056,7 +9047,7 @@
       <c r="H188" s="35"/>
       <c r="I188" s="35"/>
       <c r="J188" s="123" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="K188" s="43"/>
       <c r="L188" s="36"/>
@@ -9084,14 +9075,14 @@
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="93" t="s">
-        <v>171</v>
+        <v>197</v>
       </c>
       <c r="E189" s="1"/>
       <c r="G189" s="13"/>
       <c r="H189" s="13"/>
       <c r="I189" s="13"/>
       <c r="J189" s="119" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="K189" s="43"/>
       <c r="L189" s="2"/>
@@ -9124,7 +9115,7 @@
       <c r="H190" s="13"/>
       <c r="I190" s="13"/>
       <c r="J190" s="119" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="K190" s="43"/>
       <c r="L190" s="2"/>
@@ -9157,7 +9148,7 @@
       <c r="H191" s="13"/>
       <c r="I191" s="13"/>
       <c r="J191" s="119" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="K191" s="43"/>
       <c r="L191" s="2"/>
@@ -9190,7 +9181,7 @@
       <c r="H192" s="13"/>
       <c r="I192" s="13"/>
       <c r="J192" s="119" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="K192" s="43"/>
       <c r="L192" s="2"/>
@@ -9216,7 +9207,7 @@
     <row r="193" spans="1:30" s="16" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="29"/>
       <c r="B193" s="197" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="C193" s="198"/>
       <c r="D193" s="198"/>
@@ -9250,7 +9241,7 @@
     <row r="194" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="27"/>
       <c r="B194" s="134" t="s">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="C194" s="78"/>
       <c r="D194" s="78"/>
@@ -9318,7 +9309,7 @@
         <v>9</v>
       </c>
       <c r="B196" s="117" t="s">
-        <v>231</v>
+        <v>202</v>
       </c>
       <c r="C196" s="52"/>
       <c r="D196" s="52"/>
@@ -9328,7 +9319,7 @@
       <c r="H196" s="31"/>
       <c r="I196" s="31"/>
       <c r="J196" s="31" t="s">
-        <v>253</v>
+        <v>203</v>
       </c>
       <c r="K196" s="42">
         <v>1</v>
@@ -9360,7 +9351,7 @@
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="E197" s="1"/>
       <c r="F197" s="119"/>
@@ -9368,7 +9359,7 @@
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
       <c r="J197" s="119" t="s">
-        <v>252</v>
+        <v>205</v>
       </c>
       <c r="K197" s="43"/>
       <c r="L197" s="2"/>
@@ -9404,7 +9395,7 @@
       <c r="H198" s="13"/>
       <c r="I198" s="13"/>
       <c r="J198" s="119" t="s">
-        <v>254</v>
+        <v>206</v>
       </c>
       <c r="K198" s="43"/>
       <c r="L198" s="2"/>
@@ -9442,7 +9433,7 @@
       <c r="H199" s="19"/>
       <c r="I199" s="19"/>
       <c r="J199" s="135" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="K199" s="43"/>
       <c r="L199" s="2"/>
@@ -9476,7 +9467,7 @@
       <c r="H200" s="19"/>
       <c r="I200" s="19"/>
       <c r="J200" s="72" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="K200" s="43"/>
       <c r="L200" s="2"/>
@@ -9504,7 +9495,7 @@
         <v>10</v>
       </c>
       <c r="B201" s="52" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
       <c r="C201" s="57"/>
       <c r="D201" s="57"/>
@@ -9514,7 +9505,7 @@
       <c r="H201" s="31"/>
       <c r="I201" s="31"/>
       <c r="J201" s="31" t="s">
-        <v>257</v>
+        <v>210</v>
       </c>
       <c r="K201" s="42"/>
       <c r="L201" s="24"/>
@@ -9552,7 +9543,7 @@
       <c r="H202" s="13"/>
       <c r="I202" s="13"/>
       <c r="J202" s="119" t="s">
-        <v>258</v>
+        <v>211</v>
       </c>
       <c r="K202" s="43">
         <v>1</v>
@@ -9594,7 +9585,7 @@
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
       <c r="J203" s="13" t="s">
-        <v>259</v>
+        <v>212</v>
       </c>
       <c r="K203" s="43"/>
       <c r="L203" s="2">
@@ -9622,7 +9613,7 @@
     <row r="204" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A204" s="29"/>
       <c r="B204" s="199" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
       <c r="C204" s="200"/>
       <c r="D204" s="200"/>
@@ -9658,18 +9649,18 @@
         <v>12</v>
       </c>
       <c r="B205" s="136" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
       <c r="C205" s="55"/>
       <c r="D205" s="55"/>
       <c r="E205" s="55"/>
-      <c r="F205" s="39" t="s">
-        <v>180</v>
-      </c>
+      <c r="F205" s="39"/>
       <c r="G205" s="34"/>
       <c r="H205" s="34"/>
       <c r="I205" s="34"/>
-      <c r="J205" s="1"/>
+      <c r="J205" s="39" t="s">
+        <v>215</v>
+      </c>
       <c r="K205" s="43"/>
       <c r="L205" s="2"/>
       <c r="M205" s="2"/>
@@ -9697,13 +9688,13 @@
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
-      <c r="F206" s="40" t="s">
-        <v>181</v>
-      </c>
+      <c r="F206" s="40"/>
       <c r="G206" s="34"/>
       <c r="H206" s="34"/>
       <c r="I206" s="34"/>
-      <c r="J206" s="1"/>
+      <c r="J206" s="40" t="s">
+        <v>216</v>
+      </c>
       <c r="K206" s="43"/>
       <c r="L206" s="2"/>
       <c r="M206" s="2"/>
@@ -9731,13 +9722,13 @@
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
-      <c r="F207" s="104" t="s">
-        <v>182</v>
-      </c>
+      <c r="F207" s="104"/>
       <c r="G207" s="18"/>
       <c r="H207" s="18"/>
       <c r="I207" s="18"/>
-      <c r="J207" s="1"/>
+      <c r="J207" s="104" t="s">
+        <v>217</v>
+      </c>
       <c r="K207" s="43"/>
       <c r="L207" s="2"/>
       <c r="M207" s="2"/>
@@ -9764,13 +9755,13 @@
         <v>13</v>
       </c>
       <c r="B208" s="136" t="s">
-        <v>183</v>
+        <v>218</v>
       </c>
       <c r="C208" s="55"/>
       <c r="D208" s="55"/>
       <c r="E208" s="55"/>
       <c r="F208" s="41" t="s">
-        <v>184</v>
+        <v>219</v>
       </c>
       <c r="G208" s="59"/>
       <c r="H208" s="59"/>
@@ -9802,13 +9793,13 @@
         <v>14</v>
       </c>
       <c r="B209" s="138" t="s">
-        <v>185</v>
+        <v>220</v>
       </c>
       <c r="C209" s="56"/>
       <c r="D209" s="56"/>
       <c r="E209" s="56"/>
       <c r="F209" s="142" t="s">
-        <v>186</v>
+        <v>221</v>
       </c>
       <c r="G209" s="18"/>
       <c r="H209" s="18"/>
@@ -9840,7 +9831,7 @@
         <v>15</v>
       </c>
       <c r="B210" s="138" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="C210" s="56"/>
       <c r="D210" s="56"/>
@@ -9871,23 +9862,23 @@
       <c r="AC210" s="1"/>
       <c r="AD210" s="1"/>
     </row>
-    <row r="211" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A211" s="27">
         <v>16</v>
       </c>
       <c r="B211" s="138" t="s">
-        <v>188</v>
+        <v>223</v>
       </c>
       <c r="C211" s="56"/>
       <c r="D211" s="56"/>
       <c r="E211" s="56"/>
-      <c r="F211" s="140" t="s">
-        <v>189</v>
-      </c>
+      <c r="F211" s="140"/>
       <c r="G211" s="35"/>
       <c r="H211" s="35"/>
       <c r="I211" s="35"/>
-      <c r="J211" s="1"/>
+      <c r="J211" s="140" t="s">
+        <v>224</v>
+      </c>
       <c r="K211" s="43"/>
       <c r="L211" s="2"/>
       <c r="M211" s="2"/>
@@ -9909,19 +9900,19 @@
       <c r="AC211" s="1"/>
       <c r="AD211" s="1"/>
     </row>
-    <row r="212" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A212" s="27"/>
       <c r="B212" s="135"/>
       <c r="C212" s="14"/>
       <c r="D212" s="14"/>
       <c r="E212" s="14"/>
-      <c r="F212" s="141" t="s">
-        <v>190</v>
-      </c>
+      <c r="F212" s="141"/>
       <c r="G212" s="35"/>
       <c r="H212" s="35"/>
       <c r="I212" s="35"/>
-      <c r="J212" s="1"/>
+      <c r="J212" s="141" t="s">
+        <v>225</v>
+      </c>
       <c r="K212" s="43"/>
       <c r="L212" s="2"/>
       <c r="M212" s="2"/>
@@ -9943,19 +9934,19 @@
       <c r="AC212" s="1"/>
       <c r="AD212" s="1"/>
     </row>
-    <row r="213" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A213" s="27"/>
       <c r="B213" s="14"/>
       <c r="C213" s="14"/>
       <c r="D213" s="14"/>
       <c r="E213" s="14"/>
-      <c r="F213" s="141" t="s">
-        <v>191</v>
-      </c>
+      <c r="F213" s="141"/>
       <c r="G213" s="35"/>
       <c r="H213" s="35"/>
       <c r="I213" s="35"/>
-      <c r="J213" s="1"/>
+      <c r="J213" s="141" t="s">
+        <v>226</v>
+      </c>
       <c r="K213" s="43"/>
       <c r="L213" s="2"/>
       <c r="M213" s="2"/>
@@ -9977,19 +9968,19 @@
       <c r="AC213" s="1"/>
       <c r="AD213" s="1"/>
     </row>
-    <row r="214" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A214" s="27"/>
       <c r="B214" s="14"/>
       <c r="C214" s="14"/>
       <c r="D214" s="14"/>
       <c r="E214" s="14"/>
-      <c r="F214" s="141" t="s">
-        <v>192</v>
-      </c>
+      <c r="F214" s="141"/>
       <c r="G214" s="35"/>
       <c r="H214" s="35"/>
       <c r="I214" s="35"/>
-      <c r="J214" s="1"/>
+      <c r="J214" s="141" t="s">
+        <v>227</v>
+      </c>
       <c r="K214" s="43"/>
       <c r="L214" s="2"/>
       <c r="M214" s="2"/>
@@ -10017,13 +10008,13 @@
       <c r="C215" s="14"/>
       <c r="D215" s="14"/>
       <c r="E215" s="14"/>
-      <c r="F215" s="141" t="s">
-        <v>142</v>
-      </c>
+      <c r="F215" s="141"/>
       <c r="G215" s="35"/>
       <c r="H215" s="35"/>
       <c r="I215" s="35"/>
-      <c r="J215" s="1"/>
+      <c r="J215" s="141" t="s">
+        <v>228</v>
+      </c>
       <c r="K215" s="43"/>
       <c r="L215" s="2"/>
       <c r="M215" s="2"/>
@@ -10055,9 +10046,7 @@
       <c r="G216" s="26"/>
       <c r="H216" s="26"/>
       <c r="I216" s="26"/>
-      <c r="J216" s="46" t="s">
-        <v>193</v>
-      </c>
+      <c r="J216" s="46"/>
       <c r="K216" s="42">
         <f>SUM(K2:K215)</f>
         <v>37</v>
@@ -10133,15 +10122,15 @@
         <v>17</v>
       </c>
       <c r="B218" s="139" t="s">
-        <v>194</v>
+        <v>229</v>
       </c>
       <c r="C218" s="26"/>
       <c r="D218" s="26"/>
       <c r="E218" s="97" t="s">
-        <v>195</v>
+        <v>230</v>
       </c>
       <c r="F218" s="107" t="s">
-        <v>196</v>
+        <v>231</v>
       </c>
       <c r="G218" s="26"/>
       <c r="H218" s="26"/>
@@ -10175,7 +10164,7 @@
       <c r="D219" s="61"/>
       <c r="E219" s="61"/>
       <c r="F219" s="121" t="s">
-        <v>197</v>
+        <v>232</v>
       </c>
       <c r="G219" s="61"/>
       <c r="H219" s="61"/>
@@ -10207,13 +10196,13 @@
         <v>18</v>
       </c>
       <c r="B220" s="171" t="s">
-        <v>198</v>
+        <v>233</v>
       </c>
       <c r="C220" s="172"/>
       <c r="D220" s="173"/>
       <c r="E220" s="173"/>
       <c r="F220" s="195" t="s">
-        <v>199</v>
+        <v>234</v>
       </c>
       <c r="G220" s="1"/>
       <c r="H220" s="1"/>
@@ -10277,15 +10266,15 @@
         <v>19</v>
       </c>
       <c r="B222" s="139" t="s">
-        <v>200</v>
+        <v>235</v>
       </c>
       <c r="C222" s="26"/>
       <c r="D222" s="73"/>
       <c r="E222" s="174" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="F222" s="174" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="G222" s="26"/>
       <c r="H222" s="26"/>
@@ -10318,10 +10307,10 @@
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
       <c r="E223" s="163" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="F223" s="196" t="s">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="G223" s="1"/>
       <c r="H223" s="1"/>
@@ -10355,7 +10344,7 @@
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
       <c r="F224" s="137" t="s">
-        <v>203</v>
+        <v>238</v>
       </c>
       <c r="G224" s="1"/>
       <c r="H224" s="1"/>
@@ -10387,11 +10376,11 @@
         <v>20</v>
       </c>
       <c r="B225" s="109" t="s">
-        <v>204</v>
+        <v>239</v>
       </c>
       <c r="C225" s="1"/>
       <c r="D225" s="93" t="s">
-        <v>205</v>
+        <v>240</v>
       </c>
       <c r="E225" s="1"/>
       <c r="F225" s="1"/>
@@ -10423,7 +10412,7 @@
     <row r="226" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="27"/>
       <c r="B226" s="175" t="s">
-        <v>206</v>
+        <v>241</v>
       </c>
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
@@ -10457,7 +10446,7 @@
     <row r="227" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="27"/>
       <c r="B227" s="175" t="s">
-        <v>207</v>
+        <v>242</v>
       </c>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
@@ -10491,7 +10480,7 @@
     <row r="228" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="27"/>
       <c r="B228" s="108" t="s">
-        <v>208</v>
+        <v>243</v>
       </c>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
@@ -10712,14 +10701,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="202" t="s">
-        <v>209</v>
+        <v>244</v>
       </c>
       <c r="B1" s="202"/>
       <c r="C1" s="21" t="s">
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="D1" s="201" t="s">
-        <v>211</v>
+        <v>246</v>
       </c>
       <c r="E1" s="201"/>
       <c r="F1" s="22"/>
@@ -10727,68 +10716,68 @@
     </row>
     <row r="2" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A2" s="110" t="s">
-        <v>212</v>
+        <v>247</v>
       </c>
       <c r="B2" s="105" t="s">
-        <v>213</v>
+        <v>248</v>
       </c>
       <c r="C2" s="193" t="s">
-        <v>214</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="110" t="s">
-        <v>215</v>
+        <v>250</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>216</v>
+        <v>251</v>
       </c>
       <c r="C3" s="194" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" s="111" t="s">
-        <v>218</v>
+        <v>253</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>219</v>
+        <v>254</v>
       </c>
       <c r="C4" s="194" t="s">
-        <v>220</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="111" t="s">
-        <v>221</v>
+        <v>256</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>222</v>
+        <v>257</v>
       </c>
       <c r="C5" s="194" t="s">
-        <v>223</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="110" t="s">
-        <v>224</v>
+        <v>259</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>225</v>
+        <v>260</v>
       </c>
       <c r="C6" s="194" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="111" t="s">
-        <v>227</v>
+        <v>262</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>228</v>
+        <v>263</v>
       </c>
       <c r="C7" s="194" t="s">
-        <v>229</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -10802,26 +10791,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a834da9-6c01-4b0d-9854-214ab0844664">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA421E502B73EC48B7C481B02707A95D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8e395bb2bcb17e943266a860489f057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a834da9-6c01-4b0d-9854-214ab0844664" xmlns:ns3="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b1084d163ef6a9ae7f6b3d13802deaa" ns2:_="" ns3:_="">
     <xsd:import namespace="1a834da9-6c01-4b0d-9854-214ab0844664"/>
@@ -11076,32 +11045,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8BE695-F061-495A-A060-7569CE2A6C93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a834da9-6c01-4b0d-9854-214ab0844664">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81CDBFC0-0126-4DB7-8868-40859C987D1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11118,4 +11082,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8BE695-F061-495A-A060-7569CE2A6C93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix question1 bus and buss translations
</commit_message>
<xml_diff>
--- a/media/questions.xlsx
+++ b/media/questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ju5315jo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ju5315jo\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4320B8F-EC9B-4442-B4FA-AB6DF6D830FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7762F53-2957-4672-A17C-8D9D9A412FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Yhdistetty" sheetId="6" r:id="rId1"/>
@@ -98,6 +98,24 @@
     <t>Jos ehtoa ei ole alikysymys kysytään aina, mutta jos ehto on niin sen on täytyttävä, että kysymys tulee näkyville. esim  jos on 3.0 niin alikysymys näytetään vain jos kysymyksessä kolme on vastattu vaihtoehto 0 (auto).</t>
   </si>
   <si>
+    <t>Vietät (ja haluat viettää) paljon aikaa tien päällä. Se ei kuitenkaan tarkoita sitä, että haluat tuhlata aikaa siirtymiseen. Pidät mukavasta matkanteosta ja haluat olla varma, että saavut paikalle ajoissa. Olet valmis harkitsemaan muita tapoja liikkua, mutta ainoastaan, jos sinun ei tarvitse uhrata laadukasta matkantekoa tai mukavuutta.//Du spenderar (och vill spendera) mycket tid på vägen. Det betyder dock inte att du vill slösa tid på byten. Du gillar att resa bekvämt och du vill vara säker på att du kommer dit i tid. Du är redo att överväga andra sätt att ta dig från en plats till en annan, men bara om du inte behöver offra kvalitetsresorna eller bekvämligheten.//You (like to) spend a lot of time on the road. But that doesn't mean that you like to lose time en route. You like to travel in comfort and want to be certain that you'll arrive on time. You are willing to consider other ways of getting around. But only if you don't have to sacrifice your quality or comfort.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiedät päivittäiset kohteesi ja miten niihin pääsee. Et pidä yllätyksistä matkan aikana; elämä on sellaisenaan jo tarpeeksi stressaavaa. Olet valmis kokeilemaan nopeampia tai mukavampia vaihtoehtoja, mutta vain jos saat selkeää tietoa niistä – mieluiten yksityiskohtaisen matkasuunnitelman kera.//Du vet dina dagliga resmål och hur du tar dig till dem. Du gillar inte överraskningar under resan; livet är tillräckligt stressigt som det är. Du är villig att prova snabbare eller bekvämare alternativ, men bara om du får tydlig information om dem – gärna med en detaljerad resplan.//You know where you're going every day and how to get there. You don't like surprises en route; life is already sufficiently stressful as it is. You are willing to try out faster or more comfortable alternatives. But only if you get clear information about this, preferably with a detailed travel plan. </t>
+  </si>
+  <si>
+    <t>Haluat olla liikkeellä ja nautit ulkona kävelystä ja pyöräilystä niin talvella kuin kesällä. Pääset lyhyillä matkoilla sinne, minne haluat – ympäri vuoden. Olet ehdottomasti avoin ideoille ja vaihtoehdoille, jotka tekevät matkastasi mukavamman tai hauskemman. Sinua auttaisivat kuitenkin vinkit siitä, kuinka kulkea pitkät etäisyydet helpommin. //Du gillar att vara i rörelse och du tycker om att gå och cykla ute både vinter och sommar. Du kan ta dig dit du vill med korta resor – året runt. Du är definitivt öppen för idéer och alternativ som kommer att göra din resa bekvämare eller roligare. Men tips om hur du lättare reser långa sträckor skulle hjälpa dig. //You like to be on the move and you enjoy walking and cycling outside in both winter and summer. You can get where you want with short trips - all year round. You are definitely open to ideas and options that will make your trip more comfortable or fun. However, tips on how to travel long distances more easily would help you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olethan nokkela, joten löydät aina jonkin tavan päästä määränpäähäsi. Matkan aikana haluat rentoutua, lukea kirjoja tai kuunnella musiikkia, tai ehkä haluat keskustella muiden matkustajien kanssa. Matkustusvaihtoehtosi ovat illalla sekä kauempana kaupungista rajalliset. Sinua kiinnostaa tietää, mitä muita liikkumisvaihtoehtoja on.//Du är snabbtänkt, så du hittar alltid ett sätt att ta dig till din destination. Under resan vill du koppla av, läsa böcker eller lyssna på musik, eller kanske vill du prata med andra passagerare. Dina resemöjligheter är begränsade på kvällen och längre bort från staden. Du är intresserad av att veta vilka andra mobilitetsalternativ som finns.//Witty as you are, you always find a way to get to your destination. You like to relax en route, reading a book or chilling to some music. Or perhaps you like to chat with others. Your travel options are more limited in the evening or when you're further from the city. You'd like to know what are the alternatives. </t>
+  </si>
+  <si>
+    <t>Uusia vaihtoehtoja tai uusia reittejä? Antaa tulla! Etsit aina kaikkein sopivinta ratkaisua ja haluat olla askeleen muita edellä. Sinua kiehtoo uusi tekniikka ja oivallukset. Haluat myös tutustua kaikkiin vaihtoehtoisiin liikkumismuotoihin ja testata niitä ensimmäisenä. Uskot siihen, että aina on parantamisen varaa.//Nya alternativ eller nya rutter? Kom an! Du letar alltid efter den lämpligaste lösningen och vill ligga steget före andra. Du fascineras av ny teknik och nya insikter. Du vill också sätta dig in i alla alternativa mobilitetsmetoder och testa dem först. Du tror att det alltid finns utrymme för förbättringar.//New options, new routes? Bring it on! You're always looking for the most suitable solutions and like to be one step ahead of the pack. You are fascinated by new technology and insights. You also want to learn about all the options for your own transport and be the first to test them. You are convinced that there's always some margin for improvement.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kun jotain aloitat, haluat olla hyvin valmistautunut. Valmistautuessasi tutkit kaikkia tarjolla olevia vaihtoehtoja avoimin mielin ja ennen lähtöä kartoitat tehokkaimman reitin määränpäähäsi. Erilaiset kulkuvälineet ovat sinulle tuttuja ja olet kiinnostunut selvittämään sekä kokeilemaan uusia vaihtoehtoja.//När man startar något vill man vara väl förberedd. När du förbereder dig utforskar du alla tillgängliga alternativ med ett öppet sinne och innan du ger dig av kartlägger du den mest effektiva rutten till din destination. Du är bekant med olika transportmedel och är intresserad av att ta reda på och prova nya alternativ.//You like to be prepared when you start on something. While preparing, you examine all the available options with an open mind. You also always map the most efficient route before leaving. You have already used different types of means of transport. When relevant, you are always interested in learning about new options. </t>
+  </si>
+  <si>
     <t>Helppo Hirvi//Enkel Älg//Easy Elk</t>
   </si>
   <si>
@@ -140,7 +158,7 @@
     <t>Juna//Tåg//Train</t>
   </si>
   <si>
-    <t>Linja-auto//Bus//Buss</t>
+    <t>Linja-auto//Buss//Bus</t>
   </si>
   <si>
     <t>Mopo tai skootteri//Moped eller skoter//Moped or scooter</t>
@@ -150,6 +168,9 @@
   </si>
   <si>
     <t>Kävellen//Gående//On foot</t>
+  </si>
+  <si>
+    <t>Sähköpotkulauta, segway tai muu vastaava//Elsparkcykel, segway eller liknande//E-scooter, segway or similar</t>
   </si>
   <si>
     <t>1a</t>
@@ -325,6 +346,9 @@
     <t>Auto ja joukkoliikenne.//Bil och kollektivtrafik.//Car and public transport.</t>
   </si>
   <si>
+    <t>Auto ja kävely.//Bil och gång.//Car and walking.</t>
+  </si>
+  <si>
     <t>Polkupyörä tai sähköpotkulauta ja joukkoliikenne.//Cykel eller elsparkcykel och kollektivtrafik.//Bicycle or scooter and public transport.</t>
   </si>
   <si>
@@ -640,9 +664,15 @@
     <t xml:space="preserve">ad </t>
   </si>
   <si>
+    <t>Polkupyörä tai sähköpyörä.//Cykel tai elcykel.//Bicycle or e-bike.</t>
+  </si>
+  <si>
     <t>Joukkoliikenne.//Kollektivtrafik.//Public transportation.</t>
   </si>
   <si>
+    <t>Sähköpotkulauta.//Elsparkcykel.//E-scooter.</t>
+  </si>
+  <si>
     <t>Ei mikään näistä.//Ingen av dessa.//None of these.</t>
   </si>
   <si>
@@ -715,7 +745,7 @@
     <t>Tähän joku keino, miten saadaan erotettua hupitäyttelijät ja oikeaan dataan kuuluvat</t>
   </si>
   <si>
-    <t>Huvin vuoksi//Bara för skojs skull//Just for fun</t>
+    <t>Huvin vuoksi.//Bara för skojs skull.//Just for fun.</t>
   </si>
   <si>
     <t>Haluan saada minulle räätälöityä tietoa liikkumisesta.//Jag vill få skräddarsydd information om mobilitet.//I want to receive customized information about mobility.</t>
@@ -733,8 +763,8 @@
     <t>Tällä valinnalla kootaan kustakin profiilista oma viestintälista.</t>
   </si>
   <si>
-    <t>Haluan tilata kestävän liikkumisen uutiskirjeen. (Liikenteen ja liikkumisen uutiskirjeen henkilörekisteri https:////rekisteri.turku.fi//Saabe_data// )//Jag vill prenumerera på nyhetsbrevet om hållbar rörlighet. (
-Trafik- och mobilitetnyhetsbrevets personregister https:////rekisteri.turku.fi//Saabe_data//)//I want to subscribe to the sustainable mobility newsletter (Traffic and mobility newsletter's personal register https:////rekisteri.turku.fi//Saabe_data//)</t>
+    <t>Haluan tilata kestävän liikkumisen uutiskirjeen.  (Liikenteen ja liikkumisen uutiskirjeen henkilörekisteri https:////rekisteri.turku.fi//Saabe_data// )//Jag vill prenumerera på nyhetsbrevet om hållbar rörlighet. (
+Trafik- och mobilitetnyhetsbrevets personregister https:////rekisteri.turku.fi//Saabe_data//)//I want to subscribe to the sustainable mobility newsletter. (Traffic and mobility newsletter's personal register https:////rekisteri.turku.fi//Saabe_data//)</t>
   </si>
   <si>
     <t>En halua.//Jag vill inte.//I do not want.</t>
@@ -816,36 +846,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tiedät päivittäiset kohteesi ja miten niihin pääsee. Et pidä yllätyksistä matkan aikana; elämä on sellaisenaan jo tarpeeksi stressaavaa. Olet valmis kokeilemaan nopeampia tai mukavampia vaihtoehtoja, mutta vain jos saat selkeää tietoa niistä – mieluiten yksityiskohtaisen matkasuunnitelman kera./Du vet dina dagliga resmål och hur du tar dig till dem. Du gillar inte överraskningar under resan; livet är tillräckligt stressigt som det är. Du är villig att prova snabbare eller bekvämare alternativ, men bara om du får tydlig information om dem – gärna med en detaljerad resplan./You know where you're going every day and how to get there. You don't like surprises en route; life is already sufficiently stressful as it is. You are willing to try out faster or more comfortable alternatives. But only if you get clear information about this, preferably with a detailed travel plan. </t>
-  </si>
-  <si>
-    <t>Polkupyörä tai sähköpyörä.//Cykel tai elcykel.//Bicycle or e-bike.</t>
-  </si>
-  <si>
-    <t>Sähköpotkulauta.//Elsparkcykel.//E-scooter.</t>
-  </si>
-  <si>
-    <t>Sähköpotkulauta, segway tai muu vastaava//Elsparkcykel, segway eller liknande//E-scooter, segway or similar</t>
-  </si>
-  <si>
-    <t>Auto ja kävely.//Bil och gång.//Car and walking.</t>
-  </si>
-  <si>
-    <t>Vietät (ja haluat viettää) paljon aikaa tien päällä. Se ei kuitenkaan tarkoita sitä, että haluat tuhlata aikaa siirtymiseen. Pidät mukavasta matkanteosta ja haluat olla varma, että saavut paikalle ajoissa. Olet valmis harkitsemaan muita tapoja liikkua, mutta ainoastaan, jos sinun ei tarvitse uhrata laadukasta matkantekoa tai mukavuutta.//Du spenderar (och vill spendera) mycket tid på vägen. Det betyder dock inte att du vill slösa tid på byten. Du gillar att resa bekvämt och du vill vara säker på att du kommer dit i tid. Du är redo att överväga andra sätt att ta dig från en plats till en annan, men bara om du inte behöver offra kvalitetsresorna eller bekvämligheten.//You (like to) spend a lot of time on the road. But that doesn't mean that you like to lose time en route. You like to travel in comfort and want to be certain that you'll arrive on time. You are willing to consider other ways of getting around. But only if you don't have to sacrifice your quality or comfort.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiedät päivittäiset kohteesi ja miten niihin pääsee. Et pidä yllätyksistä matkan aikana; elämä on sellaisenaan jo tarpeeksi stressaavaa. Olet valmis kokeilemaan nopeampia tai mukavampia vaihtoehtoja, mutta vain jos saat selkeää tietoa niistä – mieluiten yksityiskohtaisen matkasuunnitelman kera.//Du vet dina dagliga resmål och hur du tar dig till dem. Du gillar inte överraskningar under resan; livet är tillräckligt stressigt som det är. Du är villig att prova snabbare eller bekvämare alternativ, men bara om du får tydlig information om dem – gärna med en detaljerad resplan.//You know where you're going every day and how to get there. You don't like surprises en route; life is already sufficiently stressful as it is. You are willing to try out faster or more comfortable alternatives. But only if you get clear information about this, preferably with a detailed travel plan. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kun jotain aloitat, haluat olla hyvin valmistautunut. Valmistautuessasi tutkit kaikkia tarjolla olevia vaihtoehtoja avoimin mielin ja ennen lähtöä kartoitat tehokkaimman reitin määränpäähäsi. Erilaiset kulkuvälineet ovat sinulle tuttuja ja olet kiinnostunut selvittämään sekä kokeilemaan uusia vaihtoehtoja.//När man startar något vill man vara väl förberedd. När du förbereder dig utforskar du alla tillgängliga alternativ med ett öppet sinne och innan du ger dig av kartlägger du den mest effektiva rutten till din destination. Du är bekant med olika transportmedel och är intresserad av att ta reda på och prova nya alternativ.//You like to be prepared when you start on something. While preparing, you examine all the available options with an open mind. You also always map the most efficient route before leaving. You have already used different types of means of transport. When relevant, you are always interested in learning about new options. </t>
-  </si>
-  <si>
-    <t>Uusia vaihtoehtoja tai uusia reittejä? Antaa tulla! Etsit aina kaikkein sopivinta ratkaisua ja haluat olla askeleen muita edellä. Sinua kiehtoo uusi tekniikka ja oivallukset. Haluat myös tutustua kaikkiin vaihtoehtoisiin liikkumismuotoihin ja testata niitä ensimmäisenä. Uskot siihen, että aina on parantamisen varaa.//Nya alternativ eller nya rutter? Kom an! Du letar alltid efter den lämpligaste lösningen och vill ligga steget före andra. Du fascineras av ny teknik och nya insikter. Du vill också sätta dig in i alla alternativa mobilitetsmetoder och testa dem först. Du tror att det alltid finns utrymme för förbättringar.//New options, new routes? Bring it on! You're always looking for the most suitable solutions and like to be one step ahead of the pack. You are fascinated by new technology and insights. You also want to learn about all the options for your own transport and be the first to test them. You are convinced that there's always some margin for improvement.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Olethan nokkela, joten löydät aina jonkin tavan päästä määränpäähäsi. Matkan aikana haluat rentoutua, lukea kirjoja tai kuunnella musiikkia, tai ehkä haluat keskustella muiden matkustajien kanssa. Matkustusvaihtoehtosi ovat illalla sekä kauempana kaupungista rajalliset. Sinua kiinnostaa tietää, mitä muita liikkumisvaihtoehtoja on.//Du är snabbtänkt, så du hittar alltid ett sätt att ta dig till din destination. Under resan vill du koppla av, läsa böcker eller lyssna på musik, eller kanske vill du prata med andra passagerare. Dina resemöjligheter är begränsade på kvällen och längre bort från staden. Du är intresserad av att veta vilka andra mobilitetsalternativ som finns.//Witty as you are, you always find a way to get to your destination. You like to relax en route, reading a book or chilling to some music. Or perhaps you like to chat with others. Your travel options are more limited in the evening or when you're further from the city. You'd like to know what are the alternatives. </t>
-  </si>
-  <si>
-    <t>Haluat olla liikkeellä ja nautit ulkona kävelystä ja pyöräilystä niin talvella kuin kesällä. Pääset lyhyillä matkoilla sinne, minne haluat – ympäri vuoden. Olet ehdottomasti avoin ideoille ja vaihtoehdoille, jotka tekevät matkastasi mukavamman tai hauskemman. Sinua auttaisivat kuitenkin vinkit siitä, kuinka kulkea pitkät etäisyydet helpommin. //Du gillar att vara i rörelse och du tycker om att gå och cykla ute både vinter och sommar. Du kan ta dig dit du vill med korta resor – året runt. Du är definitivt öppen för idéer och alternativ som kommer att göra din resa bekvämare eller roligare. Men tips om hur du lättare reser långa sträckor skulle hjälpa dig. //You like to be on the move and you enjoy walking and cycling outside in both winter and summer. You can get where you want with short trips - all year round. You are definitely open to ideas and options that will make your trip more comfortable or fun. However, tips on how to travel long distances more easily would help you.</t>
   </si>
 </sst>
 </file>
@@ -2060,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF3ACC6-6455-42D3-BCE3-944B33DD47DC}">
   <dimension ref="A1:AD235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="E71" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2165,22 +2165,22 @@
       </c>
       <c r="J2" s="7"/>
       <c r="K2" s="191" t="s">
-        <v>261</v>
+        <v>18</v>
       </c>
       <c r="L2" s="191" t="s">
-        <v>262</v>
+        <v>19</v>
       </c>
       <c r="M2" s="190" t="s">
-        <v>266</v>
+        <v>20</v>
       </c>
       <c r="N2" s="191" t="s">
-        <v>265</v>
+        <v>21</v>
       </c>
       <c r="O2" s="191" t="s">
-        <v>264</v>
+        <v>22</v>
       </c>
       <c r="P2" s="191" t="s">
-        <v>263</v>
+        <v>23</v>
       </c>
       <c r="Q2" s="9"/>
       <c r="R2" s="8"/>
@@ -2209,22 +2209,22 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="105" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="L3" s="105" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="M3" s="105" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="N3" s="105" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="O3" s="105" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="P3" s="106" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="1"/>
@@ -2246,17 +2246,17 @@
         <v>1</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C4" s="54">
         <v>1</v>
       </c>
       <c r="D4" s="54"/>
       <c r="E4" s="95" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
@@ -2337,7 +2337,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K6" s="43"/>
       <c r="L6" s="2">
@@ -2375,7 +2375,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K7" s="43">
         <v>1</v>
@@ -2413,7 +2413,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K8" s="43">
         <v>1</v>
@@ -2447,7 +2447,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="123" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="G9" s="26"/>
       <c r="H9" s="26"/>
@@ -2529,7 +2529,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K11" s="143"/>
       <c r="L11" s="144"/>
@@ -2563,7 +2563,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K12" s="143">
         <v>1</v>
@@ -2601,7 +2601,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K13" s="143">
         <v>1</v>
@@ -2635,7 +2635,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="31" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
@@ -2715,7 +2715,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K16" s="43"/>
       <c r="L16" s="2"/>
@@ -2757,7 +2757,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K17" s="43"/>
       <c r="L17" s="2"/>
@@ -2797,7 +2797,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K18" s="43"/>
       <c r="L18" s="2"/>
@@ -2829,7 +2829,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="31" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G19" s="31"/>
       <c r="H19" s="31"/>
@@ -2909,7 +2909,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K21" s="43"/>
       <c r="L21" s="2"/>
@@ -2951,7 +2951,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K22" s="43"/>
       <c r="L22" s="2"/>
@@ -2991,7 +2991,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K23" s="43"/>
       <c r="L23" s="2"/>
@@ -3023,7 +3023,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="112" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
@@ -3109,7 +3109,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K26" s="43"/>
       <c r="L26" s="2"/>
@@ -3149,7 +3149,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K27" s="43"/>
       <c r="L27" s="2"/>
@@ -3187,7 +3187,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K28" s="43"/>
       <c r="L28" s="2"/>
@@ -3219,7 +3219,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="112" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
@@ -3303,7 +3303,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K31" s="43"/>
       <c r="L31" s="2"/>
@@ -3343,7 +3343,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K32" s="43"/>
       <c r="L32" s="2"/>
@@ -3383,7 +3383,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K33" s="43"/>
       <c r="L33" s="2"/>
@@ -3415,7 +3415,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="31" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -3489,7 +3489,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K36" s="43"/>
       <c r="L36" s="2"/>
@@ -3523,7 +3523,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K37" s="43"/>
       <c r="L37" s="2"/>
@@ -3559,7 +3559,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K38" s="43"/>
       <c r="L38" s="2"/>
@@ -3591,7 +3591,7 @@
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="113" t="s">
-        <v>259</v>
+        <v>42</v>
       </c>
       <c r="G39" s="31"/>
       <c r="H39" s="31"/>
@@ -3677,7 +3677,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K41" s="43"/>
       <c r="L41" s="2"/>
@@ -3715,7 +3715,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K42" s="43"/>
       <c r="L42" s="2"/>
@@ -3753,7 +3753,7 @@
       <c r="H43" s="61"/>
       <c r="I43" s="61"/>
       <c r="J43" s="71" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K43" s="65"/>
       <c r="L43" s="66"/>
@@ -3782,16 +3782,16 @@
     </row>
     <row r="44" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B44" s="115" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C44" s="60">
         <v>1</v>
       </c>
       <c r="D44" s="161" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
@@ -3799,7 +3799,7 @@
       <c r="H44" s="18"/>
       <c r="I44" s="18"/>
       <c r="J44" s="119" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="K44" s="146"/>
       <c r="L44" s="147"/>
@@ -3827,7 +3827,7 @@
       <c r="B45" s="72"/>
       <c r="C45" s="72"/>
       <c r="D45" s="91" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
@@ -3835,7 +3835,7 @@
       <c r="H45" s="18"/>
       <c r="I45" s="18"/>
       <c r="J45" s="120" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="K45" s="146"/>
       <c r="L45" s="147"/>
@@ -3869,7 +3869,7 @@
       <c r="H46" s="18"/>
       <c r="I46" s="18"/>
       <c r="J46" s="121" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="K46" s="146"/>
       <c r="L46" s="147"/>
@@ -3903,7 +3903,7 @@
       <c r="H47" s="18"/>
       <c r="I47" s="18"/>
       <c r="J47" s="121" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="K47" s="146"/>
       <c r="L47" s="147"/>
@@ -3928,26 +3928,26 @@
     </row>
     <row r="48" spans="1:30" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A48" s="29" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B48" s="114" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C48" s="164" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D48" s="92" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F48" s="73"/>
       <c r="G48" s="73"/>
       <c r="H48" s="31"/>
       <c r="I48" s="31"/>
       <c r="J48" s="112" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="K48" s="149"/>
       <c r="L48" s="150"/>
@@ -3973,13 +3973,13 @@
     <row r="49" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A49" s="27"/>
       <c r="D49" s="92" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E49" s="11"/>
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="116" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="K49" s="146"/>
       <c r="L49" s="153"/>
@@ -4011,7 +4011,7 @@
       <c r="H50" s="11"/>
       <c r="I50" s="11"/>
       <c r="J50" s="117" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="K50" s="146"/>
       <c r="L50" s="153"/>
@@ -4043,7 +4043,7 @@
       <c r="H51" s="35"/>
       <c r="I51" s="35"/>
       <c r="J51" s="120" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K51" s="147"/>
       <c r="L51" s="159"/>
@@ -4075,7 +4075,7 @@
       <c r="H52" s="64"/>
       <c r="I52" s="64"/>
       <c r="J52" s="34" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K52" s="155"/>
       <c r="L52" s="156"/>
@@ -4100,26 +4100,26 @@
     </row>
     <row r="53" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B53" s="122" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C53" s="165" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D53" s="94" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E53" s="34" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F53" s="62"/>
       <c r="G53" s="62"/>
       <c r="H53" s="34"/>
       <c r="I53" s="34"/>
       <c r="J53" s="125" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="K53" s="146"/>
       <c r="L53" s="159"/>
@@ -4145,13 +4145,13 @@
     <row r="54" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A54" s="27"/>
       <c r="D54" s="94" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E54" s="11"/>
       <c r="H54" s="11"/>
       <c r="I54" s="11"/>
       <c r="J54" s="117" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="K54" s="146"/>
       <c r="L54" s="153"/>
@@ -4183,7 +4183,7 @@
       <c r="H55" s="11"/>
       <c r="I55" s="11"/>
       <c r="J55" s="117" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="K55" s="146"/>
       <c r="L55" s="153"/>
@@ -4215,7 +4215,7 @@
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
       <c r="J56" s="116" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="K56" s="146"/>
       <c r="L56" s="153"/>
@@ -4247,7 +4247,7 @@
       <c r="H57" s="34"/>
       <c r="I57" s="34"/>
       <c r="J57" s="125" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K57" s="146"/>
       <c r="L57" s="159"/>
@@ -4279,7 +4279,7 @@
       <c r="H58" s="35"/>
       <c r="I58" s="35"/>
       <c r="J58" s="120" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="K58" s="178"/>
       <c r="L58" s="177"/>
@@ -4311,7 +4311,7 @@
       <c r="H59" s="182"/>
       <c r="I59" s="182"/>
       <c r="J59" s="183" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K59" s="184"/>
       <c r="L59" s="185"/>
@@ -4336,24 +4336,24 @@
     </row>
     <row r="60" spans="1:30" s="62" customFormat="1" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A60" s="27" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B60" s="115" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C60" s="166" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D60" s="93" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="E60" s="34" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="H60" s="35"/>
       <c r="I60" s="35"/>
       <c r="J60" s="120" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="K60" s="146"/>
       <c r="L60" s="147"/>
@@ -4381,13 +4381,13 @@
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
       <c r="D61" s="93" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E61" s="11"/>
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
       <c r="J61" s="116" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="K61" s="146"/>
       <c r="L61" s="154"/>
@@ -4419,7 +4419,7 @@
       <c r="H62" s="11"/>
       <c r="I62" s="11"/>
       <c r="J62" s="117" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="K62" s="146"/>
       <c r="L62" s="154"/>
@@ -4451,7 +4451,7 @@
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
       <c r="J63" s="116" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="K63" s="146"/>
       <c r="L63" s="154"/>
@@ -4483,7 +4483,7 @@
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
       <c r="J64" s="116" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="K64" s="146"/>
       <c r="L64" s="154"/>
@@ -4515,7 +4515,7 @@
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
       <c r="J65" s="116" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="K65" s="146"/>
       <c r="L65" s="154"/>
@@ -4547,7 +4547,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
       <c r="J66" s="117" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="K66" s="146"/>
       <c r="L66" s="154"/>
@@ -4572,16 +4572,16 @@
     </row>
     <row r="67" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A67" s="29" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B67" s="114" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C67" s="53">
         <v>1</v>
       </c>
       <c r="D67" s="91" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E67" s="26"/>
       <c r="F67" s="73"/>
@@ -4589,7 +4589,7 @@
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
       <c r="J67" s="126" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="K67" s="149"/>
       <c r="L67" s="151"/>
@@ -4617,7 +4617,7 @@
       <c r="B68" s="18"/>
       <c r="C68" s="18"/>
       <c r="D68" s="91" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E68" s="18"/>
       <c r="F68" s="62"/>
@@ -4625,7 +4625,7 @@
       <c r="H68" s="34"/>
       <c r="I68" s="34"/>
       <c r="J68" s="125" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="K68" s="146"/>
       <c r="L68" s="147"/>
@@ -4659,7 +4659,7 @@
       <c r="H69" s="101"/>
       <c r="I69" s="101"/>
       <c r="J69" s="127" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="K69" s="155"/>
       <c r="L69" s="157"/>
@@ -4684,20 +4684,20 @@
     </row>
     <row r="70" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A70" s="27" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B70" s="128" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="102" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E70" s="1"/>
       <c r="H70" s="11"/>
       <c r="I70" s="11"/>
       <c r="J70" s="117" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="K70" s="146"/>
       <c r="L70" s="154"/>
@@ -4725,13 +4725,13 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="102" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E71" s="1"/>
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
       <c r="J71" s="117" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="K71" s="146"/>
       <c r="L71" s="154"/>
@@ -4763,7 +4763,7 @@
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
       <c r="J72" s="117" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="K72" s="146"/>
       <c r="L72" s="154"/>
@@ -4791,21 +4791,21 @@
         <v>2</v>
       </c>
       <c r="B73" s="49" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C73" s="167" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D73" s="49"/>
       <c r="E73" s="34" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F73" s="73"/>
       <c r="G73" s="73"/>
       <c r="H73" s="31"/>
       <c r="I73" s="31"/>
       <c r="J73" s="112" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="K73" s="42">
         <v>1</v>
@@ -4847,7 +4847,7 @@
       <c r="H74" s="35"/>
       <c r="I74" s="35"/>
       <c r="J74" s="120" t="s">
-        <v>260</v>
+        <v>100</v>
       </c>
       <c r="K74" s="43">
         <v>1</v>
@@ -4880,7 +4880,7 @@
       <c r="H75" s="13"/>
       <c r="I75" s="13"/>
       <c r="J75" s="116" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="K75" s="43"/>
       <c r="L75" s="2"/>
@@ -4920,7 +4920,7 @@
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
       <c r="J76" s="116" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="K76" s="43">
         <v>1</v>
@@ -4958,7 +4958,7 @@
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
       <c r="J77" s="116" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="K77" s="43"/>
       <c r="L77" s="2"/>
@@ -4996,7 +4996,7 @@
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
       <c r="J78" s="116" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="K78" s="43"/>
       <c r="L78" s="2"/>
@@ -5034,7 +5034,7 @@
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
       <c r="J79" s="116" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="K79" s="43">
         <v>1</v>
@@ -5070,7 +5070,7 @@
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
       <c r="J80" s="34" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K80" s="43"/>
       <c r="L80" s="2"/>
@@ -5098,7 +5098,7 @@
         <v>3</v>
       </c>
       <c r="B81" s="129" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C81" s="49"/>
       <c r="D81" s="49"/>
@@ -5108,7 +5108,7 @@
       <c r="H81" s="23"/>
       <c r="I81" s="23"/>
       <c r="J81" s="112" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="K81" s="42">
         <v>1</v>
@@ -5144,7 +5144,7 @@
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
       <c r="J82" s="116" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="K82" s="43"/>
       <c r="L82" s="2"/>
@@ -5182,7 +5182,7 @@
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
       <c r="J83" s="116" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="K83" s="43"/>
       <c r="L83" s="2"/>
@@ -5220,7 +5220,7 @@
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
       <c r="J84" s="116" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="K84" s="43"/>
       <c r="L84" s="2"/>
@@ -5254,7 +5254,7 @@
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
       <c r="J85" s="116" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="K85" s="43"/>
       <c r="L85" s="2"/>
@@ -5290,7 +5290,7 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
       <c r="J86" s="116" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="K86" s="43"/>
       <c r="L86" s="2"/>
@@ -5326,7 +5326,7 @@
       <c r="H87" s="17"/>
       <c r="I87" s="17"/>
       <c r="J87" s="116" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="K87" s="43"/>
       <c r="L87" s="2"/>
@@ -5356,25 +5356,25 @@
         <v>4</v>
       </c>
       <c r="B88" s="114" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C88" s="49"/>
       <c r="D88" s="51"/>
       <c r="E88" s="124" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F88" s="52" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="G88" s="163"/>
       <c r="H88" s="112" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="I88" s="173" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="J88" s="112" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="K88" s="42">
         <v>1</v>
@@ -5407,7 +5407,7 @@
       <c r="H89" s="14"/>
       <c r="I89" s="14"/>
       <c r="J89" s="116" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="K89" s="43">
         <v>1</v>
@@ -5443,7 +5443,7 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="116" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="K90" s="43">
         <v>1</v>
@@ -5481,7 +5481,7 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="116" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="K91" s="43">
         <v>1</v>
@@ -5519,7 +5519,7 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="116" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="K92" s="43"/>
       <c r="L92" s="2"/>
@@ -5555,7 +5555,7 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
       <c r="J93" s="116" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="K93" s="43">
         <v>1</v>
@@ -5591,7 +5591,7 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="116" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="K94" s="43">
         <v>1</v>
@@ -5629,7 +5629,7 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
       <c r="J95" s="116" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="K95" s="43">
         <v>1</v>
@@ -5665,7 +5665,7 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="116" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="K96" s="43">
         <v>1</v>
@@ -5703,7 +5703,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="116" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="K97" s="43">
         <v>1</v>
@@ -5739,7 +5739,7 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="116" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="K98" s="43"/>
       <c r="L98" s="2">
@@ -5775,7 +5775,7 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="116" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="K99" s="43">
         <v>1</v>
@@ -5813,7 +5813,7 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="116" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="K100" s="43">
         <v>1</v>
@@ -5851,7 +5851,7 @@
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
       <c r="J101" s="116" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="K101" s="43">
         <v>1</v>
@@ -5889,7 +5889,7 @@
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
       <c r="J102" s="34" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K102" s="43"/>
       <c r="L102" s="2"/>
@@ -5919,17 +5919,17 @@
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="52" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="G103" s="1"/>
       <c r="H103" s="112" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="I103" s="174" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="J103" s="112" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="K103" s="140">
         <v>1</v>
@@ -5963,11 +5963,11 @@
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="12" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="I104" s="12"/>
       <c r="J104" s="116" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="K104" s="143">
         <v>1</v>
@@ -6003,7 +6003,7 @@
       <c r="H105" s="12"/>
       <c r="I105" s="12"/>
       <c r="J105" s="116" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="K105" s="143">
         <v>1</v>
@@ -6039,7 +6039,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
       <c r="J106" s="116" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="K106" s="143">
         <v>1</v>
@@ -6075,7 +6075,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
       <c r="J107" s="116" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K107" s="143">
         <v>1</v>
@@ -6111,7 +6111,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
       <c r="J108" s="116" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="K108" s="143">
         <v>1</v>
@@ -6147,7 +6147,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
       <c r="J109" s="116" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="K109" s="143"/>
       <c r="L109" s="144">
@@ -6183,7 +6183,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
       <c r="J110" s="116" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="K110" s="143">
         <v>1</v>
@@ -6221,7 +6221,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
       <c r="J111" s="13" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="K111" s="143">
         <v>1</v>
@@ -6257,7 +6257,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
       <c r="J112" s="116" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="K112" s="143">
         <v>1</v>
@@ -6295,7 +6295,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="12"/>
       <c r="J113" s="116" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="K113" s="143">
         <v>1</v>
@@ -6333,7 +6333,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
       <c r="J114" s="34" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K114" s="143"/>
       <c r="L114" s="144"/>
@@ -6363,17 +6363,17 @@
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="130" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="G115" s="53"/>
       <c r="H115" s="112" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="I115" s="174" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="J115" s="112" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="K115" s="42"/>
       <c r="L115" s="24"/>
@@ -6411,7 +6411,7 @@
       <c r="H116" s="17"/>
       <c r="I116" s="17"/>
       <c r="J116" s="116" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="K116" s="43"/>
       <c r="L116" s="2"/>
@@ -6451,7 +6451,7 @@
       <c r="H117" s="1"/>
       <c r="I117" s="1"/>
       <c r="J117" s="116" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="K117" s="43"/>
       <c r="L117" s="2"/>
@@ -6491,7 +6491,7 @@
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
       <c r="J118" s="116" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="K118" s="43"/>
       <c r="L118" s="2"/>
@@ -6531,7 +6531,7 @@
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
       <c r="J119" s="116" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="K119" s="43"/>
       <c r="L119" s="2"/>
@@ -6571,7 +6571,7 @@
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
       <c r="J120" s="116" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="K120" s="43"/>
       <c r="L120" s="2"/>
@@ -6609,7 +6609,7 @@
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="116" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="K121" s="43"/>
       <c r="L121" s="2"/>
@@ -6649,7 +6649,7 @@
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
       <c r="J122" s="116" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="K122" s="43"/>
       <c r="L122" s="2">
@@ -6685,7 +6685,7 @@
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
       <c r="J123" s="116" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="K123" s="43"/>
       <c r="L123" s="2">
@@ -6723,7 +6723,7 @@
       <c r="H124" s="1"/>
       <c r="I124" s="1"/>
       <c r="J124" s="116" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K124" s="43"/>
       <c r="L124" s="2"/>
@@ -6763,7 +6763,7 @@
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
       <c r="J125" s="116" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="K125" s="43"/>
       <c r="L125" s="2">
@@ -6799,7 +6799,7 @@
       <c r="H126" s="1"/>
       <c r="I126" s="1"/>
       <c r="J126" s="34" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K126" s="43"/>
       <c r="L126" s="2"/>
@@ -6829,17 +6829,17 @@
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="114" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="G127" s="52"/>
       <c r="H127" s="112" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="I127" s="174" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="J127" s="112" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="K127" s="42"/>
       <c r="L127" s="24"/>
@@ -6877,7 +6877,7 @@
       <c r="H128" s="17"/>
       <c r="I128" s="17"/>
       <c r="J128" s="116" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="K128" s="43"/>
       <c r="L128" s="2"/>
@@ -6915,7 +6915,7 @@
       <c r="H129" s="1"/>
       <c r="I129" s="1"/>
       <c r="J129" s="116" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="K129" s="43"/>
       <c r="L129" s="2"/>
@@ -6953,7 +6953,7 @@
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
       <c r="J130" s="116" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="K130" s="43"/>
       <c r="L130" s="2"/>
@@ -6991,7 +6991,7 @@
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
       <c r="J131" s="116" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="K131" s="43"/>
       <c r="L131" s="2"/>
@@ -7027,7 +7027,7 @@
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
       <c r="J132" s="116" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="K132" s="43"/>
       <c r="L132" s="2"/>
@@ -7063,7 +7063,7 @@
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
       <c r="J133" s="116" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K133" s="43"/>
       <c r="L133" s="2"/>
@@ -7103,7 +7103,7 @@
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
       <c r="J134" s="116" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="K134" s="43"/>
       <c r="L134" s="2">
@@ -7139,7 +7139,7 @@
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
       <c r="J135" s="116" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="K135" s="43"/>
       <c r="L135" s="2"/>
@@ -7177,7 +7177,7 @@
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
       <c r="J136" s="34" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K136" s="43"/>
       <c r="L136" s="2"/>
@@ -7207,17 +7207,17 @@
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="130" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="G137" s="53"/>
       <c r="H137" s="112" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="I137" s="174" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="J137" s="112" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="K137" s="42"/>
       <c r="L137" s="24"/>
@@ -7255,7 +7255,7 @@
       <c r="H138" s="17"/>
       <c r="I138" s="17"/>
       <c r="J138" s="116" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="K138" s="43"/>
       <c r="L138" s="2"/>
@@ -7295,7 +7295,7 @@
       <c r="H139" s="1"/>
       <c r="I139" s="1"/>
       <c r="J139" s="116" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="K139" s="43"/>
       <c r="L139" s="2"/>
@@ -7333,7 +7333,7 @@
       <c r="H140" s="1"/>
       <c r="I140" s="1"/>
       <c r="J140" s="116" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="K140" s="43"/>
       <c r="L140" s="2"/>
@@ -7371,7 +7371,7 @@
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
       <c r="J141" s="116" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="K141" s="43"/>
       <c r="L141" s="2"/>
@@ -7407,7 +7407,7 @@
       <c r="H142" s="1"/>
       <c r="I142" s="1"/>
       <c r="J142" s="116" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="K142" s="43"/>
       <c r="L142" s="2"/>
@@ -7443,7 +7443,7 @@
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
       <c r="J143" s="116" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="K143" s="43"/>
       <c r="L143" s="2"/>
@@ -7479,7 +7479,7 @@
       <c r="H144" s="1"/>
       <c r="I144" s="1"/>
       <c r="J144" s="116" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="K144" s="43"/>
       <c r="L144" s="2"/>
@@ -7515,7 +7515,7 @@
       <c r="H145" s="1"/>
       <c r="I145" s="1"/>
       <c r="J145" s="116" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="K145" s="43"/>
       <c r="L145" s="2"/>
@@ -7553,7 +7553,7 @@
       <c r="H146" s="1"/>
       <c r="I146" s="1"/>
       <c r="J146" s="116" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="K146" s="43"/>
       <c r="L146" s="2">
@@ -7591,7 +7591,7 @@
       <c r="H147" s="1"/>
       <c r="I147" s="1"/>
       <c r="J147" s="116" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="K147" s="43"/>
       <c r="L147" s="2">
@@ -7627,7 +7627,7 @@
       <c r="H148" s="1"/>
       <c r="I148" s="1"/>
       <c r="J148" s="116" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="K148" s="43"/>
       <c r="L148" s="2"/>
@@ -7665,7 +7665,7 @@
       <c r="H149" s="1"/>
       <c r="I149" s="1"/>
       <c r="J149" s="34" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K149" s="43"/>
       <c r="L149" s="2"/>
@@ -7695,17 +7695,17 @@
       <c r="D150" s="18"/>
       <c r="E150" s="18"/>
       <c r="F150" s="129" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="G150" s="49"/>
       <c r="H150" s="112" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="I150" s="174" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="J150" s="112" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="K150" s="42"/>
       <c r="L150" s="24"/>
@@ -7739,7 +7739,7 @@
       <c r="H151" s="17"/>
       <c r="I151" s="17"/>
       <c r="J151" s="116" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="K151" s="43"/>
       <c r="L151" s="2"/>
@@ -7777,7 +7777,7 @@
       <c r="H152" s="1"/>
       <c r="I152" s="1"/>
       <c r="J152" s="116" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="K152" s="43"/>
       <c r="L152" s="2"/>
@@ -7813,7 +7813,7 @@
       <c r="H153" s="1"/>
       <c r="I153" s="1"/>
       <c r="J153" s="116" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="K153" s="43"/>
       <c r="L153" s="2"/>
@@ -7849,7 +7849,7 @@
       <c r="H154" s="1"/>
       <c r="I154" s="1"/>
       <c r="J154" s="116" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="K154" s="43"/>
       <c r="L154" s="2"/>
@@ -7885,7 +7885,7 @@
       <c r="H155" s="1"/>
       <c r="I155" s="1"/>
       <c r="J155" s="116" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="K155" s="43"/>
       <c r="L155" s="2">
@@ -7921,7 +7921,7 @@
       <c r="H156" s="1"/>
       <c r="I156" s="1"/>
       <c r="J156" s="116" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="K156" s="43"/>
       <c r="L156" s="2"/>
@@ -7959,7 +7959,7 @@
       <c r="H157" s="61"/>
       <c r="I157" s="18"/>
       <c r="J157" s="116" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K157" s="65"/>
       <c r="L157" s="66"/>
@@ -7987,23 +7987,23 @@
         <v>5</v>
       </c>
       <c r="B158" s="115" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C158" s="54">
         <v>3</v>
       </c>
       <c r="D158" s="93" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="E158" s="120" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="F158" s="18"/>
       <c r="G158" s="18"/>
       <c r="H158" s="18"/>
       <c r="I158" s="18"/>
       <c r="J158" s="120" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="K158" s="43"/>
       <c r="L158" s="36"/>
@@ -8031,7 +8031,7 @@
       <c r="B159" s="13"/>
       <c r="C159" s="13"/>
       <c r="D159" s="93" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="E159" s="13"/>
       <c r="F159" s="1"/>
@@ -8039,7 +8039,7 @@
       <c r="H159" s="1"/>
       <c r="I159" s="1"/>
       <c r="J159" s="34" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="K159" s="43"/>
       <c r="L159" s="2"/>
@@ -8073,7 +8073,7 @@
       <c r="H160" s="1"/>
       <c r="I160" s="1"/>
       <c r="J160" s="116" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="K160" s="43"/>
       <c r="L160" s="2"/>
@@ -8107,7 +8107,7 @@
       <c r="H161" s="1"/>
       <c r="I161" s="1"/>
       <c r="J161" s="34" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="K161" s="43"/>
       <c r="L161" s="2"/>
@@ -8141,7 +8141,7 @@
       <c r="H162" s="1"/>
       <c r="I162" s="1"/>
       <c r="J162" s="116" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="K162" s="43"/>
       <c r="L162" s="2"/>
@@ -8175,7 +8175,7 @@
       <c r="H163" s="1"/>
       <c r="I163" s="1"/>
       <c r="J163" s="34" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="K163" s="43"/>
       <c r="L163" s="2"/>
@@ -8209,7 +8209,7 @@
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
       <c r="J164" s="116" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="K164" s="43"/>
       <c r="L164" s="2"/>
@@ -8243,7 +8243,7 @@
       <c r="H165" s="1"/>
       <c r="I165" s="1"/>
       <c r="J165" s="34" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="K165" s="43"/>
       <c r="L165" s="2"/>
@@ -8277,7 +8277,7 @@
       <c r="H166" s="1"/>
       <c r="I166" s="1"/>
       <c r="J166" s="116" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="K166" s="43"/>
       <c r="L166" s="2"/>
@@ -8311,7 +8311,7 @@
       <c r="H167" s="1"/>
       <c r="I167" s="1"/>
       <c r="J167" s="34" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="K167" s="43"/>
       <c r="L167" s="2"/>
@@ -8345,7 +8345,7 @@
       <c r="H168" s="1"/>
       <c r="I168" s="1"/>
       <c r="J168" s="116" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="K168" s="43"/>
       <c r="L168" s="2"/>
@@ -8379,7 +8379,7 @@
       <c r="H169" s="1"/>
       <c r="I169" s="1"/>
       <c r="J169" s="116" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="K169" s="43"/>
       <c r="L169" s="2"/>
@@ -8413,7 +8413,7 @@
       <c r="H170" s="1"/>
       <c r="I170" s="1"/>
       <c r="J170" s="116" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="K170" s="43"/>
       <c r="L170" s="2"/>
@@ -8447,7 +8447,7 @@
       <c r="H171" s="1"/>
       <c r="I171" s="1"/>
       <c r="J171" s="34" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="K171" s="43"/>
       <c r="L171" s="2"/>
@@ -8481,7 +8481,7 @@
       <c r="H172" s="1"/>
       <c r="I172" s="1"/>
       <c r="J172" s="34" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="K172" s="43"/>
       <c r="L172" s="2"/>
@@ -8515,7 +8515,7 @@
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
       <c r="J173" s="116" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="K173" s="43"/>
       <c r="L173" s="2"/>
@@ -8549,7 +8549,7 @@
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
       <c r="J174" s="34" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="K174" s="43"/>
       <c r="L174" s="2"/>
@@ -8583,7 +8583,7 @@
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
       <c r="J175" s="34" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="K175" s="43"/>
       <c r="L175" s="2"/>
@@ -8617,7 +8617,7 @@
       <c r="H176" s="1"/>
       <c r="I176" s="1"/>
       <c r="J176" s="34" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="K176" s="43"/>
       <c r="L176" s="2"/>
@@ -8651,7 +8651,7 @@
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
       <c r="J177" s="34" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="K177" s="43"/>
       <c r="L177" s="2"/>
@@ -8685,7 +8685,7 @@
       <c r="H178" s="61"/>
       <c r="I178" s="61"/>
       <c r="J178" s="101" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K178" s="65"/>
       <c r="L178" s="66"/>
@@ -8713,21 +8713,21 @@
         <v>6</v>
       </c>
       <c r="B179" s="122" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C179" s="50">
         <v>1</v>
       </c>
       <c r="D179" s="50"/>
       <c r="E179" s="124" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F179" s="62"/>
       <c r="G179" s="35"/>
       <c r="H179" s="35"/>
       <c r="I179" s="35"/>
       <c r="J179" s="120" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="K179" s="43"/>
       <c r="L179" s="36"/>
@@ -8759,7 +8759,7 @@
       <c r="H180" s="35"/>
       <c r="I180" s="35"/>
       <c r="J180" s="34" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="K180" s="43"/>
       <c r="L180" s="36"/>
@@ -8792,7 +8792,7 @@
       <c r="H181" s="13"/>
       <c r="I181" s="13"/>
       <c r="J181" s="116" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="K181" s="43"/>
       <c r="L181" s="2"/>
@@ -8825,7 +8825,7 @@
       <c r="H182" s="13"/>
       <c r="I182" s="13"/>
       <c r="J182" s="116" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="K182" s="43"/>
       <c r="L182" s="2"/>
@@ -8858,7 +8858,7 @@
       <c r="H183" s="13"/>
       <c r="I183" s="13"/>
       <c r="J183" s="34" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="K183" s="43"/>
       <c r="L183" s="2"/>
@@ -8891,7 +8891,7 @@
       <c r="H184" s="13"/>
       <c r="I184" s="13"/>
       <c r="J184" s="116" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="K184" s="43"/>
       <c r="L184" s="2"/>
@@ -8925,7 +8925,7 @@
       <c r="H185" s="70"/>
       <c r="I185" s="70"/>
       <c r="J185" s="118" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="K185" s="65"/>
       <c r="L185" s="66"/>
@@ -8953,7 +8953,7 @@
         <v>7</v>
       </c>
       <c r="B186" s="122" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C186" s="50"/>
       <c r="D186" s="50"/>
@@ -8963,7 +8963,7 @@
       <c r="H186" s="35"/>
       <c r="I186" s="35"/>
       <c r="J186" s="35" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="K186" s="43"/>
       <c r="L186" s="36"/>
@@ -8996,7 +8996,7 @@
       <c r="H187" s="13"/>
       <c r="I187" s="13"/>
       <c r="J187" s="13" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="K187" s="43"/>
       <c r="L187" s="2"/>
@@ -9030,7 +9030,7 @@
       <c r="H188" s="70"/>
       <c r="I188" s="70"/>
       <c r="J188" s="118" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="K188" s="65"/>
       <c r="L188" s="66"/>
@@ -9058,7 +9058,7 @@
         <v>8</v>
       </c>
       <c r="B189" s="115" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C189" s="62"/>
       <c r="D189" s="162">
@@ -9070,7 +9070,7 @@
       <c r="H189" s="35"/>
       <c r="I189" s="35"/>
       <c r="J189" s="120" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="K189" s="43"/>
       <c r="L189" s="36"/>
@@ -9098,14 +9098,14 @@
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="93" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="E190" s="1"/>
       <c r="G190" s="13"/>
       <c r="H190" s="13"/>
       <c r="I190" s="13"/>
       <c r="J190" s="116" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="K190" s="43"/>
       <c r="L190" s="2"/>
@@ -9138,7 +9138,7 @@
       <c r="H191" s="13"/>
       <c r="I191" s="13"/>
       <c r="J191" s="116" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="K191" s="43"/>
       <c r="L191" s="2"/>
@@ -9171,7 +9171,7 @@
       <c r="H192" s="13"/>
       <c r="I192" s="13"/>
       <c r="J192" s="116" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="K192" s="43"/>
       <c r="L192" s="2"/>
@@ -9204,7 +9204,7 @@
       <c r="H193" s="13"/>
       <c r="I193" s="13"/>
       <c r="J193" s="116" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="K193" s="43"/>
       <c r="L193" s="2"/>
@@ -9230,7 +9230,7 @@
     <row r="194" spans="1:30" s="16" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="29"/>
       <c r="B194" s="194" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C194" s="195"/>
       <c r="D194" s="195"/>
@@ -9264,7 +9264,7 @@
     <row r="195" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="27"/>
       <c r="B195" s="131" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C195" s="78"/>
       <c r="D195" s="78"/>
@@ -9332,7 +9332,7 @@
         <v>9</v>
       </c>
       <c r="B197" s="114" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="C197" s="52"/>
       <c r="D197" s="52"/>
@@ -9342,7 +9342,7 @@
       <c r="H197" s="31"/>
       <c r="I197" s="31"/>
       <c r="J197" s="31" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="K197" s="42">
         <v>1</v>
@@ -9374,7 +9374,7 @@
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="E198" s="1"/>
       <c r="F198" s="116"/>
@@ -9382,7 +9382,7 @@
       <c r="H198" s="13"/>
       <c r="I198" s="13"/>
       <c r="J198" s="116" t="s">
-        <v>257</v>
+        <v>206</v>
       </c>
       <c r="K198" s="43"/>
       <c r="L198" s="2"/>
@@ -9420,7 +9420,7 @@
       <c r="H199" s="13"/>
       <c r="I199" s="13"/>
       <c r="J199" s="116" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="K199" s="43"/>
       <c r="L199" s="2"/>
@@ -9458,7 +9458,7 @@
       <c r="H200" s="13"/>
       <c r="I200" s="13"/>
       <c r="J200" s="116" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="K200" s="43"/>
       <c r="L200" s="2"/>
@@ -9494,7 +9494,7 @@
       <c r="H201" s="19"/>
       <c r="I201" s="19"/>
       <c r="J201" s="132" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="K201" s="43"/>
       <c r="L201" s="2"/>
@@ -9528,7 +9528,7 @@
       <c r="H202" s="19"/>
       <c r="I202" s="19"/>
       <c r="J202" s="72" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="K202" s="43"/>
       <c r="L202" s="2"/>
@@ -9556,7 +9556,7 @@
         <v>10</v>
       </c>
       <c r="B203" s="52" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="C203" s="57"/>
       <c r="D203" s="57"/>
@@ -9566,7 +9566,7 @@
       <c r="H203" s="31"/>
       <c r="I203" s="31"/>
       <c r="J203" s="31" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="K203" s="42"/>
       <c r="L203" s="24"/>
@@ -9604,7 +9604,7 @@
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
       <c r="J204" s="116" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="K204" s="43">
         <v>1</v>
@@ -9646,7 +9646,7 @@
       <c r="H205" s="13"/>
       <c r="I205" s="13"/>
       <c r="J205" s="13" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="K205" s="43"/>
       <c r="L205" s="2">
@@ -9674,7 +9674,7 @@
     <row r="206" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A206" s="29"/>
       <c r="B206" s="196" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C206" s="197"/>
       <c r="D206" s="197"/>
@@ -9710,7 +9710,7 @@
         <v>12</v>
       </c>
       <c r="B207" s="133" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="C207" s="55"/>
       <c r="D207" s="55"/>
@@ -9720,7 +9720,7 @@
       <c r="H207" s="34"/>
       <c r="I207" s="34"/>
       <c r="J207" s="39" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="K207" s="43"/>
       <c r="L207" s="2"/>
@@ -9754,7 +9754,7 @@
       <c r="H208" s="34"/>
       <c r="I208" s="34"/>
       <c r="J208" s="40" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="K208" s="43"/>
       <c r="L208" s="2"/>
@@ -9788,7 +9788,7 @@
       <c r="H209" s="18"/>
       <c r="I209" s="18"/>
       <c r="J209" s="104" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="K209" s="43"/>
       <c r="L209" s="2"/>
@@ -9816,13 +9816,13 @@
         <v>13</v>
       </c>
       <c r="B210" s="133" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="C210" s="55"/>
       <c r="D210" s="55"/>
       <c r="E210" s="55"/>
       <c r="F210" s="41" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="G210" s="59"/>
       <c r="H210" s="59"/>
@@ -9854,13 +9854,13 @@
         <v>14</v>
       </c>
       <c r="B211" s="135" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="C211" s="56"/>
       <c r="D211" s="56"/>
       <c r="E211" s="56"/>
       <c r="F211" s="139" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="G211" s="18"/>
       <c r="H211" s="18"/>
@@ -9892,7 +9892,7 @@
         <v>15</v>
       </c>
       <c r="B212" s="135" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="C212" s="56"/>
       <c r="D212" s="56"/>
@@ -9928,7 +9928,7 @@
         <v>16</v>
       </c>
       <c r="B213" s="135" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="C213" s="56"/>
       <c r="D213" s="56"/>
@@ -9938,7 +9938,7 @@
       <c r="H213" s="35"/>
       <c r="I213" s="35"/>
       <c r="J213" s="137" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="K213" s="43"/>
       <c r="L213" s="2"/>
@@ -9972,7 +9972,7 @@
       <c r="H214" s="35"/>
       <c r="I214" s="35"/>
       <c r="J214" s="138" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="K214" s="43"/>
       <c r="L214" s="2"/>
@@ -10006,7 +10006,7 @@
       <c r="H215" s="35"/>
       <c r="I215" s="35"/>
       <c r="J215" s="138" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="K215" s="43"/>
       <c r="L215" s="2"/>
@@ -10040,7 +10040,7 @@
       <c r="H216" s="35"/>
       <c r="I216" s="35"/>
       <c r="J216" s="138" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="K216" s="43"/>
       <c r="L216" s="2"/>
@@ -10074,7 +10074,7 @@
       <c r="H217" s="35"/>
       <c r="I217" s="35"/>
       <c r="J217" s="138" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="K217" s="43"/>
       <c r="L217" s="2"/>
@@ -10183,15 +10183,15 @@
         <v>17</v>
       </c>
       <c r="B220" s="136" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="C220" s="26"/>
       <c r="D220" s="26"/>
       <c r="E220" s="97" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="F220" s="107" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="G220" s="26"/>
       <c r="H220" s="26"/>
@@ -10225,7 +10225,7 @@
       <c r="D221" s="61"/>
       <c r="E221" s="61"/>
       <c r="F221" s="118" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="G221" s="61"/>
       <c r="H221" s="61"/>
@@ -10257,13 +10257,13 @@
         <v>18</v>
       </c>
       <c r="B222" s="168" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="C222" s="169"/>
       <c r="D222" s="170"/>
       <c r="E222" s="170"/>
       <c r="F222" s="192" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
       <c r="G222" s="1"/>
       <c r="H222" s="1"/>
@@ -10327,15 +10327,15 @@
         <v>19</v>
       </c>
       <c r="B224" s="136" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="C224" s="26"/>
       <c r="D224" s="73"/>
       <c r="E224" s="171" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F224" s="171" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="G224" s="26"/>
       <c r="H224" s="26"/>
@@ -10368,10 +10368,10 @@
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
       <c r="E225" s="160" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="F225" s="193" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="G225" s="1"/>
       <c r="H225" s="1"/>
@@ -10405,7 +10405,7 @@
       <c r="D226" s="1"/>
       <c r="E226" s="1"/>
       <c r="F226" s="134" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="G226" s="1"/>
       <c r="H226" s="1"/>
@@ -10437,11 +10437,11 @@
         <v>20</v>
       </c>
       <c r="B227" s="109" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="C227" s="1"/>
       <c r="D227" s="93" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="E227" s="1"/>
       <c r="F227" s="1"/>
@@ -10473,7 +10473,7 @@
     <row r="228" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="27"/>
       <c r="B228" s="172" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
@@ -10507,7 +10507,7 @@
     <row r="229" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="27"/>
       <c r="B229" s="172" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="C229" s="1"/>
       <c r="D229" s="1"/>
@@ -10541,7 +10541,7 @@
     <row r="230" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="27"/>
       <c r="B230" s="108" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="C230" s="1"/>
       <c r="D230" s="1"/>
@@ -10762,14 +10762,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="199" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="B1" s="199"/>
       <c r="C1" s="21" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="D1" s="198" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="E1" s="198"/>
       <c r="F1" s="22"/>
@@ -10777,68 +10777,68 @@
     </row>
     <row r="2" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A2" s="110" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="B2" s="105" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="C2" s="190" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="110" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="C3" s="191" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" s="111" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="C4" s="191" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="111" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="C5" s="191" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="110" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="C6" s="191" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="111" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="C7" s="191" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -10852,15 +10852,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a834da9-6c01-4b0d-9854-214ab0844664">
@@ -10869,6 +10860,15 @@
     <TaxCatchAll xmlns="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11127,26 +11127,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8BE695-F061-495A-A060-7569CE2A6C93}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
+    <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8BE695-F061-495A-A060-7569CE2A6C93}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
-    <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update question4 english translation
</commit_message>
<xml_diff>
--- a/media/questions.xlsx
+++ b/media/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ju5315jo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67999242-C782-47E2-8E8C-139F5F692DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC3428FD-B6FA-49AD-8768-B8EEA3BB924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -310,12 +310,12 @@
     <t>1.5,4-5</t>
   </si>
   <si>
+    <t xml:space="preserve">Pyöräilen ympäri vuoden.//Jag cyklar året runt.// I cycle all year round. </t>
+  </si>
+  <si>
     <t> </t>
   </si>
   <si>
-    <t xml:space="preserve">Pyöräilen ympäri vuoden.//Jag cyklar året runt.// I cycle all year round. </t>
-  </si>
-  <si>
     <t>* Esitä vain jos vastaus pyöräilyn kohdalla "4-5" tai enemmän</t>
   </si>
   <si>
@@ -389,9 +389,6 @@
   </si>
   <si>
     <t>Jalkaisin//Til fots//On Foot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tärkein syy, että käytän kulkumuotoa &lt;&lt;kysymyksen 3 vastaus tähän&gt;&gt;://Den främsta anledningen till att jag använder transportsätt &lt;&lt;svar på fråga 3 här&gt;&gt;://The main reason why &lt;&lt;answer from question 3 here&gt;&gt; I use  is: </t>
   </si>
   <si>
     <t>(valitse yksi)//(välj en)//(choose one)</t>
@@ -850,6 +847,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tiedät päivittäiset kohteesi ja miten niihin pääsee. Et pidä yllätyksistä matkan aikana; elämä on sellaisenaan jo tarpeeksi stressaavaa. Olet valmis kokeilemaan nopeampia tai mukavampia vaihtoehtoja, mutta vain jos saat selkeää tietoa niistä – mieluiten yksityiskohtaisen matkasuunnitelman kera./Du vet dina dagliga resmål och hur du tar dig till dem. Du gillar inte överraskningar under resan; livet är tillräckligt stressigt som det är. Du är villig att prova snabbare eller bekvämare alternativ, men bara om du får tydlig information om dem – gärna med en detaljerad resplan./You know where you're going every day and how to get there. You don't like surprises en route; life is already sufficiently stressful as it is. You are willing to try out faster or more comfortable alternatives. But only if you get clear information about this, preferably with a detailed travel plan. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tärkein syy, että käytän kulkumuotoa &lt;&lt;kysymyksen 3 vastaus tähän&gt;&gt;://Den främsta anledningen till att jag använder transportsätt &lt;&lt;svar på fråga 3 här&gt;&gt;://The main reason why I use &lt;&lt;answer from question 3 here&gt;&gt; is: </t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1753,22 +1753,13 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2108,7 +2099,7 @@
   <dimension ref="A1:AD248"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4655,13 +4646,13 @@
       <c r="A68" s="198" t="s">
         <v>85</v>
       </c>
-      <c r="B68" s="199" t="s">
+      <c r="B68" s="114" t="s">
         <v>86</v>
       </c>
-      <c r="C68" s="200">
-        <v>1</v>
-      </c>
-      <c r="D68" s="201" t="s">
+      <c r="C68" s="53">
+        <v>1</v>
+      </c>
+      <c r="D68" s="92" t="s">
         <v>87</v>
       </c>
       <c r="E68" s="1"/>
@@ -4669,43 +4660,43 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
-      <c r="J68" s="202" t="s">
+      <c r="J68" s="199" t="s">
+        <v>88</v>
+      </c>
+      <c r="K68" s="200" t="s">
         <v>89</v>
       </c>
-      <c r="K68" s="203" t="s">
-        <v>88</v>
-      </c>
-      <c r="L68" s="204" t="s">
-        <v>88</v>
-      </c>
-      <c r="M68" s="204" t="s">
-        <v>88</v>
-      </c>
-      <c r="N68" s="204" t="s">
-        <v>88</v>
-      </c>
-      <c r="O68" s="204" t="s">
-        <v>88</v>
-      </c>
-      <c r="P68" s="205" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q68" s="206" t="s">
-        <v>88</v>
-      </c>
-      <c r="R68" s="207"/>
-      <c r="S68" s="207"/>
-      <c r="T68" s="207"/>
-      <c r="U68" s="207"/>
-      <c r="V68" s="207"/>
-      <c r="W68" s="207"/>
-      <c r="X68" s="207"/>
-      <c r="Y68" s="207"/>
-      <c r="Z68" s="207"/>
-      <c r="AA68" s="207"/>
-      <c r="AB68" s="207"/>
-      <c r="AC68" s="207"/>
-      <c r="AD68" s="207"/>
+      <c r="L68" s="201" t="s">
+        <v>89</v>
+      </c>
+      <c r="M68" s="201" t="s">
+        <v>89</v>
+      </c>
+      <c r="N68" s="201" t="s">
+        <v>89</v>
+      </c>
+      <c r="O68" s="201" t="s">
+        <v>89</v>
+      </c>
+      <c r="P68" s="202" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q68" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R68" s="18"/>
+      <c r="S68" s="18"/>
+      <c r="T68" s="18"/>
+      <c r="U68" s="18"/>
+      <c r="V68" s="18"/>
+      <c r="W68" s="18"/>
+      <c r="X68" s="18"/>
+      <c r="Y68" s="18"/>
+      <c r="Z68" s="18"/>
+      <c r="AA68" s="18"/>
+      <c r="AB68" s="18"/>
+      <c r="AC68" s="18"/>
+      <c r="AD68" s="18"/>
     </row>
     <row r="69" spans="1:30" s="62" customFormat="1" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A69" s="27"/>
@@ -5452,25 +5443,25 @@
         <v>4</v>
       </c>
       <c r="B89" s="114" t="s">
-        <v>115</v>
+        <v>267</v>
       </c>
       <c r="C89" s="49"/>
       <c r="D89" s="51"/>
       <c r="E89" s="124" t="s">
+        <v>115</v>
+      </c>
+      <c r="F89" s="52" t="s">
         <v>116</v>
-      </c>
-      <c r="F89" s="52" t="s">
-        <v>117</v>
       </c>
       <c r="G89" s="162"/>
       <c r="H89" s="112" t="s">
+        <v>117</v>
+      </c>
+      <c r="I89" s="172" t="s">
         <v>118</v>
       </c>
-      <c r="I89" s="172" t="s">
+      <c r="J89" s="112" t="s">
         <v>119</v>
-      </c>
-      <c r="J89" s="112" t="s">
-        <v>120</v>
       </c>
       <c r="K89" s="42">
         <v>1</v>
@@ -5503,7 +5494,7 @@
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
       <c r="J90" s="116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K90" s="43">
         <v>1</v>
@@ -5539,7 +5530,7 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K91" s="43">
         <v>1</v>
@@ -5577,7 +5568,7 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="116" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K92" s="43">
         <v>1</v>
@@ -5615,7 +5606,7 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
       <c r="J93" s="116" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K93" s="43"/>
       <c r="L93" s="2"/>
@@ -5651,7 +5642,7 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="116" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K94" s="43">
         <v>1</v>
@@ -5687,7 +5678,7 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
       <c r="J95" s="116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K95" s="43">
         <v>1</v>
@@ -5725,7 +5716,7 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="116" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K96" s="43">
         <v>1</v>
@@ -5761,7 +5752,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K97" s="43">
         <v>1</v>
@@ -5799,7 +5790,7 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="116" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K98" s="43">
         <v>1</v>
@@ -5835,7 +5826,7 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K99" s="43"/>
       <c r="L99" s="2">
@@ -5871,7 +5862,7 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="116" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K100" s="43">
         <v>1</v>
@@ -5909,7 +5900,7 @@
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
       <c r="J101" s="116" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K101" s="43">
         <v>1</v>
@@ -5947,7 +5938,7 @@
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
       <c r="J102" s="116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K102" s="43">
         <v>1</v>
@@ -6015,17 +6006,17 @@
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G104" s="1"/>
       <c r="H104" s="112" t="s">
+        <v>134</v>
+      </c>
+      <c r="I104" s="173" t="s">
         <v>135</v>
       </c>
-      <c r="I104" s="173" t="s">
-        <v>136</v>
-      </c>
       <c r="J104" s="112" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K104" s="139">
         <v>1</v>
@@ -6059,11 +6050,11 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I105" s="12"/>
       <c r="J105" s="116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K105" s="142">
         <v>1</v>
@@ -6099,7 +6090,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
       <c r="J106" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K106" s="142">
         <v>1</v>
@@ -6135,7 +6126,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
       <c r="J107" s="116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K107" s="142">
         <v>1</v>
@@ -6171,7 +6162,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
       <c r="J108" s="116" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K108" s="142">
         <v>1</v>
@@ -6207,7 +6198,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
       <c r="J109" s="116" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K109" s="142">
         <v>1</v>
@@ -6243,7 +6234,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
       <c r="J110" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K110" s="142"/>
       <c r="L110" s="143">
@@ -6279,7 +6270,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
       <c r="J111" s="116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K111" s="142">
         <v>1</v>
@@ -6317,7 +6308,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
       <c r="J112" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K112" s="142">
         <v>1</v>
@@ -6353,7 +6344,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="12"/>
       <c r="J113" s="116" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K113" s="142">
         <v>1</v>
@@ -6391,7 +6382,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
       <c r="J114" s="116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K114" s="142">
         <v>1</v>
@@ -6459,17 +6450,17 @@
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="129" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G116" s="53"/>
       <c r="H116" s="112" t="s">
+        <v>140</v>
+      </c>
+      <c r="I116" s="173" t="s">
         <v>141</v>
       </c>
-      <c r="I116" s="173" t="s">
-        <v>142</v>
-      </c>
       <c r="J116" s="112" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K116" s="42"/>
       <c r="L116" s="24"/>
@@ -6507,7 +6498,7 @@
       <c r="H117" s="17"/>
       <c r="I117" s="17"/>
       <c r="J117" s="116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K117" s="43"/>
       <c r="L117" s="2"/>
@@ -6547,7 +6538,7 @@
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
       <c r="J118" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K118" s="43"/>
       <c r="L118" s="2"/>
@@ -6587,7 +6578,7 @@
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
       <c r="J119" s="116" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K119" s="43"/>
       <c r="L119" s="2"/>
@@ -6627,7 +6618,7 @@
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
       <c r="J120" s="116" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K120" s="43"/>
       <c r="L120" s="2"/>
@@ -6667,7 +6658,7 @@
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K121" s="43"/>
       <c r="L121" s="2"/>
@@ -6705,7 +6696,7 @@
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
       <c r="J122" s="116" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K122" s="43"/>
       <c r="L122" s="2"/>
@@ -6745,7 +6736,7 @@
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
       <c r="J123" s="116" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K123" s="43"/>
       <c r="L123" s="2">
@@ -6819,7 +6810,7 @@
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
       <c r="J125" s="116" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K125" s="43"/>
       <c r="L125" s="2"/>
@@ -6859,7 +6850,7 @@
       <c r="H126" s="1"/>
       <c r="I126" s="1"/>
       <c r="J126" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K126" s="43"/>
       <c r="L126" s="2">
@@ -6925,17 +6916,17 @@
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="114" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G128" s="52"/>
       <c r="H128" s="112" t="s">
+        <v>146</v>
+      </c>
+      <c r="I128" s="173" t="s">
         <v>147</v>
       </c>
-      <c r="I128" s="173" t="s">
-        <v>148</v>
-      </c>
       <c r="J128" s="112" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K128" s="42"/>
       <c r="L128" s="24"/>
@@ -6973,7 +6964,7 @@
       <c r="H129" s="17"/>
       <c r="I129" s="17"/>
       <c r="J129" s="116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K129" s="43"/>
       <c r="L129" s="2"/>
@@ -7011,7 +7002,7 @@
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
       <c r="J130" s="116" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K130" s="43"/>
       <c r="L130" s="2"/>
@@ -7049,7 +7040,7 @@
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
       <c r="J131" s="116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K131" s="43"/>
       <c r="L131" s="2"/>
@@ -7087,7 +7078,7 @@
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
       <c r="J132" s="116" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K132" s="43"/>
       <c r="L132" s="2"/>
@@ -7123,7 +7114,7 @@
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
       <c r="J133" s="116" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K133" s="43"/>
       <c r="L133" s="2"/>
@@ -7159,7 +7150,7 @@
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
       <c r="J134" s="116" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K134" s="43"/>
       <c r="L134" s="2"/>
@@ -7199,7 +7190,7 @@
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
       <c r="J135" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K135" s="43"/>
       <c r="L135" s="2">
@@ -7235,7 +7226,7 @@
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
       <c r="J136" s="116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K136" s="43"/>
       <c r="L136" s="2"/>
@@ -7303,17 +7294,17 @@
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="129" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G138" s="53"/>
       <c r="H138" s="112" t="s">
+        <v>152</v>
+      </c>
+      <c r="I138" s="173" t="s">
         <v>153</v>
       </c>
-      <c r="I138" s="173" t="s">
-        <v>154</v>
-      </c>
       <c r="J138" s="112" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K138" s="42"/>
       <c r="L138" s="24"/>
@@ -7351,7 +7342,7 @@
       <c r="H139" s="17"/>
       <c r="I139" s="17"/>
       <c r="J139" s="116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K139" s="43"/>
       <c r="L139" s="2"/>
@@ -7391,7 +7382,7 @@
       <c r="H140" s="1"/>
       <c r="I140" s="1"/>
       <c r="J140" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K140" s="43"/>
       <c r="L140" s="2"/>
@@ -7429,7 +7420,7 @@
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
       <c r="J141" s="116" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K141" s="43"/>
       <c r="L141" s="2"/>
@@ -7467,7 +7458,7 @@
       <c r="H142" s="1"/>
       <c r="I142" s="1"/>
       <c r="J142" s="116" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K142" s="43"/>
       <c r="L142" s="2"/>
@@ -7503,7 +7494,7 @@
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
       <c r="J143" s="116" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K143" s="43"/>
       <c r="L143" s="2"/>
@@ -7539,7 +7530,7 @@
       <c r="H144" s="1"/>
       <c r="I144" s="1"/>
       <c r="J144" s="116" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K144" s="43"/>
       <c r="L144" s="2"/>
@@ -7575,7 +7566,7 @@
       <c r="H145" s="1"/>
       <c r="I145" s="1"/>
       <c r="J145" s="116" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K145" s="43"/>
       <c r="L145" s="2"/>
@@ -7611,7 +7602,7 @@
       <c r="H146" s="1"/>
       <c r="I146" s="1"/>
       <c r="J146" s="116" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K146" s="43"/>
       <c r="L146" s="2"/>
@@ -7687,7 +7678,7 @@
       <c r="H148" s="1"/>
       <c r="I148" s="1"/>
       <c r="J148" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K148" s="43"/>
       <c r="L148" s="2">
@@ -7723,7 +7714,7 @@
       <c r="H149" s="1"/>
       <c r="I149" s="1"/>
       <c r="J149" s="116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K149" s="43"/>
       <c r="L149" s="2"/>
@@ -7791,17 +7782,17 @@
       <c r="D151" s="18"/>
       <c r="E151" s="18"/>
       <c r="F151" s="128" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G151" s="49"/>
       <c r="H151" s="112" t="s">
+        <v>159</v>
+      </c>
+      <c r="I151" s="173" t="s">
         <v>160</v>
       </c>
-      <c r="I151" s="173" t="s">
+      <c r="J151" s="112" t="s">
         <v>161</v>
-      </c>
-      <c r="J151" s="112" t="s">
-        <v>162</v>
       </c>
       <c r="K151" s="42"/>
       <c r="L151" s="24"/>
@@ -7835,7 +7826,7 @@
       <c r="H152" s="17"/>
       <c r="I152" s="17"/>
       <c r="J152" s="116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K152" s="43"/>
       <c r="L152" s="2"/>
@@ -7873,7 +7864,7 @@
       <c r="H153" s="1"/>
       <c r="I153" s="1"/>
       <c r="J153" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K153" s="43"/>
       <c r="L153" s="2"/>
@@ -7909,7 +7900,7 @@
       <c r="H154" s="1"/>
       <c r="I154" s="1"/>
       <c r="J154" s="116" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K154" s="43"/>
       <c r="L154" s="2"/>
@@ -7945,7 +7936,7 @@
       <c r="H155" s="1"/>
       <c r="I155" s="1"/>
       <c r="J155" s="116" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K155" s="43"/>
       <c r="L155" s="2"/>
@@ -7981,7 +7972,7 @@
       <c r="H156" s="1"/>
       <c r="I156" s="1"/>
       <c r="J156" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K156" s="43"/>
       <c r="L156" s="2">
@@ -8017,7 +8008,7 @@
       <c r="H157" s="1"/>
       <c r="I157" s="1"/>
       <c r="J157" s="116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K157" s="43"/>
       <c r="L157" s="2"/>
@@ -8089,13 +8080,13 @@
       </c>
       <c r="G159" s="1"/>
       <c r="H159" s="112" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I159" s="173" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J159" s="112" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K159" s="42"/>
       <c r="L159" s="24"/>
@@ -8131,11 +8122,11 @@
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
       <c r="H160" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I160" s="12"/>
       <c r="J160" s="116" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K160" s="43"/>
       <c r="L160" s="2"/>
@@ -8173,7 +8164,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="12"/>
       <c r="J161" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K161" s="43"/>
       <c r="L161" s="2"/>
@@ -8211,7 +8202,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="12"/>
       <c r="J162" s="116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K162" s="43"/>
       <c r="L162" s="2"/>
@@ -8249,7 +8240,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="12"/>
       <c r="J163" s="116" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K163" s="43"/>
       <c r="L163" s="2"/>
@@ -8285,7 +8276,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="12"/>
       <c r="J164" s="116" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K164" s="43"/>
       <c r="L164" s="2"/>
@@ -8321,7 +8312,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="12"/>
       <c r="J165" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K165" s="43"/>
       <c r="L165" s="2"/>
@@ -8361,7 +8352,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="12"/>
       <c r="J166" s="116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K166" s="43"/>
       <c r="L166" s="2">
@@ -8397,7 +8388,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="12"/>
       <c r="J167" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K167" s="43"/>
       <c r="L167" s="2"/>
@@ -8435,7 +8426,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="12"/>
       <c r="J168" s="116" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K168" s="43"/>
       <c r="L168" s="2"/>
@@ -8469,7 +8460,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="12"/>
       <c r="J169" s="116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K169" s="142"/>
       <c r="L169" s="143"/>
@@ -8477,7 +8468,7 @@
       <c r="N169" s="143"/>
       <c r="O169" s="143"/>
       <c r="P169" s="144" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q169" s="3"/>
       <c r="R169" s="1"/>
@@ -8533,23 +8524,23 @@
         <v>5</v>
       </c>
       <c r="B171" s="128" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C171" s="49">
         <v>3</v>
       </c>
       <c r="D171" s="91" t="s">
+        <v>164</v>
+      </c>
+      <c r="E171" s="112" t="s">
         <v>165</v>
-      </c>
-      <c r="E171" s="112" t="s">
-        <v>166</v>
       </c>
       <c r="F171" s="26"/>
       <c r="G171" s="26"/>
       <c r="H171" s="26"/>
       <c r="I171" s="26"/>
       <c r="J171" s="112" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K171" s="42"/>
       <c r="L171" s="24"/>
@@ -8577,7 +8568,7 @@
       <c r="B172" s="13"/>
       <c r="C172" s="13"/>
       <c r="D172" s="93" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E172" s="13"/>
       <c r="F172" s="1"/>
@@ -8585,7 +8576,7 @@
       <c r="H172" s="1"/>
       <c r="I172" s="1"/>
       <c r="J172" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K172" s="43"/>
       <c r="L172" s="2"/>
@@ -8619,7 +8610,7 @@
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
       <c r="J173" s="116" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K173" s="43"/>
       <c r="L173" s="2"/>
@@ -8653,7 +8644,7 @@
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
       <c r="J174" s="34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K174" s="43"/>
       <c r="L174" s="2"/>
@@ -8687,7 +8678,7 @@
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
       <c r="J175" s="116" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K175" s="43"/>
       <c r="L175" s="2"/>
@@ -8721,7 +8712,7 @@
       <c r="H176" s="1"/>
       <c r="I176" s="1"/>
       <c r="J176" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K176" s="43"/>
       <c r="L176" s="2"/>
@@ -8755,7 +8746,7 @@
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
       <c r="J177" s="116" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K177" s="43"/>
       <c r="L177" s="2"/>
@@ -8789,7 +8780,7 @@
       <c r="H178" s="1"/>
       <c r="I178" s="1"/>
       <c r="J178" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K178" s="43"/>
       <c r="L178" s="2"/>
@@ -8823,7 +8814,7 @@
       <c r="H179" s="1"/>
       <c r="I179" s="1"/>
       <c r="J179" s="116" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K179" s="43"/>
       <c r="L179" s="2"/>
@@ -8857,7 +8848,7 @@
       <c r="H180" s="1"/>
       <c r="I180" s="1"/>
       <c r="J180" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K180" s="43"/>
       <c r="L180" s="2"/>
@@ -8891,7 +8882,7 @@
       <c r="H181" s="1"/>
       <c r="I181" s="1"/>
       <c r="J181" s="116" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K181" s="43"/>
       <c r="L181" s="2"/>
@@ -8925,7 +8916,7 @@
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
       <c r="J182" s="116" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K182" s="43"/>
       <c r="L182" s="2"/>
@@ -8959,7 +8950,7 @@
       <c r="H183" s="1"/>
       <c r="I183" s="1"/>
       <c r="J183" s="116" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K183" s="43"/>
       <c r="L183" s="2"/>
@@ -8993,7 +8984,7 @@
       <c r="H184" s="1"/>
       <c r="I184" s="1"/>
       <c r="J184" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K184" s="43"/>
       <c r="L184" s="2"/>
@@ -9027,7 +9018,7 @@
       <c r="H185" s="1"/>
       <c r="I185" s="1"/>
       <c r="J185" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K185" s="43"/>
       <c r="L185" s="2"/>
@@ -9061,7 +9052,7 @@
       <c r="H186" s="1"/>
       <c r="I186" s="1"/>
       <c r="J186" s="116" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K186" s="43"/>
       <c r="L186" s="2"/>
@@ -9095,7 +9086,7 @@
       <c r="H187" s="1"/>
       <c r="I187" s="1"/>
       <c r="J187" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K187" s="43"/>
       <c r="L187" s="2"/>
@@ -9129,7 +9120,7 @@
       <c r="H188" s="1"/>
       <c r="I188" s="1"/>
       <c r="J188" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K188" s="43"/>
       <c r="L188" s="2"/>
@@ -9163,7 +9154,7 @@
       <c r="H189" s="1"/>
       <c r="I189" s="1"/>
       <c r="J189" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="K189" s="43"/>
       <c r="L189" s="2"/>
@@ -9197,7 +9188,7 @@
       <c r="H190" s="1"/>
       <c r="I190" s="1"/>
       <c r="J190" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K190" s="43"/>
       <c r="L190" s="2"/>
@@ -9259,21 +9250,21 @@
         <v>6</v>
       </c>
       <c r="B192" s="122" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C192" s="50">
         <v>1</v>
       </c>
       <c r="D192" s="50"/>
       <c r="E192" s="124" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F192" s="62"/>
       <c r="G192" s="35"/>
       <c r="H192" s="35"/>
       <c r="I192" s="35"/>
       <c r="J192" s="120" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K192" s="43"/>
       <c r="L192" s="36"/>
@@ -9305,7 +9296,7 @@
       <c r="H193" s="35"/>
       <c r="I193" s="35"/>
       <c r="J193" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K193" s="43"/>
       <c r="L193" s="36"/>
@@ -9338,7 +9329,7 @@
       <c r="H194" s="13"/>
       <c r="I194" s="13"/>
       <c r="J194" s="116" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K194" s="43"/>
       <c r="L194" s="2"/>
@@ -9371,7 +9362,7 @@
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
       <c r="J195" s="116" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K195" s="43"/>
       <c r="L195" s="2"/>
@@ -9404,7 +9395,7 @@
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
       <c r="J196" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K196" s="43"/>
       <c r="L196" s="2"/>
@@ -9437,7 +9428,7 @@
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
       <c r="J197" s="116" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K197" s="43"/>
       <c r="L197" s="2"/>
@@ -9471,7 +9462,7 @@
       <c r="H198" s="70"/>
       <c r="I198" s="70"/>
       <c r="J198" s="118" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K198" s="65"/>
       <c r="L198" s="66"/>
@@ -9499,7 +9490,7 @@
         <v>7</v>
       </c>
       <c r="B199" s="122" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C199" s="50"/>
       <c r="D199" s="50"/>
@@ -9509,7 +9500,7 @@
       <c r="H199" s="35"/>
       <c r="I199" s="35"/>
       <c r="J199" s="35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K199" s="43"/>
       <c r="L199" s="36"/>
@@ -9542,7 +9533,7 @@
       <c r="H200" s="13"/>
       <c r="I200" s="13"/>
       <c r="J200" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K200" s="43"/>
       <c r="L200" s="2"/>
@@ -9576,7 +9567,7 @@
       <c r="H201" s="70"/>
       <c r="I201" s="70"/>
       <c r="J201" s="118" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K201" s="65"/>
       <c r="L201" s="66"/>
@@ -9604,7 +9595,7 @@
         <v>8</v>
       </c>
       <c r="B202" s="115" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C202" s="62"/>
       <c r="D202" s="161">
@@ -9616,7 +9607,7 @@
       <c r="H202" s="35"/>
       <c r="I202" s="35"/>
       <c r="J202" s="120" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K202" s="43"/>
       <c r="L202" s="36"/>
@@ -9644,14 +9635,14 @@
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="93" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E203" s="1"/>
       <c r="G203" s="13"/>
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
       <c r="J203" s="116" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K203" s="43"/>
       <c r="L203" s="2"/>
@@ -9684,7 +9675,7 @@
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
       <c r="J204" s="116" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K204" s="43"/>
       <c r="L204" s="2"/>
@@ -9717,7 +9708,7 @@
       <c r="H205" s="13"/>
       <c r="I205" s="13"/>
       <c r="J205" s="116" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K205" s="43"/>
       <c r="L205" s="2"/>
@@ -9775,13 +9766,13 @@
     </row>
     <row r="207" spans="1:30" s="16" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="29"/>
-      <c r="B207" s="208" t="s">
-        <v>203</v>
-      </c>
-      <c r="C207" s="209"/>
-      <c r="D207" s="209"/>
-      <c r="E207" s="209"/>
-      <c r="F207" s="209"/>
+      <c r="B207" s="203" t="s">
+        <v>202</v>
+      </c>
+      <c r="C207" s="204"/>
+      <c r="D207" s="204"/>
+      <c r="E207" s="204"/>
+      <c r="F207" s="204"/>
       <c r="G207" s="103"/>
       <c r="H207" s="103"/>
       <c r="I207" s="103"/>
@@ -9810,7 +9801,7 @@
     <row r="208" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="27"/>
       <c r="B208" s="130" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C208" s="78"/>
       <c r="D208" s="78"/>
@@ -9878,7 +9869,7 @@
         <v>9</v>
       </c>
       <c r="B210" s="114" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C210" s="52"/>
       <c r="D210" s="52"/>
@@ -9920,7 +9911,7 @@
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E211" s="1"/>
       <c r="F211" s="116"/>
@@ -9966,7 +9957,7 @@
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
       <c r="J212" s="116" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K212" s="43"/>
       <c r="L212" s="2"/>
@@ -10004,7 +9995,7 @@
       <c r="H213" s="13"/>
       <c r="I213" s="13"/>
       <c r="J213" s="116" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K213" s="43"/>
       <c r="L213" s="2"/>
@@ -10040,7 +10031,7 @@
       <c r="H214" s="19"/>
       <c r="I214" s="19"/>
       <c r="J214" s="131" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K214" s="43"/>
       <c r="L214" s="2"/>
@@ -10074,7 +10065,7 @@
       <c r="H215" s="19"/>
       <c r="I215" s="19"/>
       <c r="J215" s="72" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K215" s="43"/>
       <c r="L215" s="2"/>
@@ -10102,7 +10093,7 @@
         <v>10</v>
       </c>
       <c r="B216" s="52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C216" s="57"/>
       <c r="D216" s="57"/>
@@ -10112,7 +10103,7 @@
       <c r="H216" s="31"/>
       <c r="I216" s="31"/>
       <c r="J216" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K216" s="42"/>
       <c r="L216" s="24"/>
@@ -10150,7 +10141,7 @@
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
       <c r="J217" s="116" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K217" s="43">
         <v>1</v>
@@ -10192,7 +10183,7 @@
       <c r="H218" s="13"/>
       <c r="I218" s="13"/>
       <c r="J218" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K218" s="43"/>
       <c r="L218" s="2">
@@ -10219,13 +10210,13 @@
     </row>
     <row r="219" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A219" s="29"/>
-      <c r="B219" s="210" t="s">
-        <v>215</v>
-      </c>
-      <c r="C219" s="211"/>
-      <c r="D219" s="211"/>
-      <c r="E219" s="211"/>
-      <c r="F219" s="211"/>
+      <c r="B219" s="205" t="s">
+        <v>214</v>
+      </c>
+      <c r="C219" s="206"/>
+      <c r="D219" s="206"/>
+      <c r="E219" s="206"/>
+      <c r="F219" s="206"/>
       <c r="G219" s="103"/>
       <c r="H219" s="103"/>
       <c r="I219" s="103"/>
@@ -10256,7 +10247,7 @@
         <v>12</v>
       </c>
       <c r="B220" s="132" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C220" s="55"/>
       <c r="D220" s="55"/>
@@ -10266,7 +10257,7 @@
       <c r="H220" s="34"/>
       <c r="I220" s="34"/>
       <c r="J220" s="39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K220" s="43"/>
       <c r="L220" s="2"/>
@@ -10300,7 +10291,7 @@
       <c r="H221" s="34"/>
       <c r="I221" s="34"/>
       <c r="J221" s="40" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K221" s="43"/>
       <c r="L221" s="2"/>
@@ -10334,7 +10325,7 @@
       <c r="H222" s="18"/>
       <c r="I222" s="18"/>
       <c r="J222" s="104" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K222" s="43"/>
       <c r="L222" s="2"/>
@@ -10362,13 +10353,13 @@
         <v>13</v>
       </c>
       <c r="B223" s="132" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C223" s="55"/>
       <c r="D223" s="55"/>
       <c r="E223" s="55"/>
       <c r="F223" s="41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G223" s="59"/>
       <c r="H223" s="59"/>
@@ -10400,13 +10391,13 @@
         <v>14</v>
       </c>
       <c r="B224" s="134" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C224" s="56"/>
       <c r="D224" s="56"/>
       <c r="E224" s="56"/>
       <c r="F224" s="138" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G224" s="18"/>
       <c r="H224" s="18"/>
@@ -10438,7 +10429,7 @@
         <v>15</v>
       </c>
       <c r="B225" s="134" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C225" s="56"/>
       <c r="D225" s="56"/>
@@ -10474,7 +10465,7 @@
         <v>16</v>
       </c>
       <c r="B226" s="134" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C226" s="56"/>
       <c r="D226" s="56"/>
@@ -10484,7 +10475,7 @@
       <c r="H226" s="35"/>
       <c r="I226" s="35"/>
       <c r="J226" s="136" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K226" s="43"/>
       <c r="L226" s="2"/>
@@ -10518,7 +10509,7 @@
       <c r="H227" s="35"/>
       <c r="I227" s="35"/>
       <c r="J227" s="137" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K227" s="43"/>
       <c r="L227" s="2"/>
@@ -10552,7 +10543,7 @@
       <c r="H228" s="35"/>
       <c r="I228" s="35"/>
       <c r="J228" s="137" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K228" s="43"/>
       <c r="L228" s="2"/>
@@ -10586,7 +10577,7 @@
       <c r="H229" s="35"/>
       <c r="I229" s="35"/>
       <c r="J229" s="137" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K229" s="43"/>
       <c r="L229" s="2"/>
@@ -10620,7 +10611,7 @@
       <c r="H230" s="35"/>
       <c r="I230" s="35"/>
       <c r="J230" s="137" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K230" s="43"/>
       <c r="L230" s="2"/>
@@ -10730,15 +10721,15 @@
         <v>17</v>
       </c>
       <c r="B233" s="135" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C233" s="26"/>
       <c r="D233" s="26"/>
       <c r="E233" s="97" t="s">
+        <v>231</v>
+      </c>
+      <c r="F233" s="126" t="s">
         <v>232</v>
-      </c>
-      <c r="F233" s="126" t="s">
-        <v>233</v>
       </c>
       <c r="G233" s="26"/>
       <c r="H233" s="26"/>
@@ -10772,7 +10763,7 @@
       <c r="D234" s="61"/>
       <c r="E234" s="61"/>
       <c r="F234" s="107" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G234" s="61"/>
       <c r="I234" s="18"/>
@@ -10803,13 +10794,13 @@
         <v>18</v>
       </c>
       <c r="B235" s="167" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C235" s="168"/>
       <c r="D235" s="169"/>
       <c r="E235" s="169"/>
       <c r="F235" s="191" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G235" s="1"/>
       <c r="H235" s="1"/>
@@ -10873,15 +10864,15 @@
         <v>19</v>
       </c>
       <c r="B237" s="135" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C237" s="26"/>
       <c r="D237" s="73"/>
       <c r="E237" s="193" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F237" s="170" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G237" s="26"/>
       <c r="H237" s="26"/>
@@ -10914,10 +10905,10 @@
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
       <c r="E238" s="159" t="s">
+        <v>238</v>
+      </c>
+      <c r="F238" s="192" t="s">
         <v>239</v>
-      </c>
-      <c r="F238" s="192" t="s">
-        <v>240</v>
       </c>
       <c r="G238" s="1"/>
       <c r="H238" s="1"/>
@@ -10951,7 +10942,7 @@
       <c r="D239" s="1"/>
       <c r="E239" s="1"/>
       <c r="F239" s="133" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G239" s="1"/>
       <c r="H239" s="1"/>
@@ -10983,11 +10974,11 @@
         <v>20</v>
       </c>
       <c r="B240" s="109" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C240" s="1"/>
       <c r="D240" s="93" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E240" s="1"/>
       <c r="F240" s="1"/>
@@ -11019,7 +11010,7 @@
     <row r="241" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="27"/>
       <c r="B241" s="171" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
@@ -11053,7 +11044,7 @@
     <row r="242" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="27"/>
       <c r="B242" s="171" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C242" s="1"/>
       <c r="D242" s="1"/>
@@ -11087,7 +11078,7 @@
     <row r="243" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="27"/>
       <c r="B243" s="108" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C243" s="1"/>
       <c r="D243" s="1"/>
@@ -11307,84 +11298,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="208" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" s="208"/>
+      <c r="C1" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="B1" s="213"/>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="207" t="s">
         <v>248</v>
       </c>
-      <c r="D1" s="212" t="s">
-        <v>249</v>
-      </c>
-      <c r="E1" s="212"/>
+      <c r="E1" s="207"/>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A2" s="110" t="s">
+        <v>249</v>
+      </c>
+      <c r="B2" s="105" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="105" t="s">
+      <c r="C2" s="189" t="s">
         <v>251</v>
-      </c>
-      <c r="C2" s="189" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="110" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="105" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="C3" s="190" t="s">
         <v>254</v>
-      </c>
-      <c r="C3" s="190" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" s="111" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="105" t="s">
         <v>256</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="C4" s="190" t="s">
         <v>257</v>
-      </c>
-      <c r="C4" s="190" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="111" t="s">
+        <v>258</v>
+      </c>
+      <c r="B5" s="106" t="s">
         <v>259</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="C5" s="190" t="s">
         <v>260</v>
-      </c>
-      <c r="C5" s="190" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="110" t="s">
+        <v>261</v>
+      </c>
+      <c r="B6" s="105" t="s">
         <v>262</v>
       </c>
-      <c r="B6" s="105" t="s">
+      <c r="C6" s="190" t="s">
         <v>263</v>
-      </c>
-      <c r="C6" s="190" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="111" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="105" t="s">
         <v>265</v>
       </c>
-      <c r="B7" s="105" t="s">
+      <c r="C7" s="190" t="s">
         <v>266</v>
-      </c>
-      <c r="C7" s="190" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -11409,15 +11400,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA421E502B73EC48B7C481B02707A95D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8e395bb2bcb17e943266a860489f057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a834da9-6c01-4b0d-9854-214ab0844664" xmlns:ns3="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b1084d163ef6a9ae7f6b3d13802deaa" ns2:_="" ns3:_="">
     <xsd:import namespace="1a834da9-6c01-4b0d-9854-214ab0844664"/>
@@ -11672,32 +11654,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8BE695-F061-495A-A060-7569CE2A6C93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81CDBFC0-0126-4DB7-8868-40859C987D1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11714,4 +11697,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8BE695-F061-495A-A060-7569CE2A6C93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix invalid sub question condition in question 4
</commit_message>
<xml_diff>
--- a/media/questions.xlsx
+++ b/media/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ju5315jo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC3428FD-B6FA-49AD-8768-B8EEA3BB924F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4307D21B-B190-455E-B0E2-18829D6B479B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="269">
   <si>
     <t>#</t>
   </si>
@@ -391,6 +391,9 @@
     <t>Jalkaisin//Til fots//On Foot</t>
   </si>
   <si>
+    <t xml:space="preserve">Tärkein syy, että käytän kulkumuotoa &lt;&lt;kysymyksen 3 vastaus tähän&gt;&gt;://Den främsta anledningen till att jag använder transportsätt &lt;&lt;svar på fråga 3 här&gt;&gt;://The main reason why I use &lt;&lt;answer from question 3 here&gt;&gt; is: </t>
+  </si>
+  <si>
     <t>(valitse yksi)//(välj en)//(choose one)</t>
   </si>
   <si>
@@ -849,7 +852,7 @@
     <t xml:space="preserve">Tiedät päivittäiset kohteesi ja miten niihin pääsee. Et pidä yllätyksistä matkan aikana; elämä on sellaisenaan jo tarpeeksi stressaavaa. Olet valmis kokeilemaan nopeampia tai mukavampia vaihtoehtoja, mutta vain jos saat selkeää tietoa niistä – mieluiten yksityiskohtaisen matkasuunnitelman kera./Du vet dina dagliga resmål och hur du tar dig till dem. Du gillar inte överraskningar under resan; livet är tillräckligt stressigt som det är. Du är villig att prova snabbare eller bekvämare alternativ, men bara om du får tydlig information om dem – gärna med en detaljerad resplan./You know where you're going every day and how to get there. You don't like surprises en route; life is already sufficiently stressful as it is. You are willing to try out faster or more comfortable alternatives. But only if you get clear information about this, preferably with a detailed travel plan. </t>
   </si>
   <si>
-    <t xml:space="preserve">Tärkein syy, että käytän kulkumuotoa &lt;&lt;kysymyksen 3 vastaus tähän&gt;&gt;://Den främsta anledningen till att jag använder transportsätt &lt;&lt;svar på fråga 3 här&gt;&gt;://The main reason why I use &lt;&lt;answer from question 3 here&gt;&gt; is: </t>
+    <t>3.6</t>
   </si>
 </sst>
 </file>
@@ -2098,8 +2101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF3ACC6-6455-42D3-BCE3-944B33DD47DC}">
   <dimension ref="A1:AD248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5443,25 +5446,25 @@
         <v>4</v>
       </c>
       <c r="B89" s="114" t="s">
-        <v>267</v>
+        <v>115</v>
       </c>
       <c r="C89" s="49"/>
       <c r="D89" s="51"/>
       <c r="E89" s="124" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F89" s="52" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G89" s="162"/>
       <c r="H89" s="112" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I89" s="172" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J89" s="112" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K89" s="42">
         <v>1</v>
@@ -5494,7 +5497,7 @@
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
       <c r="J90" s="116" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K90" s="43">
         <v>1</v>
@@ -5530,7 +5533,7 @@
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="116" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K91" s="43">
         <v>1</v>
@@ -5568,7 +5571,7 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="116" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K92" s="43">
         <v>1</v>
@@ -5606,7 +5609,7 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
       <c r="J93" s="116" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K93" s="43"/>
       <c r="L93" s="2"/>
@@ -5642,7 +5645,7 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="116" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K94" s="43">
         <v>1</v>
@@ -5678,7 +5681,7 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
       <c r="J95" s="116" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K95" s="43">
         <v>1</v>
@@ -5716,7 +5719,7 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="116" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K96" s="43">
         <v>1</v>
@@ -5752,7 +5755,7 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="116" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K97" s="43">
         <v>1</v>
@@ -5790,7 +5793,7 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="116" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K98" s="43">
         <v>1</v>
@@ -5826,7 +5829,7 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="116" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K99" s="43"/>
       <c r="L99" s="2">
@@ -5862,7 +5865,7 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="116" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K100" s="43">
         <v>1</v>
@@ -5900,7 +5903,7 @@
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
       <c r="J101" s="116" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K101" s="43">
         <v>1</v>
@@ -5938,7 +5941,7 @@
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
       <c r="J102" s="116" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K102" s="43">
         <v>1</v>
@@ -6006,17 +6009,17 @@
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="52" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G104" s="1"/>
       <c r="H104" s="112" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I104" s="173" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J104" s="112" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K104" s="139">
         <v>1</v>
@@ -6050,11 +6053,11 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I105" s="12"/>
       <c r="J105" s="116" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K105" s="142">
         <v>1</v>
@@ -6090,7 +6093,7 @@
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
       <c r="J106" s="116" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K106" s="142">
         <v>1</v>
@@ -6126,7 +6129,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
       <c r="J107" s="116" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K107" s="142">
         <v>1</v>
@@ -6162,7 +6165,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
       <c r="J108" s="116" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K108" s="142">
         <v>1</v>
@@ -6198,7 +6201,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
       <c r="J109" s="116" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K109" s="142">
         <v>1</v>
@@ -6234,7 +6237,7 @@
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
       <c r="J110" s="116" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K110" s="142"/>
       <c r="L110" s="143">
@@ -6270,7 +6273,7 @@
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
       <c r="J111" s="116" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K111" s="142">
         <v>1</v>
@@ -6308,7 +6311,7 @@
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
       <c r="J112" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K112" s="142">
         <v>1</v>
@@ -6344,7 +6347,7 @@
       <c r="H113" s="12"/>
       <c r="I113" s="12"/>
       <c r="J113" s="116" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K113" s="142">
         <v>1</v>
@@ -6382,7 +6385,7 @@
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
       <c r="J114" s="116" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K114" s="142">
         <v>1</v>
@@ -6450,17 +6453,17 @@
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="129" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G116" s="53"/>
       <c r="H116" s="112" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I116" s="173" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J116" s="112" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K116" s="42"/>
       <c r="L116" s="24"/>
@@ -6498,7 +6501,7 @@
       <c r="H117" s="17"/>
       <c r="I117" s="17"/>
       <c r="J117" s="116" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K117" s="43"/>
       <c r="L117" s="2"/>
@@ -6538,7 +6541,7 @@
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
       <c r="J118" s="116" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K118" s="43"/>
       <c r="L118" s="2"/>
@@ -6578,7 +6581,7 @@
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
       <c r="J119" s="116" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K119" s="43"/>
       <c r="L119" s="2"/>
@@ -6618,7 +6621,7 @@
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
       <c r="J120" s="116" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K120" s="43"/>
       <c r="L120" s="2"/>
@@ -6658,7 +6661,7 @@
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="116" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K121" s="43"/>
       <c r="L121" s="2"/>
@@ -6696,7 +6699,7 @@
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
       <c r="J122" s="116" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K122" s="43"/>
       <c r="L122" s="2"/>
@@ -6736,7 +6739,7 @@
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
       <c r="J123" s="116" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K123" s="43"/>
       <c r="L123" s="2">
@@ -6810,7 +6813,7 @@
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
       <c r="J125" s="116" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K125" s="43"/>
       <c r="L125" s="2"/>
@@ -6850,7 +6853,7 @@
       <c r="H126" s="1"/>
       <c r="I126" s="1"/>
       <c r="J126" s="116" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K126" s="43"/>
       <c r="L126" s="2">
@@ -6916,17 +6919,17 @@
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="114" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G128" s="52"/>
       <c r="H128" s="112" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I128" s="173" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J128" s="112" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K128" s="42"/>
       <c r="L128" s="24"/>
@@ -6964,7 +6967,7 @@
       <c r="H129" s="17"/>
       <c r="I129" s="17"/>
       <c r="J129" s="116" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K129" s="43"/>
       <c r="L129" s="2"/>
@@ -7002,7 +7005,7 @@
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
       <c r="J130" s="116" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K130" s="43"/>
       <c r="L130" s="2"/>
@@ -7040,7 +7043,7 @@
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
       <c r="J131" s="116" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K131" s="43"/>
       <c r="L131" s="2"/>
@@ -7078,7 +7081,7 @@
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
       <c r="J132" s="116" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K132" s="43"/>
       <c r="L132" s="2"/>
@@ -7114,7 +7117,7 @@
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
       <c r="J133" s="116" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K133" s="43"/>
       <c r="L133" s="2"/>
@@ -7150,7 +7153,7 @@
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
       <c r="J134" s="116" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K134" s="43"/>
       <c r="L134" s="2"/>
@@ -7190,7 +7193,7 @@
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
       <c r="J135" s="116" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K135" s="43"/>
       <c r="L135" s="2">
@@ -7226,7 +7229,7 @@
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
       <c r="J136" s="116" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K136" s="43"/>
       <c r="L136" s="2"/>
@@ -7294,17 +7297,17 @@
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="129" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G138" s="53"/>
       <c r="H138" s="112" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I138" s="173" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J138" s="112" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K138" s="42"/>
       <c r="L138" s="24"/>
@@ -7342,7 +7345,7 @@
       <c r="H139" s="17"/>
       <c r="I139" s="17"/>
       <c r="J139" s="116" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K139" s="43"/>
       <c r="L139" s="2"/>
@@ -7382,7 +7385,7 @@
       <c r="H140" s="1"/>
       <c r="I140" s="1"/>
       <c r="J140" s="116" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K140" s="43"/>
       <c r="L140" s="2"/>
@@ -7420,7 +7423,7 @@
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
       <c r="J141" s="116" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K141" s="43"/>
       <c r="L141" s="2"/>
@@ -7458,7 +7461,7 @@
       <c r="H142" s="1"/>
       <c r="I142" s="1"/>
       <c r="J142" s="116" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K142" s="43"/>
       <c r="L142" s="2"/>
@@ -7494,7 +7497,7 @@
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
       <c r="J143" s="116" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K143" s="43"/>
       <c r="L143" s="2"/>
@@ -7530,7 +7533,7 @@
       <c r="H144" s="1"/>
       <c r="I144" s="1"/>
       <c r="J144" s="116" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K144" s="43"/>
       <c r="L144" s="2"/>
@@ -7566,7 +7569,7 @@
       <c r="H145" s="1"/>
       <c r="I145" s="1"/>
       <c r="J145" s="116" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K145" s="43"/>
       <c r="L145" s="2"/>
@@ -7602,7 +7605,7 @@
       <c r="H146" s="1"/>
       <c r="I146" s="1"/>
       <c r="J146" s="116" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K146" s="43"/>
       <c r="L146" s="2"/>
@@ -7678,7 +7681,7 @@
       <c r="H148" s="1"/>
       <c r="I148" s="1"/>
       <c r="J148" s="116" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K148" s="43"/>
       <c r="L148" s="2">
@@ -7714,7 +7717,7 @@
       <c r="H149" s="1"/>
       <c r="I149" s="1"/>
       <c r="J149" s="116" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K149" s="43"/>
       <c r="L149" s="2"/>
@@ -7782,17 +7785,17 @@
       <c r="D151" s="18"/>
       <c r="E151" s="18"/>
       <c r="F151" s="128" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G151" s="49"/>
       <c r="H151" s="112" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I151" s="173" t="s">
-        <v>160</v>
+        <v>268</v>
       </c>
       <c r="J151" s="112" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K151" s="42"/>
       <c r="L151" s="24"/>
@@ -7826,7 +7829,7 @@
       <c r="H152" s="17"/>
       <c r="I152" s="17"/>
       <c r="J152" s="116" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K152" s="43"/>
       <c r="L152" s="2"/>
@@ -7864,7 +7867,7 @@
       <c r="H153" s="1"/>
       <c r="I153" s="1"/>
       <c r="J153" s="116" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K153" s="43"/>
       <c r="L153" s="2"/>
@@ -7900,7 +7903,7 @@
       <c r="H154" s="1"/>
       <c r="I154" s="1"/>
       <c r="J154" s="116" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K154" s="43"/>
       <c r="L154" s="2"/>
@@ -7936,7 +7939,7 @@
       <c r="H155" s="1"/>
       <c r="I155" s="1"/>
       <c r="J155" s="116" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K155" s="43"/>
       <c r="L155" s="2"/>
@@ -7972,7 +7975,7 @@
       <c r="H156" s="1"/>
       <c r="I156" s="1"/>
       <c r="J156" s="116" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K156" s="43"/>
       <c r="L156" s="2">
@@ -8008,7 +8011,7 @@
       <c r="H157" s="1"/>
       <c r="I157" s="1"/>
       <c r="J157" s="116" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K157" s="43"/>
       <c r="L157" s="2"/>
@@ -8080,13 +8083,13 @@
       </c>
       <c r="G159" s="1"/>
       <c r="H159" s="112" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I159" s="173" t="s">
-        <v>135</v>
+        <v>161</v>
       </c>
       <c r="J159" s="112" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="K159" s="42"/>
       <c r="L159" s="24"/>
@@ -8122,11 +8125,11 @@
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
       <c r="H160" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I160" s="12"/>
       <c r="J160" s="116" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K160" s="43"/>
       <c r="L160" s="2"/>
@@ -8164,7 +8167,7 @@
       <c r="H161" s="12"/>
       <c r="I161" s="12"/>
       <c r="J161" s="116" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K161" s="43"/>
       <c r="L161" s="2"/>
@@ -8202,7 +8205,7 @@
       <c r="H162" s="12"/>
       <c r="I162" s="12"/>
       <c r="J162" s="116" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K162" s="43"/>
       <c r="L162" s="2"/>
@@ -8240,7 +8243,7 @@
       <c r="H163" s="12"/>
       <c r="I163" s="12"/>
       <c r="J163" s="116" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K163" s="43"/>
       <c r="L163" s="2"/>
@@ -8276,7 +8279,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="12"/>
       <c r="J164" s="116" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K164" s="43"/>
       <c r="L164" s="2"/>
@@ -8312,7 +8315,7 @@
       <c r="H165" s="12"/>
       <c r="I165" s="12"/>
       <c r="J165" s="116" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K165" s="43"/>
       <c r="L165" s="2"/>
@@ -8352,7 +8355,7 @@
       <c r="H166" s="12"/>
       <c r="I166" s="12"/>
       <c r="J166" s="116" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K166" s="43"/>
       <c r="L166" s="2">
@@ -8388,7 +8391,7 @@
       <c r="H167" s="12"/>
       <c r="I167" s="12"/>
       <c r="J167" s="13" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K167" s="43"/>
       <c r="L167" s="2"/>
@@ -8426,7 +8429,7 @@
       <c r="H168" s="12"/>
       <c r="I168" s="12"/>
       <c r="J168" s="116" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K168" s="43"/>
       <c r="L168" s="2"/>
@@ -8460,7 +8463,7 @@
       <c r="H169" s="12"/>
       <c r="I169" s="12"/>
       <c r="J169" s="116" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K169" s="142"/>
       <c r="L169" s="143"/>
@@ -8468,7 +8471,7 @@
       <c r="N169" s="143"/>
       <c r="O169" s="143"/>
       <c r="P169" s="144" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q169" s="3"/>
       <c r="R169" s="1"/>
@@ -8524,23 +8527,23 @@
         <v>5</v>
       </c>
       <c r="B171" s="128" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C171" s="49">
         <v>3</v>
       </c>
       <c r="D171" s="91" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E171" s="112" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F171" s="26"/>
       <c r="G171" s="26"/>
       <c r="H171" s="26"/>
       <c r="I171" s="26"/>
       <c r="J171" s="112" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K171" s="42"/>
       <c r="L171" s="24"/>
@@ -8568,7 +8571,7 @@
       <c r="B172" s="13"/>
       <c r="C172" s="13"/>
       <c r="D172" s="93" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E172" s="13"/>
       <c r="F172" s="1"/>
@@ -8576,7 +8579,7 @@
       <c r="H172" s="1"/>
       <c r="I172" s="1"/>
       <c r="J172" s="34" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K172" s="43"/>
       <c r="L172" s="2"/>
@@ -8610,7 +8613,7 @@
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
       <c r="J173" s="116" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K173" s="43"/>
       <c r="L173" s="2"/>
@@ -8644,7 +8647,7 @@
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
       <c r="J174" s="34" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K174" s="43"/>
       <c r="L174" s="2"/>
@@ -8678,7 +8681,7 @@
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
       <c r="J175" s="116" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K175" s="43"/>
       <c r="L175" s="2"/>
@@ -8712,7 +8715,7 @@
       <c r="H176" s="1"/>
       <c r="I176" s="1"/>
       <c r="J176" s="34" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K176" s="43"/>
       <c r="L176" s="2"/>
@@ -8746,7 +8749,7 @@
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
       <c r="J177" s="116" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K177" s="43"/>
       <c r="L177" s="2"/>
@@ -8780,7 +8783,7 @@
       <c r="H178" s="1"/>
       <c r="I178" s="1"/>
       <c r="J178" s="34" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K178" s="43"/>
       <c r="L178" s="2"/>
@@ -8814,7 +8817,7 @@
       <c r="H179" s="1"/>
       <c r="I179" s="1"/>
       <c r="J179" s="116" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K179" s="43"/>
       <c r="L179" s="2"/>
@@ -8848,7 +8851,7 @@
       <c r="H180" s="1"/>
       <c r="I180" s="1"/>
       <c r="J180" s="34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K180" s="43"/>
       <c r="L180" s="2"/>
@@ -8882,7 +8885,7 @@
       <c r="H181" s="1"/>
       <c r="I181" s="1"/>
       <c r="J181" s="116" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K181" s="43"/>
       <c r="L181" s="2"/>
@@ -8916,7 +8919,7 @@
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
       <c r="J182" s="116" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="K182" s="43"/>
       <c r="L182" s="2"/>
@@ -8950,7 +8953,7 @@
       <c r="H183" s="1"/>
       <c r="I183" s="1"/>
       <c r="J183" s="116" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K183" s="43"/>
       <c r="L183" s="2"/>
@@ -8984,7 +8987,7 @@
       <c r="H184" s="1"/>
       <c r="I184" s="1"/>
       <c r="J184" s="34" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K184" s="43"/>
       <c r="L184" s="2"/>
@@ -9018,7 +9021,7 @@
       <c r="H185" s="1"/>
       <c r="I185" s="1"/>
       <c r="J185" s="34" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K185" s="43"/>
       <c r="L185" s="2"/>
@@ -9052,7 +9055,7 @@
       <c r="H186" s="1"/>
       <c r="I186" s="1"/>
       <c r="J186" s="116" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K186" s="43"/>
       <c r="L186" s="2"/>
@@ -9086,7 +9089,7 @@
       <c r="H187" s="1"/>
       <c r="I187" s="1"/>
       <c r="J187" s="34" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K187" s="43"/>
       <c r="L187" s="2"/>
@@ -9120,7 +9123,7 @@
       <c r="H188" s="1"/>
       <c r="I188" s="1"/>
       <c r="J188" s="34" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K188" s="43"/>
       <c r="L188" s="2"/>
@@ -9154,7 +9157,7 @@
       <c r="H189" s="1"/>
       <c r="I189" s="1"/>
       <c r="J189" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K189" s="43"/>
       <c r="L189" s="2"/>
@@ -9188,7 +9191,7 @@
       <c r="H190" s="1"/>
       <c r="I190" s="1"/>
       <c r="J190" s="34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K190" s="43"/>
       <c r="L190" s="2"/>
@@ -9250,21 +9253,21 @@
         <v>6</v>
       </c>
       <c r="B192" s="122" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C192" s="50">
         <v>1</v>
       </c>
       <c r="D192" s="50"/>
       <c r="E192" s="124" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F192" s="62"/>
       <c r="G192" s="35"/>
       <c r="H192" s="35"/>
       <c r="I192" s="35"/>
       <c r="J192" s="120" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K192" s="43"/>
       <c r="L192" s="36"/>
@@ -9296,7 +9299,7 @@
       <c r="H193" s="35"/>
       <c r="I193" s="35"/>
       <c r="J193" s="34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K193" s="43"/>
       <c r="L193" s="36"/>
@@ -9329,7 +9332,7 @@
       <c r="H194" s="13"/>
       <c r="I194" s="13"/>
       <c r="J194" s="116" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K194" s="43"/>
       <c r="L194" s="2"/>
@@ -9362,7 +9365,7 @@
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
       <c r="J195" s="116" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K195" s="43"/>
       <c r="L195" s="2"/>
@@ -9395,7 +9398,7 @@
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
       <c r="J196" s="34" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K196" s="43"/>
       <c r="L196" s="2"/>
@@ -9428,7 +9431,7 @@
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
       <c r="J197" s="116" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K197" s="43"/>
       <c r="L197" s="2"/>
@@ -9462,7 +9465,7 @@
       <c r="H198" s="70"/>
       <c r="I198" s="70"/>
       <c r="J198" s="118" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K198" s="65"/>
       <c r="L198" s="66"/>
@@ -9490,7 +9493,7 @@
         <v>7</v>
       </c>
       <c r="B199" s="122" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C199" s="50"/>
       <c r="D199" s="50"/>
@@ -9500,7 +9503,7 @@
       <c r="H199" s="35"/>
       <c r="I199" s="35"/>
       <c r="J199" s="35" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="K199" s="43"/>
       <c r="L199" s="36"/>
@@ -9533,7 +9536,7 @@
       <c r="H200" s="13"/>
       <c r="I200" s="13"/>
       <c r="J200" s="13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K200" s="43"/>
       <c r="L200" s="2"/>
@@ -9567,7 +9570,7 @@
       <c r="H201" s="70"/>
       <c r="I201" s="70"/>
       <c r="J201" s="118" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K201" s="65"/>
       <c r="L201" s="66"/>
@@ -9595,7 +9598,7 @@
         <v>8</v>
       </c>
       <c r="B202" s="115" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C202" s="62"/>
       <c r="D202" s="161">
@@ -9607,7 +9610,7 @@
       <c r="H202" s="35"/>
       <c r="I202" s="35"/>
       <c r="J202" s="120" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="K202" s="43"/>
       <c r="L202" s="36"/>
@@ -9635,14 +9638,14 @@
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="93" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E203" s="1"/>
       <c r="G203" s="13"/>
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
       <c r="J203" s="116" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K203" s="43"/>
       <c r="L203" s="2"/>
@@ -9675,7 +9678,7 @@
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
       <c r="J204" s="116" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K204" s="43"/>
       <c r="L204" s="2"/>
@@ -9708,7 +9711,7 @@
       <c r="H205" s="13"/>
       <c r="I205" s="13"/>
       <c r="J205" s="116" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K205" s="43"/>
       <c r="L205" s="2"/>
@@ -9767,7 +9770,7 @@
     <row r="207" spans="1:30" s="16" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="29"/>
       <c r="B207" s="203" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C207" s="204"/>
       <c r="D207" s="204"/>
@@ -9801,7 +9804,7 @@
     <row r="208" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="27"/>
       <c r="B208" s="130" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C208" s="78"/>
       <c r="D208" s="78"/>
@@ -9869,7 +9872,7 @@
         <v>9</v>
       </c>
       <c r="B210" s="114" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C210" s="52"/>
       <c r="D210" s="52"/>
@@ -9911,7 +9914,7 @@
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E211" s="1"/>
       <c r="F211" s="116"/>
@@ -9957,7 +9960,7 @@
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
       <c r="J212" s="116" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K212" s="43"/>
       <c r="L212" s="2"/>
@@ -9995,7 +9998,7 @@
       <c r="H213" s="13"/>
       <c r="I213" s="13"/>
       <c r="J213" s="116" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="K213" s="43"/>
       <c r="L213" s="2"/>
@@ -10031,7 +10034,7 @@
       <c r="H214" s="19"/>
       <c r="I214" s="19"/>
       <c r="J214" s="131" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K214" s="43"/>
       <c r="L214" s="2"/>
@@ -10065,7 +10068,7 @@
       <c r="H215" s="19"/>
       <c r="I215" s="19"/>
       <c r="J215" s="72" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K215" s="43"/>
       <c r="L215" s="2"/>
@@ -10093,7 +10096,7 @@
         <v>10</v>
       </c>
       <c r="B216" s="52" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C216" s="57"/>
       <c r="D216" s="57"/>
@@ -10103,7 +10106,7 @@
       <c r="H216" s="31"/>
       <c r="I216" s="31"/>
       <c r="J216" s="31" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="K216" s="42"/>
       <c r="L216" s="24"/>
@@ -10141,7 +10144,7 @@
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
       <c r="J217" s="116" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="K217" s="43">
         <v>1</v>
@@ -10183,7 +10186,7 @@
       <c r="H218" s="13"/>
       <c r="I218" s="13"/>
       <c r="J218" s="13" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="K218" s="43"/>
       <c r="L218" s="2">
@@ -10211,7 +10214,7 @@
     <row r="219" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A219" s="29"/>
       <c r="B219" s="205" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C219" s="206"/>
       <c r="D219" s="206"/>
@@ -10247,7 +10250,7 @@
         <v>12</v>
       </c>
       <c r="B220" s="132" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C220" s="55"/>
       <c r="D220" s="55"/>
@@ -10257,7 +10260,7 @@
       <c r="H220" s="34"/>
       <c r="I220" s="34"/>
       <c r="J220" s="39" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="K220" s="43"/>
       <c r="L220" s="2"/>
@@ -10291,7 +10294,7 @@
       <c r="H221" s="34"/>
       <c r="I221" s="34"/>
       <c r="J221" s="40" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K221" s="43"/>
       <c r="L221" s="2"/>
@@ -10325,7 +10328,7 @@
       <c r="H222" s="18"/>
       <c r="I222" s="18"/>
       <c r="J222" s="104" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K222" s="43"/>
       <c r="L222" s="2"/>
@@ -10353,13 +10356,13 @@
         <v>13</v>
       </c>
       <c r="B223" s="132" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C223" s="55"/>
       <c r="D223" s="55"/>
       <c r="E223" s="55"/>
       <c r="F223" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G223" s="59"/>
       <c r="H223" s="59"/>
@@ -10391,13 +10394,13 @@
         <v>14</v>
       </c>
       <c r="B224" s="134" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C224" s="56"/>
       <c r="D224" s="56"/>
       <c r="E224" s="56"/>
       <c r="F224" s="138" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G224" s="18"/>
       <c r="H224" s="18"/>
@@ -10429,7 +10432,7 @@
         <v>15</v>
       </c>
       <c r="B225" s="134" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C225" s="56"/>
       <c r="D225" s="56"/>
@@ -10465,7 +10468,7 @@
         <v>16</v>
       </c>
       <c r="B226" s="134" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C226" s="56"/>
       <c r="D226" s="56"/>
@@ -10475,7 +10478,7 @@
       <c r="H226" s="35"/>
       <c r="I226" s="35"/>
       <c r="J226" s="136" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="K226" s="43"/>
       <c r="L226" s="2"/>
@@ -10509,7 +10512,7 @@
       <c r="H227" s="35"/>
       <c r="I227" s="35"/>
       <c r="J227" s="137" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="K227" s="43"/>
       <c r="L227" s="2"/>
@@ -10543,7 +10546,7 @@
       <c r="H228" s="35"/>
       <c r="I228" s="35"/>
       <c r="J228" s="137" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K228" s="43"/>
       <c r="L228" s="2"/>
@@ -10577,7 +10580,7 @@
       <c r="H229" s="35"/>
       <c r="I229" s="35"/>
       <c r="J229" s="137" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="K229" s="43"/>
       <c r="L229" s="2"/>
@@ -10611,7 +10614,7 @@
       <c r="H230" s="35"/>
       <c r="I230" s="35"/>
       <c r="J230" s="137" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K230" s="43"/>
       <c r="L230" s="2"/>
@@ -10721,15 +10724,15 @@
         <v>17</v>
       </c>
       <c r="B233" s="135" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C233" s="26"/>
       <c r="D233" s="26"/>
       <c r="E233" s="97" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F233" s="126" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G233" s="26"/>
       <c r="H233" s="26"/>
@@ -10763,7 +10766,7 @@
       <c r="D234" s="61"/>
       <c r="E234" s="61"/>
       <c r="F234" s="107" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G234" s="61"/>
       <c r="I234" s="18"/>
@@ -10794,13 +10797,13 @@
         <v>18</v>
       </c>
       <c r="B235" s="167" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C235" s="168"/>
       <c r="D235" s="169"/>
       <c r="E235" s="169"/>
       <c r="F235" s="191" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G235" s="1"/>
       <c r="H235" s="1"/>
@@ -10864,15 +10867,15 @@
         <v>19</v>
       </c>
       <c r="B237" s="135" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C237" s="26"/>
       <c r="D237" s="73"/>
       <c r="E237" s="193" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F237" s="170" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G237" s="26"/>
       <c r="H237" s="26"/>
@@ -10905,10 +10908,10 @@
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
       <c r="E238" s="159" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F238" s="192" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G238" s="1"/>
       <c r="H238" s="1"/>
@@ -10942,7 +10945,7 @@
       <c r="D239" s="1"/>
       <c r="E239" s="1"/>
       <c r="F239" s="133" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G239" s="1"/>
       <c r="H239" s="1"/>
@@ -10974,11 +10977,11 @@
         <v>20</v>
       </c>
       <c r="B240" s="109" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C240" s="1"/>
       <c r="D240" s="93" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E240" s="1"/>
       <c r="F240" s="1"/>
@@ -11010,7 +11013,7 @@
     <row r="241" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="27"/>
       <c r="B241" s="171" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
@@ -11044,7 +11047,7 @@
     <row r="242" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="27"/>
       <c r="B242" s="171" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C242" s="1"/>
       <c r="D242" s="1"/>
@@ -11078,7 +11081,7 @@
     <row r="243" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="27"/>
       <c r="B243" s="108" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C243" s="1"/>
       <c r="D243" s="1"/>
@@ -11299,14 +11302,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="208" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B1" s="208"/>
       <c r="C1" s="21" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D1" s="207" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E1" s="207"/>
       <c r="F1" s="22"/>
@@ -11314,68 +11317,68 @@
     </row>
     <row r="2" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A2" s="110" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B2" s="105" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C2" s="189" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="110" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C3" s="190" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" s="111" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C4" s="190" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="111" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C5" s="190" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="110" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C6" s="190" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="111" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C7" s="190" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -11389,17 +11392,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a834da9-6c01-4b0d-9854-214ab0844664">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA421E502B73EC48B7C481B02707A95D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8e395bb2bcb17e943266a860489f057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a834da9-6c01-4b0d-9854-214ab0844664" xmlns:ns3="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b1084d163ef6a9ae7f6b3d13802deaa" ns2:_="" ns3:_="">
     <xsd:import namespace="1a834da9-6c01-4b0d-9854-214ab0844664"/>
@@ -11654,6 +11646,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a834da9-6c01-4b0d-9854-214ab0844664">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11664,23 +11667,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81CDBFC0-0126-4DB7-8868-40859C987D1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11699,6 +11685,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8BE695-F061-495A-A060-7569CE2A6C93}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Remove duplicate option in question5
</commit_message>
<xml_diff>
--- a/media/questions.xlsx
+++ b/media/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ju5315jo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4307D21B-B190-455E-B0E2-18829D6B479B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{229D1C4E-547C-4759-9838-D0B060C34720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5112" yWindow="1920" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Yhdistetty" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="269">
   <si>
     <t>#</t>
   </si>
@@ -529,13 +529,16 @@
     <t>Tärkein syy, miksi kävelen on://Den främsta anledningen till att jag går är://The main reason why I walk is:</t>
   </si>
   <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>Matkan hinta.//Resans pris.//Cost of the journey.</t>
+  </si>
+  <si>
+    <t>Tärkein syy, miksi käytän Sähköpotkulauta, segway tai muu vastaava on://Den främsta anledningen till att jag använder Elsparkcykel, segway eller liknande är: //The main reason why I use e-scooter, segway or similar is:</t>
+  </si>
+  <si>
     <t>3.5</t>
-  </si>
-  <si>
-    <t>Matkan hinta.//Resans pris.//Cost of the journey.</t>
-  </si>
-  <si>
-    <t>Tärkein syy, miksi käytän Sähköpotkulauta, segway tai muu vastaava on://Den främsta anledningen till att jag använder Elsparkcykel, segway eller liknande är: //The main reason why I use e-scooter, segway or similar is:</t>
   </si>
   <si>
     <t>Mikä tai mitkä seuraavista saisivat sinut muuttamaan liikkumistottumuksiasi?//Vad skulle få dig att ändra dina mobilitetsvanor?//What would inspire you to change your travel habits?</t>
@@ -850,9 +853,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tiedät päivittäiset kohteesi ja miten niihin pääsee. Et pidä yllätyksistä matkan aikana; elämä on sellaisenaan jo tarpeeksi stressaavaa. Olet valmis kokeilemaan nopeampia tai mukavampia vaihtoehtoja, mutta vain jos saat selkeää tietoa niistä – mieluiten yksityiskohtaisen matkasuunnitelman kera./Du vet dina dagliga resmål och hur du tar dig till dem. Du gillar inte överraskningar under resan; livet är tillräckligt stressigt som det är. Du är villig att prova snabbare eller bekvämare alternativ, men bara om du får tydlig information om dem – gärna med en detaljerad resplan./You know where you're going every day and how to get there. You don't like surprises en route; life is already sufficiently stressful as it is. You are willing to try out faster or more comfortable alternatives. But only if you get clear information about this, preferably with a detailed travel plan. </t>
-  </si>
-  <si>
-    <t>3.6</t>
   </si>
 </sst>
 </file>
@@ -1798,10 +1798,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
@@ -2099,10 +2095,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF3ACC6-6455-42D3-BCE3-944B33DD47DC}">
-  <dimension ref="A1:AD248"/>
+  <dimension ref="A1:AD247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B159" sqref="B159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4013,7 +4009,7 @@
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:30" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A49" s="27"/>
       <c r="D49" s="92" t="s">
         <v>58</v>
@@ -7792,7 +7788,7 @@
         <v>160</v>
       </c>
       <c r="I151" s="173" t="s">
-        <v>268</v>
+        <v>161</v>
       </c>
       <c r="J151" s="112" t="s">
         <v>162</v>
@@ -8086,7 +8082,7 @@
         <v>163</v>
       </c>
       <c r="I159" s="173" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="J159" s="112" t="s">
         <v>120</v>
@@ -8527,23 +8523,23 @@
         <v>5</v>
       </c>
       <c r="B171" s="128" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C171" s="49">
         <v>3</v>
       </c>
       <c r="D171" s="91" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E171" s="112" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F171" s="26"/>
       <c r="G171" s="26"/>
       <c r="H171" s="26"/>
       <c r="I171" s="26"/>
       <c r="J171" s="112" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K171" s="42"/>
       <c r="L171" s="24"/>
@@ -8571,7 +8567,7 @@
       <c r="B172" s="13"/>
       <c r="C172" s="13"/>
       <c r="D172" s="93" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E172" s="13"/>
       <c r="F172" s="1"/>
@@ -8579,7 +8575,7 @@
       <c r="H172" s="1"/>
       <c r="I172" s="1"/>
       <c r="J172" s="34" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K172" s="43"/>
       <c r="L172" s="2"/>
@@ -8613,7 +8609,7 @@
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
       <c r="J173" s="116" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K173" s="43"/>
       <c r="L173" s="2"/>
@@ -8647,7 +8643,7 @@
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
       <c r="J174" s="34" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K174" s="43"/>
       <c r="L174" s="2"/>
@@ -8681,7 +8677,7 @@
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
       <c r="J175" s="116" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K175" s="43"/>
       <c r="L175" s="2"/>
@@ -8715,7 +8711,7 @@
       <c r="H176" s="1"/>
       <c r="I176" s="1"/>
       <c r="J176" s="34" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K176" s="43"/>
       <c r="L176" s="2"/>
@@ -8749,7 +8745,7 @@
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
       <c r="J177" s="116" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K177" s="43"/>
       <c r="L177" s="2"/>
@@ -8783,7 +8779,7 @@
       <c r="H178" s="1"/>
       <c r="I178" s="1"/>
       <c r="J178" s="34" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K178" s="43"/>
       <c r="L178" s="2"/>
@@ -8817,7 +8813,7 @@
       <c r="H179" s="1"/>
       <c r="I179" s="1"/>
       <c r="J179" s="116" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K179" s="43"/>
       <c r="L179" s="2"/>
@@ -8840,7 +8836,7 @@
       <c r="AC179" s="1"/>
       <c r="AD179" s="1"/>
     </row>
-    <row r="180" spans="1:30" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:30" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A180" s="27"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -8850,8 +8846,8 @@
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
       <c r="I180" s="1"/>
-      <c r="J180" s="34" t="s">
-        <v>176</v>
+      <c r="J180" s="116" t="s">
+        <v>178</v>
       </c>
       <c r="K180" s="43"/>
       <c r="L180" s="2"/>
@@ -8874,7 +8870,7 @@
       <c r="AC180" s="1"/>
       <c r="AD180" s="1"/>
     </row>
-    <row r="181" spans="1:30" ht="91.8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A181" s="27"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -8885,7 +8881,7 @@
       <c r="H181" s="1"/>
       <c r="I181" s="1"/>
       <c r="J181" s="116" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="K181" s="43"/>
       <c r="L181" s="2"/>
@@ -8908,7 +8904,7 @@
       <c r="AC181" s="1"/>
       <c r="AD181" s="1"/>
     </row>
-    <row r="182" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="27"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -8919,7 +8915,7 @@
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
       <c r="J182" s="116" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="K182" s="43"/>
       <c r="L182" s="2"/>
@@ -8942,7 +8938,7 @@
       <c r="AC182" s="1"/>
       <c r="AD182" s="1"/>
     </row>
-    <row r="183" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:30" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A183" s="27"/>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -8952,8 +8948,8 @@
       <c r="G183" s="1"/>
       <c r="H183" s="1"/>
       <c r="I183" s="1"/>
-      <c r="J183" s="116" t="s">
-        <v>179</v>
+      <c r="J183" s="34" t="s">
+        <v>181</v>
       </c>
       <c r="K183" s="43"/>
       <c r="L183" s="2"/>
@@ -8987,7 +8983,7 @@
       <c r="H184" s="1"/>
       <c r="I184" s="1"/>
       <c r="J184" s="34" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K184" s="43"/>
       <c r="L184" s="2"/>
@@ -9010,7 +9006,7 @@
       <c r="AC184" s="1"/>
       <c r="AD184" s="1"/>
     </row>
-    <row r="185" spans="1:30" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A185" s="27"/>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -9020,8 +9016,8 @@
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
       <c r="I185" s="1"/>
-      <c r="J185" s="34" t="s">
-        <v>181</v>
+      <c r="J185" s="116" t="s">
+        <v>183</v>
       </c>
       <c r="K185" s="43"/>
       <c r="L185" s="2"/>
@@ -9044,7 +9040,7 @@
       <c r="AC185" s="1"/>
       <c r="AD185" s="1"/>
     </row>
-    <row r="186" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:30" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A186" s="27"/>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -9054,8 +9050,8 @@
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
       <c r="I186" s="1"/>
-      <c r="J186" s="116" t="s">
-        <v>182</v>
+      <c r="J186" s="34" t="s">
+        <v>184</v>
       </c>
       <c r="K186" s="43"/>
       <c r="L186" s="2"/>
@@ -9089,7 +9085,7 @@
       <c r="H187" s="1"/>
       <c r="I187" s="1"/>
       <c r="J187" s="34" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="K187" s="43"/>
       <c r="L187" s="2"/>
@@ -9123,7 +9119,7 @@
       <c r="H188" s="1"/>
       <c r="I188" s="1"/>
       <c r="J188" s="34" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="K188" s="43"/>
       <c r="L188" s="2"/>
@@ -9146,7 +9142,7 @@
       <c r="AC188" s="1"/>
       <c r="AD188" s="1"/>
     </row>
-    <row r="189" spans="1:30" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:30" ht="72.599999999999994" x14ac:dyDescent="0.3">
       <c r="A189" s="27"/>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -9157,7 +9153,7 @@
       <c r="H189" s="1"/>
       <c r="I189" s="1"/>
       <c r="J189" s="34" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="K189" s="43"/>
       <c r="L189" s="2"/>
@@ -9180,26 +9176,26 @@
       <c r="AC189" s="1"/>
       <c r="AD189" s="1"/>
     </row>
-    <row r="190" spans="1:30" ht="72.599999999999994" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A190" s="27"/>
-      <c r="B190" s="1"/>
-      <c r="C190" s="1"/>
-      <c r="D190" s="1"/>
-      <c r="E190" s="1"/>
-      <c r="F190" s="1"/>
-      <c r="G190" s="1"/>
-      <c r="H190" s="1"/>
-      <c r="I190" s="1"/>
-      <c r="J190" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="K190" s="43"/>
-      <c r="L190" s="2"/>
-      <c r="M190" s="2"/>
-      <c r="N190" s="2"/>
-      <c r="O190" s="2"/>
-      <c r="P190" s="45"/>
-      <c r="Q190" s="3"/>
+      <c r="B190" s="63"/>
+      <c r="C190" s="61"/>
+      <c r="D190" s="61"/>
+      <c r="E190" s="61"/>
+      <c r="F190" s="61"/>
+      <c r="G190" s="61"/>
+      <c r="H190" s="61"/>
+      <c r="I190" s="61"/>
+      <c r="J190" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="K190" s="65"/>
+      <c r="L190" s="66"/>
+      <c r="M190" s="66"/>
+      <c r="N190" s="66"/>
+      <c r="O190" s="66"/>
+      <c r="P190" s="67"/>
+      <c r="Q190" s="68"/>
       <c r="R190" s="1"/>
       <c r="S190" s="1"/>
       <c r="T190" s="1"/>
@@ -9214,26 +9210,34 @@
       <c r="AC190" s="1"/>
       <c r="AD190" s="1"/>
     </row>
-    <row r="191" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A191" s="27"/>
-      <c r="B191" s="63"/>
-      <c r="C191" s="61"/>
-      <c r="D191" s="61"/>
-      <c r="E191" s="61"/>
-      <c r="F191" s="61"/>
-      <c r="G191" s="61"/>
-      <c r="H191" s="61"/>
-      <c r="I191" s="61"/>
-      <c r="J191" s="101" t="s">
-        <v>62</v>
-      </c>
-      <c r="K191" s="65"/>
-      <c r="L191" s="66"/>
-      <c r="M191" s="66"/>
-      <c r="N191" s="66"/>
-      <c r="O191" s="66"/>
-      <c r="P191" s="67"/>
-      <c r="Q191" s="68"/>
+    <row r="191" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A191" s="29">
+        <v>6</v>
+      </c>
+      <c r="B191" s="122" t="s">
+        <v>188</v>
+      </c>
+      <c r="C191" s="50">
+        <v>1</v>
+      </c>
+      <c r="D191" s="50"/>
+      <c r="E191" s="124" t="s">
+        <v>116</v>
+      </c>
+      <c r="F191" s="62"/>
+      <c r="G191" s="35"/>
+      <c r="H191" s="35"/>
+      <c r="I191" s="35"/>
+      <c r="J191" s="120" t="s">
+        <v>189</v>
+      </c>
+      <c r="K191" s="43"/>
+      <c r="L191" s="36"/>
+      <c r="M191" s="36"/>
+      <c r="N191" s="36"/>
+      <c r="O191" s="36"/>
+      <c r="P191" s="45"/>
+      <c r="Q191" s="3"/>
       <c r="R191" s="1"/>
       <c r="S191" s="1"/>
       <c r="T191" s="1"/>
@@ -9248,26 +9252,16 @@
       <c r="AC191" s="1"/>
       <c r="AD191" s="1"/>
     </row>
-    <row r="192" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A192" s="29">
-        <v>6</v>
-      </c>
-      <c r="B192" s="122" t="s">
-        <v>187</v>
-      </c>
-      <c r="C192" s="50">
-        <v>1</v>
-      </c>
-      <c r="D192" s="50"/>
-      <c r="E192" s="124" t="s">
-        <v>116</v>
-      </c>
-      <c r="F192" s="62"/>
+    <row r="192" spans="1:30" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A192" s="27"/>
+      <c r="C192" s="18"/>
+      <c r="D192" s="18"/>
+      <c r="E192" s="18"/>
       <c r="G192" s="35"/>
       <c r="H192" s="35"/>
       <c r="I192" s="35"/>
-      <c r="J192" s="120" t="s">
-        <v>188</v>
+      <c r="J192" s="34" t="s">
+        <v>190</v>
       </c>
       <c r="K192" s="43"/>
       <c r="L192" s="36"/>
@@ -9290,22 +9284,23 @@
       <c r="AC192" s="1"/>
       <c r="AD192" s="1"/>
     </row>
-    <row r="193" spans="1:30" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A193" s="27"/>
-      <c r="C193" s="18"/>
-      <c r="D193" s="18"/>
-      <c r="E193" s="18"/>
-      <c r="G193" s="35"/>
-      <c r="H193" s="35"/>
-      <c r="I193" s="35"/>
-      <c r="J193" s="34" t="s">
-        <v>189</v>
+      <c r="B193" s="1"/>
+      <c r="C193" s="1"/>
+      <c r="D193" s="1"/>
+      <c r="E193" s="1"/>
+      <c r="G193" s="13"/>
+      <c r="H193" s="13"/>
+      <c r="I193" s="13"/>
+      <c r="J193" s="116" t="s">
+        <v>191</v>
       </c>
       <c r="K193" s="43"/>
-      <c r="L193" s="36"/>
-      <c r="M193" s="36"/>
-      <c r="N193" s="36"/>
-      <c r="O193" s="36"/>
+      <c r="L193" s="2"/>
+      <c r="M193" s="2"/>
+      <c r="N193" s="2"/>
+      <c r="O193" s="2"/>
       <c r="P193" s="45"/>
       <c r="Q193" s="3"/>
       <c r="R193" s="1"/>
@@ -9332,7 +9327,7 @@
       <c r="H194" s="13"/>
       <c r="I194" s="13"/>
       <c r="J194" s="116" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="K194" s="43"/>
       <c r="L194" s="2"/>
@@ -9355,7 +9350,7 @@
       <c r="AC194" s="1"/>
       <c r="AD194" s="1"/>
     </row>
-    <row r="195" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:30" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A195" s="27"/>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -9364,8 +9359,8 @@
       <c r="G195" s="13"/>
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
-      <c r="J195" s="116" t="s">
-        <v>191</v>
+      <c r="J195" s="34" t="s">
+        <v>193</v>
       </c>
       <c r="K195" s="43"/>
       <c r="L195" s="2"/>
@@ -9388,7 +9383,7 @@
       <c r="AC195" s="1"/>
       <c r="AD195" s="1"/>
     </row>
-    <row r="196" spans="1:30" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A196" s="27"/>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -9397,8 +9392,8 @@
       <c r="G196" s="13"/>
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
-      <c r="J196" s="34" t="s">
-        <v>192</v>
+      <c r="J196" s="116" t="s">
+        <v>194</v>
       </c>
       <c r="K196" s="43"/>
       <c r="L196" s="2"/>
@@ -9422,24 +9417,25 @@
       <c r="AD196" s="1"/>
     </row>
     <row r="197" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A197" s="27"/>
-      <c r="B197" s="1"/>
-      <c r="C197" s="1"/>
-      <c r="D197" s="1"/>
-      <c r="E197" s="1"/>
-      <c r="G197" s="13"/>
-      <c r="H197" s="13"/>
-      <c r="I197" s="13"/>
-      <c r="J197" s="116" t="s">
-        <v>193</v>
-      </c>
-      <c r="K197" s="43"/>
-      <c r="L197" s="2"/>
-      <c r="M197" s="2"/>
-      <c r="N197" s="2"/>
-      <c r="O197" s="2"/>
-      <c r="P197" s="45"/>
-      <c r="Q197" s="3"/>
+      <c r="A197" s="69"/>
+      <c r="B197" s="61"/>
+      <c r="C197" s="61"/>
+      <c r="D197" s="61"/>
+      <c r="E197" s="61"/>
+      <c r="F197" s="22"/>
+      <c r="G197" s="70"/>
+      <c r="H197" s="70"/>
+      <c r="I197" s="70"/>
+      <c r="J197" s="118" t="s">
+        <v>195</v>
+      </c>
+      <c r="K197" s="65"/>
+      <c r="L197" s="66"/>
+      <c r="M197" s="66"/>
+      <c r="N197" s="66"/>
+      <c r="O197" s="66"/>
+      <c r="P197" s="67"/>
+      <c r="Q197" s="68"/>
       <c r="R197" s="1"/>
       <c r="S197" s="1"/>
       <c r="T197" s="1"/>
@@ -9454,26 +9450,30 @@
       <c r="AC197" s="1"/>
       <c r="AD197" s="1"/>
     </row>
-    <row r="198" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A198" s="69"/>
-      <c r="B198" s="61"/>
-      <c r="C198" s="61"/>
-      <c r="D198" s="61"/>
-      <c r="E198" s="61"/>
-      <c r="F198" s="22"/>
-      <c r="G198" s="70"/>
-      <c r="H198" s="70"/>
-      <c r="I198" s="70"/>
-      <c r="J198" s="118" t="s">
-        <v>194</v>
-      </c>
-      <c r="K198" s="65"/>
-      <c r="L198" s="66"/>
-      <c r="M198" s="66"/>
-      <c r="N198" s="66"/>
-      <c r="O198" s="66"/>
-      <c r="P198" s="67"/>
-      <c r="Q198" s="68"/>
+    <row r="198" spans="1:30" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="27">
+        <v>7</v>
+      </c>
+      <c r="B198" s="122" t="s">
+        <v>196</v>
+      </c>
+      <c r="C198" s="50"/>
+      <c r="D198" s="50"/>
+      <c r="E198" s="50"/>
+      <c r="F198" s="62"/>
+      <c r="G198" s="35"/>
+      <c r="H198" s="35"/>
+      <c r="I198" s="35"/>
+      <c r="J198" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="K198" s="43"/>
+      <c r="L198" s="36"/>
+      <c r="M198" s="36"/>
+      <c r="N198" s="36"/>
+      <c r="O198" s="36"/>
+      <c r="P198" s="45"/>
+      <c r="Q198" s="3"/>
       <c r="R198" s="1"/>
       <c r="S198" s="1"/>
       <c r="T198" s="1"/>
@@ -9488,28 +9488,23 @@
       <c r="AC198" s="1"/>
       <c r="AD198" s="1"/>
     </row>
-    <row r="199" spans="1:30" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="27">
-        <v>7</v>
-      </c>
-      <c r="B199" s="122" t="s">
-        <v>195</v>
-      </c>
-      <c r="C199" s="50"/>
-      <c r="D199" s="50"/>
-      <c r="E199" s="50"/>
-      <c r="F199" s="62"/>
-      <c r="G199" s="35"/>
-      <c r="H199" s="35"/>
-      <c r="I199" s="35"/>
-      <c r="J199" s="35" t="s">
-        <v>196</v>
+    <row r="199" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="27"/>
+      <c r="B199" s="1"/>
+      <c r="C199" s="1"/>
+      <c r="D199" s="1"/>
+      <c r="E199" s="1"/>
+      <c r="G199" s="13"/>
+      <c r="H199" s="13"/>
+      <c r="I199" s="13"/>
+      <c r="J199" s="13" t="s">
+        <v>198</v>
       </c>
       <c r="K199" s="43"/>
-      <c r="L199" s="36"/>
-      <c r="M199" s="36"/>
-      <c r="N199" s="36"/>
-      <c r="O199" s="36"/>
+      <c r="L199" s="2"/>
+      <c r="M199" s="2"/>
+      <c r="N199" s="2"/>
+      <c r="O199" s="2"/>
       <c r="P199" s="45"/>
       <c r="Q199" s="3"/>
       <c r="R199" s="1"/>
@@ -9526,25 +9521,26 @@
       <c r="AC199" s="1"/>
       <c r="AD199" s="1"/>
     </row>
-    <row r="200" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="27"/>
-      <c r="B200" s="1"/>
-      <c r="C200" s="1"/>
-      <c r="D200" s="1"/>
-      <c r="E200" s="1"/>
-      <c r="G200" s="13"/>
-      <c r="H200" s="13"/>
-      <c r="I200" s="13"/>
-      <c r="J200" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="K200" s="43"/>
-      <c r="L200" s="2"/>
-      <c r="M200" s="2"/>
-      <c r="N200" s="2"/>
-      <c r="O200" s="2"/>
-      <c r="P200" s="45"/>
-      <c r="Q200" s="3"/>
+    <row r="200" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A200" s="69"/>
+      <c r="B200" s="61"/>
+      <c r="C200" s="61"/>
+      <c r="D200" s="61"/>
+      <c r="E200" s="61"/>
+      <c r="F200" s="22"/>
+      <c r="G200" s="70"/>
+      <c r="H200" s="70"/>
+      <c r="I200" s="70"/>
+      <c r="J200" s="118" t="s">
+        <v>195</v>
+      </c>
+      <c r="K200" s="65"/>
+      <c r="L200" s="66"/>
+      <c r="M200" s="66"/>
+      <c r="N200" s="66"/>
+      <c r="O200" s="66"/>
+      <c r="P200" s="67"/>
+      <c r="Q200" s="68"/>
       <c r="R200" s="1"/>
       <c r="S200" s="1"/>
       <c r="T200" s="1"/>
@@ -9559,26 +9555,32 @@
       <c r="AC200" s="1"/>
       <c r="AD200" s="1"/>
     </row>
-    <row r="201" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A201" s="69"/>
-      <c r="B201" s="61"/>
-      <c r="C201" s="61"/>
-      <c r="D201" s="61"/>
-      <c r="E201" s="61"/>
-      <c r="F201" s="22"/>
-      <c r="G201" s="70"/>
-      <c r="H201" s="70"/>
-      <c r="I201" s="70"/>
-      <c r="J201" s="118" t="s">
-        <v>194</v>
-      </c>
-      <c r="K201" s="65"/>
-      <c r="L201" s="66"/>
-      <c r="M201" s="66"/>
-      <c r="N201" s="66"/>
-      <c r="O201" s="66"/>
-      <c r="P201" s="67"/>
-      <c r="Q201" s="68"/>
+    <row r="201" spans="1:30" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A201" s="27">
+        <v>8</v>
+      </c>
+      <c r="B201" s="115" t="s">
+        <v>199</v>
+      </c>
+      <c r="C201" s="62"/>
+      <c r="D201" s="161">
+        <v>7.1</v>
+      </c>
+      <c r="E201" s="54"/>
+      <c r="F201" s="62"/>
+      <c r="G201" s="35"/>
+      <c r="H201" s="35"/>
+      <c r="I201" s="35"/>
+      <c r="J201" s="120" t="s">
+        <v>200</v>
+      </c>
+      <c r="K201" s="43"/>
+      <c r="L201" s="36"/>
+      <c r="M201" s="36"/>
+      <c r="N201" s="36"/>
+      <c r="O201" s="36"/>
+      <c r="P201" s="45"/>
+      <c r="Q201" s="3"/>
       <c r="R201" s="1"/>
       <c r="S201" s="1"/>
       <c r="T201" s="1"/>
@@ -9593,30 +9595,25 @@
       <c r="AC201" s="1"/>
       <c r="AD201" s="1"/>
     </row>
-    <row r="202" spans="1:30" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A202" s="27">
-        <v>8</v>
-      </c>
-      <c r="B202" s="115" t="s">
-        <v>198</v>
-      </c>
-      <c r="C202" s="62"/>
-      <c r="D202" s="161">
-        <v>7.1</v>
-      </c>
-      <c r="E202" s="54"/>
-      <c r="F202" s="62"/>
-      <c r="G202" s="35"/>
-      <c r="H202" s="35"/>
-      <c r="I202" s="35"/>
-      <c r="J202" s="120" t="s">
-        <v>199</v>
+    <row r="202" spans="1:30" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A202" s="27"/>
+      <c r="B202" s="1"/>
+      <c r="C202" s="1"/>
+      <c r="D202" s="93" t="s">
+        <v>201</v>
+      </c>
+      <c r="E202" s="1"/>
+      <c r="G202" s="13"/>
+      <c r="H202" s="13"/>
+      <c r="I202" s="13"/>
+      <c r="J202" s="116" t="s">
+        <v>202</v>
       </c>
       <c r="K202" s="43"/>
-      <c r="L202" s="36"/>
-      <c r="M202" s="36"/>
-      <c r="N202" s="36"/>
-      <c r="O202" s="36"/>
+      <c r="L202" s="2"/>
+      <c r="M202" s="2"/>
+      <c r="N202" s="2"/>
+      <c r="O202" s="2"/>
       <c r="P202" s="45"/>
       <c r="Q202" s="3"/>
       <c r="R202" s="1"/>
@@ -9633,19 +9630,17 @@
       <c r="AC202" s="1"/>
       <c r="AD202" s="1"/>
     </row>
-    <row r="203" spans="1:30" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:30" ht="51" x14ac:dyDescent="0.3">
       <c r="A203" s="27"/>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
-      <c r="D203" s="93" t="s">
-        <v>200</v>
-      </c>
+      <c r="D203" s="1"/>
       <c r="E203" s="1"/>
       <c r="G203" s="13"/>
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
       <c r="J203" s="116" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="K203" s="43"/>
       <c r="L203" s="2"/>
@@ -9668,7 +9663,7 @@
       <c r="AC203" s="1"/>
       <c r="AD203" s="1"/>
     </row>
-    <row r="204" spans="1:30" ht="51" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A204" s="27"/>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -9678,7 +9673,7 @@
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
       <c r="J204" s="116" t="s">
-        <v>202</v>
+        <v>124</v>
       </c>
       <c r="K204" s="43"/>
       <c r="L204" s="2"/>
@@ -9701,7 +9696,7 @@
       <c r="AC204" s="1"/>
       <c r="AD204" s="1"/>
     </row>
-    <row r="205" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="27"/>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -9711,7 +9706,7 @@
       <c r="H205" s="13"/>
       <c r="I205" s="13"/>
       <c r="J205" s="116" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
       <c r="K205" s="43"/>
       <c r="L205" s="2"/>
@@ -9734,86 +9729,85 @@
       <c r="AC205" s="1"/>
       <c r="AD205" s="1"/>
     </row>
-    <row r="206" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="27"/>
-      <c r="B206" s="1"/>
-      <c r="C206" s="1"/>
-      <c r="D206" s="1"/>
-      <c r="E206" s="1"/>
-      <c r="G206" s="13"/>
-      <c r="H206" s="13"/>
-      <c r="I206" s="13"/>
-      <c r="J206" s="116" t="s">
-        <v>62</v>
-      </c>
-      <c r="K206" s="43"/>
-      <c r="L206" s="2"/>
-      <c r="M206" s="2"/>
-      <c r="N206" s="2"/>
-      <c r="O206" s="2"/>
-      <c r="P206" s="45"/>
-      <c r="Q206" s="3"/>
-      <c r="R206" s="1"/>
-      <c r="S206" s="1"/>
-      <c r="T206" s="1"/>
-      <c r="U206" s="1"/>
-      <c r="V206" s="1"/>
-      <c r="W206" s="1"/>
-      <c r="X206" s="1"/>
-      <c r="Y206" s="1"/>
-      <c r="Z206" s="1"/>
-      <c r="AA206" s="1"/>
-      <c r="AB206" s="1"/>
-      <c r="AC206" s="1"/>
-      <c r="AD206" s="1"/>
-    </row>
-    <row r="207" spans="1:30" s="16" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="29"/>
-      <c r="B207" s="203" t="s">
-        <v>203</v>
-      </c>
-      <c r="C207" s="204"/>
-      <c r="D207" s="204"/>
-      <c r="E207" s="204"/>
-      <c r="F207" s="204"/>
-      <c r="G207" s="103"/>
-      <c r="H207" s="103"/>
-      <c r="I207" s="103"/>
-      <c r="J207" s="74"/>
-      <c r="K207" s="75"/>
-      <c r="L207" s="76"/>
-      <c r="M207" s="76"/>
-      <c r="N207" s="76"/>
-      <c r="O207" s="76"/>
-      <c r="P207" s="77"/>
-      <c r="Q207" s="37"/>
-      <c r="R207" s="14"/>
-      <c r="S207" s="14"/>
-      <c r="T207" s="14"/>
-      <c r="U207" s="14"/>
-      <c r="V207" s="14"/>
-      <c r="W207" s="14"/>
-      <c r="X207" s="14"/>
-      <c r="Y207" s="14"/>
-      <c r="Z207" s="14"/>
-      <c r="AA207" s="14"/>
-      <c r="AB207" s="14"/>
-      <c r="AC207" s="14"/>
-      <c r="AD207" s="14"/>
-    </row>
-    <row r="208" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:30" s="16" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A206" s="29"/>
+      <c r="B206" s="203" t="s">
+        <v>204</v>
+      </c>
+      <c r="C206" s="204"/>
+      <c r="D206" s="204"/>
+      <c r="E206" s="204"/>
+      <c r="F206" s="204"/>
+      <c r="G206" s="103"/>
+      <c r="H206" s="103"/>
+      <c r="I206" s="103"/>
+      <c r="J206" s="74"/>
+      <c r="K206" s="75"/>
+      <c r="L206" s="76"/>
+      <c r="M206" s="76"/>
+      <c r="N206" s="76"/>
+      <c r="O206" s="76"/>
+      <c r="P206" s="77"/>
+      <c r="Q206" s="37"/>
+      <c r="R206" s="14"/>
+      <c r="S206" s="14"/>
+      <c r="T206" s="14"/>
+      <c r="U206" s="14"/>
+      <c r="V206" s="14"/>
+      <c r="W206" s="14"/>
+      <c r="X206" s="14"/>
+      <c r="Y206" s="14"/>
+      <c r="Z206" s="14"/>
+      <c r="AA206" s="14"/>
+      <c r="AB206" s="14"/>
+      <c r="AC206" s="14"/>
+      <c r="AD206" s="14"/>
+    </row>
+    <row r="207" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A207" s="27"/>
+      <c r="B207" s="130" t="s">
+        <v>205</v>
+      </c>
+      <c r="C207" s="78"/>
+      <c r="D207" s="78"/>
+      <c r="E207" s="78"/>
+      <c r="F207" s="79"/>
+      <c r="G207" s="79"/>
+      <c r="H207" s="79"/>
+      <c r="I207" s="79"/>
+      <c r="J207" s="79"/>
+      <c r="K207" s="80"/>
+      <c r="L207" s="81"/>
+      <c r="M207" s="81"/>
+      <c r="N207" s="81"/>
+      <c r="O207" s="81"/>
+      <c r="P207" s="82"/>
+      <c r="Q207" s="3"/>
+      <c r="R207" s="1"/>
+      <c r="S207" s="1"/>
+      <c r="T207" s="1"/>
+      <c r="U207" s="1"/>
+      <c r="V207" s="1"/>
+      <c r="W207" s="1"/>
+      <c r="X207" s="1"/>
+      <c r="Y207" s="1"/>
+      <c r="Z207" s="1"/>
+      <c r="AA207" s="1"/>
+      <c r="AB207" s="1"/>
+      <c r="AC207" s="1"/>
+      <c r="AD207" s="1"/>
+    </row>
+    <row r="208" spans="1:30" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="27"/>
-      <c r="B208" s="130" t="s">
-        <v>204</v>
-      </c>
-      <c r="C208" s="78"/>
-      <c r="D208" s="78"/>
-      <c r="E208" s="78"/>
-      <c r="F208" s="79"/>
-      <c r="G208" s="79"/>
-      <c r="H208" s="79"/>
-      <c r="I208" s="79"/>
-      <c r="J208" s="79"/>
+      <c r="B208" s="83"/>
+      <c r="C208" s="83"/>
+      <c r="D208" s="83"/>
+      <c r="E208" s="83"/>
+      <c r="F208" s="84"/>
+      <c r="G208" s="84"/>
+      <c r="H208" s="84"/>
+      <c r="I208" s="84"/>
+      <c r="J208" s="84"/>
       <c r="K208" s="80"/>
       <c r="L208" s="81"/>
       <c r="M208" s="81"/>
@@ -9835,24 +9829,34 @@
       <c r="AC208" s="1"/>
       <c r="AD208" s="1"/>
     </row>
-    <row r="209" spans="1:30" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="27"/>
-      <c r="B209" s="83"/>
-      <c r="C209" s="83"/>
-      <c r="D209" s="83"/>
-      <c r="E209" s="83"/>
-      <c r="F209" s="84"/>
-      <c r="G209" s="84"/>
-      <c r="H209" s="84"/>
-      <c r="I209" s="84"/>
-      <c r="J209" s="84"/>
-      <c r="K209" s="80"/>
-      <c r="L209" s="81"/>
-      <c r="M209" s="81"/>
-      <c r="N209" s="81"/>
-      <c r="O209" s="81"/>
-      <c r="P209" s="82"/>
-      <c r="Q209" s="3"/>
+    <row r="209" spans="1:30" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A209" s="29">
+        <v>9</v>
+      </c>
+      <c r="B209" s="114" t="s">
+        <v>206</v>
+      </c>
+      <c r="C209" s="52"/>
+      <c r="D209" s="52"/>
+      <c r="E209" s="52"/>
+      <c r="F209" s="31"/>
+      <c r="G209" s="31"/>
+      <c r="H209" s="31"/>
+      <c r="I209" s="31"/>
+      <c r="J209" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="K209" s="42">
+        <v>1</v>
+      </c>
+      <c r="L209" s="24">
+        <v>1</v>
+      </c>
+      <c r="M209" s="24"/>
+      <c r="N209" s="24"/>
+      <c r="O209" s="24"/>
+      <c r="P209" s="44"/>
+      <c r="Q209" s="25"/>
       <c r="R209" s="1"/>
       <c r="S209" s="1"/>
       <c r="T209" s="1"/>
@@ -9867,34 +9871,32 @@
       <c r="AC209" s="1"/>
       <c r="AD209" s="1"/>
     </row>
-    <row r="210" spans="1:30" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="29">
-        <v>9</v>
-      </c>
-      <c r="B210" s="114" t="s">
-        <v>205</v>
-      </c>
-      <c r="C210" s="52"/>
-      <c r="D210" s="52"/>
-      <c r="E210" s="52"/>
-      <c r="F210" s="31"/>
-      <c r="G210" s="31"/>
-      <c r="H210" s="31"/>
-      <c r="I210" s="31"/>
-      <c r="J210" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="K210" s="42">
-        <v>1</v>
-      </c>
-      <c r="L210" s="24">
-        <v>1</v>
-      </c>
-      <c r="M210" s="24"/>
-      <c r="N210" s="24"/>
-      <c r="O210" s="24"/>
-      <c r="P210" s="44"/>
-      <c r="Q210" s="25"/>
+    <row r="210" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A210" s="27"/>
+      <c r="B210" s="1"/>
+      <c r="C210" s="1"/>
+      <c r="D210" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E210" s="1"/>
+      <c r="F210" s="116"/>
+      <c r="G210" s="13"/>
+      <c r="H210" s="13"/>
+      <c r="I210" s="13"/>
+      <c r="J210" s="116" t="s">
+        <v>41</v>
+      </c>
+      <c r="K210" s="43"/>
+      <c r="L210" s="2"/>
+      <c r="M210" s="2">
+        <v>1</v>
+      </c>
+      <c r="N210" s="2"/>
+      <c r="O210" s="2">
+        <v>1</v>
+      </c>
+      <c r="P210" s="45"/>
+      <c r="Q210" s="3"/>
       <c r="R210" s="1"/>
       <c r="S210" s="1"/>
       <c r="T210" s="1"/>
@@ -9913,23 +9915,21 @@
       <c r="A211" s="27"/>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
-      <c r="D211" s="1" t="s">
-        <v>206</v>
-      </c>
+      <c r="D211" s="1"/>
       <c r="E211" s="1"/>
       <c r="F211" s="116"/>
       <c r="G211" s="13"/>
       <c r="H211" s="13"/>
       <c r="I211" s="13"/>
       <c r="J211" s="116" t="s">
-        <v>41</v>
+        <v>208</v>
       </c>
       <c r="K211" s="43"/>
       <c r="L211" s="2"/>
-      <c r="M211" s="2">
-        <v>1</v>
-      </c>
-      <c r="N211" s="2"/>
+      <c r="M211" s="2"/>
+      <c r="N211" s="2">
+        <v>1</v>
+      </c>
       <c r="O211" s="2">
         <v>1</v>
       </c>
@@ -9960,14 +9960,12 @@
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
       <c r="J212" s="116" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="K212" s="43"/>
       <c r="L212" s="2"/>
       <c r="M212" s="2"/>
-      <c r="N212" s="2">
-        <v>1</v>
-      </c>
+      <c r="N212" s="2"/>
       <c r="O212" s="2">
         <v>1</v>
       </c>
@@ -9987,26 +9985,24 @@
       <c r="AC212" s="1"/>
       <c r="AD212" s="1"/>
     </row>
-    <row r="213" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A213" s="27"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
       <c r="E213" s="1"/>
-      <c r="F213" s="116"/>
-      <c r="G213" s="13"/>
-      <c r="H213" s="13"/>
-      <c r="I213" s="13"/>
-      <c r="J213" s="116" t="s">
-        <v>208</v>
+      <c r="F213" s="131"/>
+      <c r="G213" s="19"/>
+      <c r="H213" s="19"/>
+      <c r="I213" s="19"/>
+      <c r="J213" s="131" t="s">
+        <v>210</v>
       </c>
       <c r="K213" s="43"/>
       <c r="L213" s="2"/>
       <c r="M213" s="2"/>
       <c r="N213" s="2"/>
-      <c r="O213" s="2">
-        <v>1</v>
-      </c>
+      <c r="O213" s="2"/>
       <c r="P213" s="45"/>
       <c r="Q213" s="3"/>
       <c r="R213" s="1"/>
@@ -10033,8 +10029,8 @@
       <c r="G214" s="19"/>
       <c r="H214" s="19"/>
       <c r="I214" s="19"/>
-      <c r="J214" s="131" t="s">
-        <v>209</v>
+      <c r="J214" s="72" t="s">
+        <v>211</v>
       </c>
       <c r="K214" s="43"/>
       <c r="L214" s="2"/>
@@ -10057,26 +10053,34 @@
       <c r="AC214" s="1"/>
       <c r="AD214" s="1"/>
     </row>
-    <row r="215" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A215" s="27"/>
-      <c r="B215" s="1"/>
-      <c r="C215" s="1"/>
-      <c r="D215" s="1"/>
-      <c r="E215" s="1"/>
-      <c r="F215" s="131"/>
-      <c r="G215" s="19"/>
-      <c r="H215" s="19"/>
-      <c r="I215" s="19"/>
-      <c r="J215" s="72" t="s">
-        <v>210</v>
-      </c>
-      <c r="K215" s="43"/>
-      <c r="L215" s="2"/>
-      <c r="M215" s="2"/>
-      <c r="N215" s="2"/>
-      <c r="O215" s="2"/>
-      <c r="P215" s="45"/>
-      <c r="Q215" s="3"/>
+    <row r="215" spans="1:30" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A215" s="29">
+        <v>10</v>
+      </c>
+      <c r="B215" s="52" t="s">
+        <v>212</v>
+      </c>
+      <c r="C215" s="57"/>
+      <c r="D215" s="57"/>
+      <c r="E215" s="57"/>
+      <c r="F215" s="31"/>
+      <c r="G215" s="31"/>
+      <c r="H215" s="31"/>
+      <c r="I215" s="31"/>
+      <c r="J215" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="K215" s="42"/>
+      <c r="L215" s="24"/>
+      <c r="M215" s="24"/>
+      <c r="N215" s="24"/>
+      <c r="O215" s="24">
+        <v>1</v>
+      </c>
+      <c r="P215" s="44">
+        <v>1</v>
+      </c>
+      <c r="Q215" s="25"/>
       <c r="R215" s="1"/>
       <c r="S215" s="1"/>
       <c r="T215" s="1"/>
@@ -10091,34 +10095,34 @@
       <c r="AC215" s="1"/>
       <c r="AD215" s="1"/>
     </row>
-    <row r="216" spans="1:30" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A216" s="29">
-        <v>10</v>
-      </c>
-      <c r="B216" s="52" t="s">
-        <v>211</v>
-      </c>
-      <c r="C216" s="57"/>
-      <c r="D216" s="57"/>
-      <c r="E216" s="57"/>
-      <c r="F216" s="31"/>
-      <c r="G216" s="31"/>
-      <c r="H216" s="31"/>
-      <c r="I216" s="31"/>
-      <c r="J216" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="K216" s="42"/>
-      <c r="L216" s="24"/>
-      <c r="M216" s="24"/>
-      <c r="N216" s="24"/>
-      <c r="O216" s="24">
-        <v>1</v>
-      </c>
-      <c r="P216" s="44">
-        <v>1</v>
-      </c>
-      <c r="Q216" s="25"/>
+    <row r="216" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A216" s="27"/>
+      <c r="B216" s="1"/>
+      <c r="C216" s="1"/>
+      <c r="D216" s="1"/>
+      <c r="E216" s="1"/>
+      <c r="F216" s="116"/>
+      <c r="G216" s="13"/>
+      <c r="H216" s="13"/>
+      <c r="I216" s="13"/>
+      <c r="J216" s="116" t="s">
+        <v>214</v>
+      </c>
+      <c r="K216" s="43">
+        <v>1</v>
+      </c>
+      <c r="L216" s="2"/>
+      <c r="M216" s="2">
+        <v>1</v>
+      </c>
+      <c r="N216" s="2">
+        <v>1</v>
+      </c>
+      <c r="O216" s="2">
+        <v>1</v>
+      </c>
+      <c r="P216" s="45"/>
+      <c r="Q216" s="3"/>
       <c r="R216" s="1"/>
       <c r="S216" s="1"/>
       <c r="T216" s="1"/>
@@ -10133,32 +10137,26 @@
       <c r="AC216" s="1"/>
       <c r="AD216" s="1"/>
     </row>
-    <row r="217" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A217" s="27"/>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
       <c r="E217" s="1"/>
-      <c r="F217" s="116"/>
+      <c r="F217" s="13"/>
       <c r="G217" s="13"/>
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
-      <c r="J217" s="116" t="s">
-        <v>213</v>
-      </c>
-      <c r="K217" s="43">
-        <v>1</v>
-      </c>
-      <c r="L217" s="2"/>
-      <c r="M217" s="2">
-        <v>1</v>
-      </c>
-      <c r="N217" s="2">
-        <v>1</v>
-      </c>
-      <c r="O217" s="2">
-        <v>1</v>
-      </c>
+      <c r="J217" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="K217" s="43"/>
+      <c r="L217" s="2">
+        <v>1</v>
+      </c>
+      <c r="M217" s="2"/>
+      <c r="N217" s="2"/>
+      <c r="O217" s="2"/>
       <c r="P217" s="45"/>
       <c r="Q217" s="3"/>
       <c r="R217" s="1"/>
@@ -10176,27 +10174,25 @@
       <c r="AD217" s="1"/>
     </row>
     <row r="218" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A218" s="27"/>
-      <c r="B218" s="1"/>
-      <c r="C218" s="1"/>
-      <c r="D218" s="1"/>
-      <c r="E218" s="1"/>
-      <c r="F218" s="13"/>
-      <c r="G218" s="13"/>
-      <c r="H218" s="13"/>
-      <c r="I218" s="13"/>
-      <c r="J218" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="K218" s="43"/>
-      <c r="L218" s="2">
-        <v>1</v>
-      </c>
-      <c r="M218" s="2"/>
-      <c r="N218" s="2"/>
-      <c r="O218" s="2"/>
-      <c r="P218" s="45"/>
-      <c r="Q218" s="3"/>
+      <c r="A218" s="29"/>
+      <c r="B218" s="205" t="s">
+        <v>216</v>
+      </c>
+      <c r="C218" s="206"/>
+      <c r="D218" s="206"/>
+      <c r="E218" s="206"/>
+      <c r="F218" s="206"/>
+      <c r="G218" s="103"/>
+      <c r="H218" s="103"/>
+      <c r="I218" s="103"/>
+      <c r="J218" s="85"/>
+      <c r="K218" s="86"/>
+      <c r="L218" s="87"/>
+      <c r="M218" s="87"/>
+      <c r="N218" s="87"/>
+      <c r="O218" s="87"/>
+      <c r="P218" s="88"/>
+      <c r="Q218" s="89"/>
       <c r="R218" s="1"/>
       <c r="S218" s="1"/>
       <c r="T218" s="1"/>
@@ -10212,25 +10208,29 @@
       <c r="AD218" s="1"/>
     </row>
     <row r="219" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A219" s="29"/>
-      <c r="B219" s="205" t="s">
-        <v>215</v>
-      </c>
-      <c r="C219" s="206"/>
-      <c r="D219" s="206"/>
-      <c r="E219" s="206"/>
-      <c r="F219" s="206"/>
-      <c r="G219" s="103"/>
-      <c r="H219" s="103"/>
-      <c r="I219" s="103"/>
-      <c r="J219" s="85"/>
-      <c r="K219" s="86"/>
-      <c r="L219" s="87"/>
-      <c r="M219" s="87"/>
-      <c r="N219" s="87"/>
-      <c r="O219" s="87"/>
-      <c r="P219" s="88"/>
-      <c r="Q219" s="89"/>
+      <c r="A219" s="27">
+        <v>12</v>
+      </c>
+      <c r="B219" s="132" t="s">
+        <v>217</v>
+      </c>
+      <c r="C219" s="55"/>
+      <c r="D219" s="55"/>
+      <c r="E219" s="55"/>
+      <c r="F219" s="39"/>
+      <c r="G219" s="34"/>
+      <c r="H219" s="34"/>
+      <c r="I219" s="34"/>
+      <c r="J219" s="39" t="s">
+        <v>218</v>
+      </c>
+      <c r="K219" s="43"/>
+      <c r="L219" s="2"/>
+      <c r="M219" s="2"/>
+      <c r="N219" s="2"/>
+      <c r="O219" s="2"/>
+      <c r="P219" s="45"/>
+      <c r="Q219" s="3"/>
       <c r="R219" s="1"/>
       <c r="S219" s="1"/>
       <c r="T219" s="1"/>
@@ -10246,21 +10246,17 @@
       <c r="AD219" s="1"/>
     </row>
     <row r="220" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A220" s="27">
-        <v>12</v>
-      </c>
-      <c r="B220" s="132" t="s">
-        <v>216</v>
-      </c>
-      <c r="C220" s="55"/>
-      <c r="D220" s="55"/>
-      <c r="E220" s="55"/>
-      <c r="F220" s="39"/>
+      <c r="A220" s="27"/>
+      <c r="B220" s="133"/>
+      <c r="C220" s="1"/>
+      <c r="D220" s="1"/>
+      <c r="E220" s="1"/>
+      <c r="F220" s="40"/>
       <c r="G220" s="34"/>
       <c r="H220" s="34"/>
       <c r="I220" s="34"/>
-      <c r="J220" s="39" t="s">
-        <v>217</v>
+      <c r="J220" s="40" t="s">
+        <v>219</v>
       </c>
       <c r="K220" s="43"/>
       <c r="L220" s="2"/>
@@ -10289,12 +10285,12 @@
       <c r="C221" s="1"/>
       <c r="D221" s="1"/>
       <c r="E221" s="1"/>
-      <c r="F221" s="40"/>
-      <c r="G221" s="34"/>
-      <c r="H221" s="34"/>
-      <c r="I221" s="34"/>
-      <c r="J221" s="40" t="s">
-        <v>218</v>
+      <c r="F221" s="104"/>
+      <c r="G221" s="18"/>
+      <c r="H221" s="18"/>
+      <c r="I221" s="18"/>
+      <c r="J221" s="104" t="s">
+        <v>220</v>
       </c>
       <c r="K221" s="43"/>
       <c r="L221" s="2"/>
@@ -10318,18 +10314,22 @@
       <c r="AD221" s="1"/>
     </row>
     <row r="222" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A222" s="27"/>
-      <c r="B222" s="133"/>
-      <c r="C222" s="1"/>
-      <c r="D222" s="1"/>
-      <c r="E222" s="1"/>
-      <c r="F222" s="104"/>
-      <c r="G222" s="18"/>
-      <c r="H222" s="18"/>
-      <c r="I222" s="18"/>
-      <c r="J222" s="104" t="s">
-        <v>219</v>
-      </c>
+      <c r="A222" s="27">
+        <v>13</v>
+      </c>
+      <c r="B222" s="132" t="s">
+        <v>221</v>
+      </c>
+      <c r="C222" s="55"/>
+      <c r="D222" s="55"/>
+      <c r="E222" s="55"/>
+      <c r="F222" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="G222" s="59"/>
+      <c r="H222" s="59"/>
+      <c r="I222" s="59"/>
+      <c r="J222" s="1"/>
       <c r="K222" s="43"/>
       <c r="L222" s="2"/>
       <c r="M222" s="2"/>
@@ -10351,22 +10351,22 @@
       <c r="AC222" s="1"/>
       <c r="AD222" s="1"/>
     </row>
-    <row r="223" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A223" s="27">
-        <v>13</v>
-      </c>
-      <c r="B223" s="132" t="s">
-        <v>220</v>
-      </c>
-      <c r="C223" s="55"/>
-      <c r="D223" s="55"/>
-      <c r="E223" s="55"/>
-      <c r="F223" s="41" t="s">
-        <v>221</v>
-      </c>
-      <c r="G223" s="59"/>
-      <c r="H223" s="59"/>
-      <c r="I223" s="59"/>
+        <v>14</v>
+      </c>
+      <c r="B223" s="134" t="s">
+        <v>223</v>
+      </c>
+      <c r="C223" s="56"/>
+      <c r="D223" s="56"/>
+      <c r="E223" s="56"/>
+      <c r="F223" s="138" t="s">
+        <v>224</v>
+      </c>
+      <c r="G223" s="18"/>
+      <c r="H223" s="18"/>
+      <c r="I223" s="18"/>
       <c r="J223" s="1"/>
       <c r="K223" s="43"/>
       <c r="L223" s="2"/>
@@ -10389,19 +10389,17 @@
       <c r="AC223" s="1"/>
       <c r="AD223" s="1"/>
     </row>
-    <row r="224" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:30" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="27">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B224" s="134" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C224" s="56"/>
       <c r="D224" s="56"/>
       <c r="E224" s="56"/>
-      <c r="F224" s="138" t="s">
-        <v>223</v>
-      </c>
+      <c r="F224" s="38"/>
       <c r="G224" s="18"/>
       <c r="H224" s="18"/>
       <c r="I224" s="18"/>
@@ -10427,21 +10425,23 @@
       <c r="AC224" s="1"/>
       <c r="AD224" s="1"/>
     </row>
-    <row r="225" spans="1:30" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A225" s="27">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B225" s="134" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C225" s="56"/>
       <c r="D225" s="56"/>
       <c r="E225" s="56"/>
-      <c r="F225" s="38"/>
-      <c r="G225" s="18"/>
-      <c r="H225" s="18"/>
-      <c r="I225" s="18"/>
-      <c r="J225" s="1"/>
+      <c r="F225" s="136"/>
+      <c r="G225" s="35"/>
+      <c r="H225" s="35"/>
+      <c r="I225" s="35"/>
+      <c r="J225" s="136" t="s">
+        <v>227</v>
+      </c>
       <c r="K225" s="43"/>
       <c r="L225" s="2"/>
       <c r="M225" s="2"/>
@@ -10464,21 +10464,17 @@
       <c r="AD225" s="1"/>
     </row>
     <row r="226" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A226" s="27">
-        <v>16</v>
-      </c>
-      <c r="B226" s="134" t="s">
-        <v>225</v>
-      </c>
-      <c r="C226" s="56"/>
-      <c r="D226" s="56"/>
-      <c r="E226" s="56"/>
-      <c r="F226" s="136"/>
+      <c r="A226" s="27"/>
+      <c r="B226" s="131"/>
+      <c r="C226" s="14"/>
+      <c r="D226" s="14"/>
+      <c r="E226" s="14"/>
+      <c r="F226" s="137"/>
       <c r="G226" s="35"/>
       <c r="H226" s="35"/>
       <c r="I226" s="35"/>
-      <c r="J226" s="136" t="s">
-        <v>226</v>
+      <c r="J226" s="137" t="s">
+        <v>228</v>
       </c>
       <c r="K226" s="43"/>
       <c r="L226" s="2"/>
@@ -10501,9 +10497,9 @@
       <c r="AC226" s="1"/>
       <c r="AD226" s="1"/>
     </row>
-    <row r="227" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A227" s="27"/>
-      <c r="B227" s="131"/>
+      <c r="B227" s="14"/>
       <c r="C227" s="14"/>
       <c r="D227" s="14"/>
       <c r="E227" s="14"/>
@@ -10512,7 +10508,7 @@
       <c r="H227" s="35"/>
       <c r="I227" s="35"/>
       <c r="J227" s="137" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K227" s="43"/>
       <c r="L227" s="2"/>
@@ -10546,7 +10542,7 @@
       <c r="H228" s="35"/>
       <c r="I228" s="35"/>
       <c r="J228" s="137" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="K228" s="43"/>
       <c r="L228" s="2"/>
@@ -10569,7 +10565,7 @@
       <c r="AC228" s="1"/>
       <c r="AD228" s="1"/>
     </row>
-    <row r="229" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A229" s="27"/>
       <c r="B229" s="14"/>
       <c r="C229" s="14"/>
@@ -10580,7 +10576,7 @@
       <c r="H229" s="35"/>
       <c r="I229" s="35"/>
       <c r="J229" s="137" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="K229" s="43"/>
       <c r="L229" s="2"/>
@@ -10604,25 +10600,41 @@
       <c r="AD229" s="1"/>
     </row>
     <row r="230" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A230" s="27"/>
-      <c r="B230" s="14"/>
-      <c r="C230" s="14"/>
-      <c r="D230" s="14"/>
-      <c r="E230" s="14"/>
-      <c r="F230" s="137"/>
-      <c r="G230" s="35"/>
-      <c r="H230" s="35"/>
-      <c r="I230" s="35"/>
-      <c r="J230" s="137" t="s">
-        <v>230</v>
-      </c>
-      <c r="K230" s="43"/>
-      <c r="L230" s="2"/>
-      <c r="M230" s="2"/>
-      <c r="N230" s="2"/>
-      <c r="O230" s="2"/>
-      <c r="P230" s="45"/>
-      <c r="Q230" s="3"/>
+      <c r="A230" s="29"/>
+      <c r="B230" s="26"/>
+      <c r="C230" s="26"/>
+      <c r="D230" s="26"/>
+      <c r="E230" s="26"/>
+      <c r="F230" s="26"/>
+      <c r="G230" s="26"/>
+      <c r="H230" s="26"/>
+      <c r="I230" s="26"/>
+      <c r="J230" s="46"/>
+      <c r="K230" s="42">
+        <f t="shared" ref="K230:P230" si="0">SUM(K2:K229)</f>
+        <v>38</v>
+      </c>
+      <c r="L230" s="24">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="M230" s="24">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="N230" s="24">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="O230" s="24">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="P230" s="44">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="Q230" s="25"/>
       <c r="R230" s="1"/>
       <c r="S230" s="1"/>
       <c r="T230" s="1"/>
@@ -10638,41 +10650,23 @@
       <c r="AD230" s="1"/>
     </row>
     <row r="231" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A231" s="29"/>
-      <c r="B231" s="26"/>
-      <c r="C231" s="26"/>
-      <c r="D231" s="26"/>
-      <c r="E231" s="26"/>
-      <c r="F231" s="26"/>
-      <c r="G231" s="26"/>
-      <c r="H231" s="26"/>
-      <c r="I231" s="26"/>
-      <c r="J231" s="46"/>
-      <c r="K231" s="42">
-        <f t="shared" ref="K231:P231" si="0">SUM(K2:K230)</f>
-        <v>38</v>
-      </c>
-      <c r="L231" s="24">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="M231" s="24">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="N231" s="24">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="O231" s="24">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="P231" s="44">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="Q231" s="25"/>
+      <c r="A231" s="27"/>
+      <c r="B231" s="18"/>
+      <c r="C231" s="18"/>
+      <c r="D231" s="18"/>
+      <c r="E231" s="18"/>
+      <c r="F231" s="18"/>
+      <c r="G231" s="18"/>
+      <c r="H231" s="18"/>
+      <c r="I231" s="18"/>
+      <c r="J231" s="96"/>
+      <c r="K231" s="36"/>
+      <c r="L231" s="36"/>
+      <c r="M231" s="36"/>
+      <c r="N231" s="36"/>
+      <c r="O231" s="36"/>
+      <c r="P231" s="45"/>
+      <c r="Q231" s="3"/>
       <c r="R231" s="1"/>
       <c r="S231" s="1"/>
       <c r="T231" s="1"/>
@@ -10687,23 +10681,31 @@
       <c r="AC231" s="1"/>
       <c r="AD231" s="1"/>
     </row>
-    <row r="232" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A232" s="27"/>
-      <c r="B232" s="18"/>
-      <c r="C232" s="18"/>
-      <c r="D232" s="18"/>
-      <c r="E232" s="18"/>
-      <c r="F232" s="18"/>
-      <c r="G232" s="18"/>
-      <c r="H232" s="18"/>
-      <c r="I232" s="18"/>
-      <c r="J232" s="96"/>
-      <c r="K232" s="36"/>
-      <c r="L232" s="36"/>
-      <c r="M232" s="36"/>
-      <c r="N232" s="36"/>
-      <c r="O232" s="36"/>
-      <c r="P232" s="45"/>
+    <row r="232" spans="1:30" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="27">
+        <v>17</v>
+      </c>
+      <c r="B232" s="135" t="s">
+        <v>232</v>
+      </c>
+      <c r="C232" s="26"/>
+      <c r="D232" s="26"/>
+      <c r="E232" s="97" t="s">
+        <v>233</v>
+      </c>
+      <c r="F232" s="126" t="s">
+        <v>234</v>
+      </c>
+      <c r="G232" s="26"/>
+      <c r="H232" s="26"/>
+      <c r="I232" s="26"/>
+      <c r="J232" s="26"/>
+      <c r="K232" s="24"/>
+      <c r="L232" s="24"/>
+      <c r="M232" s="24"/>
+      <c r="N232" s="24"/>
+      <c r="O232" s="24"/>
+      <c r="P232" s="44"/>
       <c r="Q232" s="3"/>
       <c r="R232" s="1"/>
       <c r="S232" s="1"/>
@@ -10719,31 +10721,24 @@
       <c r="AC232" s="1"/>
       <c r="AD232" s="1"/>
     </row>
-    <row r="233" spans="1:30" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="27">
-        <v>17</v>
-      </c>
-      <c r="B233" s="135" t="s">
-        <v>231</v>
-      </c>
-      <c r="C233" s="26"/>
-      <c r="D233" s="26"/>
-      <c r="E233" s="97" t="s">
-        <v>232</v>
-      </c>
-      <c r="F233" s="126" t="s">
-        <v>233</v>
-      </c>
-      <c r="G233" s="26"/>
-      <c r="H233" s="26"/>
-      <c r="I233" s="26"/>
-      <c r="J233" s="26"/>
-      <c r="K233" s="24"/>
-      <c r="L233" s="24"/>
-      <c r="M233" s="24"/>
-      <c r="N233" s="24"/>
-      <c r="O233" s="24"/>
-      <c r="P233" s="44"/>
+    <row r="233" spans="1:30" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="69"/>
+      <c r="B233" s="61"/>
+      <c r="C233" s="61"/>
+      <c r="D233" s="61"/>
+      <c r="E233" s="61"/>
+      <c r="F233" s="107" t="s">
+        <v>235</v>
+      </c>
+      <c r="G233" s="61"/>
+      <c r="I233" s="18"/>
+      <c r="J233" s="18"/>
+      <c r="K233" s="36"/>
+      <c r="L233" s="66"/>
+      <c r="M233" s="66"/>
+      <c r="N233" s="66"/>
+      <c r="O233" s="66"/>
+      <c r="P233" s="67"/>
       <c r="Q233" s="3"/>
       <c r="R233" s="1"/>
       <c r="S233" s="1"/>
@@ -10759,24 +10754,29 @@
       <c r="AC233" s="1"/>
       <c r="AD233" s="1"/>
     </row>
-    <row r="234" spans="1:30" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="69"/>
-      <c r="B234" s="61"/>
-      <c r="C234" s="61"/>
-      <c r="D234" s="61"/>
-      <c r="E234" s="61"/>
-      <c r="F234" s="107" t="s">
-        <v>234</v>
-      </c>
-      <c r="G234" s="61"/>
-      <c r="I234" s="18"/>
-      <c r="J234" s="18"/>
-      <c r="K234" s="36"/>
-      <c r="L234" s="66"/>
-      <c r="M234" s="66"/>
-      <c r="N234" s="66"/>
-      <c r="O234" s="66"/>
-      <c r="P234" s="67"/>
+    <row r="234" spans="1:30" ht="266.39999999999998" x14ac:dyDescent="0.3">
+      <c r="A234" s="27">
+        <v>18</v>
+      </c>
+      <c r="B234" s="167" t="s">
+        <v>236</v>
+      </c>
+      <c r="C234" s="168"/>
+      <c r="D234" s="169"/>
+      <c r="E234" s="169"/>
+      <c r="F234" s="191" t="s">
+        <v>237</v>
+      </c>
+      <c r="G234" s="1"/>
+      <c r="H234" s="1"/>
+      <c r="I234" s="1"/>
+      <c r="J234" s="26"/>
+      <c r="K234" s="98"/>
+      <c r="L234" s="6"/>
+      <c r="M234" s="6"/>
+      <c r="N234" s="6"/>
+      <c r="O234" s="6"/>
+      <c r="P234" s="6"/>
       <c r="Q234" s="3"/>
       <c r="R234" s="1"/>
       <c r="S234" s="1"/>
@@ -10792,24 +10792,18 @@
       <c r="AC234" s="1"/>
       <c r="AD234" s="1"/>
     </row>
-    <row r="235" spans="1:30" ht="266.39999999999998" x14ac:dyDescent="0.3">
-      <c r="A235" s="27">
-        <v>18</v>
-      </c>
-      <c r="B235" s="167" t="s">
-        <v>235</v>
-      </c>
-      <c r="C235" s="168"/>
-      <c r="D235" s="169"/>
-      <c r="E235" s="169"/>
-      <c r="F235" s="191" t="s">
-        <v>236</v>
-      </c>
+    <row r="235" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A235" s="27"/>
+      <c r="B235" s="99"/>
+      <c r="C235" s="1"/>
+      <c r="D235" s="11"/>
+      <c r="E235" s="11"/>
+      <c r="F235" s="11"/>
       <c r="G235" s="1"/>
       <c r="H235" s="1"/>
       <c r="I235" s="1"/>
-      <c r="J235" s="26"/>
-      <c r="K235" s="98"/>
+      <c r="J235" s="18"/>
+      <c r="K235" s="100"/>
       <c r="L235" s="6"/>
       <c r="M235" s="6"/>
       <c r="N235" s="6"/>
@@ -10830,23 +10824,31 @@
       <c r="AC235" s="1"/>
       <c r="AD235" s="1"/>
     </row>
-    <row r="236" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A236" s="27"/>
-      <c r="B236" s="99"/>
-      <c r="C236" s="1"/>
-      <c r="D236" s="11"/>
-      <c r="E236" s="11"/>
-      <c r="F236" s="11"/>
-      <c r="G236" s="1"/>
-      <c r="H236" s="1"/>
-      <c r="I236" s="1"/>
-      <c r="J236" s="18"/>
-      <c r="K236" s="100"/>
-      <c r="L236" s="6"/>
-      <c r="M236" s="6"/>
-      <c r="N236" s="6"/>
-      <c r="O236" s="6"/>
-      <c r="P236" s="6"/>
+    <row r="236" spans="1:30" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="29">
+        <v>19</v>
+      </c>
+      <c r="B236" s="135" t="s">
+        <v>238</v>
+      </c>
+      <c r="C236" s="26"/>
+      <c r="D236" s="73"/>
+      <c r="E236" s="193" t="s">
+        <v>239</v>
+      </c>
+      <c r="F236" s="170" t="s">
+        <v>137</v>
+      </c>
+      <c r="G236" s="26"/>
+      <c r="H236" s="26"/>
+      <c r="I236" s="26"/>
+      <c r="J236" s="26"/>
+      <c r="K236" s="98"/>
+      <c r="L236" s="98"/>
+      <c r="M236" s="98"/>
+      <c r="N236" s="98"/>
+      <c r="O236" s="98"/>
+      <c r="P236" s="98"/>
       <c r="Q236" s="3"/>
       <c r="R236" s="1"/>
       <c r="S236" s="1"/>
@@ -10862,31 +10864,27 @@
       <c r="AC236" s="1"/>
       <c r="AD236" s="1"/>
     </row>
-    <row r="237" spans="1:30" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="29">
-        <v>19</v>
-      </c>
-      <c r="B237" s="135" t="s">
-        <v>237</v>
-      </c>
-      <c r="C237" s="26"/>
-      <c r="D237" s="73"/>
-      <c r="E237" s="193" t="s">
-        <v>238</v>
-      </c>
-      <c r="F237" s="170" t="s">
-        <v>137</v>
-      </c>
-      <c r="G237" s="26"/>
-      <c r="H237" s="26"/>
-      <c r="I237" s="26"/>
-      <c r="J237" s="26"/>
-      <c r="K237" s="98"/>
-      <c r="L237" s="98"/>
-      <c r="M237" s="98"/>
-      <c r="N237" s="98"/>
-      <c r="O237" s="98"/>
-      <c r="P237" s="98"/>
+    <row r="237" spans="1:30" ht="133.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A237" s="27"/>
+      <c r="B237" s="90"/>
+      <c r="C237" s="1"/>
+      <c r="D237" s="1"/>
+      <c r="E237" s="159" t="s">
+        <v>240</v>
+      </c>
+      <c r="F237" s="192" t="s">
+        <v>241</v>
+      </c>
+      <c r="G237" s="1"/>
+      <c r="H237" s="1"/>
+      <c r="I237" s="1"/>
+      <c r="J237" s="18"/>
+      <c r="K237" s="36"/>
+      <c r="L237" s="2"/>
+      <c r="M237" s="2"/>
+      <c r="N237" s="2"/>
+      <c r="O237" s="2"/>
+      <c r="P237" s="2"/>
       <c r="Q237" s="3"/>
       <c r="R237" s="1"/>
       <c r="S237" s="1"/>
@@ -10902,27 +10900,25 @@
       <c r="AC237" s="1"/>
       <c r="AD237" s="1"/>
     </row>
-    <row r="238" spans="1:30" ht="133.80000000000001" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A238" s="27"/>
-      <c r="B238" s="90"/>
+      <c r="B238" s="1"/>
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
-      <c r="E238" s="159" t="s">
-        <v>239</v>
-      </c>
-      <c r="F238" s="192" t="s">
-        <v>240</v>
+      <c r="E238" s="1"/>
+      <c r="F238" s="133" t="s">
+        <v>242</v>
       </c>
       <c r="G238" s="1"/>
       <c r="H238" s="1"/>
       <c r="I238" s="1"/>
-      <c r="J238" s="18"/>
-      <c r="K238" s="36"/>
-      <c r="L238" s="2"/>
-      <c r="M238" s="2"/>
-      <c r="N238" s="2"/>
-      <c r="O238" s="2"/>
-      <c r="P238" s="2"/>
+      <c r="J238" s="1"/>
+      <c r="K238" s="6"/>
+      <c r="L238" s="6"/>
+      <c r="M238" s="6"/>
+      <c r="N238" s="6"/>
+      <c r="O238" s="6"/>
+      <c r="P238" s="6"/>
       <c r="Q238" s="3"/>
       <c r="R238" s="1"/>
       <c r="S238" s="1"/>
@@ -10938,25 +10934,29 @@
       <c r="AC238" s="1"/>
       <c r="AD238" s="1"/>
     </row>
-    <row r="239" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A239" s="27"/>
-      <c r="B239" s="1"/>
+    <row r="239" spans="1:30" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A239" s="27">
+        <v>20</v>
+      </c>
+      <c r="B239" s="109" t="s">
+        <v>243</v>
+      </c>
       <c r="C239" s="1"/>
-      <c r="D239" s="1"/>
+      <c r="D239" s="93" t="s">
+        <v>244</v>
+      </c>
       <c r="E239" s="1"/>
-      <c r="F239" s="133" t="s">
-        <v>241</v>
-      </c>
+      <c r="F239" s="1"/>
       <c r="G239" s="1"/>
       <c r="H239" s="1"/>
       <c r="I239" s="1"/>
       <c r="J239" s="1"/>
-      <c r="K239" s="6"/>
-      <c r="L239" s="6"/>
-      <c r="M239" s="6"/>
-      <c r="N239" s="6"/>
-      <c r="O239" s="6"/>
-      <c r="P239" s="6"/>
+      <c r="K239" s="2"/>
+      <c r="L239" s="2"/>
+      <c r="M239" s="2"/>
+      <c r="N239" s="2"/>
+      <c r="O239" s="2"/>
+      <c r="P239" s="2"/>
       <c r="Q239" s="3"/>
       <c r="R239" s="1"/>
       <c r="S239" s="1"/>
@@ -10972,29 +10972,25 @@
       <c r="AC239" s="1"/>
       <c r="AD239" s="1"/>
     </row>
-    <row r="240" spans="1:30" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="27">
-        <v>20</v>
-      </c>
-      <c r="B240" s="109" t="s">
-        <v>242</v>
+    <row r="240" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A240" s="27"/>
+      <c r="B240" s="171" t="s">
+        <v>245</v>
       </c>
       <c r="C240" s="1"/>
-      <c r="D240" s="93" t="s">
-        <v>243</v>
-      </c>
+      <c r="D240" s="1"/>
       <c r="E240" s="1"/>
       <c r="F240" s="1"/>
       <c r="G240" s="1"/>
       <c r="H240" s="1"/>
       <c r="I240" s="1"/>
       <c r="J240" s="1"/>
-      <c r="K240" s="2"/>
-      <c r="L240" s="2"/>
-      <c r="M240" s="2"/>
-      <c r="N240" s="2"/>
-      <c r="O240" s="2"/>
-      <c r="P240" s="2"/>
+      <c r="K240" s="6"/>
+      <c r="L240" s="6"/>
+      <c r="M240" s="6"/>
+      <c r="N240" s="6"/>
+      <c r="O240" s="6"/>
+      <c r="P240" s="6"/>
       <c r="Q240" s="3"/>
       <c r="R240" s="1"/>
       <c r="S240" s="1"/>
@@ -11013,7 +11009,7 @@
     <row r="241" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="27"/>
       <c r="B241" s="171" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
@@ -11044,10 +11040,10 @@
       <c r="AC241" s="1"/>
       <c r="AD241" s="1"/>
     </row>
-    <row r="242" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="27"/>
-      <c r="B242" s="171" t="s">
-        <v>245</v>
+      <c r="B242" s="108" t="s">
+        <v>247</v>
       </c>
       <c r="C242" s="1"/>
       <c r="D242" s="1"/>
@@ -11057,12 +11053,12 @@
       <c r="H242" s="1"/>
       <c r="I242" s="1"/>
       <c r="J242" s="1"/>
-      <c r="K242" s="6"/>
-      <c r="L242" s="6"/>
-      <c r="M242" s="6"/>
-      <c r="N242" s="6"/>
-      <c r="O242" s="6"/>
-      <c r="P242" s="6"/>
+      <c r="K242" s="2"/>
+      <c r="L242" s="2"/>
+      <c r="M242" s="2"/>
+      <c r="N242" s="2"/>
+      <c r="O242" s="2"/>
+      <c r="P242" s="2"/>
       <c r="Q242" s="3"/>
       <c r="R242" s="1"/>
       <c r="S242" s="1"/>
@@ -11078,11 +11074,9 @@
       <c r="AC242" s="1"/>
       <c r="AD242" s="1"/>
     </row>
-    <row r="243" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:30" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="27"/>
-      <c r="B243" s="108" t="s">
-        <v>246</v>
-      </c>
+      <c r="B243" s="1"/>
       <c r="C243" s="1"/>
       <c r="D243" s="1"/>
       <c r="E243" s="1"/>
@@ -11240,42 +11234,10 @@
       <c r="AC247" s="1"/>
       <c r="AD247" s="1"/>
     </row>
-    <row r="248" spans="1:30" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A248" s="27"/>
-      <c r="B248" s="1"/>
-      <c r="C248" s="1"/>
-      <c r="D248" s="1"/>
-      <c r="E248" s="1"/>
-      <c r="F248" s="1"/>
-      <c r="G248" s="1"/>
-      <c r="H248" s="1"/>
-      <c r="I248" s="1"/>
-      <c r="J248" s="1"/>
-      <c r="K248" s="2"/>
-      <c r="L248" s="2"/>
-      <c r="M248" s="2"/>
-      <c r="N248" s="2"/>
-      <c r="O248" s="2"/>
-      <c r="P248" s="2"/>
-      <c r="Q248" s="3"/>
-      <c r="R248" s="1"/>
-      <c r="S248" s="1"/>
-      <c r="T248" s="1"/>
-      <c r="U248" s="1"/>
-      <c r="V248" s="1"/>
-      <c r="W248" s="1"/>
-      <c r="X248" s="1"/>
-      <c r="Y248" s="1"/>
-      <c r="Z248" s="1"/>
-      <c r="AA248" s="1"/>
-      <c r="AB248" s="1"/>
-      <c r="AC248" s="1"/>
-      <c r="AD248" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B207:F207"/>
-    <mergeCell ref="B219:F219"/>
+    <mergeCell ref="B206:F206"/>
+    <mergeCell ref="B218:F218"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -11302,14 +11264,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="208" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B1" s="208"/>
       <c r="C1" s="21" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D1" s="207" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E1" s="207"/>
       <c r="F1" s="22"/>
@@ -11317,68 +11279,68 @@
     </row>
     <row r="2" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A2" s="110" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B2" s="105" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C2" s="189" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="110" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C3" s="190" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" s="111" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C4" s="190" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="111" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C5" s="190" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="110" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C6" s="190" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="111" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C7" s="190" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -11392,6 +11354,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a834da9-6c01-4b0d-9854-214ab0844664">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA421E502B73EC48B7C481B02707A95D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8e395bb2bcb17e943266a860489f057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a834da9-6c01-4b0d-9854-214ab0844664" xmlns:ns3="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b1084d163ef6a9ae7f6b3d13802deaa" ns2:_="" ns3:_="">
     <xsd:import namespace="1a834da9-6c01-4b0d-9854-214ab0844664"/>
@@ -11646,17 +11619,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a834da9-6c01-4b0d-9854-214ab0844664">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11667,6 +11629,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
+    <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81CDBFC0-0126-4DB7-8868-40859C987D1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11685,23 +11664,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8BE695-F061-495A-A060-7569CE2A6C93}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Question2 add option public transport and walking
</commit_message>
<xml_diff>
--- a/media/questions.xlsx
+++ b/media/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ju5315jo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4307D21B-B190-455E-B0E2-18829D6B479B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A99C02E-C0F1-481B-B192-25AF46085584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="270">
   <si>
     <t>#</t>
   </si>
@@ -529,13 +529,16 @@
     <t>Tärkein syy, miksi kävelen on://Den främsta anledningen till att jag går är://The main reason why I walk is:</t>
   </si>
   <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>Matkan hinta.//Resans pris.//Cost of the journey.</t>
+  </si>
+  <si>
+    <t>Tärkein syy, miksi käytän Sähköpotkulauta, segway tai muu vastaava on://Den främsta anledningen till att jag använder Elsparkcykel, segway eller liknande är: //The main reason why I use e-scooter, segway or similar is:</t>
+  </si>
+  <si>
     <t>3.5</t>
-  </si>
-  <si>
-    <t>Matkan hinta.//Resans pris.//Cost of the journey.</t>
-  </si>
-  <si>
-    <t>Tärkein syy, miksi käytän Sähköpotkulauta, segway tai muu vastaava on://Den främsta anledningen till att jag använder Elsparkcykel, segway eller liknande är: //The main reason why I use e-scooter, segway or similar is:</t>
   </si>
   <si>
     <t>Mikä tai mitkä seuraavista saisivat sinut muuttamaan liikkumistottumuksiasi?//Vad skulle få dig att ändra dina mobilitetsvanor?//What would inspire you to change your travel habits?</t>
@@ -852,7 +855,7 @@
     <t xml:space="preserve">Tiedät päivittäiset kohteesi ja miten niihin pääsee. Et pidä yllätyksistä matkan aikana; elämä on sellaisenaan jo tarpeeksi stressaavaa. Olet valmis kokeilemaan nopeampia tai mukavampia vaihtoehtoja, mutta vain jos saat selkeää tietoa niistä – mieluiten yksityiskohtaisen matkasuunnitelman kera./Du vet dina dagliga resmål och hur du tar dig till dem. Du gillar inte överraskningar under resan; livet är tillräckligt stressigt som det är. Du är villig att prova snabbare eller bekvämare alternativ, men bara om du får tydlig information om dem – gärna med en detaljerad resplan./You know where you're going every day and how to get there. You don't like surprises en route; life is already sufficiently stressful as it is. You are willing to try out faster or more comfortable alternatives. But only if you get clear information about this, preferably with a detailed travel plan. </t>
   </si>
   <si>
-    <t>3.6</t>
+    <t>Joukkoliikenne ja kävely.//Kollektivtrafik och gång.//Public transport and walking.</t>
   </si>
 </sst>
 </file>
@@ -1237,7 +1240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="209">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1780,6 +1783,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2101,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF3ACC6-6455-42D3-BCE3-944B33DD47DC}">
   <dimension ref="A1:AD248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="D72" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J76" sqref="J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4013,7 +4019,7 @@
       <c r="AC48" s="1"/>
       <c r="AD48" s="1"/>
     </row>
-    <row r="49" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:30" ht="48.6" x14ac:dyDescent="0.3">
       <c r="A49" s="27"/>
       <c r="D49" s="92" t="s">
         <v>58</v>
@@ -4962,25 +4968,26 @@
       <c r="AC75" s="1"/>
       <c r="AD75" s="1"/>
     </row>
-    <row r="76" spans="1:30" ht="51" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A76" s="27"/>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="116" t="s">
-        <v>102</v>
+      <c r="B76" s="54"/>
+      <c r="C76" s="165"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="62"/>
+      <c r="G76" s="62"/>
+      <c r="H76" s="35"/>
+      <c r="I76" s="35"/>
+      <c r="J76" s="209" t="s">
+        <v>269</v>
       </c>
       <c r="K76" s="43"/>
-      <c r="L76" s="2"/>
-      <c r="M76" s="2">
-        <v>1</v>
-      </c>
-      <c r="N76" s="2">
-        <v>1</v>
-      </c>
-      <c r="O76" s="2">
+      <c r="L76" s="36"/>
+      <c r="M76" s="36"/>
+      <c r="N76" s="36">
+        <v>1</v>
+      </c>
+      <c r="O76" s="36">
         <v>1</v>
       </c>
       <c r="P76" s="45">
@@ -5001,26 +5008,27 @@
       <c r="AC76" s="1"/>
       <c r="AD76" s="1"/>
     </row>
-    <row r="77" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:30" ht="51" x14ac:dyDescent="0.3">
       <c r="A77" s="27"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
       <c r="J77" s="116" t="s">
-        <v>103</v>
-      </c>
-      <c r="K77" s="43">
-        <v>1</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="K77" s="43"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2">
         <v>1</v>
       </c>
-      <c r="N77" s="2"/>
-      <c r="O77" s="2"/>
+      <c r="N77" s="2">
+        <v>1</v>
+      </c>
+      <c r="O77" s="2">
+        <v>1</v>
+      </c>
       <c r="P77" s="45">
         <v>1</v>
       </c>
@@ -5039,7 +5047,7 @@
       <c r="AC77" s="1"/>
       <c r="AD77" s="1"/>
     </row>
-    <row r="78" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A78" s="27"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -5048,17 +5056,17 @@
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
       <c r="J78" s="116" t="s">
-        <v>104</v>
-      </c>
-      <c r="K78" s="43"/>
+        <v>103</v>
+      </c>
+      <c r="K78" s="43">
+        <v>1</v>
+      </c>
       <c r="L78" s="2"/>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2">
-        <v>1</v>
-      </c>
-      <c r="O78" s="2">
-        <v>1</v>
-      </c>
+      <c r="M78" s="2">
+        <v>1</v>
+      </c>
+      <c r="N78" s="2"/>
+      <c r="O78" s="2"/>
       <c r="P78" s="45">
         <v>1</v>
       </c>
@@ -5077,7 +5085,7 @@
       <c r="AC78" s="1"/>
       <c r="AD78" s="1"/>
     </row>
-    <row r="79" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A79" s="27"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -5086,14 +5094,14 @@
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
       <c r="J79" s="116" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K79" s="43"/>
       <c r="L79" s="2"/>
-      <c r="M79" s="2">
-        <v>1</v>
-      </c>
-      <c r="N79" s="2"/>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2">
+        <v>1</v>
+      </c>
       <c r="O79" s="2">
         <v>1</v>
       </c>
@@ -5115,7 +5123,7 @@
       <c r="AC79" s="1"/>
       <c r="AD79" s="1"/>
     </row>
-    <row r="80" spans="1:30" ht="51" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A80" s="27"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -5124,18 +5132,20 @@
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
       <c r="J80" s="116" t="s">
-        <v>106</v>
-      </c>
-      <c r="K80" s="43">
-        <v>1</v>
-      </c>
-      <c r="L80" s="2">
-        <v>1</v>
-      </c>
-      <c r="M80" s="2"/>
+        <v>105</v>
+      </c>
+      <c r="K80" s="43"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2">
+        <v>1</v>
+      </c>
       <c r="N80" s="2"/>
-      <c r="O80" s="2"/>
-      <c r="P80" s="45"/>
+      <c r="O80" s="2">
+        <v>1</v>
+      </c>
+      <c r="P80" s="45">
+        <v>1</v>
+      </c>
       <c r="Q80" s="3"/>
       <c r="R80" s="1"/>
       <c r="S80" s="1"/>
@@ -5151,7 +5161,7 @@
       <c r="AC80" s="1"/>
       <c r="AD80" s="1"/>
     </row>
-    <row r="81" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:30" ht="51" x14ac:dyDescent="0.3">
       <c r="A81" s="27"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -5159,11 +5169,15 @@
       <c r="E81" s="1"/>
       <c r="H81" s="13"/>
       <c r="I81" s="13"/>
-      <c r="J81" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="K81" s="43"/>
-      <c r="L81" s="2"/>
+      <c r="J81" s="116" t="s">
+        <v>106</v>
+      </c>
+      <c r="K81" s="43">
+        <v>1</v>
+      </c>
+      <c r="L81" s="2">
+        <v>1</v>
+      </c>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
@@ -5183,34 +5197,24 @@
       <c r="AC81" s="1"/>
       <c r="AD81" s="1"/>
     </row>
-    <row r="82" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
-      <c r="A82" s="29">
-        <v>3</v>
-      </c>
-      <c r="B82" s="128" t="s">
-        <v>107</v>
-      </c>
-      <c r="C82" s="49"/>
-      <c r="D82" s="49"/>
-      <c r="E82" s="49"/>
-      <c r="F82" s="73"/>
-      <c r="G82" s="73"/>
-      <c r="H82" s="23"/>
-      <c r="I82" s="23"/>
-      <c r="J82" s="112" t="s">
-        <v>108</v>
-      </c>
-      <c r="K82" s="42">
-        <v>1</v>
-      </c>
-      <c r="L82" s="24">
-        <v>1</v>
-      </c>
-      <c r="M82" s="24"/>
-      <c r="N82" s="24"/>
-      <c r="O82" s="24"/>
-      <c r="P82" s="44"/>
-      <c r="Q82" s="25"/>
+    <row r="82" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="27"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="K82" s="43"/>
+      <c r="L82" s="2"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
+      <c r="O82" s="2"/>
+      <c r="P82" s="45"/>
+      <c r="Q82" s="3"/>
       <c r="R82" s="1"/>
       <c r="S82" s="1"/>
       <c r="T82" s="1"/>
@@ -5225,30 +5229,34 @@
       <c r="AC82" s="1"/>
       <c r="AD82" s="1"/>
     </row>
-    <row r="83" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="27"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="17"/>
-      <c r="J83" s="116" t="s">
-        <v>109</v>
-      </c>
-      <c r="K83" s="43"/>
-      <c r="L83" s="2"/>
-      <c r="M83" s="2"/>
-      <c r="N83" s="2">
-        <v>1</v>
-      </c>
-      <c r="O83" s="2">
-        <v>1</v>
-      </c>
-      <c r="P83" s="45">
-        <v>1</v>
-      </c>
-      <c r="Q83" s="3"/>
+    <row r="83" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A83" s="29">
+        <v>3</v>
+      </c>
+      <c r="B83" s="128" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" s="49"/>
+      <c r="D83" s="49"/>
+      <c r="E83" s="49"/>
+      <c r="F83" s="73"/>
+      <c r="G83" s="73"/>
+      <c r="H83" s="23"/>
+      <c r="I83" s="23"/>
+      <c r="J83" s="112" t="s">
+        <v>108</v>
+      </c>
+      <c r="K83" s="42">
+        <v>1</v>
+      </c>
+      <c r="L83" s="24">
+        <v>1</v>
+      </c>
+      <c r="M83" s="24"/>
+      <c r="N83" s="24"/>
+      <c r="O83" s="24"/>
+      <c r="P83" s="44"/>
+      <c r="Q83" s="25"/>
       <c r="R83" s="1"/>
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
@@ -5272,7 +5280,7 @@
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
       <c r="J84" s="116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K84" s="43"/>
       <c r="L84" s="2"/>
@@ -5301,7 +5309,7 @@
       <c r="AC84" s="1"/>
       <c r="AD84" s="1"/>
     </row>
-    <row r="85" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="27"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -5310,16 +5318,20 @@
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
       <c r="J85" s="116" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K85" s="43"/>
       <c r="L85" s="2"/>
       <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
+      <c r="N85" s="2">
+        <v>1</v>
+      </c>
       <c r="O85" s="2">
         <v>1</v>
       </c>
-      <c r="P85" s="45"/>
+      <c r="P85" s="45">
+        <v>1</v>
+      </c>
       <c r="Q85" s="3"/>
       <c r="R85" s="1"/>
       <c r="S85" s="1"/>
@@ -5344,18 +5356,16 @@
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
       <c r="J86" s="116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K86" s="43"/>
       <c r="L86" s="2"/>
-      <c r="M86" s="2">
-        <v>1</v>
-      </c>
+      <c r="M86" s="2"/>
       <c r="N86" s="2"/>
-      <c r="O86" s="2"/>
-      <c r="P86" s="45">
-        <v>1</v>
-      </c>
+      <c r="O86" s="2">
+        <v>1</v>
+      </c>
+      <c r="P86" s="45"/>
       <c r="Q86" s="3"/>
       <c r="R86" s="1"/>
       <c r="S86" s="1"/>
@@ -5380,7 +5390,7 @@
       <c r="H87" s="17"/>
       <c r="I87" s="17"/>
       <c r="J87" s="116" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K87" s="43"/>
       <c r="L87" s="2"/>
@@ -5407,7 +5417,7 @@
       <c r="AC87" s="1"/>
       <c r="AD87" s="1"/>
     </row>
-    <row r="88" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A88" s="27"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -5416,11 +5426,13 @@
       <c r="H88" s="17"/>
       <c r="I88" s="17"/>
       <c r="J88" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K88" s="43"/>
       <c r="L88" s="2"/>
-      <c r="M88" s="2"/>
+      <c r="M88" s="2">
+        <v>1</v>
+      </c>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
       <c r="P88" s="45">
@@ -5441,39 +5453,25 @@
       <c r="AC88" s="1"/>
       <c r="AD88" s="1"/>
     </row>
-    <row r="89" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="29">
-        <v>4</v>
-      </c>
-      <c r="B89" s="114" t="s">
-        <v>115</v>
-      </c>
-      <c r="C89" s="49"/>
-      <c r="D89" s="51"/>
-      <c r="E89" s="124" t="s">
-        <v>116</v>
-      </c>
-      <c r="F89" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="G89" s="162"/>
-      <c r="H89" s="112" t="s">
-        <v>118</v>
-      </c>
-      <c r="I89" s="172" t="s">
-        <v>119</v>
-      </c>
-      <c r="J89" s="112" t="s">
-        <v>120</v>
-      </c>
-      <c r="K89" s="42">
-        <v>1</v>
-      </c>
-      <c r="L89" s="24"/>
-      <c r="M89" s="24"/>
-      <c r="N89" s="24"/>
-      <c r="O89" s="24"/>
-      <c r="P89" s="44"/>
+    <row r="89" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="27"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="1"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="17"/>
+      <c r="J89" s="116" t="s">
+        <v>114</v>
+      </c>
+      <c r="K89" s="43"/>
+      <c r="L89" s="2"/>
+      <c r="M89" s="2"/>
+      <c r="N89" s="2"/>
+      <c r="O89" s="2"/>
+      <c r="P89" s="45">
+        <v>1</v>
+      </c>
       <c r="Q89" s="3"/>
       <c r="R89" s="1"/>
       <c r="S89" s="1"/>
@@ -5489,24 +5487,39 @@
       <c r="AC89" s="1"/>
       <c r="AD89" s="1"/>
     </row>
-    <row r="90" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="27"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="H90" s="14"/>
-      <c r="I90" s="14"/>
-      <c r="J90" s="116" t="s">
-        <v>121</v>
-      </c>
-      <c r="K90" s="43">
-        <v>1</v>
-      </c>
-      <c r="L90" s="2"/>
-      <c r="M90" s="2"/>
-      <c r="N90" s="2"/>
-      <c r="O90" s="2"/>
-      <c r="P90" s="45"/>
+    <row r="90" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
+      <c r="A90" s="29">
+        <v>4</v>
+      </c>
+      <c r="B90" s="114" t="s">
+        <v>115</v>
+      </c>
+      <c r="C90" s="49"/>
+      <c r="D90" s="51"/>
+      <c r="E90" s="124" t="s">
+        <v>116</v>
+      </c>
+      <c r="F90" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="G90" s="162"/>
+      <c r="H90" s="112" t="s">
+        <v>118</v>
+      </c>
+      <c r="I90" s="172" t="s">
+        <v>119</v>
+      </c>
+      <c r="J90" s="112" t="s">
+        <v>120</v>
+      </c>
+      <c r="K90" s="42">
+        <v>1</v>
+      </c>
+      <c r="L90" s="24"/>
+      <c r="M90" s="24"/>
+      <c r="N90" s="24"/>
+      <c r="O90" s="24"/>
+      <c r="P90" s="44"/>
       <c r="Q90" s="3"/>
       <c r="R90" s="1"/>
       <c r="S90" s="1"/>
@@ -5524,16 +5537,13 @@
     </row>
     <row r="91" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="27"/>
-      <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-      <c r="I91" s="1"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
       <c r="J91" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K91" s="43">
         <v>1</v>
@@ -5542,9 +5552,7 @@
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
-      <c r="P91" s="45">
-        <v>1</v>
-      </c>
+      <c r="P91" s="45"/>
       <c r="Q91" s="3"/>
       <c r="R91" s="1"/>
       <c r="S91" s="1"/>
@@ -5560,7 +5568,7 @@
       <c r="AC91" s="1"/>
       <c r="AD91" s="1"/>
     </row>
-    <row r="92" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="27"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -5571,7 +5579,7 @@
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="116" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K92" s="43">
         <v>1</v>
@@ -5598,7 +5606,7 @@
       <c r="AC92" s="1"/>
       <c r="AD92" s="1"/>
     </row>
-    <row r="93" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="27"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -5609,9 +5617,11 @@
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
       <c r="J93" s="116" t="s">
-        <v>124</v>
-      </c>
-      <c r="K93" s="43"/>
+        <v>123</v>
+      </c>
+      <c r="K93" s="43">
+        <v>1</v>
+      </c>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
@@ -5634,7 +5644,7 @@
       <c r="AC93" s="1"/>
       <c r="AD93" s="1"/>
     </row>
-    <row r="94" spans="1:30" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="27"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -5645,16 +5655,16 @@
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="116" t="s">
-        <v>125</v>
-      </c>
-      <c r="K94" s="43">
-        <v>1</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="K94" s="43"/>
       <c r="L94" s="2"/>
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
-      <c r="P94" s="45"/>
+      <c r="P94" s="45">
+        <v>1</v>
+      </c>
       <c r="Q94" s="3"/>
       <c r="R94" s="1"/>
       <c r="S94" s="1"/>
@@ -5670,7 +5680,7 @@
       <c r="AC94" s="1"/>
       <c r="AD94" s="1"/>
     </row>
-    <row r="95" spans="1:30" ht="51" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:30" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="27"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -5681,7 +5691,7 @@
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
       <c r="J95" s="116" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K95" s="43">
         <v>1</v>
@@ -5690,9 +5700,7 @@
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
-      <c r="P95" s="45">
-        <v>1</v>
-      </c>
+      <c r="P95" s="45"/>
       <c r="Q95" s="3"/>
       <c r="R95" s="1"/>
       <c r="S95" s="1"/>
@@ -5719,7 +5727,7 @@
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="116" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K96" s="43">
         <v>1</v>
@@ -5728,7 +5736,9 @@
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
-      <c r="P96" s="45"/>
+      <c r="P96" s="45">
+        <v>1</v>
+      </c>
       <c r="Q96" s="3"/>
       <c r="R96" s="1"/>
       <c r="S96" s="1"/>
@@ -5744,7 +5754,7 @@
       <c r="AC96" s="1"/>
       <c r="AD96" s="1"/>
     </row>
-    <row r="97" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:30" ht="51" x14ac:dyDescent="0.3">
       <c r="A97" s="27"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -5755,14 +5765,12 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="116" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K97" s="43">
         <v>1</v>
       </c>
-      <c r="L97" s="2">
-        <v>1</v>
-      </c>
+      <c r="L97" s="2"/>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -5782,7 +5790,7 @@
       <c r="AC97" s="1"/>
       <c r="AD97" s="1"/>
     </row>
-    <row r="98" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A98" s="27"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -5793,12 +5801,14 @@
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="116" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K98" s="43">
         <v>1</v>
       </c>
-      <c r="L98" s="2"/>
+      <c r="L98" s="2">
+        <v>1</v>
+      </c>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
@@ -5829,12 +5839,12 @@
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="116" t="s">
-        <v>130</v>
-      </c>
-      <c r="K99" s="43"/>
-      <c r="L99" s="2">
-        <v>1</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="K99" s="43">
+        <v>1</v>
+      </c>
+      <c r="L99" s="2"/>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
@@ -5854,7 +5864,7 @@
       <c r="AC99" s="1"/>
       <c r="AD99" s="1"/>
     </row>
-    <row r="100" spans="1:30" ht="51" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A100" s="27"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -5865,11 +5875,9 @@
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="116" t="s">
-        <v>131</v>
-      </c>
-      <c r="K100" s="43">
-        <v>1</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="K100" s="43"/>
       <c r="L100" s="2">
         <v>1</v>
       </c>
@@ -5892,7 +5900,7 @@
       <c r="AC100" s="1"/>
       <c r="AD100" s="1"/>
     </row>
-    <row r="101" spans="1:30" ht="71.400000000000006" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:30" ht="51" x14ac:dyDescent="0.3">
       <c r="A101" s="27"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -5903,7 +5911,7 @@
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
       <c r="J101" s="116" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K101" s="43">
         <v>1</v>
@@ -5930,7 +5938,7 @@
       <c r="AC101" s="1"/>
       <c r="AD101" s="1"/>
     </row>
-    <row r="102" spans="1:30" ht="102" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:30" ht="71.400000000000006" x14ac:dyDescent="0.3">
       <c r="A102" s="27"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -5941,18 +5949,18 @@
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
       <c r="J102" s="116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K102" s="43">
         <v>1</v>
       </c>
-      <c r="L102" s="2"/>
+      <c r="L102" s="2">
+        <v>1</v>
+      </c>
       <c r="M102" s="2"/>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
-      <c r="P102" s="45">
-        <v>1</v>
-      </c>
+      <c r="P102" s="45"/>
       <c r="Q102" s="3"/>
       <c r="R102" s="1"/>
       <c r="S102" s="1"/>
@@ -5968,7 +5976,7 @@
       <c r="AC102" s="1"/>
       <c r="AD102" s="1"/>
     </row>
-    <row r="103" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:30" ht="102" x14ac:dyDescent="0.3">
       <c r="A103" s="27"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -5978,15 +5986,19 @@
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
-      <c r="J103" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="K103" s="43"/>
+      <c r="J103" s="116" t="s">
+        <v>133</v>
+      </c>
+      <c r="K103" s="43">
+        <v>1</v>
+      </c>
       <c r="L103" s="2"/>
       <c r="M103" s="2"/>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
-      <c r="P103" s="45"/>
+      <c r="P103" s="45">
+        <v>1</v>
+      </c>
       <c r="Q103" s="3"/>
       <c r="R103" s="1"/>
       <c r="S103" s="1"/>
@@ -6002,33 +6014,25 @@
       <c r="AC103" s="1"/>
       <c r="AD103" s="1"/>
     </row>
-    <row r="104" spans="1:30" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:30" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="27"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
-      <c r="F104" s="52" t="s">
-        <v>134</v>
-      </c>
+      <c r="F104" s="1"/>
       <c r="G104" s="1"/>
-      <c r="H104" s="112" t="s">
-        <v>135</v>
-      </c>
-      <c r="I104" s="173" t="s">
-        <v>136</v>
-      </c>
-      <c r="J104" s="112" t="s">
-        <v>120</v>
-      </c>
-      <c r="K104" s="139">
-        <v>1</v>
-      </c>
-      <c r="L104" s="140"/>
-      <c r="M104" s="140"/>
-      <c r="N104" s="140"/>
-      <c r="O104" s="140"/>
-      <c r="P104" s="141"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+      <c r="J104" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="K104" s="43"/>
+      <c r="L104" s="2"/>
+      <c r="M104" s="2"/>
+      <c r="N104" s="2"/>
+      <c r="O104" s="2"/>
+      <c r="P104" s="45"/>
       <c r="Q104" s="3"/>
       <c r="R104" s="1"/>
       <c r="S104" s="1"/>
@@ -6050,23 +6054,27 @@
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
+      <c r="F105" s="52" t="s">
+        <v>134</v>
+      </c>
       <c r="G105" s="1"/>
-      <c r="H105" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="I105" s="12"/>
-      <c r="J105" s="116" t="s">
-        <v>121</v>
-      </c>
-      <c r="K105" s="142">
-        <v>1</v>
-      </c>
-      <c r="L105" s="143"/>
-      <c r="M105" s="143"/>
-      <c r="N105" s="143"/>
-      <c r="O105" s="143"/>
-      <c r="P105" s="144"/>
+      <c r="H105" s="112" t="s">
+        <v>135</v>
+      </c>
+      <c r="I105" s="173" t="s">
+        <v>136</v>
+      </c>
+      <c r="J105" s="112" t="s">
+        <v>120</v>
+      </c>
+      <c r="K105" s="139">
+        <v>1</v>
+      </c>
+      <c r="L105" s="140"/>
+      <c r="M105" s="140"/>
+      <c r="N105" s="140"/>
+      <c r="O105" s="140"/>
+      <c r="P105" s="141"/>
       <c r="Q105" s="3"/>
       <c r="R105" s="1"/>
       <c r="S105" s="1"/>
@@ -6082,7 +6090,7 @@
       <c r="AC105" s="1"/>
       <c r="AD105" s="1"/>
     </row>
-    <row r="106" spans="1:30" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:30" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="27"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -6090,10 +6098,12 @@
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
-      <c r="H106" s="12"/>
+      <c r="H106" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="I106" s="12"/>
       <c r="J106" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K106" s="142">
         <v>1</v>
@@ -6118,7 +6128,7 @@
       <c r="AC106" s="1"/>
       <c r="AD106" s="1"/>
     </row>
-    <row r="107" spans="1:30" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:30" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="27"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -6129,7 +6139,7 @@
       <c r="H107" s="12"/>
       <c r="I107" s="12"/>
       <c r="J107" s="116" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K107" s="142">
         <v>1</v>
@@ -6154,7 +6164,7 @@
       <c r="AC107" s="1"/>
       <c r="AD107" s="1"/>
     </row>
-    <row r="108" spans="1:30" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:30" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="27"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -6165,7 +6175,7 @@
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
       <c r="J108" s="116" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K108" s="142">
         <v>1</v>
@@ -6190,7 +6200,7 @@
       <c r="AC108" s="1"/>
       <c r="AD108" s="1"/>
     </row>
-    <row r="109" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:30" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="27"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -6201,7 +6211,7 @@
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
       <c r="J109" s="116" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="K109" s="142">
         <v>1</v>
@@ -6226,7 +6236,7 @@
       <c r="AC109" s="1"/>
       <c r="AD109" s="1"/>
     </row>
-    <row r="110" spans="1:30" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="27"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -6237,12 +6247,12 @@
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
       <c r="J110" s="116" t="s">
-        <v>130</v>
-      </c>
-      <c r="K110" s="142"/>
-      <c r="L110" s="143">
-        <v>1</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="K110" s="142">
+        <v>1</v>
+      </c>
+      <c r="L110" s="143"/>
       <c r="M110" s="143"/>
       <c r="N110" s="143"/>
       <c r="O110" s="143"/>
@@ -6273,11 +6283,9 @@
       <c r="H111" s="12"/>
       <c r="I111" s="12"/>
       <c r="J111" s="116" t="s">
-        <v>128</v>
-      </c>
-      <c r="K111" s="142">
-        <v>1</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="K111" s="142"/>
       <c r="L111" s="143">
         <v>1</v>
       </c>
@@ -6300,7 +6308,7 @@
       <c r="AC111" s="1"/>
       <c r="AD111" s="1"/>
     </row>
-    <row r="112" spans="1:30" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:30" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="27"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -6310,13 +6318,15 @@
       <c r="G112" s="1"/>
       <c r="H112" s="12"/>
       <c r="I112" s="12"/>
-      <c r="J112" s="13" t="s">
-        <v>139</v>
+      <c r="J112" s="116" t="s">
+        <v>128</v>
       </c>
       <c r="K112" s="142">
         <v>1</v>
       </c>
-      <c r="L112" s="143"/>
+      <c r="L112" s="143">
+        <v>1</v>
+      </c>
       <c r="M112" s="143"/>
       <c r="N112" s="143"/>
       <c r="O112" s="143"/>
@@ -6336,7 +6346,7 @@
       <c r="AC112" s="1"/>
       <c r="AD112" s="1"/>
     </row>
-    <row r="113" spans="1:30" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:30" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="27"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -6346,15 +6356,13 @@
       <c r="G113" s="1"/>
       <c r="H113" s="12"/>
       <c r="I113" s="12"/>
-      <c r="J113" s="116" t="s">
-        <v>132</v>
+      <c r="J113" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="K113" s="142">
         <v>1</v>
       </c>
-      <c r="L113" s="143">
-        <v>1</v>
-      </c>
+      <c r="L113" s="143"/>
       <c r="M113" s="143"/>
       <c r="N113" s="143"/>
       <c r="O113" s="143"/>
@@ -6374,7 +6382,7 @@
       <c r="AC113" s="1"/>
       <c r="AD113" s="1"/>
     </row>
-    <row r="114" spans="1:30" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:30" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="27"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -6385,18 +6393,18 @@
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
       <c r="J114" s="116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K114" s="142">
         <v>1</v>
       </c>
-      <c r="L114" s="143"/>
+      <c r="L114" s="143">
+        <v>1</v>
+      </c>
       <c r="M114" s="143"/>
       <c r="N114" s="143"/>
       <c r="O114" s="143"/>
-      <c r="P114" s="144">
-        <v>1</v>
-      </c>
+      <c r="P114" s="144"/>
       <c r="Q114" s="3"/>
       <c r="R114" s="1"/>
       <c r="S114" s="1"/>
@@ -6412,7 +6420,7 @@
       <c r="AC114" s="1"/>
       <c r="AD114" s="1"/>
     </row>
-    <row r="115" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:30" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="27"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -6422,15 +6430,19 @@
       <c r="G115" s="1"/>
       <c r="H115" s="12"/>
       <c r="I115" s="12"/>
-      <c r="J115" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="K115" s="142"/>
+      <c r="J115" s="116" t="s">
+        <v>133</v>
+      </c>
+      <c r="K115" s="142">
+        <v>1</v>
+      </c>
       <c r="L115" s="143"/>
       <c r="M115" s="143"/>
       <c r="N115" s="143"/>
       <c r="O115" s="143"/>
-      <c r="P115" s="144"/>
+      <c r="P115" s="144">
+        <v>1</v>
+      </c>
       <c r="Q115" s="3"/>
       <c r="R115" s="1"/>
       <c r="S115" s="1"/>
@@ -6446,35 +6458,25 @@
       <c r="AC115" s="1"/>
       <c r="AD115" s="1"/>
     </row>
-    <row r="116" spans="1:30" ht="102" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="27"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
-      <c r="F116" s="129" t="s">
-        <v>140</v>
-      </c>
-      <c r="G116" s="53"/>
-      <c r="H116" s="112" t="s">
-        <v>141</v>
-      </c>
-      <c r="I116" s="173" t="s">
-        <v>142</v>
-      </c>
-      <c r="J116" s="112" t="s">
-        <v>120</v>
-      </c>
-      <c r="K116" s="42"/>
-      <c r="L116" s="24"/>
-      <c r="M116" s="24"/>
-      <c r="N116" s="24">
-        <v>1</v>
-      </c>
-      <c r="O116" s="24"/>
-      <c r="P116" s="44">
-        <v>1</v>
-      </c>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1"/>
+      <c r="H116" s="12"/>
+      <c r="I116" s="12"/>
+      <c r="J116" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="K116" s="142"/>
+      <c r="L116" s="143"/>
+      <c r="M116" s="143"/>
+      <c r="N116" s="143"/>
+      <c r="O116" s="143"/>
+      <c r="P116" s="144"/>
       <c r="Q116" s="3"/>
       <c r="R116" s="1"/>
       <c r="S116" s="1"/>
@@ -6490,29 +6492,33 @@
       <c r="AC116" s="1"/>
       <c r="AD116" s="1"/>
     </row>
-    <row r="117" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:30" ht="102" x14ac:dyDescent="0.3">
       <c r="A117" s="27"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
-      <c r="F117" s="17"/>
-      <c r="G117" s="17"/>
-      <c r="H117" s="17"/>
-      <c r="I117" s="17"/>
-      <c r="J117" s="116" t="s">
-        <v>121</v>
-      </c>
-      <c r="K117" s="43"/>
-      <c r="L117" s="2"/>
-      <c r="M117" s="2"/>
-      <c r="N117" s="2">
-        <v>1</v>
-      </c>
-      <c r="O117" s="2">
-        <v>1</v>
-      </c>
-      <c r="P117" s="45">
+      <c r="F117" s="129" t="s">
+        <v>140</v>
+      </c>
+      <c r="G117" s="53"/>
+      <c r="H117" s="112" t="s">
+        <v>141</v>
+      </c>
+      <c r="I117" s="173" t="s">
+        <v>142</v>
+      </c>
+      <c r="J117" s="112" t="s">
+        <v>120</v>
+      </c>
+      <c r="K117" s="42"/>
+      <c r="L117" s="24"/>
+      <c r="M117" s="24"/>
+      <c r="N117" s="24">
+        <v>1</v>
+      </c>
+      <c r="O117" s="24"/>
+      <c r="P117" s="44">
         <v>1</v>
       </c>
       <c r="Q117" s="3"/>
@@ -6536,12 +6542,12 @@
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
-      <c r="H118" s="1"/>
-      <c r="I118" s="1"/>
+      <c r="F118" s="17"/>
+      <c r="G118" s="17"/>
+      <c r="H118" s="17"/>
+      <c r="I118" s="17"/>
       <c r="J118" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K118" s="43"/>
       <c r="L118" s="2"/>
@@ -6570,7 +6576,7 @@
       <c r="AC118" s="1"/>
       <c r="AD118" s="1"/>
     </row>
-    <row r="119" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A119" s="27"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -6581,7 +6587,7 @@
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
       <c r="J119" s="116" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K119" s="43"/>
       <c r="L119" s="2"/>
@@ -6610,7 +6616,7 @@
       <c r="AC119" s="1"/>
       <c r="AD119" s="1"/>
     </row>
-    <row r="120" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A120" s="27"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -6621,7 +6627,7 @@
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
       <c r="J120" s="116" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="K120" s="43"/>
       <c r="L120" s="2"/>
@@ -6650,7 +6656,7 @@
       <c r="AC120" s="1"/>
       <c r="AD120" s="1"/>
     </row>
-    <row r="121" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A121" s="27"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -6661,7 +6667,7 @@
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="116" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="K121" s="43"/>
       <c r="L121" s="2"/>
@@ -6672,7 +6678,9 @@
       <c r="O121" s="2">
         <v>1</v>
       </c>
-      <c r="P121" s="45"/>
+      <c r="P121" s="45">
+        <v>1</v>
+      </c>
       <c r="Q121" s="3"/>
       <c r="R121" s="1"/>
       <c r="S121" s="1"/>
@@ -6688,7 +6696,7 @@
       <c r="AC121" s="1"/>
       <c r="AD121" s="1"/>
     </row>
-    <row r="122" spans="1:30" ht="81.599999999999994" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A122" s="27"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -6699,7 +6707,7 @@
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
       <c r="J122" s="116" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="K122" s="43"/>
       <c r="L122" s="2"/>
@@ -6710,9 +6718,7 @@
       <c r="O122" s="2">
         <v>1</v>
       </c>
-      <c r="P122" s="45">
-        <v>1</v>
-      </c>
+      <c r="P122" s="45"/>
       <c r="Q122" s="3"/>
       <c r="R122" s="1"/>
       <c r="S122" s="1"/>
@@ -6728,7 +6734,7 @@
       <c r="AC122" s="1"/>
       <c r="AD122" s="1"/>
     </row>
-    <row r="123" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:30" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A123" s="27"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -6739,16 +6745,20 @@
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
       <c r="J123" s="116" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K123" s="43"/>
-      <c r="L123" s="2">
-        <v>1</v>
-      </c>
+      <c r="L123" s="2"/>
       <c r="M123" s="2"/>
-      <c r="N123" s="2"/>
-      <c r="O123" s="2"/>
-      <c r="P123" s="45"/>
+      <c r="N123" s="2">
+        <v>1</v>
+      </c>
+      <c r="O123" s="2">
+        <v>1</v>
+      </c>
+      <c r="P123" s="45">
+        <v>1</v>
+      </c>
       <c r="Q123" s="3"/>
       <c r="R123" s="1"/>
       <c r="S123" s="1"/>
@@ -6764,7 +6774,7 @@
       <c r="AC123" s="1"/>
       <c r="AD123" s="1"/>
     </row>
-    <row r="124" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A124" s="27"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -6775,16 +6785,14 @@
       <c r="H124" s="1"/>
       <c r="I124" s="1"/>
       <c r="J124" s="116" t="s">
-        <v>57</v>
+        <v>145</v>
       </c>
       <c r="K124" s="43"/>
       <c r="L124" s="2">
         <v>1</v>
       </c>
       <c r="M124" s="2"/>
-      <c r="N124" s="2">
-        <v>1</v>
-      </c>
+      <c r="N124" s="2"/>
       <c r="O124" s="2"/>
       <c r="P124" s="45"/>
       <c r="Q124" s="3"/>
@@ -6802,7 +6810,7 @@
       <c r="AC124" s="1"/>
       <c r="AD124" s="1"/>
     </row>
-    <row r="125" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="27"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -6813,20 +6821,18 @@
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
       <c r="J125" s="116" t="s">
-        <v>138</v>
+        <v>57</v>
       </c>
       <c r="K125" s="43"/>
-      <c r="L125" s="2"/>
+      <c r="L125" s="2">
+        <v>1</v>
+      </c>
       <c r="M125" s="2"/>
       <c r="N125" s="2">
         <v>1</v>
       </c>
-      <c r="O125" s="2">
-        <v>1</v>
-      </c>
-      <c r="P125" s="45">
-        <v>1</v>
-      </c>
+      <c r="O125" s="2"/>
+      <c r="P125" s="45"/>
       <c r="Q125" s="3"/>
       <c r="R125" s="1"/>
       <c r="S125" s="1"/>
@@ -6842,7 +6848,7 @@
       <c r="AC125" s="1"/>
       <c r="AD125" s="1"/>
     </row>
-    <row r="126" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A126" s="27"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -6853,16 +6859,20 @@
       <c r="H126" s="1"/>
       <c r="I126" s="1"/>
       <c r="J126" s="116" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="K126" s="43"/>
-      <c r="L126" s="2">
-        <v>1</v>
-      </c>
+      <c r="L126" s="2"/>
       <c r="M126" s="2"/>
-      <c r="N126" s="2"/>
-      <c r="O126" s="2"/>
-      <c r="P126" s="45"/>
+      <c r="N126" s="2">
+        <v>1</v>
+      </c>
+      <c r="O126" s="2">
+        <v>1</v>
+      </c>
+      <c r="P126" s="45">
+        <v>1</v>
+      </c>
       <c r="Q126" s="3"/>
       <c r="R126" s="1"/>
       <c r="S126" s="1"/>
@@ -6878,7 +6888,7 @@
       <c r="AC126" s="1"/>
       <c r="AD126" s="1"/>
     </row>
-    <row r="127" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A127" s="27"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -6888,11 +6898,13 @@
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
       <c r="I127" s="1"/>
-      <c r="J127" s="34" t="s">
-        <v>62</v>
+      <c r="J127" s="116" t="s">
+        <v>130</v>
       </c>
       <c r="K127" s="43"/>
-      <c r="L127" s="2"/>
+      <c r="L127" s="2">
+        <v>1</v>
+      </c>
       <c r="M127" s="2"/>
       <c r="N127" s="2"/>
       <c r="O127" s="2"/>
@@ -6912,35 +6924,25 @@
       <c r="AC127" s="1"/>
       <c r="AD127" s="1"/>
     </row>
-    <row r="128" spans="1:30" ht="91.8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="27"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
-      <c r="F128" s="114" t="s">
-        <v>146</v>
-      </c>
-      <c r="G128" s="52"/>
-      <c r="H128" s="112" t="s">
-        <v>147</v>
-      </c>
-      <c r="I128" s="173" t="s">
-        <v>148</v>
-      </c>
-      <c r="J128" s="112" t="s">
-        <v>120</v>
-      </c>
-      <c r="K128" s="42"/>
-      <c r="L128" s="24"/>
-      <c r="M128" s="24"/>
-      <c r="N128" s="24"/>
-      <c r="O128" s="24">
-        <v>1</v>
-      </c>
-      <c r="P128" s="44">
-        <v>1</v>
-      </c>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
+      <c r="J128" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="K128" s="43"/>
+      <c r="L128" s="2"/>
+      <c r="M128" s="2"/>
+      <c r="N128" s="2"/>
+      <c r="O128" s="2"/>
+      <c r="P128" s="45"/>
       <c r="Q128" s="3"/>
       <c r="R128" s="1"/>
       <c r="S128" s="1"/>
@@ -6956,27 +6958,33 @@
       <c r="AC128" s="1"/>
       <c r="AD128" s="1"/>
     </row>
-    <row r="129" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:30" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A129" s="27"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
-      <c r="F129" s="17"/>
-      <c r="G129" s="17"/>
-      <c r="H129" s="17"/>
-      <c r="I129" s="17"/>
-      <c r="J129" s="116" t="s">
-        <v>121</v>
-      </c>
-      <c r="K129" s="43"/>
-      <c r="L129" s="2"/>
-      <c r="M129" s="2"/>
-      <c r="N129" s="2"/>
-      <c r="O129" s="2">
-        <v>1</v>
-      </c>
-      <c r="P129" s="45">
+      <c r="F129" s="114" t="s">
+        <v>146</v>
+      </c>
+      <c r="G129" s="52"/>
+      <c r="H129" s="112" t="s">
+        <v>147</v>
+      </c>
+      <c r="I129" s="173" t="s">
+        <v>148</v>
+      </c>
+      <c r="J129" s="112" t="s">
+        <v>120</v>
+      </c>
+      <c r="K129" s="42"/>
+      <c r="L129" s="24"/>
+      <c r="M129" s="24"/>
+      <c r="N129" s="24"/>
+      <c r="O129" s="24">
+        <v>1</v>
+      </c>
+      <c r="P129" s="44">
         <v>1</v>
       </c>
       <c r="Q129" s="3"/>
@@ -6994,26 +7002,26 @@
       <c r="AC129" s="1"/>
       <c r="AD129" s="1"/>
     </row>
-    <row r="130" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A130" s="27"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
-      <c r="F130" s="1"/>
-      <c r="G130" s="1"/>
-      <c r="H130" s="1"/>
-      <c r="I130" s="1"/>
+      <c r="F130" s="17"/>
+      <c r="G130" s="17"/>
+      <c r="H130" s="17"/>
+      <c r="I130" s="17"/>
       <c r="J130" s="116" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="K130" s="43"/>
       <c r="L130" s="2"/>
-      <c r="M130" s="2">
-        <v>1</v>
-      </c>
+      <c r="M130" s="2"/>
       <c r="N130" s="2"/>
-      <c r="O130" s="2"/>
+      <c r="O130" s="2">
+        <v>1</v>
+      </c>
       <c r="P130" s="45">
         <v>1</v>
       </c>
@@ -7032,7 +7040,7 @@
       <c r="AC130" s="1"/>
       <c r="AD130" s="1"/>
     </row>
-    <row r="131" spans="1:30" ht="51" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="27"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -7043,18 +7051,18 @@
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
       <c r="J131" s="116" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="K131" s="43"/>
       <c r="L131" s="2"/>
-      <c r="M131" s="2"/>
-      <c r="N131" s="2">
-        <v>1</v>
-      </c>
-      <c r="O131" s="2">
-        <v>1</v>
-      </c>
-      <c r="P131" s="45"/>
+      <c r="M131" s="2">
+        <v>1</v>
+      </c>
+      <c r="N131" s="2"/>
+      <c r="O131" s="2"/>
+      <c r="P131" s="45">
+        <v>1</v>
+      </c>
       <c r="Q131" s="3"/>
       <c r="R131" s="1"/>
       <c r="S131" s="1"/>
@@ -7070,7 +7078,7 @@
       <c r="AC131" s="1"/>
       <c r="AD131" s="1"/>
     </row>
-    <row r="132" spans="1:30" ht="71.400000000000006" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:30" ht="51" x14ac:dyDescent="0.3">
       <c r="A132" s="27"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -7081,16 +7089,18 @@
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
       <c r="J132" s="116" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="K132" s="43"/>
       <c r="L132" s="2"/>
       <c r="M132" s="2"/>
-      <c r="N132" s="2"/>
-      <c r="O132" s="2"/>
-      <c r="P132" s="45">
-        <v>1</v>
-      </c>
+      <c r="N132" s="2">
+        <v>1</v>
+      </c>
+      <c r="O132" s="2">
+        <v>1</v>
+      </c>
+      <c r="P132" s="45"/>
       <c r="Q132" s="3"/>
       <c r="R132" s="1"/>
       <c r="S132" s="1"/>
@@ -7106,7 +7116,7 @@
       <c r="AC132" s="1"/>
       <c r="AD132" s="1"/>
     </row>
-    <row r="133" spans="1:30" ht="102" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:30" ht="71.400000000000006" x14ac:dyDescent="0.3">
       <c r="A133" s="27"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -7117,7 +7127,7 @@
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
       <c r="J133" s="116" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K133" s="43"/>
       <c r="L133" s="2"/>
@@ -7142,7 +7152,7 @@
       <c r="AC133" s="1"/>
       <c r="AD133" s="1"/>
     </row>
-    <row r="134" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:30" ht="102" x14ac:dyDescent="0.3">
       <c r="A134" s="27"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -7153,17 +7163,13 @@
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
       <c r="J134" s="116" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="K134" s="43"/>
       <c r="L134" s="2"/>
       <c r="M134" s="2"/>
-      <c r="N134" s="2">
-        <v>1</v>
-      </c>
-      <c r="O134" s="2">
-        <v>1</v>
-      </c>
+      <c r="N134" s="2"/>
+      <c r="O134" s="2"/>
       <c r="P134" s="45">
         <v>1</v>
       </c>
@@ -7182,7 +7188,7 @@
       <c r="AC134" s="1"/>
       <c r="AD134" s="1"/>
     </row>
-    <row r="135" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A135" s="27"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -7193,16 +7199,20 @@
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
       <c r="J135" s="116" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="K135" s="43"/>
-      <c r="L135" s="2">
-        <v>1</v>
-      </c>
+      <c r="L135" s="2"/>
       <c r="M135" s="2"/>
-      <c r="N135" s="2"/>
-      <c r="O135" s="2"/>
-      <c r="P135" s="45"/>
+      <c r="N135" s="2">
+        <v>1</v>
+      </c>
+      <c r="O135" s="2">
+        <v>1</v>
+      </c>
+      <c r="P135" s="45">
+        <v>1</v>
+      </c>
       <c r="Q135" s="3"/>
       <c r="R135" s="1"/>
       <c r="S135" s="1"/>
@@ -7218,7 +7228,7 @@
       <c r="AC135" s="1"/>
       <c r="AD135" s="1"/>
     </row>
-    <row r="136" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A136" s="27"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -7229,17 +7239,15 @@
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
       <c r="J136" s="116" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K136" s="43"/>
-      <c r="L136" s="2"/>
+      <c r="L136" s="2">
+        <v>1</v>
+      </c>
       <c r="M136" s="2"/>
-      <c r="N136" s="2">
-        <v>1</v>
-      </c>
-      <c r="O136" s="2">
-        <v>1</v>
-      </c>
+      <c r="N136" s="2"/>
+      <c r="O136" s="2"/>
       <c r="P136" s="45"/>
       <c r="Q136" s="3"/>
       <c r="R136" s="1"/>
@@ -7256,7 +7264,7 @@
       <c r="AC136" s="1"/>
       <c r="AD136" s="1"/>
     </row>
-    <row r="137" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A137" s="27"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -7266,14 +7274,18 @@
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
       <c r="I137" s="1"/>
-      <c r="J137" s="34" t="s">
-        <v>62</v>
+      <c r="J137" s="116" t="s">
+        <v>128</v>
       </c>
       <c r="K137" s="43"/>
       <c r="L137" s="2"/>
       <c r="M137" s="2"/>
-      <c r="N137" s="2"/>
-      <c r="O137" s="2"/>
+      <c r="N137" s="2">
+        <v>1</v>
+      </c>
+      <c r="O137" s="2">
+        <v>1</v>
+      </c>
       <c r="P137" s="45"/>
       <c r="Q137" s="3"/>
       <c r="R137" s="1"/>
@@ -7290,35 +7302,25 @@
       <c r="AC137" s="1"/>
       <c r="AD137" s="1"/>
     </row>
-    <row r="138" spans="1:30" ht="91.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="27"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
-      <c r="F138" s="129" t="s">
-        <v>152</v>
-      </c>
-      <c r="G138" s="53"/>
-      <c r="H138" s="112" t="s">
-        <v>153</v>
-      </c>
-      <c r="I138" s="173" t="s">
-        <v>154</v>
-      </c>
-      <c r="J138" s="112" t="s">
-        <v>120</v>
-      </c>
-      <c r="K138" s="42"/>
-      <c r="L138" s="24"/>
-      <c r="M138" s="24">
-        <v>1</v>
-      </c>
-      <c r="N138" s="24"/>
-      <c r="O138" s="24">
-        <v>1</v>
-      </c>
-      <c r="P138" s="44"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+      <c r="J138" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="K138" s="43"/>
+      <c r="L138" s="2"/>
+      <c r="M138" s="2"/>
+      <c r="N138" s="2"/>
+      <c r="O138" s="2"/>
+      <c r="P138" s="45"/>
       <c r="Q138" s="3"/>
       <c r="R138" s="1"/>
       <c r="S138" s="1"/>
@@ -7334,31 +7336,35 @@
       <c r="AC138" s="1"/>
       <c r="AD138" s="1"/>
     </row>
-    <row r="139" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:30" ht="91.8" x14ac:dyDescent="0.3">
       <c r="A139" s="27"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
-      <c r="F139" s="17"/>
-      <c r="G139" s="17"/>
-      <c r="H139" s="17"/>
-      <c r="I139" s="17"/>
-      <c r="J139" s="116" t="s">
-        <v>121</v>
-      </c>
-      <c r="K139" s="43"/>
-      <c r="L139" s="2"/>
-      <c r="M139" s="2">
-        <v>1</v>
-      </c>
-      <c r="N139" s="2"/>
-      <c r="O139" s="2">
-        <v>1</v>
-      </c>
-      <c r="P139" s="45">
-        <v>1</v>
-      </c>
+      <c r="F139" s="129" t="s">
+        <v>152</v>
+      </c>
+      <c r="G139" s="53"/>
+      <c r="H139" s="112" t="s">
+        <v>153</v>
+      </c>
+      <c r="I139" s="173" t="s">
+        <v>154</v>
+      </c>
+      <c r="J139" s="112" t="s">
+        <v>120</v>
+      </c>
+      <c r="K139" s="42"/>
+      <c r="L139" s="24"/>
+      <c r="M139" s="24">
+        <v>1</v>
+      </c>
+      <c r="N139" s="24"/>
+      <c r="O139" s="24">
+        <v>1</v>
+      </c>
+      <c r="P139" s="44"/>
       <c r="Q139" s="3"/>
       <c r="R139" s="1"/>
       <c r="S139" s="1"/>
@@ -7380,12 +7386,12 @@
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
-      <c r="F140" s="1"/>
-      <c r="G140" s="1"/>
-      <c r="H140" s="1"/>
-      <c r="I140" s="1"/>
+      <c r="F140" s="17"/>
+      <c r="G140" s="17"/>
+      <c r="H140" s="17"/>
+      <c r="I140" s="17"/>
       <c r="J140" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K140" s="43"/>
       <c r="L140" s="2"/>
@@ -7396,7 +7402,9 @@
       <c r="O140" s="2">
         <v>1</v>
       </c>
-      <c r="P140" s="45"/>
+      <c r="P140" s="45">
+        <v>1</v>
+      </c>
       <c r="Q140" s="3"/>
       <c r="R140" s="1"/>
       <c r="S140" s="1"/>
@@ -7412,7 +7420,7 @@
       <c r="AC140" s="1"/>
       <c r="AD140" s="1"/>
     </row>
-    <row r="141" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:30" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A141" s="27"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -7423,7 +7431,7 @@
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
       <c r="J141" s="116" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="K141" s="43"/>
       <c r="L141" s="2"/>
@@ -7431,10 +7439,10 @@
         <v>1</v>
       </c>
       <c r="N141" s="2"/>
-      <c r="O141" s="2"/>
-      <c r="P141" s="45">
-        <v>1</v>
-      </c>
+      <c r="O141" s="2">
+        <v>1</v>
+      </c>
+      <c r="P141" s="45"/>
       <c r="Q141" s="3"/>
       <c r="R141" s="1"/>
       <c r="S141" s="1"/>
@@ -7461,7 +7469,7 @@
       <c r="H142" s="1"/>
       <c r="I142" s="1"/>
       <c r="J142" s="116" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="K142" s="43"/>
       <c r="L142" s="2"/>
@@ -7470,7 +7478,9 @@
       </c>
       <c r="N142" s="2"/>
       <c r="O142" s="2"/>
-      <c r="P142" s="45"/>
+      <c r="P142" s="45">
+        <v>1</v>
+      </c>
       <c r="Q142" s="3"/>
       <c r="R142" s="1"/>
       <c r="S142" s="1"/>
@@ -7497,7 +7507,7 @@
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
       <c r="J143" s="116" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="K143" s="43"/>
       <c r="L143" s="2"/>
@@ -7522,7 +7532,7 @@
       <c r="AC143" s="1"/>
       <c r="AD143" s="1"/>
     </row>
-    <row r="144" spans="1:30" ht="102" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="27"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -7533,7 +7543,7 @@
       <c r="H144" s="1"/>
       <c r="I144" s="1"/>
       <c r="J144" s="116" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K144" s="43"/>
       <c r="L144" s="2"/>
@@ -7558,7 +7568,7 @@
       <c r="AC144" s="1"/>
       <c r="AD144" s="1"/>
     </row>
-    <row r="145" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:30" ht="102" x14ac:dyDescent="0.3">
       <c r="A145" s="27"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -7569,7 +7579,7 @@
       <c r="H145" s="1"/>
       <c r="I145" s="1"/>
       <c r="J145" s="116" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K145" s="43"/>
       <c r="L145" s="2"/>
@@ -7594,7 +7604,7 @@
       <c r="AC145" s="1"/>
       <c r="AD145" s="1"/>
     </row>
-    <row r="146" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A146" s="27"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -7605,7 +7615,7 @@
       <c r="H146" s="1"/>
       <c r="I146" s="1"/>
       <c r="J146" s="116" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="K146" s="43"/>
       <c r="L146" s="2"/>
@@ -7614,9 +7624,7 @@
       </c>
       <c r="N146" s="2"/>
       <c r="O146" s="2"/>
-      <c r="P146" s="45">
-        <v>1</v>
-      </c>
+      <c r="P146" s="45"/>
       <c r="Q146" s="3"/>
       <c r="R146" s="1"/>
       <c r="S146" s="1"/>
@@ -7632,7 +7640,7 @@
       <c r="AC146" s="1"/>
       <c r="AD146" s="1"/>
     </row>
-    <row r="147" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A147" s="27"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -7643,18 +7651,18 @@
       <c r="H147" s="1"/>
       <c r="I147" s="1"/>
       <c r="J147" s="116" t="s">
-        <v>57</v>
+        <v>138</v>
       </c>
       <c r="K147" s="43"/>
-      <c r="L147" s="2">
-        <v>1</v>
-      </c>
+      <c r="L147" s="2"/>
       <c r="M147" s="2">
         <v>1</v>
       </c>
       <c r="N147" s="2"/>
       <c r="O147" s="2"/>
-      <c r="P147" s="45"/>
+      <c r="P147" s="45">
+        <v>1</v>
+      </c>
       <c r="Q147" s="3"/>
       <c r="R147" s="1"/>
       <c r="S147" s="1"/>
@@ -7681,13 +7689,15 @@
       <c r="H148" s="1"/>
       <c r="I148" s="1"/>
       <c r="J148" s="116" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="K148" s="43"/>
       <c r="L148" s="2">
         <v>1</v>
       </c>
-      <c r="M148" s="2"/>
+      <c r="M148" s="2">
+        <v>1</v>
+      </c>
       <c r="N148" s="2"/>
       <c r="O148" s="2"/>
       <c r="P148" s="45"/>
@@ -7706,7 +7716,7 @@
       <c r="AC148" s="1"/>
       <c r="AD148" s="1"/>
     </row>
-    <row r="149" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="27"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -7717,17 +7727,15 @@
       <c r="H149" s="1"/>
       <c r="I149" s="1"/>
       <c r="J149" s="116" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K149" s="43"/>
-      <c r="L149" s="2"/>
+      <c r="L149" s="2">
+        <v>1</v>
+      </c>
       <c r="M149" s="2"/>
-      <c r="N149" s="2">
-        <v>1</v>
-      </c>
-      <c r="O149" s="2">
-        <v>1</v>
-      </c>
+      <c r="N149" s="2"/>
+      <c r="O149" s="2"/>
       <c r="P149" s="45"/>
       <c r="Q149" s="3"/>
       <c r="R149" s="1"/>
@@ -7744,7 +7752,7 @@
       <c r="AC149" s="1"/>
       <c r="AD149" s="1"/>
     </row>
-    <row r="150" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A150" s="27"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -7754,14 +7762,18 @@
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
       <c r="I150" s="1"/>
-      <c r="J150" s="34" t="s">
-        <v>62</v>
+      <c r="J150" s="116" t="s">
+        <v>128</v>
       </c>
       <c r="K150" s="43"/>
       <c r="L150" s="2"/>
       <c r="M150" s="2"/>
-      <c r="N150" s="2"/>
-      <c r="O150" s="2"/>
+      <c r="N150" s="2">
+        <v>1</v>
+      </c>
+      <c r="O150" s="2">
+        <v>1</v>
+      </c>
       <c r="P150" s="45"/>
       <c r="Q150" s="3"/>
       <c r="R150" s="1"/>
@@ -7778,33 +7790,25 @@
       <c r="AC150" s="1"/>
       <c r="AD150" s="1"/>
     </row>
-    <row r="151" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="27"/>
-      <c r="B151" s="18"/>
-      <c r="C151" s="18"/>
-      <c r="D151" s="18"/>
-      <c r="E151" s="18"/>
-      <c r="F151" s="128" t="s">
-        <v>159</v>
-      </c>
-      <c r="G151" s="49"/>
-      <c r="H151" s="112" t="s">
-        <v>160</v>
-      </c>
-      <c r="I151" s="173" t="s">
-        <v>268</v>
-      </c>
-      <c r="J151" s="112" t="s">
-        <v>162</v>
-      </c>
-      <c r="K151" s="42"/>
-      <c r="L151" s="24"/>
-      <c r="M151" s="24"/>
-      <c r="N151" s="24"/>
-      <c r="O151" s="24"/>
-      <c r="P151" s="44">
-        <v>1</v>
-      </c>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+      <c r="J151" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="K151" s="43"/>
+      <c r="L151" s="2"/>
+      <c r="M151" s="2"/>
+      <c r="N151" s="2"/>
+      <c r="O151" s="2"/>
+      <c r="P151" s="45"/>
       <c r="Q151" s="3"/>
       <c r="R151" s="1"/>
       <c r="S151" s="1"/>
@@ -7820,25 +7824,31 @@
       <c r="AC151" s="1"/>
       <c r="AD151" s="1"/>
     </row>
-    <row r="152" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A152" s="27"/>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
-      <c r="D152" s="1"/>
-      <c r="E152" s="1"/>
-      <c r="H152" s="17"/>
-      <c r="I152" s="17"/>
-      <c r="J152" s="116" t="s">
-        <v>121</v>
-      </c>
-      <c r="K152" s="43"/>
-      <c r="L152" s="2"/>
-      <c r="M152" s="2"/>
-      <c r="N152" s="2"/>
-      <c r="O152" s="2">
-        <v>1</v>
-      </c>
-      <c r="P152" s="45">
+      <c r="B152" s="18"/>
+      <c r="C152" s="18"/>
+      <c r="D152" s="18"/>
+      <c r="E152" s="18"/>
+      <c r="F152" s="128" t="s">
+        <v>159</v>
+      </c>
+      <c r="G152" s="49"/>
+      <c r="H152" s="112" t="s">
+        <v>160</v>
+      </c>
+      <c r="I152" s="173" t="s">
+        <v>161</v>
+      </c>
+      <c r="J152" s="112" t="s">
+        <v>162</v>
+      </c>
+      <c r="K152" s="42"/>
+      <c r="L152" s="24"/>
+      <c r="M152" s="24"/>
+      <c r="N152" s="24"/>
+      <c r="O152" s="24"/>
+      <c r="P152" s="44">
         <v>1</v>
       </c>
       <c r="Q152" s="3"/>
@@ -7862,12 +7872,10 @@
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
-      <c r="F153" s="1"/>
-      <c r="G153" s="1"/>
-      <c r="H153" s="1"/>
-      <c r="I153" s="1"/>
+      <c r="H153" s="17"/>
+      <c r="I153" s="17"/>
       <c r="J153" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K153" s="43"/>
       <c r="L153" s="2"/>
@@ -7876,7 +7884,9 @@
       <c r="O153" s="2">
         <v>1</v>
       </c>
-      <c r="P153" s="45"/>
+      <c r="P153" s="45">
+        <v>1</v>
+      </c>
       <c r="Q153" s="3"/>
       <c r="R153" s="1"/>
       <c r="S153" s="1"/>
@@ -7903,16 +7913,16 @@
       <c r="H154" s="1"/>
       <c r="I154" s="1"/>
       <c r="J154" s="116" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="K154" s="43"/>
       <c r="L154" s="2"/>
       <c r="M154" s="2"/>
       <c r="N154" s="2"/>
-      <c r="O154" s="2"/>
-      <c r="P154" s="45">
-        <v>1</v>
-      </c>
+      <c r="O154" s="2">
+        <v>1</v>
+      </c>
+      <c r="P154" s="45"/>
       <c r="Q154" s="3"/>
       <c r="R154" s="1"/>
       <c r="S154" s="1"/>
@@ -7939,7 +7949,7 @@
       <c r="H155" s="1"/>
       <c r="I155" s="1"/>
       <c r="J155" s="116" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K155" s="43"/>
       <c r="L155" s="2"/>
@@ -7975,16 +7985,16 @@
       <c r="H156" s="1"/>
       <c r="I156" s="1"/>
       <c r="J156" s="116" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="K156" s="43"/>
-      <c r="L156" s="2">
-        <v>1</v>
-      </c>
+      <c r="L156" s="2"/>
       <c r="M156" s="2"/>
       <c r="N156" s="2"/>
       <c r="O156" s="2"/>
-      <c r="P156" s="45"/>
+      <c r="P156" s="45">
+        <v>1</v>
+      </c>
       <c r="Q156" s="3"/>
       <c r="R156" s="1"/>
       <c r="S156" s="1"/>
@@ -8000,7 +8010,7 @@
       <c r="AC156" s="1"/>
       <c r="AD156" s="1"/>
     </row>
-    <row r="157" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="27"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -8011,17 +8021,15 @@
       <c r="H157" s="1"/>
       <c r="I157" s="1"/>
       <c r="J157" s="116" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K157" s="43"/>
-      <c r="L157" s="2"/>
+      <c r="L157" s="2">
+        <v>1</v>
+      </c>
       <c r="M157" s="2"/>
-      <c r="N157" s="2">
-        <v>1</v>
-      </c>
-      <c r="O157" s="2">
-        <v>1</v>
-      </c>
+      <c r="N157" s="2"/>
+      <c r="O157" s="2"/>
       <c r="P157" s="45"/>
       <c r="Q157" s="3"/>
       <c r="R157" s="1"/>
@@ -8038,26 +8046,30 @@
       <c r="AC157" s="1"/>
       <c r="AD157" s="1"/>
     </row>
-    <row r="158" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="69"/>
-      <c r="B158" s="61"/>
-      <c r="C158" s="61"/>
-      <c r="D158" s="61"/>
-      <c r="E158" s="61"/>
-      <c r="F158" s="61"/>
-      <c r="G158" s="61"/>
-      <c r="H158" s="61"/>
-      <c r="I158" s="18"/>
+    <row r="158" spans="1:30" ht="40.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A158" s="27"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="1"/>
+      <c r="D158" s="1"/>
+      <c r="E158" s="1"/>
+      <c r="F158" s="1"/>
+      <c r="G158" s="1"/>
+      <c r="H158" s="1"/>
+      <c r="I158" s="1"/>
       <c r="J158" s="116" t="s">
-        <v>62</v>
-      </c>
-      <c r="K158" s="65"/>
-      <c r="L158" s="66"/>
-      <c r="M158" s="66"/>
-      <c r="N158" s="66"/>
-      <c r="O158" s="66"/>
-      <c r="P158" s="67"/>
-      <c r="Q158" s="68"/>
+        <v>128</v>
+      </c>
+      <c r="K158" s="43"/>
+      <c r="L158" s="2"/>
+      <c r="M158" s="2"/>
+      <c r="N158" s="2">
+        <v>1</v>
+      </c>
+      <c r="O158" s="2">
+        <v>1</v>
+      </c>
+      <c r="P158" s="45"/>
+      <c r="Q158" s="3"/>
       <c r="R158" s="1"/>
       <c r="S158" s="1"/>
       <c r="T158" s="1"/>
@@ -8072,36 +8084,26 @@
       <c r="AC158" s="1"/>
       <c r="AD158" s="1"/>
     </row>
-    <row r="159" spans="1:30" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="27"/>
-      <c r="B159" s="1"/>
-      <c r="C159" s="1"/>
-      <c r="D159" s="1"/>
-      <c r="E159" s="1"/>
-      <c r="F159" s="197" t="s">
-        <v>43</v>
-      </c>
-      <c r="G159" s="1"/>
-      <c r="H159" s="112" t="s">
-        <v>163</v>
-      </c>
-      <c r="I159" s="173" t="s">
-        <v>161</v>
-      </c>
-      <c r="J159" s="112" t="s">
-        <v>120</v>
-      </c>
-      <c r="K159" s="42"/>
-      <c r="L159" s="24"/>
-      <c r="M159" s="24"/>
-      <c r="N159" s="24"/>
-      <c r="O159" s="24">
-        <v>1</v>
-      </c>
-      <c r="P159" s="44">
-        <v>1</v>
-      </c>
-      <c r="Q159" s="3"/>
+    <row r="159" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="69"/>
+      <c r="B159" s="61"/>
+      <c r="C159" s="61"/>
+      <c r="D159" s="61"/>
+      <c r="E159" s="61"/>
+      <c r="F159" s="61"/>
+      <c r="G159" s="61"/>
+      <c r="H159" s="61"/>
+      <c r="I159" s="18"/>
+      <c r="J159" s="116" t="s">
+        <v>62</v>
+      </c>
+      <c r="K159" s="65"/>
+      <c r="L159" s="66"/>
+      <c r="M159" s="66"/>
+      <c r="N159" s="66"/>
+      <c r="O159" s="66"/>
+      <c r="P159" s="67"/>
+      <c r="Q159" s="68"/>
       <c r="R159" s="1"/>
       <c r="S159" s="1"/>
       <c r="T159" s="1"/>
@@ -8122,23 +8124,27 @@
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
       <c r="E160" s="1"/>
-      <c r="F160" s="1"/>
+      <c r="F160" s="197" t="s">
+        <v>43</v>
+      </c>
       <c r="G160" s="1"/>
-      <c r="H160" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="I160" s="12"/>
-      <c r="J160" s="116" t="s">
-        <v>121</v>
-      </c>
-      <c r="K160" s="43"/>
-      <c r="L160" s="2"/>
-      <c r="M160" s="2"/>
-      <c r="N160" s="2"/>
-      <c r="O160" s="2">
-        <v>1</v>
-      </c>
-      <c r="P160" s="45">
+      <c r="H160" s="112" t="s">
+        <v>163</v>
+      </c>
+      <c r="I160" s="173" t="s">
+        <v>164</v>
+      </c>
+      <c r="J160" s="112" t="s">
+        <v>120</v>
+      </c>
+      <c r="K160" s="42"/>
+      <c r="L160" s="24"/>
+      <c r="M160" s="24"/>
+      <c r="N160" s="24"/>
+      <c r="O160" s="24">
+        <v>1</v>
+      </c>
+      <c r="P160" s="44">
         <v>1</v>
       </c>
       <c r="Q160" s="3"/>
@@ -8156,7 +8162,7 @@
       <c r="AC160" s="1"/>
       <c r="AD160" s="1"/>
     </row>
-    <row r="161" spans="1:30" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:30" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="27"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -8164,18 +8170,20 @@
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
-      <c r="H161" s="12"/>
+      <c r="H161" s="12" t="s">
+        <v>137</v>
+      </c>
       <c r="I161" s="12"/>
       <c r="J161" s="116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K161" s="43"/>
       <c r="L161" s="2"/>
-      <c r="M161" s="2">
-        <v>1</v>
-      </c>
+      <c r="M161" s="2"/>
       <c r="N161" s="2"/>
-      <c r="O161" s="2"/>
+      <c r="O161" s="2">
+        <v>1</v>
+      </c>
       <c r="P161" s="45">
         <v>1</v>
       </c>
@@ -8194,7 +8202,7 @@
       <c r="AC161" s="1"/>
       <c r="AD161" s="1"/>
     </row>
-    <row r="162" spans="1:30" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:30" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="27"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -8205,18 +8213,18 @@
       <c r="H162" s="12"/>
       <c r="I162" s="12"/>
       <c r="J162" s="116" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K162" s="43"/>
       <c r="L162" s="2"/>
-      <c r="M162" s="2"/>
-      <c r="N162" s="2">
-        <v>1</v>
-      </c>
-      <c r="O162" s="2">
-        <v>1</v>
-      </c>
-      <c r="P162" s="45"/>
+      <c r="M162" s="2">
+        <v>1</v>
+      </c>
+      <c r="N162" s="2"/>
+      <c r="O162" s="2"/>
+      <c r="P162" s="45">
+        <v>1</v>
+      </c>
       <c r="Q162" s="3"/>
       <c r="R162" s="1"/>
       <c r="S162" s="1"/>
@@ -8232,7 +8240,7 @@
       <c r="AC162" s="1"/>
       <c r="AD162" s="1"/>
     </row>
-    <row r="163" spans="1:30" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:30" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="27"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -8243,16 +8251,18 @@
       <c r="H163" s="12"/>
       <c r="I163" s="12"/>
       <c r="J163" s="116" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="K163" s="43"/>
       <c r="L163" s="2"/>
       <c r="M163" s="2"/>
-      <c r="N163" s="2"/>
-      <c r="O163" s="2"/>
-      <c r="P163" s="45">
-        <v>1</v>
-      </c>
+      <c r="N163" s="2">
+        <v>1</v>
+      </c>
+      <c r="O163" s="2">
+        <v>1</v>
+      </c>
+      <c r="P163" s="45"/>
       <c r="Q163" s="3"/>
       <c r="R163" s="1"/>
       <c r="S163" s="1"/>
@@ -8268,7 +8278,7 @@
       <c r="AC163" s="1"/>
       <c r="AD163" s="1"/>
     </row>
-    <row r="164" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:30" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="27"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -8279,7 +8289,7 @@
       <c r="H164" s="12"/>
       <c r="I164" s="12"/>
       <c r="J164" s="116" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="K164" s="43"/>
       <c r="L164" s="2"/>
@@ -8304,7 +8314,7 @@
       <c r="AC164" s="1"/>
       <c r="AD164" s="1"/>
     </row>
-    <row r="165" spans="1:30" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="27"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -8315,17 +8325,13 @@
       <c r="H165" s="12"/>
       <c r="I165" s="12"/>
       <c r="J165" s="116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K165" s="43"/>
       <c r="L165" s="2"/>
       <c r="M165" s="2"/>
-      <c r="N165" s="2">
-        <v>1</v>
-      </c>
-      <c r="O165" s="2">
-        <v>1</v>
-      </c>
+      <c r="N165" s="2"/>
+      <c r="O165" s="2"/>
       <c r="P165" s="45">
         <v>1</v>
       </c>
@@ -8355,16 +8361,20 @@
       <c r="H166" s="12"/>
       <c r="I166" s="12"/>
       <c r="J166" s="116" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K166" s="43"/>
-      <c r="L166" s="2">
-        <v>1</v>
-      </c>
+      <c r="L166" s="2"/>
       <c r="M166" s="2"/>
-      <c r="N166" s="2"/>
-      <c r="O166" s="2"/>
-      <c r="P166" s="45"/>
+      <c r="N166" s="2">
+        <v>1</v>
+      </c>
+      <c r="O166" s="2">
+        <v>1</v>
+      </c>
+      <c r="P166" s="45">
+        <v>1</v>
+      </c>
       <c r="Q166" s="3"/>
       <c r="R166" s="1"/>
       <c r="S166" s="1"/>
@@ -8380,7 +8390,7 @@
       <c r="AC166" s="1"/>
       <c r="AD166" s="1"/>
     </row>
-    <row r="167" spans="1:30" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:30" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="27"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -8390,18 +8400,16 @@
       <c r="G167" s="1"/>
       <c r="H167" s="12"/>
       <c r="I167" s="12"/>
-      <c r="J167" s="13" t="s">
-        <v>139</v>
+      <c r="J167" s="116" t="s">
+        <v>128</v>
       </c>
       <c r="K167" s="43"/>
-      <c r="L167" s="2"/>
+      <c r="L167" s="2">
+        <v>1</v>
+      </c>
       <c r="M167" s="2"/>
-      <c r="N167" s="2">
-        <v>1</v>
-      </c>
-      <c r="O167" s="2">
-        <v>1</v>
-      </c>
+      <c r="N167" s="2"/>
+      <c r="O167" s="2"/>
       <c r="P167" s="45"/>
       <c r="Q167" s="3"/>
       <c r="R167" s="1"/>
@@ -8418,7 +8426,7 @@
       <c r="AC167" s="1"/>
       <c r="AD167" s="1"/>
     </row>
-    <row r="168" spans="1:30" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:30" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="27"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -8428,14 +8436,18 @@
       <c r="G168" s="1"/>
       <c r="H168" s="12"/>
       <c r="I168" s="12"/>
-      <c r="J168" s="116" t="s">
-        <v>132</v>
+      <c r="J168" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="K168" s="43"/>
       <c r="L168" s="2"/>
       <c r="M168" s="2"/>
-      <c r="N168" s="2"/>
-      <c r="O168" s="2"/>
+      <c r="N168" s="2">
+        <v>1</v>
+      </c>
+      <c r="O168" s="2">
+        <v>1</v>
+      </c>
       <c r="P168" s="45"/>
       <c r="Q168" s="3"/>
       <c r="R168" s="1"/>
@@ -8452,7 +8464,7 @@
       <c r="AC168" s="1"/>
       <c r="AD168" s="1"/>
     </row>
-    <row r="169" spans="1:30" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:30" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="27"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -8463,16 +8475,14 @@
       <c r="H169" s="12"/>
       <c r="I169" s="12"/>
       <c r="J169" s="116" t="s">
-        <v>133</v>
-      </c>
-      <c r="K169" s="142"/>
-      <c r="L169" s="143"/>
-      <c r="M169" s="143"/>
-      <c r="N169" s="143"/>
-      <c r="O169" s="143"/>
-      <c r="P169" s="144" t="s">
-        <v>137</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="K169" s="43"/>
+      <c r="L169" s="2"/>
+      <c r="M169" s="2"/>
+      <c r="N169" s="2"/>
+      <c r="O169" s="2"/>
+      <c r="P169" s="45"/>
       <c r="Q169" s="3"/>
       <c r="R169" s="1"/>
       <c r="S169" s="1"/>
@@ -8488,7 +8498,7 @@
       <c r="AC169" s="1"/>
       <c r="AD169" s="1"/>
     </row>
-    <row r="170" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:30" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="27"/>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -8498,15 +8508,17 @@
       <c r="G170" s="1"/>
       <c r="H170" s="12"/>
       <c r="I170" s="12"/>
-      <c r="J170" s="34" t="s">
-        <v>62</v>
+      <c r="J170" s="116" t="s">
+        <v>133</v>
       </c>
       <c r="K170" s="142"/>
       <c r="L170" s="143"/>
       <c r="M170" s="143"/>
       <c r="N170" s="143"/>
       <c r="O170" s="143"/>
-      <c r="P170" s="144"/>
+      <c r="P170" s="144" t="s">
+        <v>137</v>
+      </c>
       <c r="Q170" s="3"/>
       <c r="R170" s="1"/>
       <c r="S170" s="1"/>
@@ -8522,97 +8534,97 @@
       <c r="AC170" s="1"/>
       <c r="AD170" s="1"/>
     </row>
-    <row r="171" spans="1:30" s="73" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="29">
+    <row r="171" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="27"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="1"/>
+      <c r="H171" s="12"/>
+      <c r="I171" s="12"/>
+      <c r="J171" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="K171" s="142"/>
+      <c r="L171" s="143"/>
+      <c r="M171" s="143"/>
+      <c r="N171" s="143"/>
+      <c r="O171" s="143"/>
+      <c r="P171" s="144"/>
+      <c r="Q171" s="3"/>
+      <c r="R171" s="1"/>
+      <c r="S171" s="1"/>
+      <c r="T171" s="1"/>
+      <c r="U171" s="1"/>
+      <c r="V171" s="1"/>
+      <c r="W171" s="1"/>
+      <c r="X171" s="1"/>
+      <c r="Y171" s="1"/>
+      <c r="Z171" s="1"/>
+      <c r="AA171" s="1"/>
+      <c r="AB171" s="1"/>
+      <c r="AC171" s="1"/>
+      <c r="AD171" s="1"/>
+    </row>
+    <row r="172" spans="1:30" s="73" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="29">
         <v>5</v>
       </c>
-      <c r="B171" s="128" t="s">
-        <v>164</v>
-      </c>
-      <c r="C171" s="49">
+      <c r="B172" s="128" t="s">
+        <v>165</v>
+      </c>
+      <c r="C172" s="49">
         <v>3</v>
       </c>
-      <c r="D171" s="91" t="s">
-        <v>165</v>
-      </c>
-      <c r="E171" s="112" t="s">
+      <c r="D172" s="91" t="s">
         <v>166</v>
       </c>
-      <c r="F171" s="26"/>
-      <c r="G171" s="26"/>
-      <c r="H171" s="26"/>
-      <c r="I171" s="26"/>
-      <c r="J171" s="112" t="s">
+      <c r="E172" s="112" t="s">
         <v>167</v>
       </c>
-      <c r="K171" s="42"/>
-      <c r="L171" s="24"/>
-      <c r="M171" s="24"/>
-      <c r="N171" s="24"/>
-      <c r="O171" s="24"/>
-      <c r="P171" s="44"/>
-      <c r="Q171" s="25"/>
-      <c r="R171" s="26"/>
-      <c r="S171" s="26"/>
-      <c r="T171" s="26"/>
-      <c r="U171" s="26"/>
-      <c r="V171" s="26"/>
-      <c r="W171" s="26"/>
-      <c r="X171" s="26"/>
-      <c r="Y171" s="26"/>
-      <c r="Z171" s="26"/>
-      <c r="AA171" s="26"/>
-      <c r="AB171" s="26"/>
-      <c r="AC171" s="26"/>
-      <c r="AD171" s="26"/>
-    </row>
-    <row r="172" spans="1:30" ht="42" x14ac:dyDescent="0.3">
-      <c r="A172" s="27"/>
-      <c r="B172" s="13"/>
-      <c r="C172" s="13"/>
-      <c r="D172" s="93" t="s">
+      <c r="F172" s="26"/>
+      <c r="G172" s="26"/>
+      <c r="H172" s="26"/>
+      <c r="I172" s="26"/>
+      <c r="J172" s="112" t="s">
         <v>168</v>
       </c>
-      <c r="E172" s="13"/>
-      <c r="F172" s="1"/>
-      <c r="G172" s="1"/>
-      <c r="H172" s="1"/>
-      <c r="I172" s="1"/>
-      <c r="J172" s="34" t="s">
+      <c r="K172" s="42"/>
+      <c r="L172" s="24"/>
+      <c r="M172" s="24"/>
+      <c r="N172" s="24"/>
+      <c r="O172" s="24"/>
+      <c r="P172" s="44"/>
+      <c r="Q172" s="25"/>
+      <c r="R172" s="26"/>
+      <c r="S172" s="26"/>
+      <c r="T172" s="26"/>
+      <c r="U172" s="26"/>
+      <c r="V172" s="26"/>
+      <c r="W172" s="26"/>
+      <c r="X172" s="26"/>
+      <c r="Y172" s="26"/>
+      <c r="Z172" s="26"/>
+      <c r="AA172" s="26"/>
+      <c r="AB172" s="26"/>
+      <c r="AC172" s="26"/>
+      <c r="AD172" s="26"/>
+    </row>
+    <row r="173" spans="1:30" ht="42" x14ac:dyDescent="0.3">
+      <c r="A173" s="27"/>
+      <c r="B173" s="13"/>
+      <c r="C173" s="13"/>
+      <c r="D173" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="K172" s="43"/>
-      <c r="L172" s="2"/>
-      <c r="M172" s="2"/>
-      <c r="N172" s="2"/>
-      <c r="O172" s="2"/>
-      <c r="P172" s="45"/>
-      <c r="Q172" s="3"/>
-      <c r="R172" s="1"/>
-      <c r="S172" s="1"/>
-      <c r="T172" s="1"/>
-      <c r="U172" s="1"/>
-      <c r="V172" s="1"/>
-      <c r="W172" s="1"/>
-      <c r="X172" s="1"/>
-      <c r="Y172" s="1"/>
-      <c r="Z172" s="1"/>
-      <c r="AA172" s="1"/>
-      <c r="AB172" s="1"/>
-      <c r="AC172" s="1"/>
-      <c r="AD172" s="1"/>
-    </row>
-    <row r="173" spans="1:30" ht="51" x14ac:dyDescent="0.3">
-      <c r="A173" s="27"/>
-      <c r="B173" s="1"/>
-      <c r="C173" s="1"/>
-      <c r="D173" s="1"/>
-      <c r="E173" s="1"/>
+      <c r="E173" s="13"/>
       <c r="F173" s="1"/>
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
-      <c r="J173" s="116" t="s">
+      <c r="J173" s="34" t="s">
         <v>170</v>
       </c>
       <c r="K173" s="43"/>
@@ -8636,7 +8648,7 @@
       <c r="AC173" s="1"/>
       <c r="AD173" s="1"/>
     </row>
-    <row r="174" spans="1:30" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:30" ht="51" x14ac:dyDescent="0.3">
       <c r="A174" s="27"/>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -8646,7 +8658,7 @@
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
-      <c r="J174" s="34" t="s">
+      <c r="J174" s="116" t="s">
         <v>171</v>
       </c>
       <c r="K174" s="43"/>
@@ -8670,7 +8682,7 @@
       <c r="AC174" s="1"/>
       <c r="AD174" s="1"/>
     </row>
-    <row r="175" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:30" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A175" s="27"/>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -8680,7 +8692,7 @@
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
-      <c r="J175" s="116" t="s">
+      <c r="J175" s="34" t="s">
         <v>172</v>
       </c>
       <c r="K175" s="43"/>
@@ -8704,7 +8716,7 @@
       <c r="AC175" s="1"/>
       <c r="AD175" s="1"/>
     </row>
-    <row r="176" spans="1:30" ht="42" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A176" s="27"/>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -8714,7 +8726,7 @@
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
       <c r="I176" s="1"/>
-      <c r="J176" s="34" t="s">
+      <c r="J176" s="116" t="s">
         <v>173</v>
       </c>
       <c r="K176" s="43"/>
@@ -8738,7 +8750,7 @@
       <c r="AC176" s="1"/>
       <c r="AD176" s="1"/>
     </row>
-    <row r="177" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:30" ht="42" x14ac:dyDescent="0.3">
       <c r="A177" s="27"/>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -8748,7 +8760,7 @@
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
-      <c r="J177" s="116" t="s">
+      <c r="J177" s="34" t="s">
         <v>174</v>
       </c>
       <c r="K177" s="43"/>
@@ -8772,7 +8784,7 @@
       <c r="AC177" s="1"/>
       <c r="AD177" s="1"/>
     </row>
-    <row r="178" spans="1:30" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:30" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A178" s="27"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -8782,7 +8794,7 @@
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
       <c r="I178" s="1"/>
-      <c r="J178" s="34" t="s">
+      <c r="J178" s="116" t="s">
         <v>175</v>
       </c>
       <c r="K178" s="43"/>
@@ -8806,7 +8818,7 @@
       <c r="AC178" s="1"/>
       <c r="AD178" s="1"/>
     </row>
-    <row r="179" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:30" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A179" s="27"/>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -8816,7 +8828,7 @@
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
       <c r="I179" s="1"/>
-      <c r="J179" s="116" t="s">
+      <c r="J179" s="34" t="s">
         <v>176</v>
       </c>
       <c r="K179" s="43"/>
@@ -8840,7 +8852,7 @@
       <c r="AC179" s="1"/>
       <c r="AD179" s="1"/>
     </row>
-    <row r="180" spans="1:30" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:30" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A180" s="27"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -8850,8 +8862,8 @@
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
       <c r="I180" s="1"/>
-      <c r="J180" s="34" t="s">
-        <v>176</v>
+      <c r="J180" s="116" t="s">
+        <v>177</v>
       </c>
       <c r="K180" s="43"/>
       <c r="L180" s="2"/>
@@ -8885,7 +8897,7 @@
       <c r="H181" s="1"/>
       <c r="I181" s="1"/>
       <c r="J181" s="116" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="K181" s="43"/>
       <c r="L181" s="2"/>
@@ -8919,7 +8931,7 @@
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
       <c r="J182" s="116" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K182" s="43"/>
       <c r="L182" s="2"/>
@@ -8953,7 +8965,7 @@
       <c r="H183" s="1"/>
       <c r="I183" s="1"/>
       <c r="J183" s="116" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K183" s="43"/>
       <c r="L183" s="2"/>
@@ -8987,7 +8999,7 @@
       <c r="H184" s="1"/>
       <c r="I184" s="1"/>
       <c r="J184" s="34" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="K184" s="43"/>
       <c r="L184" s="2"/>
@@ -9021,7 +9033,7 @@
       <c r="H185" s="1"/>
       <c r="I185" s="1"/>
       <c r="J185" s="34" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K185" s="43"/>
       <c r="L185" s="2"/>
@@ -9055,7 +9067,7 @@
       <c r="H186" s="1"/>
       <c r="I186" s="1"/>
       <c r="J186" s="116" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K186" s="43"/>
       <c r="L186" s="2"/>
@@ -9089,7 +9101,7 @@
       <c r="H187" s="1"/>
       <c r="I187" s="1"/>
       <c r="J187" s="34" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K187" s="43"/>
       <c r="L187" s="2"/>
@@ -9123,7 +9135,7 @@
       <c r="H188" s="1"/>
       <c r="I188" s="1"/>
       <c r="J188" s="34" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K188" s="43"/>
       <c r="L188" s="2"/>
@@ -9157,7 +9169,7 @@
       <c r="H189" s="1"/>
       <c r="I189" s="1"/>
       <c r="J189" s="34" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="K189" s="43"/>
       <c r="L189" s="2"/>
@@ -9191,7 +9203,7 @@
       <c r="H190" s="1"/>
       <c r="I190" s="1"/>
       <c r="J190" s="34" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K190" s="43"/>
       <c r="L190" s="2"/>
@@ -9253,7 +9265,7 @@
         <v>6</v>
       </c>
       <c r="B192" s="122" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C192" s="50">
         <v>1</v>
@@ -9267,7 +9279,7 @@
       <c r="H192" s="35"/>
       <c r="I192" s="35"/>
       <c r="J192" s="120" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="K192" s="43"/>
       <c r="L192" s="36"/>
@@ -9299,7 +9311,7 @@
       <c r="H193" s="35"/>
       <c r="I193" s="35"/>
       <c r="J193" s="34" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K193" s="43"/>
       <c r="L193" s="36"/>
@@ -9332,7 +9344,7 @@
       <c r="H194" s="13"/>
       <c r="I194" s="13"/>
       <c r="J194" s="116" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K194" s="43"/>
       <c r="L194" s="2"/>
@@ -9365,7 +9377,7 @@
       <c r="H195" s="13"/>
       <c r="I195" s="13"/>
       <c r="J195" s="116" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K195" s="43"/>
       <c r="L195" s="2"/>
@@ -9398,7 +9410,7 @@
       <c r="H196" s="13"/>
       <c r="I196" s="13"/>
       <c r="J196" s="34" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K196" s="43"/>
       <c r="L196" s="2"/>
@@ -9431,7 +9443,7 @@
       <c r="H197" s="13"/>
       <c r="I197" s="13"/>
       <c r="J197" s="116" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K197" s="43"/>
       <c r="L197" s="2"/>
@@ -9465,7 +9477,7 @@
       <c r="H198" s="70"/>
       <c r="I198" s="70"/>
       <c r="J198" s="118" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K198" s="65"/>
       <c r="L198" s="66"/>
@@ -9493,7 +9505,7 @@
         <v>7</v>
       </c>
       <c r="B199" s="122" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C199" s="50"/>
       <c r="D199" s="50"/>
@@ -9503,7 +9515,7 @@
       <c r="H199" s="35"/>
       <c r="I199" s="35"/>
       <c r="J199" s="35" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="K199" s="43"/>
       <c r="L199" s="36"/>
@@ -9536,7 +9548,7 @@
       <c r="H200" s="13"/>
       <c r="I200" s="13"/>
       <c r="J200" s="13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="K200" s="43"/>
       <c r="L200" s="2"/>
@@ -9570,7 +9582,7 @@
       <c r="H201" s="70"/>
       <c r="I201" s="70"/>
       <c r="J201" s="118" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K201" s="65"/>
       <c r="L201" s="66"/>
@@ -9598,7 +9610,7 @@
         <v>8</v>
       </c>
       <c r="B202" s="115" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C202" s="62"/>
       <c r="D202" s="161">
@@ -9610,7 +9622,7 @@
       <c r="H202" s="35"/>
       <c r="I202" s="35"/>
       <c r="J202" s="120" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="K202" s="43"/>
       <c r="L202" s="36"/>
@@ -9638,14 +9650,14 @@
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="93" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E203" s="1"/>
       <c r="G203" s="13"/>
       <c r="H203" s="13"/>
       <c r="I203" s="13"/>
       <c r="J203" s="116" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K203" s="43"/>
       <c r="L203" s="2"/>
@@ -9678,7 +9690,7 @@
       <c r="H204" s="13"/>
       <c r="I204" s="13"/>
       <c r="J204" s="116" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K204" s="43"/>
       <c r="L204" s="2"/>
@@ -9770,7 +9782,7 @@
     <row r="207" spans="1:30" s="16" customFormat="1" ht="15.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="29"/>
       <c r="B207" s="203" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C207" s="204"/>
       <c r="D207" s="204"/>
@@ -9804,7 +9816,7 @@
     <row r="208" spans="1:30" ht="12.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="27"/>
       <c r="B208" s="130" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C208" s="78"/>
       <c r="D208" s="78"/>
@@ -9872,7 +9884,7 @@
         <v>9</v>
       </c>
       <c r="B210" s="114" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C210" s="52"/>
       <c r="D210" s="52"/>
@@ -9914,7 +9926,7 @@
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E211" s="1"/>
       <c r="F211" s="116"/>
@@ -9960,7 +9972,7 @@
       <c r="H212" s="13"/>
       <c r="I212" s="13"/>
       <c r="J212" s="116" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="K212" s="43"/>
       <c r="L212" s="2"/>
@@ -9998,7 +10010,7 @@
       <c r="H213" s="13"/>
       <c r="I213" s="13"/>
       <c r="J213" s="116" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K213" s="43"/>
       <c r="L213" s="2"/>
@@ -10034,7 +10046,7 @@
       <c r="H214" s="19"/>
       <c r="I214" s="19"/>
       <c r="J214" s="131" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="K214" s="43"/>
       <c r="L214" s="2"/>
@@ -10068,7 +10080,7 @@
       <c r="H215" s="19"/>
       <c r="I215" s="19"/>
       <c r="J215" s="72" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="K215" s="43"/>
       <c r="L215" s="2"/>
@@ -10096,7 +10108,7 @@
         <v>10</v>
       </c>
       <c r="B216" s="52" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C216" s="57"/>
       <c r="D216" s="57"/>
@@ -10106,7 +10118,7 @@
       <c r="H216" s="31"/>
       <c r="I216" s="31"/>
       <c r="J216" s="31" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="K216" s="42"/>
       <c r="L216" s="24"/>
@@ -10144,7 +10156,7 @@
       <c r="H217" s="13"/>
       <c r="I217" s="13"/>
       <c r="J217" s="116" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="K217" s="43">
         <v>1</v>
@@ -10186,7 +10198,7 @@
       <c r="H218" s="13"/>
       <c r="I218" s="13"/>
       <c r="J218" s="13" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="K218" s="43"/>
       <c r="L218" s="2">
@@ -10214,7 +10226,7 @@
     <row r="219" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A219" s="29"/>
       <c r="B219" s="205" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C219" s="206"/>
       <c r="D219" s="206"/>
@@ -10250,7 +10262,7 @@
         <v>12</v>
       </c>
       <c r="B220" s="132" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C220" s="55"/>
       <c r="D220" s="55"/>
@@ -10260,7 +10272,7 @@
       <c r="H220" s="34"/>
       <c r="I220" s="34"/>
       <c r="J220" s="39" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="K220" s="43"/>
       <c r="L220" s="2"/>
@@ -10294,7 +10306,7 @@
       <c r="H221" s="34"/>
       <c r="I221" s="34"/>
       <c r="J221" s="40" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="K221" s="43"/>
       <c r="L221" s="2"/>
@@ -10328,7 +10340,7 @@
       <c r="H222" s="18"/>
       <c r="I222" s="18"/>
       <c r="J222" s="104" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="K222" s="43"/>
       <c r="L222" s="2"/>
@@ -10356,13 +10368,13 @@
         <v>13</v>
       </c>
       <c r="B223" s="132" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C223" s="55"/>
       <c r="D223" s="55"/>
       <c r="E223" s="55"/>
       <c r="F223" s="41" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G223" s="59"/>
       <c r="H223" s="59"/>
@@ -10394,13 +10406,13 @@
         <v>14</v>
       </c>
       <c r="B224" s="134" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C224" s="56"/>
       <c r="D224" s="56"/>
       <c r="E224" s="56"/>
       <c r="F224" s="138" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G224" s="18"/>
       <c r="H224" s="18"/>
@@ -10432,7 +10444,7 @@
         <v>15</v>
       </c>
       <c r="B225" s="134" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C225" s="56"/>
       <c r="D225" s="56"/>
@@ -10468,7 +10480,7 @@
         <v>16</v>
       </c>
       <c r="B226" s="134" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C226" s="56"/>
       <c r="D226" s="56"/>
@@ -10478,7 +10490,7 @@
       <c r="H226" s="35"/>
       <c r="I226" s="35"/>
       <c r="J226" s="136" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="K226" s="43"/>
       <c r="L226" s="2"/>
@@ -10512,7 +10524,7 @@
       <c r="H227" s="35"/>
       <c r="I227" s="35"/>
       <c r="J227" s="137" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="K227" s="43"/>
       <c r="L227" s="2"/>
@@ -10546,7 +10558,7 @@
       <c r="H228" s="35"/>
       <c r="I228" s="35"/>
       <c r="J228" s="137" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="K228" s="43"/>
       <c r="L228" s="2"/>
@@ -10580,7 +10592,7 @@
       <c r="H229" s="35"/>
       <c r="I229" s="35"/>
       <c r="J229" s="137" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="K229" s="43"/>
       <c r="L229" s="2"/>
@@ -10614,7 +10626,7 @@
       <c r="H230" s="35"/>
       <c r="I230" s="35"/>
       <c r="J230" s="137" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="K230" s="43"/>
       <c r="L230" s="2"/>
@@ -10662,15 +10674,15 @@
       </c>
       <c r="N231" s="24">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O231" s="24">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P231" s="44">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q231" s="25"/>
       <c r="R231" s="1"/>
@@ -10724,15 +10736,15 @@
         <v>17</v>
       </c>
       <c r="B233" s="135" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C233" s="26"/>
       <c r="D233" s="26"/>
       <c r="E233" s="97" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F233" s="126" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G233" s="26"/>
       <c r="H233" s="26"/>
@@ -10766,7 +10778,7 @@
       <c r="D234" s="61"/>
       <c r="E234" s="61"/>
       <c r="F234" s="107" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="G234" s="61"/>
       <c r="I234" s="18"/>
@@ -10797,13 +10809,13 @@
         <v>18</v>
       </c>
       <c r="B235" s="167" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C235" s="168"/>
       <c r="D235" s="169"/>
       <c r="E235" s="169"/>
       <c r="F235" s="191" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G235" s="1"/>
       <c r="H235" s="1"/>
@@ -10867,12 +10879,12 @@
         <v>19</v>
       </c>
       <c r="B237" s="135" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C237" s="26"/>
       <c r="D237" s="73"/>
       <c r="E237" s="193" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F237" s="170" t="s">
         <v>137</v>
@@ -10908,10 +10920,10 @@
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
       <c r="E238" s="159" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F238" s="192" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="G238" s="1"/>
       <c r="H238" s="1"/>
@@ -10945,7 +10957,7 @@
       <c r="D239" s="1"/>
       <c r="E239" s="1"/>
       <c r="F239" s="133" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G239" s="1"/>
       <c r="H239" s="1"/>
@@ -10977,11 +10989,11 @@
         <v>20</v>
       </c>
       <c r="B240" s="109" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C240" s="1"/>
       <c r="D240" s="93" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E240" s="1"/>
       <c r="F240" s="1"/>
@@ -11013,7 +11025,7 @@
     <row r="241" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="27"/>
       <c r="B241" s="171" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
@@ -11047,7 +11059,7 @@
     <row r="242" spans="1:30" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="27"/>
       <c r="B242" s="171" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C242" s="1"/>
       <c r="D242" s="1"/>
@@ -11081,7 +11093,7 @@
     <row r="243" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="27"/>
       <c r="B243" s="108" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C243" s="1"/>
       <c r="D243" s="1"/>
@@ -11302,14 +11314,14 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="208" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B1" s="208"/>
       <c r="C1" s="21" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D1" s="207" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E1" s="207"/>
       <c r="F1" s="22"/>
@@ -11317,68 +11329,68 @@
     </row>
     <row r="2" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A2" s="110" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B2" s="105" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C2" s="189" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" s="110" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B3" s="105" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C3" s="190" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" s="111" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B4" s="105" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C4" s="190" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="111" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B5" s="106" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C5" s="190" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A6" s="110" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B6" s="105" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C6" s="190" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="111" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B7" s="105" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C7" s="190" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -11392,6 +11404,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA421E502B73EC48B7C481B02707A95D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a8e395bb2bcb17e943266a860489f057">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a834da9-6c01-4b0d-9854-214ab0844664" xmlns:ns3="3e128f30-cef5-496e-8ae1-acf69bdb7a7e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9b1084d163ef6a9ae7f6b3d13802deaa" ns2:_="" ns3:_="">
     <xsd:import namespace="1a834da9-6c01-4b0d-9854-214ab0844664"/>
@@ -11646,7 +11667,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a834da9-6c01-4b0d-9854-214ab0844664">
@@ -11657,16 +11678,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8BE695-F061-495A-A060-7569CE2A6C93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81CDBFC0-0126-4DB7-8868-40859C987D1F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11685,27 +11705,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{826F9CCE-BEBF-4C0A-A820-CB0577938037}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="1a834da9-6c01-4b0d-9854-214ab0844664"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="3e128f30-cef5-496e-8ae1-acf69bdb7a7e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C8BE695-F061-495A-A060-7569CE2A6C93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>